<commit_message>
Completed separate context & refactoring
</commit_message>
<xml_diff>
--- a/dataset/testing.xlsx
+++ b/dataset/testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajed/PycharmProjects/Study-on-ChatGPT/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13270BA6-ED78-9449-B064-41E94A618A58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3AC808-969D-9341-B038-12D09E06F3AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="760" windowWidth="28040" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="24">
   <si>
     <t>id</t>
   </si>
@@ -32,6 +32,12 @@
   </si>
   <si>
     <t>question</t>
+  </si>
+  <si>
+    <t>answer (shared_context)</t>
+  </si>
+  <si>
+    <t>answer (separate_context)</t>
   </si>
   <si>
     <t>a</t>
@@ -61,10 +67,35 @@
     <t>Explain what is wrong with the given code. Describe the fault precisely by proposing a modification to the code.</t>
   </si>
   <si>
+    <t>There is a bug in the given code because the loop condition `i &gt; 0` should be `i &gt;= 0` in order to search all elements in the array `x`. The loop condition `i &gt; 0` only searches the elements from index 1 to the last index, which means that the element at index 0 will not be searched. This can be fixed by modifying the loop condition to `i &gt;= 0`. Here is the modified code:
+```
+public static int findLast (int[] x, int y)
+{       
+  for (int i=x.length-1; i &gt;= 0; i--)
+  {
+     if (x[i] == y) 
+     {
+        return i;
+     }
+  }
+  return -1;
+}
+```</t>
+  </si>
+  <si>
     <t>b</t>
   </si>
   <si>
     <t>If possible, give a test case that does not execute the fault. If not, briefly explain why not.</t>
+  </si>
+  <si>
+    <t>A test case that does not execute the fault would be to pass in an array `x` that does not contain the value `y`. For example:
+```
+int[] x = {1, 2, 3, 4, 5};
+int y = 6;
+assert(findLast(x, y) == -1);
+```
+This test case will not execute the fault because the value `y` is not present in the array `x`, so the loop will execute all the way to the end and return `-1` as expected.</t>
   </si>
   <si>
     <t>c</t>
@@ -153,12 +184,6 @@
       }
       return count;
    }</t>
-  </si>
-  <si>
-    <t>answer (shared_context)</t>
-  </si>
-  <si>
-    <t>answer (separate_context)</t>
   </si>
 </sst>
 </file>
@@ -187,7 +212,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -210,17 +235,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -230,8 +244,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -549,16 +563,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="3" max="3" width="38.1640625" customWidth="1"/>
-    <col min="4" max="4" width="122" customWidth="1"/>
-    <col min="5" max="5" width="138.6640625" customWidth="1"/>
-    <col min="6" max="6" width="63.5" customWidth="1"/>
+    <col min="4" max="4" width="93.83203125" customWidth="1"/>
+    <col min="5" max="5" width="75.5" customWidth="1"/>
+    <col min="6" max="6" width="106.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -575,35 +588,44 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="289">
       <c r="A2">
         <v>5.0999999999999996</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="170">
       <c r="A3">
         <v>5.0999999999999996</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -611,10 +633,13 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -622,10 +647,13 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -633,10 +661,13 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -644,10 +675,13 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -655,13 +689,13 @@
         <v>5.2</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -669,10 +703,13 @@
         <v>5.2</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -680,10 +717,13 @@
         <v>5.2</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -691,10 +731,13 @@
         <v>5.2</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -702,10 +745,13 @@
         <v>5.2</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -713,10 +759,13 @@
         <v>5.2</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -724,13 +773,13 @@
         <v>5.3</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -738,10 +787,13 @@
         <v>5.3</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -749,10 +801,13 @@
         <v>5.3</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -760,10 +815,13 @@
         <v>5.3</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -771,10 +829,13 @@
         <v>5.3</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -782,10 +843,13 @@
         <v>5.3</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
       </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -793,13 +857,13 @@
         <v>5.4</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -807,10 +871,13 @@
         <v>5.4</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
       </c>
       <c r="D21" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -818,10 +885,13 @@
         <v>5.4</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="C22" t="s">
+        <v>23</v>
       </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -829,10 +899,13 @@
         <v>5.4</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -840,10 +913,13 @@
         <v>5.4</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="C24" t="s">
+        <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -851,10 +927,13 @@
         <v>5.4</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactoring & completed chapter 1 (Shared Context)
</commit_message>
<xml_diff>
--- a/dataset/testing.xlsx
+++ b/dataset/testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajed/PycharmProjects/Study-on-ChatGPT/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33455C4-7F19-9B43-8A44-469B078A0982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B46EEEE-880C-7C48-95BD-8E56A7BA5582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="28040" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="28040" windowHeight="17300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ch1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="108">
   <si>
     <t>id</t>
   </si>
@@ -569,23 +569,138 @@
 a modification to the code.</t>
   </si>
   <si>
+    <t xml:space="preserve">There are several issues with the given code:
+1. The `Vehicle` class should implement the `Cloneable` interface and override the `clone()` method with a `public` access modifier, rather than using a default (package-private) access modifier. This is because the `clone()` method of the `Object` class, which is being overridden by the `Vehicle` class, has a `protected` access modifier. Thus, the `clone()` method of the `Vehicle` class should have a `public` access modifier to make it visible to code outside of the package.
+2. The `clone()` method of the `Vehicle` class should call the `clone()` method of the `Object` class and handle the `CloneNotSupportedException` that it may throw, rather than simply creating a new instance of the `Vehicle` class. This is because the `clone()` method of the `Object` class performs a field-by-field copy of the object being cloned, which is necessary to create a true copy of the object. Simply creating a new instance of the `Vehicle` class only creates a new object with the same field values, but it is not a true copy of the original object.
+3. The `clone()` method of the `Truck` class should also call the `clone()` method of the `Object` class and handle the `CloneNotSupportedException` that it may throw, in addition to calling the `clone()` method of the `Vehicle` class. This is necessary to ensure that a true copy of the `Truck` object is created, rather than just a new object with the same field values.
+4. The `clone()` method of the `Truck` class should cast the result of the call to the `clone()` method of the `Vehicle` class to a `Truck` object before assigning a value to the `y` field. This is because the `clone()` method of the `Vehicle` class returns an `Object`, which must be cast to a `Truck` object before it can be used as a `Truck` object.
+To address these issues, the code could be modified as follows:
+```
+class Vehicle implements Cloneable
+{
+    private int x;
+    public Vehicle (int y) { x = y;}
+    @Override
+    public Vehicle clone() throws CloneNotSupportedException
+    {
+        return (Vehicle) super.clone();
+    }
+    // other methods omitted
+}
+class Truck extends Vehicle
+{
+    private int y;
+    public Truck (int z) { super (z); y = z;}
+    @Override
+    public Truck clone() throws CloneNotSupportedException
+    {
+        Truck result = (Truck) super.clone();
+        result.y = this.y;
+        return result;
+    }
+    // other methods omitted
+}
+```
+</t>
+  </si>
+  <si>
     <t>If possible, give a test case that does not execute the fault. If not, briefly explain why
 not.</t>
   </si>
   <si>
+    <t xml:space="preserve">
+It is not possible to give a test case that does not execute the fault in the given code, because the fault is present in the implementation of the `clone()` method in both the `Vehicle` and `Truck` classes. The fault in the `Vehicle` class is that it does not call the `clone()` method of the `Object` class and handle the `CloneNotSupportedException` that it may throw, and instead simply creates a new instance of the `Vehicle` class. The fault in the `Truck` class is that it also does not call the `clone()` method of the `Object` class and handle the `CloneNotSupportedException` that it may throw, and instead relies on the faulty implementation in the `Vehicle` class. Additionally, the `Truck` class casts the result of the call to the `clone()` method of the `Vehicle` class to a `Truck` object without checking if the object is actually an instance of the `Truck` class, which can result in a `ClassCastException` being thrown at runtime.
+Therefore, any test case that calls the `clone()` method on a `Truck` object will execute the fault, because it will result in either a `CloneNotSupportedException` being thrown (if the `clone()` method of the `Object` class is called and throws the exception) or a `ClassCastException` being thrown (if the `clone()` method of the `Object` class is not called and the result of the call to the `clone()` method of the `Vehicle` class is cast to a `Truck` object without checking its type).
+</t>
+  </si>
+  <si>
     <t>If possible, give a test case that executes the fault, but does not result in an error state.
 If not, briefly explain why not.</t>
   </si>
   <si>
+    <t xml:space="preserve">
+It is not possible to give a test case that executes the fault but does not result in an error state, because the fault in the given code always results in an error state. The fault in the `Vehicle` class is that it does not call the `clone()` method of the `Object` class and handle the `CloneNotSupportedException` that it may throw, and instead simply creates a new instance of the `Vehicle` class. This results in a `CloneNotSupportedException` being thrown when the `clone()` method is called, because the `clone()` method of the `Object` class is not being called to perform the necessary field-by-field copy of the object being cloned.
+The fault in the `Truck` class is that it also does not call the `clone()` method of the `Object` class and handle the `CloneNotSupportedException` that it may throw, and instead relies on the faulty implementation in the `Vehicle` class. Additionally, the `Truck` class casts the result of the call to the `clone()` method of the `Vehicle` class to a `Truck` object without checking if the object is actually an instance of the `Truck` class, which can result in a `ClassCastException` being thrown at runtime. Therefore, any test case that calls the `clone()` method on a `Truck` object will result in either a `CloneNotSupportedException` being thrown (if the `clone()` method of the `Object` class is called and throws the exception) or a `ClassCastException` being thrown (if the `clone()` method of the `Object` class is not called and the result of the call to the `clone()` method of the `Vehicle` class is cast to a `Truck` object without checking its type).
+</t>
+  </si>
+  <si>
     <t>If possible, give a test case that results in an error, but not a failure. If not, briefly
 explain why not. Hint: Don’t forget about the program counter.</t>
   </si>
   <si>
+    <t xml:space="preserve">
+It is not possible to give a test case that results in an error but not a failure, because an error in a program always results in a failure. An error in a program is a problem that occurs during the execution of the program and prevents it from continuing to run normally. Examples of errors include exceptions being thrown, the program entering an infinite loop, or the program crashing due to a system error.
+In the case of the given code, any test case that calls the `clone()` method on a `Truck` object will result in either a `CloneNotSupportedException` being thrown (if the `clone()` method of the `Object` class is called and throws the exception) or a `ClassCastException` being thrown (if the `clone()` method of the `Object` class is not called and the result of the call to the `clone()` method of the `Vehicle` class is cast to a `Truck` object without checking its type). In either case, the program will terminate abruptly, resulting in a failure.
+It is not possible to recover from an error in a program, because the program's execution has been disrupted and it is no longer possible to continue running the program in a predictable and correct manner. Therefore, any test case that executes the fault in the given code will result in a failure.
+</t>
+  </si>
+  <si>
     <t>In the given code, describe the first error state. Be sure to describe the complete state.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+The first error state in the given code occurs when the `clone()` method of the `Truck` class is called and the `clone()` method of the `Object` class is called and throws a `CloneNotSupportedException`.
+When this occurs, the following sequence of events takes place:
+1. The `clone()` method of the `Truck` class is called on a `Truck` object.
+2. The `clone()` method of the `Vehicle` class is called, because it is being overridden by the `Truck` class.
+3. The `clone()` method of the `Object` class is called, because it is being overridden by the `Vehicle` class.
+4. The `clone()` method of the `Object` class throws a `CloneNotSupportedException`, because the object being cloned does not implement the `Cloneable` interface.
+5. The `clone()` method of the `Vehicle` class catches the `CloneNotSupportedException` and does not handle it, because it is not implemented to do so.
+6. The `clone()` method of the `Truck` class catches the `CloneNotSupportedException` and does not handle it, because it is not implemented to do so.
+7. The `clone()` method of the `Truck` class returns control to the calling code, and the `CloneNotSupportedException` is propagated to the calling code.
+In this error state, the program is terminated and a `CloneNotSupportedException` is thrown, indicating that the object being cloned does not support cloning. This error state results in a failure of the program.
+</t>
   </si>
   <si>
     <t>Implement your repair and verify that the given test now produces the expected output.
 Submit a screen printout or other evidence that your new program works.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+To repair the given code and make it produce the expected output, the `clone()` method of the `Vehicle` class should be modified to call the `clone()` method of the `Object` class and handle the `CloneNotSupportedException` that it may throw, and the `clone()` method of the `Truck` class should be modified to call the `clone()` method of the `Object` class, handle the `CloneNotSupportedException` that it may throw, and cast the result of the call to the `clone()` method of the `Vehicle` class to a `Truck` object before assigning a value to the `y` field.
+Here is the repaired code:
+```
+class Vehicle implements Cloneable
+{
+    private int x;
+    public Vehicle (int y) { x = y;}
+    @Override
+    public Vehicle clone() throws CloneNotSupportedException
+    {
+        return (Vehicle) super.clone();
+    }
+    // other methods omitted
+}
+class Truck extends Vehicle
+{
+    private int y;
+    public Truck (int z) { super (z); y = z;}
+    @Override
+    public Truck clone() throws CloneNotSupportedException
+    {
+        Truck result = (Truck) super.clone();
+        result.y = this.y;
+        return result;
+    }
+    // other methods omitted
+}
+```
+To verify that the repaired code produces the expected output, I will write a test case that calls the `clone()` method on a `Truck` object and checks that the resulting object has the same field values as the original object and is of the same class:
+```
+Truck suv = new Truck (4);
+Truck co = suv.clone();
+if (suv.x == co.x &amp;&amp; suv.getClass() == co.getClass()) {
+    System.out.println("Test passed");
+} else {
+    System.out.println("Test failed");
+}
+```
+When I run this test case with the repaired code, it produces the expected output: "Test passed". This indicates that the repaired code is correct and produces the expected output.
+Here is a screen printout of the test case being run:
+```
+Test passed
+```
+</t>
   </si>
   <si>
     <t xml:space="preserve"> Consider the following three example classes. These are OO faults taken from Joshua Bloch’s
@@ -613,6 +728,85 @@
 // and that equals()is faulty.</t>
   </si>
   <si>
+    <t xml:space="preserve">The problem with the given code is that the `BigDecimal` class has inconsistent implementation of the `equals` and `compareTo` methods. The `equals` method returns `false` for the `BigDecimal` objects `x` and `y`, but the `compareTo` method returns `0` for the same objects, indicating that they are equal. This inconsistency can lead to unexpected behavior when using the `BigDecimal` objects with collections that rely on either the `equals` or `compareTo` methods for comparison, such as the `TreeSet` and `HashSet` in the example.
+To fix this issue, one possible modification to the code would be to override the `equals` method in the `BigDecimal` class to use the same comparison logic as the `compareTo` method. This would ensure that the `equals` and `compareTo` methods are consistent with each other and behave as expected when used with collections.
+Alternatively, if it is not possible or desirable to modify the `BigDecimal` class, the code could use a different collection class that does not rely on either the `equals` or `compareTo` methods for comparison, such as a `LinkedHashSet` or a `List`. This would allow the code to work correctly even with the inconsistent implementation of the `equals` and `compareTo` methods in the `BigDecimal` class.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+It is not possible to give a test case that does not execute the fault in the given code, because the fault is inherent in the implementation of the `BigDecimal` class. The fault occurs whenever the `BigDecimal` objects `x` and `y` are used with a collection that relies on either the `equals` or `compareTo` methods for comparison, regardless of the specific values of `x` and `y`.
+The fault occurs because the `equals` and `compareTo` methods of the `BigDecimal` class are implemented in a way that is inconsistent with each other. The `equals` method returns `false` for the `BigDecimal` objects `x` and `y`, but the `compareTo` method returns `0` for the same objects, indicating that they are equal. This inconsistency can lead to unexpected behavior when using the `BigDecimal` objects with collections that rely on either the `equals` or `compareTo` methods for comparison.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+A test case that executes the fault but does not result in an error state for the given code would be as follows:
+```
+public static void main(String[] args) {
+    BigDecimal x = new BigDecimal("1.0");
+    BigDecimal y = new BigDecimal("1.00");
+    Set&lt;BigDecimal&gt; BigDecimalTree = new TreeSet&lt;BigDecimal&gt;();
+    BigDecimalTree.add(x);
+    BigDecimalTree.add(y);
+    Set&lt;BigDecimal&gt; BigDecimalHash = new HashSet&lt;BigDecimal&gt;();
+    BigDecimalHash.add(x);
+    BigDecimalHash.add(y);
+    System.out.println("BigDecimalTree = " + BigDecimalTree);
+    System.out.println("BigDecimalHash = " + BigDecimalHash);
+}
+```
+This test case executes the fault by using the `BigDecimal` objects `x` and `y` with a `TreeSet` and a `HashSet`, which rely on the `compareTo` and `equals` methods, respectively, for comparison. The fault occurs because the `equals` and `compareTo` methods of the `BigDecimal` class are implemented in a way that is inconsistent with each other. The `equals` method returns `false` for the `BigDecimal` objects `x` and `y`, but the `compareTo` method returns `0` for the same objects, indicating that they are equal. As a result, the `TreeSet` ends up with only one element, while the `HashSet` has two elements.
+This test case does not result in an error state, because the code does not contain any syntax errors or runtime exceptions. However, the test case does produce unexpected results, which may indicate a problem with the code.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+It is not possible to give a test case that results in an error but not a failure for the given code, because the code does not contain any syntax errors or runtime exceptions. The code simply creates and uses two `BigDecimal` objects and two collections, which are all valid operations.
+The fault in the given code is not an error, but rather an inconsistency in the implementation of the `equals` and `compareTo` methods of the `BigDecimal` class. This inconsistency can lead to unexpected behavior when using the `BigDecimal` objects with collections that rely on either the `equals` or `compareTo` methods for comparison, such as the `TreeSet` and `HashSet` in the example. However, this behavior is not considered an error, as it does not result in a syntax error or a runtime exception.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+There is no error state in the given code. The code simply creates and uses two `BigDecimal` objects and two collections, which are all valid operations.
+The fault in the given code is not an error, but rather an inconsistency in the implementation of the `equals` and `compareTo` methods of the `BigDecimal` class. This inconsistency can lead to unexpected behavior when using the `BigDecimal` objects with collections that rely on either the `equals` or `compareTo` methods for comparison, such as the `TreeSet` and `HashSet` in the example. However, this behavior is not considered an error, as it does not result in a syntax error or a runtime exception.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+To fix the fault in the given code, one possible modification would be to override the `equals` method in the `BigDecimal` class to use the same comparison logic as the `compareTo` method. This would ensure that the `equals` and `compareTo` methods are consistent with each other and behave as expected when used with collections.
+Here is an example of how this could be done:
+```
+public class BigDecimal {
+    // existing implementation of compareTo method
+    public int compareTo(BigDecimal other) {
+        // implementation details
+    }
+    @Override
+    public boolean equals(Object other) {
+        if (other == this) {
+            return true;
+        }
+        if (!(other instanceof BigDecimal)) {
+            return false;
+        }
+        return compareTo((BigDecimal) other) == 0;
+    }
+}
+```
+With this modification, the test case from earlier would produce the expected output:
+```
+BigDecimalTree = 1
+BigDecimalHash = 1, 1
+```
+Here is a screen printout of the test case being executed with the modified `BigDecimal` class:
+```
+BigDecimalTree = [1]
+BigDecimalHash = [1, 1]
+```
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">Consider the following three example classes. These are OO faults taken from Joshua Bloch’s
 Effective Java, Second Edition. Answer the following questions about each.
 class Point
@@ -659,110 +853,118 @@
 a modification to the code.</t>
   </si>
   <si>
-    <t xml:space="preserve">There is a fault in the `ColorPoint` class's implementation of the `equals` method. Specifically, the `equals` method in the `ColorPoint` class does not properly handle cases where it is passed an instance of the superclass `Point` as the argument. This is a problem because the `equals` method in the `Point` class does not consider the `color` field when determining if two points are equal, but the `equals` method in the `ColorPoint` class does consider the `color` field. This means that when the `equals` method in the `ColorPoint` class is called with an instance of `Point` as the argument, it will always return `false`, even if the `Point` and `ColorPoint` objects have the same `x` and `y` values.
-To fix this fault, the `equals` method in the `ColorPoint` class should be modified to properly handle cases where it is passed an instance of the superclass `Point` as the argument. One way to do this would be to add a check at the beginning of the method to determine if the argument is an instance of `Point`, and if it is, to compare the `x` and `y` values of the `ColorPoint` and `Point` objects directly, rather than calling the `equals` method of the `Point` class.
-For example:
-```
-@Override public boolean equals (Object o)
+    <t xml:space="preserve">There are a few issues with the given code.
+First, in the `Point` class, the `equals` method does not properly override the `equals` method in the `Object` class. The `equals` method in the `Object` class checks for object reference equality (i.e., whether two references refer to the same object), while the `equals` method in the `Point` class checks for value equality (i.e., whether two `Point` objects have the same values for their `x` and `y` fields). To properly override the `equals` method, the `Point` class should add an `@Override` annotation to the method and also include a check for object reference equality at the beginning of the method. The modified `equals` method in the `Point` class should look like this:
+```
+@Override
+public boolean equals(Object o) {
+    if (o == this) return true;
+    if (!(o instanceof Point)) return false;
+    Point p = (Point) o;
+    return (p.x == this.x) &amp;&amp; (p.y == this.y);
+}
+```
+Second, in the `ColorPoint` class, the `equals` method does not properly handle the case where it is passed an object that is not an instance of `ColorPoint`. In this case, the method should return `false` rather than throwing a `ClassCastException`. To fix this issue, the `equals` method in the `ColorPoint` class should include a check for object reference equality at the beginning of the method, similar to what was done in the modified `equals` method in the `Point` class. The modified `equals` method in the `ColorPoint` class should look like this:
+```
+@Override
+public boolean equals(Object o) {
+    if (o == this) return true;
+    if (!(o instanceof ColorPoint)) return false;
+    ColorPoint cp = (ColorPoint) o;
+    return super.equals(cp) &amp;&amp; (cp.color == this.color);
+}
+```
+Finally, the tests at the end of the code are not checking the expected behavior of the `equals` methods. The first test, `p.equals(cp1)`, is expected to return `true`, but it will actually return `false` because `p` and `cp1` are not equal according to the `equals` method in the `Point` class. The second test, `cp1.equals(p)`, is expected to return `true`, but it will actually throw a `ClassCastException` because the `equals` method in the `ColorPoint` class is attempting to cast the `Point` object `p` to a `ColorPoint` object. The third test, `cp1.equals(cp2)`, is expected to return `false`, but it will actually return `true` because the `equals` method in the `ColorPoint` class is not considering the `color` field when checking for equality.
+To fix these issues, the tests should be modified to use the modified `equals` methods described above. The modified tests should look like this:
+```
+Point p = new Point (1,2);
+ColorPoint cp1 = new ColorPoint (1,2,RED);
+ColorPoint cp2 = new ColorPoint (1,2,BLUE);
+assertTrue(p.equals(cp1)); // Test 1: p
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+It is not possible to give a test case that does not execute the fault in the given code because the fault is present in the implementation of the `equals` method in both the `Point` and `ColorPoint` classes. The fault in the `Point` class is that the method does not properly override the `equals` method in the `Object` class, and the fault in the `ColorPoint` class is that the method does not properly handle the case where it is passed an object that is not an instance of `ColorPoint`. These faults are present in the implementation of the `equals` method in both classes and will be executed every time the method is called.
+To avoid executing the fault, the implementation of the `equals` method in both classes must be modified to properly override the `equals` method in the `Object` class and handle the case where it is passed an object that is not an instance of the class. The modified `equals` methods for both classes were provided in the previous response.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+It is not possible to give a test case that executes the fault in the given code but does not result in an error state because the fault in the `Point` class will always result in an error state (i.e., a `ClassCastException` will be thrown) when the `equals` method is called with an object that is not an instance of the `Point` class. The fault in the `ColorPoint` class will also always result in an error state (i.e., a `ClassCastException` will be thrown) when the `equals` method is called with an object that is not an instance of the `ColorPoint` class.
+To avoid these error states, the implementation of the `equals` method in both classes must be modified to properly handle the case where it is passed an object that is not an instance of the class. The modified `equals` methods for both classes were provided in a previous response.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+It is not possible to give a test case that results in an error but not a failure for the given code because the fault in the `Point` class will always result in a failure (i.e., a `ClassCastException` will be thrown) when the `equals` method is called with an object that is not an instance of the `Point` class. The fault in the `ColorPoint` class will also always result in a failure (i.e., a `ClassCastException` will be thrown) when the `equals` method is called with an object that is not an instance of the `ColorPoint` class.
+To avoid these failures, the implementation of the `equals` method in both classes must be modified to properly handle the case where it is passed an object that is not an instance of the class. The modified `equals` methods for both classes were provided in a previous response.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In the given code, describe the first error state. Be sure to describe the complete state.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+The first error state in the given code occurs when the `equals` method in the `Point` class is called with an object that is not an instance of the `Point` class. When this happens, a `ClassCastException` will be thrown when the code attempts to cast the object to a `Point` object at Location A.
+The complete state of the error includes the following:
+- The `Point` object that the `equals` method was called on (e.g., `p` in the test `p.equals(cp1)`)
+- The object that was passed as an argument to the `equals` method (e.g., `cp1` in the test `p.equals(cp1)`)
+- The line of code where the `ClassCastException` is thrown (i.e., `Point p = (Point) o;` at Location A)
+- The `ClassCastException` object that is thrown, which includes the following information:
+  - The message describing the error (e.g., "Cannot cast com.example.ColorPoint to com.example.Point")
+  - The stack trace showing the sequence of method calls leading up to the exception
+This error state will occur whenever the `equals` method in the `Point` class is called with an object that is not an instance of the `Point` class, regardless of the values of the fields in the objects being compared.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+To fix the faults in the given code, the implementation of the `equals` method in both the `Point` and `ColorPoint` classes must be modified. The modified `equals` methods should include an `@Override` annotation and a check for object reference equality at the beginning of the method to properly override the `equals` method in the `Object` class and handle the case where the method is passed an object that is not an instance of the class.
+Here is the modified code with the fixed `equals` methods:
+```
+class Point
 {
-    if (o instanceof Point) {
+    private int x; private int y;
+    public Point (int x, int y) { this.x=x; this.y=y; }
+    @Override
+    public boolean equals(Object o) {
+        if (o == this) return true;
+        if (!(o instanceof Point)) return false;
         Point p = (Point) o;
         return (p.x == this.x) &amp;&amp; (p.y == this.y);
     }
-    if (!(o instanceof ColorPoint)) return false;
-    ColorPoint cp = (ColorPoint) o;
-    return (super.equals(cp) &amp;&amp; (cp.color == this.color));
-}
-```
-Alternatively, the `equals` method in the `Point` class could be modified to consider the `color` field when determining if two points are equal. This would allow the `equals` method in the `ColorPoint` class to simply call the `equals` method of the `Point` class and compare the `color` fields directly, without the need for any special handling of instances of the `Point` class.
-For example:
-```
-@Override public boolean equals (Object o)
+}
+class ColorPoint extends Point
 {
-    if (!(o instanceof Point)) return false;
-    Point p = (Point) o;
-    return (p.x == this.x) &amp;&amp; (p.y == this.y) &amp;&amp; ((p instanceof ColorPoint &amp;&amp; ((ColorPoint) p).color == this.color) || !(p instanceof ColorPoint));
-}
-```
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-It is not possible to give a test case that does not execute the fault, because the fault exists in the implementation of the `equals` method in the `ColorPoint` class. Any test case that calls the `equals` method on an instance of the `ColorPoint` class will execute the fault.
-For example, consider the following test cases:
+    private Color color;
+    // Fault: Superclass instantiable; subclass state extended
+    public ColorPoint (int x, int y, Color color)
+    {
+        super (x,y);
+        this.color=color;
+    }
+    @Override
+    public boolean equals(Object o) {
+        if (o == this) return true;
+        if (!(o instanceof ColorPoint)) return false;
+        ColorPoint cp = (ColorPoint) o;
+        return super.equals(cp) &amp;&amp; (cp.color == this.color);
+    }
+}
+```
+With these changes, the tests at the end of the code will produce the expected output. Here is the modified test code:
 ```
 Point p = new Point (1,2);
 ColorPoint cp1 = new ColorPoint (1,2,RED);
 ColorPoint cp2 = new ColorPoint (1,2,BLUE);
-p.equals (cp1); // Test 1: Result = true;
-cp1.equals (p); // Test 2: Result = false;
-cp1.equals (cp2); // Test 3: Result = false;
-```
-All of these test cases will execute the fault, because they all call the `equals` method on an instance of the `ColorPoint` class. The first test case will return `true`, because the `Point` class's `equals` method does not consider the `color` field and the `Point` and `ColorPoint` objects have the same `x` and `y` values. The second and third test cases will return `false`, because the `ColorPoint` class's `equals` method does consider the `color` field and the `ColorPoint` objects have different `color` values.
-To avoid executing the fault, it would be necessary to modify the implementation of the `equals` method in the `ColorPoint` class, as described in the previous answer.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-It is not possible to give a test case that executes the fault but does not result in an error state, because the fault in the `ColorPoint` class's implementation of the `equals` method results in the method returning the wrong value for some input.
-For example, consider the following test case:
-```
-Point p = new Point (1,2);
-ColorPoint cp1 = new ColorPoint (1,2,RED);
-p.equals (cp1); // Test 4: Result = true;
-```
-This test case will execute the fault, because it calls the `equals` method on an instance of the `ColorPoint` class and passes an instance of the `Point` class as the argument. The fault in the `ColorPoint` class's implementation of the `equals` method causes the method to return `false` in this case, even though the `Point` and `ColorPoint` objects have the same `x` and `y` values.
-Therefore, it is not possible to give a test case that executes the fault but does not result in an error state, because the fault always results in an incorrect return value.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-It is not possible to give a test case that results in an error but not a failure, because the fault in the `ColorPoint` class's implementation of the `equals` method does not result in an error.
-The fault in the `ColorPoint` class's implementation of the `equals` method results in the method returning the wrong value for some input, but it does not result in an error such as an exception being thrown or the program crashing. Instead, the method simply returns an incorrect value, which may cause issues if the incorrect return value is used in other parts of the program, but it does not result in an error.
-Therefore, it is not possible to give a test case that results in an error but not a failure, because the fault does not result in an error.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> In the given code, describe the first error state. Be sure to describe the complete state.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-There is no error state in the given code. The fault in the `ColorPoint` class's implementation of the `equals` method results in the method returning the wrong value for some input, but it does not result in an error such as an exception being thrown or the program crashing. Instead, the method simply returns an incorrect value, which may cause issues if the incorrect return value is used in other parts of the program, but it does not result in an error state.
-Therefore, there is no first error state in the given code.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-To fix the fault in the `ColorPoint` class's implementation of the `equals` method, one option would be to modify the method as follows:
-```
-@Override public boolean equals (Object o)
-{
-    if (o instanceof Point) {
-        Point p = (Point) o;
-        return (p.x == this.x) &amp;&amp; (p.y == this.y);
-    }
-    if (!(o instanceof ColorPoint)) return false;
-    ColorPoint cp = (ColorPoint) o;
-    return (super.equals(cp) &amp;&amp; (cp.color == this.color));
-}
-```
-This modified implementation of the `equals` method properly handles cases where it is passed an instance of the superclass `Point` as the argument, and compares the `x` and `y` values of the `ColorPoint` and `Point` objects directly.
-To verify that this repair works as intended, we can re-run the original test cases with the modified `ColorPoint` class:
-```
-Point p = new Point (1,2);
-ColorPoint cp1 = new ColorPoint (1,2,RED);
-ColorPoint cp2 = new ColorPoint (1,2,BLUE);
-System.out.println(p.equals (cp1)); // Test 1: Result = true;
-System.out.println(cp1.equals (p)); // Test 2: Result = true;
-System.out.println(cp1.equals (cp2)); // Test 3: Result = false;
-```
-This produces the following output:
-```
-true
-true
-false
-```
-which is the expected output. This demonstrates that the repair to the `ColorPoint` class's implementation of the `equals` method is successful, and the test cases now produce the expected output.
+assertTrue(p.equals(cp1)); // Test 1: p.equals(cp1) = true
+assertTrue(cp1.equals(p)); // Test 2: cp1.equals(p) = true
+assertFalse(cp1.equals(cp2)); // Test 3: cp1.equals(cp2) = false
+```
+Here is a screen printout showing that the modified code works as expected:
+```
+All tests passed.
+```
 </t>
   </si>
   <si>
@@ -842,6 +1044,30 @@
     <t>Develop JUnit tests for the BoundedQueue class. Make sure your tests check every method, but we will not evaluate the quality of your test designs and do not expect you to satisfy any test criteria. Turn in a printout of your JUnit tests and either a printout or a screen shot showing the results of each test.</t>
   </si>
   <si>
+    <t xml:space="preserve">Here is an example of JUnit tests for the BoundedQueue class:
+```
+import static org.junit.Assert.*;
+import org.junit.Before;
+import org.junit.Test;
+public class BoundedQueueTest {
+    private BoundedQueue queue;
+    @Before
+    public void setUp() throws Exception {
+        queue = new BoundedQueue(5);
+    }
+    @Test
+    public void testEnQueue() {
+        // Test enqueuing elements
+        queue.enQueue(1);
+        queue.enQueue(2);
+        queue.enQueue(3);
+        assertEquals("[1, 2, 3]", queue.toString());
+        // Test enqueuing element when queue is full
+        try {
+            queue.enQueue(4);
+</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 
 import java.util.*;
 public class Min
@@ -879,6 +1105,34 @@
     <t>Delete the explict throw of NullPointerException in the Min program (figure 3.2). Verify that the JUnit test for a list with a single null element now fails.</t>
   </si>
   <si>
+    <t xml:space="preserve">To delete the explicit throw of NullPointerException in the Min program, you can simply remove the following line of code:
+if (result == null) throw new NullPointerException ("Min.min");
+After removing this line, the modified Min program would look like this:
+import java.util.*;
+public class Min
+{
+/**
+* Returns the minimum element in a list
+* @param list Comparable list of elements to search
+* return the minimum element in the list
+* @throws NullPointerException (NPE) if list is null or
+* if any list elements are null
+* @throws ClassCastException (CCE) if list elements are not mutually comparable
+* @throws MlegalArgumentException if list is empty
+*/
+public static &lt;T extends Comparable&lt;? super T&gt;&gt; T min (List&lt;? extends T&gt; lst)
+{
+if (list.size() == 0)
+throw new IllegalArgumentException ("Min.min”);
+}
+Iterator&lt;? extends T&gt; itr = list.iterator():
+T result = itr.next():
+while (itr.hasNext())
+f
+T comp = itr
+</t>
+  </si>
+  <si>
     <t>The following JUnit test method for the sort() method has a non-syntactic flaw.
 @Test
 public void testSort()
@@ -896,6 +1150,10 @@
     <t>Find the flaw and describe it in terms of the RIPR model. Be as precise, specific, and concise as you can. For full credit, you must use the terminology introduced in the book.
 In the test method, names is an instance of an object that stores strings and has methods add(), sort(), and getFirst(), which do exactly what you would expect from their names.
 You can assume that the object names has been properly instantiated and the add() and getFirst() methods have already been tested and work correctly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The non-syntactic flaw in the test method is that there is a line of code "23" which is not a valid Java statement. This violates the rule of well-formedness in the RIPR model, as a well-formed program must have a syntactically correct structure. 
+</t>
   </si>
   <si>
     <t>Consider the following example class. PrimeNumbers has three methods. The first, computePrimes(), takes one integer input and computes that many prime numbers. iterator() returns an Iterator that will iterate through the primes, and toString() returns a string representation.
@@ -941,18 +1199,88 @@
     <t>Write a test that does not reach the fault. If a test cannot be created, explain why.</t>
   </si>
   <si>
+    <t xml:space="preserve">Test 1:
+1. Call computePrimes() with input value 2.
+2. Call toString() to retrieve the list of prime numbers computed.
+3. Verify that the list contains 2.
+Expected result: The list contains 2.
+Test 2:
+1. Call computePrimes() with input value 5.
+2. Call toString() to retrieve the list of prime numbers computed.
+3. Verify that the list contains 2, 3, 5, 7, 11.
+Expected result: The list contains 2, 3, 5, 7, 11.
+Test 3:
+1. Call computePrimes() with input value 3.
+2. Call iterator() to retrieve an iterator for the list of prime numbers computed.
+3. Iterate through the iterator and verify that the prime numbers encountered are 2, 3, and 5.
+Expected result: The iterator returns 2, 3, and 5.
+Test 4:
+1. Call computePrimes() with input value 100.
+2. Call iterator() to retrieve an iterator for the list of prime numbers computed.
+3. Iterate through the iterator and verify that the prime numbers encountered do not include any prime numbers ending in 9 (e.g. 19, 29, 59, 79, 89).
+Expected result: The iterator does not return any prime numbers ending in 9.
+Test 5: (Test oracle required)
+1. Call computePrimes() with input value 100.
+2. Call iterator() to retrieve an iterator for the list of prime numbers computed.
+3. Iterate through the iterator and verify that the prime numbers encountered are correct by comparing them to a known list of prime numbers (test oracle).
+Expected result: The iterator returns the same list of prime numbers as the known list of prime numbers.
+</t>
+  </si>
+  <si>
     <t>Write a test that reaches the fault, but does not infect. If a test cannot be created, explain why.</t>
   </si>
   <si>
+    <t xml:space="preserve">
+Test 6:
+1. Call computePrimes() with input value 5.
+2. Call toString() to retrieve the list of prime numbers computed.
+3. Verify that the list contains 2, 3, 5, 7, 11.
+Expected result: The list contains 2, 3, 5, 7, 11.
+This test reaches the fault, as it would include a prime number ending in 9 (e.g. 19) if the fault did not exist. However, it does not "infect" the result, as it does not verify the presence of any prime numbers ending in 9 and therefore will not fail if they are not present.
+</t>
+  </si>
+  <si>
     <t>Write a test that infects the state, but does not propagate. If a test cannot be created, explain why.</t>
   </si>
   <si>
+    <t xml:space="preserve">
+Test 7:
+1. Call computePrimes() with input value 5.
+2. Call iterator() to retrieve an iterator for the list of prime numbers computed.
+3. Iterate through the iterator and verify that the prime numbers encountered are 2, 3, 5, 7, 11.
+Expected result: The iterator returns 2, 3, 5, 7, 11.
+This test infects the state by reaching the fault and including a prime number ending in 9 in the list of prime numbers, but it does not propagate the infection as it does not verify the presence or absence of any other prime numbers beyond the first 5. Therefore, it will not fail if the fault causes additional prime numbers to be omitted beyond the first 5.
+</t>
+  </si>
+  <si>
     <t>Write a test that propagates, but does not reveal. If a test cannot be created, explain why.</t>
   </si>
   <si>
+    <t xml:space="preserve">
+Test 8:
+1. Call computePrimes() with input value 100.
+2. Call iterator() to retrieve an iterator for the list of prime numbers computed.
+3. Iterate through the iterator and verify that the prime numbers encountered are correct by comparing them to a known list of prime numbers (test oracle).
+4. Call toString() to retrieve a string representation of the list of prime numbers.
+5. Verify that the string representation is correct by comparing it to a known string representation of the list of prime numbers.
+Expected result: The iterator returns the same list of prime numbers as the known list of prime numbers, and the string representation of the list is correct.
+This test propagates the infection caused by the fault by verifying the presence or absence of all prime numbers up to 100, but it does not reveal the infection as it only compares the result to a known correct result, rather than explicitly checking for the presence or absence of specific prime numbers ending in 9. Therefore, it will not fail if the fault causes some prime numbers ending in 9 to be omitted.
+</t>
+  </si>
+  <si>
     <t>Write a test that reveals the fault. If a test cannot be created, explain why.</t>
   </si>
   <si>
+    <t xml:space="preserve">
+Test 9:
+1. Call computePrimes() with input value 100.
+2. Call iterator() to retrieve an iterator for the list of prime numbers computed.
+3. Iterate through the iterator and verify that the prime numbers encountered do not include any prime numbers ending in 9 (e.g. 19, 29, 59, 79, 89).
+Expected result: The iterator does not return any prime numbers ending in 9.
+This test reveals the fault by explicitly checking for the presence or absence of prime numbers ending in 9 and will fail if the fault causes any of these numbers to be omitted.
+</t>
+  </si>
+  <si>
     <t>When overriding the equals() method, programmers are also required to override the hashCode() method; otherwise clients cannot store instances of these objects in common Collection structures such as HashSet. For example, the Point class from Chapter 1 is defective in this regard.</t>
   </si>
   <si>
@@ -972,13 +1300,151 @@
   </si>
   <si>
     <t>Replace each occurrence of a set with a list in the JUnit theory removeThenAddDoesNotChangeSet. Is the resulting theory valid or invalid? How many of the tests that pass the precondition also pass the postcondition? Explain.</t>
+  </si>
+  <si>
+    <t>It is not possible for me to accurately answer this question without more information about the JUnit theory "removeThenAddDoesNotChangeSet" and the context in which it is being used.
+In general, replacing a set with a list in a JUnit theory may result in the theory becoming invalid, depending on how the set and list are used in the theory. If the set and list are used in ways that are not interchangeable, such as using set-specific methods on a list, then the theory may become invalid.
+Without knowing more about the theory and the specific replacements being made, it is not possible to determine how many of the tests that pass the precondition will also pass the postcondition. It is also not possible to determine whether the resulting theory will be valid or invalid.</t>
+  </si>
+  <si>
+    <t>To demonstrate the problem with the Point class, let's first define the class:
+Copy code
+class Point {
+  int x;
+  int y;
+  public Point(int x, int y) {
+    this.x = x;
+    this.y = y;
+  }
+  // Overrides equals() method, but not hashCode()
+  public boolean equals(Object o) {
+    if (!(o instanceof Point)) return false;
+    Point p = (Point) o;
+    return p.x == x &amp;&amp; p.y == y;
+  }
+}
+Now, let's try to use a HashSet to store a few Point objects:
+Set&lt;Point&gt; set = new HashSet&lt;&gt;();
+Point p1 = new Point(1, 2);
+Point p2 = new Point(3, 4);
+Point p3 = new Point(1, 2);
+set.add(p1);
+set.add(p2);
+set.add(p3);
+System.out.println(set.size());  // Outputs: 3
+As we can see, the HashSet contains 3 elements even though p1 and p3 are equal. This is because the HashSet uses the hashCode() method to determine if two objects are equal, and in this case, the hashCode() method has not been overridden. Since the hashCode() method for p1 and p3 will be different (since they are distinct objects), the HashSet will consider them to be different elements and will add both to the set.
+To fix this issue, we need to override the hashCode() method in the Point class:
+class Point {
+  int x;
+  int y;
+  public Point(int x, int y) {
+    this.x = x;
+    this.y = y;
+  }
+  // Overrides equals() method
+  public boolean equals(Object o) {
+    if (!(o instanceof Point)) return false;
+    Point p = (Point) o;
+    return p.x == x &amp;&amp; p.y == y;
+  }
+  // Overrides hashCode() method
+  public int hashCode() {
+    return Objects.hash(x, y);
+  }
+}
+With the hashCode() method overridden, the HashSet will now correctly store only 2 elements:
+Set&lt;Point&gt; set = new HashSet&lt;&gt;();
+Point p1 = new Point(1, 2);
+Point p2 = new Point(3, 4);
+Point p3 = new Point(1, 2);
+set.add(p1);
+set.add(p2);
+set.add(p3);
+System.out.println(set.size());  // Outputs: 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The equals() and hashCode() methods are used together in Java to implement the contract of object equality, as defined by the Objects.equals() and Objects.hash() methods.
+According to this contract, if two objects are equal (as determined by the equals() method), then their hashCode() values must be equal as well. Conversely, if two objects have equal hashCode() values, they do not necessarily have to be equal (as determined by the equals() method).
+In other words, the relationship between equals() and hashCode() is defined by the following mathematical relationship:
+if a.equals(b) then a.hashCode() == b.hashCode()
+This relationship is important because it allows objects to be stored and retrieved efficiently in common data structures such as HashMap, HashSet, and Hashtable.
+It's also worth noting that the hashCode() method should be implemented such that it returns the same value for two equal objects every time it is called on those objects, as long as the objects are not modified. This allows the hashCode() method to be used as a way to identify unique objects and helps to ensure the efficiency of data structures that rely on it.
+</t>
+  </si>
+  <si>
+    <t>Here is a simple JUnit test that demonstrates that the Point class does not satisfy the required relationship between equals() and hashCode():
+import org.junit.Test;
+import static org.junit.Assert.*;
+public class PointTest {
+  @Test
+  public void testEqualsAndHashCode() {
+    Point p1 = new Point(1, 2);
+    Point p2 = new Point(1, 2);
+    Point p3 = new Point(3, 4);
+    assertTrue(p1.equals(p2));
+    assertFalse(p1.hashCode() == p2.hashCode());  // Fails
+  }
+}
+In this test, we create two Point objects, p1 and p2, which are equal (as determined by the equals() method). However, the test fails because the hashCode() values of p1 and p2 are not equal, indicating that the hashCode() method is not properly implemented.
+To fix this issue, the hashCode() method in the Point class needs to be overridden as described in the previous answer. Once the hashCode() method is properly implemented, the test should pass.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To repair the fault in the Point class, the hashCode() method needs to be overridden as follows:
+class Point {
+  int x;
+  int y;
+  public Point(int x, int y) {
+    this.x = x;
+    this.y = y;
+  }
+  // Overrides equals() method
+  public boolean equals(Object o) {
+    if (!(o instanceof Point)) return false;
+    Point p = (Point) o;
+    return p.x == x &amp;&amp; p.y == y;
+  }
+  // Overrides hashCode() method
+  public int hashCode() {
+    return Objects.hash(x, y);
+  }
+}
+With the hashCode() method overridden, the Point class will now satisfy the required relationship between equals() and hashCode() and can be used with common data structures such as HashMap, HashSet, and Hashtable without any issues.
+It's worth noting that the hashCode() method implementation shown above uses the Objects.hash() utility method to compute the hash code for the Point object. This method takes the x and y fields of the Point object as arguments and returns a hash code that is based on their values. This ensures that the hash code is consistent with the definition of equality for the Point class (as defined by the equals() method).
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To rewrite the JUnit test as a JUnit theory, we can use the @Theory annotation and the @DataPoints annotation to specify a set of data points that will be used to evaluate the theory.
+Here is the revised JUnit test:
+import org.junit.experimental.theories.DataPoint;
+import org.junit.experimental.theories.Theories;
+import org.junit.experimental.theories.Theory;
+import org.junit.runner.RunWith;
+import static org.junit.Assert.*;
+@RunWith(Theories.class)
+public class PointTest {
+  @DataPoint
+  public static Point p1 = new Point(1, 2);
+  @DataPoint
+  public static Point p2 = new Point(1, 2);
+  @DataPoint
+  public static Point p3 = new Point(3, 4);
+  @Theory
+  public void testEqualsAndHashCode(Point p1, Point p2) {
+    assertTrue(p1.equals(p2));
+    assertTrue(p1.hashCode() == p2.hashCode());
+  }
+}
+In this revised test, the @DataPoint annotation is used to define three Point objects that will be used as data points for the theory. The theory itself is defined using the @Theory annotation and takes two Point objects as arguments. The theory asserts that if two Point objects are equal (as determined by the equals() method), then their hashCode() values must also be equal.
+To evaluate the theory, JUnit will generate a set of test cases using the data points defined in the test class. For each test case, JUnit will pass two Point objects to the theory and evaluate the assertions. If any of the assertions fail, the theory will be considered to have failed.
+In this case, since the Point class has been repaired and the hashCode() method is properly implemented, the theory should pass for all test cases.
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -990,11 +1456,7 @@
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1005,7 +1467,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1028,44 +1490,17 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1383,20 +1818,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.83203125" customWidth="1"/>
-    <col min="3" max="3" width="110" customWidth="1"/>
-    <col min="4" max="4" width="62.6640625" customWidth="1"/>
-    <col min="5" max="5" width="87.33203125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="55.1640625" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="16.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="63.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="51.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="75.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.5" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1409,689 +1846,725 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="404">
-      <c r="A2">
+    <row r="2" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="323">
-      <c r="A3">
+    <row r="3" spans="1:6" ht="323" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
+    <row r="4" spans="1:6" ht="323" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
+    <row r="5" spans="1:6" ht="323" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6">
+    <row r="6" spans="1:6" ht="323" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7">
+    <row r="7" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8">
+    <row r="8" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>5.2</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9">
+    <row r="9" spans="1:6" ht="306" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>5.2</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10">
+    <row r="10" spans="1:6" ht="306" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>5.2</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11">
+    <row r="11" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
         <v>5.2</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12">
+    <row r="12" spans="1:6" ht="306" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
         <v>5.2</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13">
+    <row r="13" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
         <v>5.2</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="A14">
+    <row r="14" spans="1:6" ht="340" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
         <v>5.3</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="A15">
+    <row r="15" spans="1:6" ht="340" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
         <v>5.3</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="A16">
+    <row r="16" spans="1:6" ht="340" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
         <v>5.3</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
-      <c r="A17">
+    <row r="17" spans="1:5" ht="340" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
         <v>5.3</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18">
+    <row r="18" spans="1:5" ht="340" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
         <v>5.3</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
-      <c r="A19">
+    <row r="19" spans="1:5" ht="340" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
         <v>5.3</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20">
+    <row r="20" spans="1:5" ht="388" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
         <v>5.4</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
-      <c r="A21">
+    <row r="21" spans="1:5" ht="372" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
         <v>5.4</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
-      <c r="A22">
+    <row r="22" spans="1:5" ht="372" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
         <v>5.4</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
-      <c r="A23">
+    <row r="23" spans="1:5" ht="372" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
         <v>5.4</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
-      <c r="A24">
+    <row r="24" spans="1:5" ht="372" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
         <v>5.4</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
-      <c r="A25">
+    <row r="25" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
         <v>5.4</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
-      <c r="A26">
+    <row r="26" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
         <v>7.1</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27">
+      <c r="E26" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
         <v>7.1</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D27" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28">
+      <c r="D27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
         <v>7.1</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29">
-        <v>7.1</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="E33" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C29" t="s">
-        <v>46</v>
-      </c>
-      <c r="D29" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30">
-        <v>7.1</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="C35" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C30" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="C36" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31">
-        <v>7.1</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="E40" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C31" t="s">
-        <v>46</v>
-      </c>
-      <c r="D31" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32">
-        <v>7.2</v>
-      </c>
-      <c r="B32" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" t="s">
-        <v>53</v>
-      </c>
-      <c r="D32" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33">
-        <v>7.2</v>
-      </c>
-      <c r="B33" t="s">
-        <v>10</v>
-      </c>
-      <c r="C33" t="s">
-        <v>53</v>
-      </c>
-      <c r="D33" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34">
-        <v>7.2</v>
-      </c>
-      <c r="B34" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" t="s">
-        <v>53</v>
-      </c>
-      <c r="D34" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35">
-        <v>7.2</v>
-      </c>
-      <c r="B35" t="s">
-        <v>16</v>
-      </c>
-      <c r="C35" t="s">
-        <v>53</v>
-      </c>
-      <c r="D35" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36">
-        <v>7.2</v>
-      </c>
-      <c r="B36" t="s">
-        <v>19</v>
-      </c>
-      <c r="C36" t="s">
-        <v>53</v>
-      </c>
-      <c r="D36" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37">
-        <v>7.2</v>
-      </c>
-      <c r="B37" t="s">
-        <v>22</v>
-      </c>
-      <c r="C37" t="s">
-        <v>53</v>
-      </c>
-      <c r="D37" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38">
-        <v>7.3</v>
-      </c>
-      <c r="B38" t="s">
-        <v>6</v>
-      </c>
-      <c r="C38" t="s">
-        <v>54</v>
-      </c>
-      <c r="D38" t="s">
-        <v>55</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39">
-        <v>7.3</v>
-      </c>
-      <c r="B39" t="s">
-        <v>10</v>
-      </c>
-      <c r="C39" t="s">
-        <v>54</v>
-      </c>
-      <c r="D39" t="s">
-        <v>48</v>
-      </c>
-      <c r="E39" s="6" t="s">
+      <c r="C43" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40">
-        <v>7.3</v>
-      </c>
-      <c r="B40" t="s">
-        <v>13</v>
-      </c>
-      <c r="C40" t="s">
-        <v>54</v>
-      </c>
-      <c r="D40" t="s">
-        <v>49</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41">
-        <v>7.3</v>
-      </c>
-      <c r="B41" t="s">
-        <v>16</v>
-      </c>
-      <c r="C41" t="s">
-        <v>54</v>
-      </c>
-      <c r="D41" t="s">
-        <v>50</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42">
-        <v>7.3</v>
-      </c>
-      <c r="B42" t="s">
-        <v>19</v>
-      </c>
-      <c r="C42" t="s">
-        <v>54</v>
-      </c>
-      <c r="D42" t="s">
-        <v>60</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43">
-        <v>7.3</v>
-      </c>
-      <c r="B43" t="s">
-        <v>22</v>
-      </c>
-      <c r="C43" t="s">
-        <v>54</v>
-      </c>
-      <c r="D43" t="s">
-        <v>52</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>62</v>
+      <c r="E43" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -2103,216 +2576,262 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="96.6640625" customWidth="1"/>
-    <col min="4" max="4" width="96.33203125" customWidth="1"/>
-    <col min="5" max="5" width="66.6640625" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="11.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="50" style="1" customWidth="1"/>
+    <col min="4" max="4" width="69.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="52.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2">
+    <row r="2" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
+      <c r="C2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
+      <c r="C3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="255" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
+      <c r="C4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6">
+      <c r="C5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7">
+      <c r="C6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8">
+      <c r="C7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9">
+      <c r="C8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>6</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10">
+      <c r="C9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11">
+      <c r="C10" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C11" t="s">
-        <v>75</v>
-      </c>
-      <c r="D11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12">
+      <c r="C11" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
         <v>9</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13">
+      <c r="C12" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
         <v>9</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14">
+      <c r="C13" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
         <v>9</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C14" t="s">
-        <v>75</v>
-      </c>
-      <c r="D14" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15">
+      <c r="C14" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="289" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
         <v>10</v>
       </c>
-      <c r="D15" t="s">
-        <v>81</v>
+      <c r="D15" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug fix & completed chapter 1 (separate Context)
</commit_message>
<xml_diff>
--- a/dataset/testing.xlsx
+++ b/dataset/testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajed/PycharmProjects/Study-on-ChatGPT/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B46EEEE-880C-7C48-95BD-8E56A7BA5582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A15395-22B6-D946-AE73-93973852771B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="28040" windowHeight="17300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="28040" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ch1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="150">
   <si>
     <t>id</t>
   </si>
@@ -87,6 +87,25 @@
 </t>
   </si>
   <si>
+    <t>The given code has a logical error in the for loop that causes it to miss the last element of the array when searching for the last index of a given value. The loop's termination condition is `i &gt; 0`, which means that it will stop iterating one element before the last element of the array. To fix this, the termination condition should be changed to `i &gt;= 0`. So the for loop should be updated as follows:
+```
+for (int i=x.length-1; i &gt;= 0; i--)
+```
+Additionally, the return statement -1 should be outside of the loop, in the case where the element is not found.
+```
+   int result = -1;
+    for (int i=x.length-1; i &gt;= 0; i--)
+      {
+         if (x[i] == y) 
+         {
+            result = i;
+         }
+      }
+      return result;
+```
+This ensures that the function will return -1 only when the element is not found, but will return the last index at which the element was found if the element is in the array.</t>
+  </si>
+  <si>
     <t>b</t>
   </si>
   <si>
@@ -100,6 +119,17 @@
 </t>
   </si>
   <si>
+    <t>A test case that does not execute the fault in this code would be to call the `findLast` method with valid non-null input, where the array `x` contains the value `y` at least once. For example, the following test case would not execute the fault:
+```
+int[] testArray = {1, 2, 3, 4, 5, 5};
+int testValue = 5;
+int lastIndex = findLast(testArray, testValue);
+assert lastIndex == 5;
+```
+Here the test passes as the last index of value `5` in array `testArray` is `5` and it was correctly returned from the function. 
+The fault in the code is the loop condition `i &gt; 0`, it should be `i &gt;= 0` so the loop covers the full range of the array, and it can correctly check the last element of the array. As the condition is `i &gt; 0` the loop will stop before checking the last element, so the function will return -1 in the cases where last element is the element we are looking for, which would be an incorrect result.</t>
+  </si>
+  <si>
     <t>c</t>
   </si>
   <si>
@@ -113,6 +143,14 @@
 </t>
   </si>
   <si>
+    <t>This function appears to search an array of integers (x) for a given value (y), and returns the last index at which that value is found. If the value is not present in the array, the function returns -1. If the input array is null, the function throws a NullPointerException.
+It has a bug, When searching the array in the for-loop, it has a condition to i &gt; 0 instead of i &gt;= 0. which means the function only looks at elements of the array with indexes 1 through n-1, rather than all elements.
+A test case that executes the fault, but does not result in an error state, would involve passing an array that contains the value y at index 0. In this case, the function will not find the value y in the array, because it never looks at the element at index 0, and will incorrectly return -1.
+For example:
+findLast([5,2,3,5], 5) 
+The function will incorrectly return -1 instead of 3</t>
+  </si>
+  <si>
     <t>d</t>
   </si>
   <si>
@@ -126,6 +164,11 @@
 </t>
   </si>
   <si>
+    <t>This method will not result in an error because it properly handles the case where the input array is null by throwing a `NullPointerException`. Additionally, it properly handles the case where the specified value is not found in the array by returning -1. 
+However, it is possible that this method could cause a failure if the input array is not properly checked for nullity before being passed to this method. For example, if the input array is null, and the code that calls this method does not handle the `NullPointerException`, that would cause a failure in the program.
+And also, the for loop which is for finding last index of an element, it's only checking for the last element, As the loop is starting from x.length-1 and it's checking the element only till i&gt;0, so it's not checking for the first index. If we want the function to work correctly, it should be i&gt;=0</t>
+  </si>
+  <si>
     <t>e</t>
   </si>
   <si>
@@ -137,6 +180,10 @@
 The given code contains a fault in the for loop's continuation condition, which will result in an incorrect value being returned by the function. However, this fault does not result in an exception being thrown, so it is not an error in the sense of an exceptional event occurring during the execution of the code.
 Therefore, there are no error states that can be encountered while the code is executing.
 </t>
+  </si>
+  <si>
+    <t>The given code defines a public static method called "findLast" that takes in an integer array "x" and an integer "y" as arguments. The function is supposed to find the last index of the element "y" in the array "x" and return it. If the element "y" is not present in the array, the function should return -1. The function also throws a NullPointerException if the input array "x" is null.
+One of the errors in this code is that the loop used to traverse the array "x" is starting from the last element and going to the second last element. The loop should start at the last element, which is x.length-1, and check if the element at that index is "y". If it is not, then the loop should move to the second last element by decrementing the index i and check again. This loop should continue until either the element "y" is found or the index i becomes less than 0, at which point the loop should exit and return -1, indicating that the element "y" was not found in the array. So the error is on the for loop. It should be "for (int i=x.length-1; i &gt;= 0; i--)".</t>
   </si>
   <si>
     <t>f</t>
@@ -226,6 +273,42 @@
 </t>
   </si>
   <si>
+    <t>The given function has a small error in the for loop condition. The loop should iterate until `i &gt;= 0` instead of `i &gt; 0`. This is because the last element in the array has an index of `x.length - 1`, and we need to include that index in our search.
+Here is the corrected version of the function:
+```
+   public static int findLast (int[] x, int y)
+   {       
+    for (int i=x.length-1; i &gt;= 0; i--)
+      {
+         if (x[i] == y) 
+         {
+            return i;
+         }
+      }
+      return -1;
+   }
+```
+To verify that this version of the function works, you can write test cases using the `assertEquals` method from the `junit` library. 
+```
+import static org.junit.Assert.assertEquals;
+import org.junit.Test;
+public class FindLastTest {
+    @Test
+    public void testFindLast() {
+        int[] array1 = {1, 2, 3, 4, 5};
+        int[] array2 = {1, 2, 3, 4, 5, 5};
+        int[] array3 = {1, 2, 3, 4, 5, 5, 5};
+        int[] array4 = {};
+        assertEquals(4, findLast(array1, 5));
+        assertEquals(5, findLast(array2, 5));
+        assertEquals(6, findLast(array3, 5));
+        assertEquals(-1, findLast(array4, 5));
+    }
+}
+```
+You can see that we are testing for different scenario. Where last element is not present in array, where last element is present in array and where last element is present multiple times.</t>
+  </si>
+  <si>
     <t>/**
    * Find LAST index of zero
    *
@@ -268,6 +351,31 @@
 </t>
   </si>
   <si>
+    <t>The given code is a method that finds the last index of the element 0 in an input array, `x`. It does this by iterating through the array in a forwards order, and returning the first index at which it finds a 0. However, this method has a few issues:
+(1) The method does not handle the case where the last element in the array is 0. The method will only return the index of the first 0 it finds, rather than the last.
+(2) If the input array does not contain 0, the method will return -1, which is the intended behavior. However, it will return -1 even if the input array is empty or if it is not initialized.
+To fix these issues, one way to modify the code as follows:
+```
+   public static int lastZero (int[] x) {
+    if (x == null) {
+      throw new NullPointerException("Input array is null");
+    }
+    if (x.length == 0) {
+      return -1;
+    }
+    int lastZeroIndex = -1;
+    for (int i = x.length - 1; i &gt;= 0; i--) {
+      if (x[i] == 0) {
+        lastZeroIndex = i;
+      }
+    }
+    return lastZeroIndex;
+   }
+```
+We first check the input array if it is null or has a length of 0, returning -1 if either of those cases are true. Then we added an int variable named lastZeroIndex initialized as -1. After that, we are iterating from the end of the array. And when we found 0, we update the lastZeroIndex with current i.
+In this way, it guarantees that even if the last element of the array is 0, the method will still return the correct index. And if no 0 is found in the array, then lastZeroIndex will remain -1 and that will be returned.</t>
+  </si>
+  <si>
     <t xml:space="preserve">
 Since the given code does not contain any faults, any test case that passes a valid input (i.e., an non-null array of integers) to the method would not execute the fault.
 For example, the following test case would not execute the fault:
@@ -280,10 +388,25 @@
 </t>
   </si>
   <si>
+    <t>A test case that does not execute the fault in this method would be to pass in an array that contains at least one zero as an element, and the last element in the array is a zero.
+For example, int[] x = {1, 2, 3, 0} would be a valid test case, as the method would find the last zero in the</t>
+  </si>
+  <si>
     <t xml:space="preserve">
 Since the given code does not contain any faults, it is not possible to provide a test case that executes a fault but does not result in an error state.
 The code simply searches for the last occurrence of the value 0 in an array of integers and returns the index of that occurrence. If the value 0 is not found in the array, the method returns -1. There is no way for the method to execute a fault in this behavior.
 </t>
+  </si>
+  <si>
+    <t>This method will throw a `NullPointerException` if the input array `x` is null. Therefore, a test case that passes a null value as the input parameter would cause this exception to be thrown.
+If the array is not null, a test case that returns the expected output but not an error state would be an input array containing at least one `0` and the last element of the array is `0` so the method will return the last index of `0` in the array.
+example: 
+int[] x = {1,2,3,0,5,0}; 
+assert( lastZero(x) == 5);
+Another test case can be if the array contain only 0's.
+example:
+int[] x = {0,0,0,0,0}; 
+assert( lastZero(x) == 4);</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -310,11 +433,24 @@
 </t>
   </si>
   <si>
+    <t>This method does not have any potential test cases that would result in an error, but not a failure. The only exception thrown by the method is a `NullPointerException` which is thrown when the input array `x` is null. This exception is thrown before the program counter reaches any other lines of code in the method, so it would be considered a failure.
+Additionally, the implementation of the function is simple and doesn't have any logical error that could prevent it from returning the expected value. It will always return the last index of zero in the array or -1 if the zero is not present. If a test case is passed to this function it will successfully complete its execution by returning the value.
+It is possible that if the array is not of int type then the function would throw an exception but in the given implementation it is clearly mentioned that the input to the function is int array which eliminates this case as well.</t>
+  </si>
+  <si>
     <t xml:space="preserve">
 Since the given code does not contain any faults, it is not possible to describe an error state for any test case.
 The code simply searches for the last occurrence of the value 0 in an array of integers and returns the index of that occurrence. If the value 0 is not found in the array, the method returns -1. There is no way for the method to produce an error in this behavior.
 However, if the input to the method is null, a NullPointerException will be thrown, as specified in the method's Javadoc comment. This would be an error, but not a failure, since the program would not crash and the execution would continue after the exception is caught. In this case, the first error state would be the point at which the NullPointerException is thrown, when the program attempts to access the length of a null array.
 </t>
+  </si>
+  <si>
+    <t>The first error state would occur if the input array 'x' is null, causing a `NullPointerException` to be thrown. This is because the method checks for a null input by using a `NullPointerException` and doesn't have any null check, in the body of the method, on the array passed in.
+The state of the error would be:
+- Input array: null
+- Index of last 0: N/A 
+- Exception thrown: NullPointerException with the message "x is null"
+When the method is called with a null array, the for loop in the method body would not be executed because the array does not exist. Instead, the `NullPointerException` would be thrown immediately when the method attempts to access the length of the null array, because it's a null reference.</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -355,6 +491,27 @@
 ```
 This output is the expected result, since the input array is null and the method throws a NullPointerException as specified in the Javadoc comment.
 </t>
+  </si>
+  <si>
+    <t>To find the last index of zero in an array, you can iterate through the array in reverse order and check if the current element is equal to zero. If it is, return the index. If the loop completes without finding a zero, return -1. Here is an updated implementation of the `lastZero` method:
+```
+public static int lastZero (int[] x) {
+    for (int i = x.length - 1; i &gt;= 0; i--) {
+        if (x[i] == 0) {
+            return i;
+        }
+    }
+    return -1;
+}
+```
+You can test your implementation by creating an array of integers and calling the `lastZero` method on it, and comparing the result to what you expect it to be:
+```
+int[] testArray = {1, 2, 3, 0, 4, 5, 0};
+int lastZeroIndex = lastZero(testArray);
+System.out.println("Last zero index: " + lastZeroIndex);
+```
+Expected Output: `Last zero index: 6`
+If the output match the expectation, you can say that the solution is working fine and also can capture the output in some image and that can be your evidence of the solution working.</t>
   </si>
   <si>
     <t>/** 
@@ -383,16 +540,69 @@
 </t>
   </si>
   <si>
+    <t>There are a few things that are wrong with the given code:
+1. The method doesn't check for a null input array. If the input array is null, the code will throw a `NullPointerException` when it tries to access the length of the array. To fix this, you can add a null check at the beginning of the method, like this:
+```
+if (x == null) {
+    throw new NullPointerException("Input array cannot be null");
+}
+```
+2. The method counts positive numbers and zero but doesn't differentiate between them. If you want to count positive numbers only, the if statement should be modified as follows:
+```
+if (x[i] &gt; 0)
+{
+   count++;
+}
+```
+3. Using Java naming convention, it is preferred to have the method name start with small case letter, 
+so it would be better to name it countPositive instead of CountPositive.
+With these modifications, the updated code should look like this:
+```
+public static int countPositive(int[] x) {
+    if (x == null) {
+        throw new NullPointerException("Input array cannot be null");
+    }
+    int count = 0;
+    for (int i = 0; i &lt; x.length; i++) {
+        if (x[i] &gt; 0) {
+            count++;
+        }
+    }
+    return count;
+}
+```
+So, the major issue with the code was the first point, this might lead to a unexpected behavior. Additionally, minor issues is to not make a distinction between positive numbers and zeroes and using naming conventions</t>
+  </si>
+  <si>
     <t xml:space="preserve">
 Since there is no fault or error present in the given code, there is no need to provide a test case to demonstrate the absence of a fault. Any valid test case (that is, a test case that passes in an array of integers as a parameter) will execute correctly with the given implementation. 
 If you have a specific issue or error in mind that you would like to test, please provide more information about the fault or error you are trying to address. 
 </t>
   </si>
   <si>
+    <t>A test case that would not execute the fault would be to pass a non-null array to the function that contains only positive elements. For example: 
+```
+int[] testArray = {1, 2, 3, 4, 5};
+assert(countPositive(testArray) == 5);
+```
+This test case does not execute the fault because the input array is non-null and contains only positive elements, so the for loop will execute normally and correctly count the number of positive elements in the array.
+Also, passing an empty array, array with only negative element, Zero as a element would also not execute the fault as the function is only counting the positive element.</t>
+  </si>
+  <si>
     <t xml:space="preserve">
 Since there is no fault or error present in the given code, there is no need to provide a test case to demonstrate the execution of a fault. The code will execute correctly for any valid input. 
 If you have a specific issue or error in mind that you would like to test, please provide more information about the fault or error you are trying to address. 
 </t>
+  </si>
+  <si>
+    <t>This code counts the number of positive elements in an array, and throws a NullPointerException if the input array is null. A test case that executes the fault but does not result in an error state would involve passing in a null array to the method.
+For example,
+```
+int[] arr = null;
+int result = countPositive(arr);
+```
+This will execute the fault (the method is checking for a null array and throwing an exception) but as the program does not check for the exception throw, it will not result in an error state and the program will terminate immediately.
+It should be noted that this behaviour is considered poor practice and in production code should be handled to prevent unexpected termination and to provide meaningful error messages to users.</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -402,15 +612,100 @@
 </t>
   </si>
   <si>
+    <t>This code snippet throws a `NullPointerException` if the input array `x` is null. This exception is thrown when a program attempts to use a null object reference, which occurs in this case when the `x.length` property is accessed on a null object.
+A test case that would result in an error, but not a failure would be if the input array is null. For example:
+```
+int[] testArray = null;
+try {
+    int count = countPositive(testArray);
+} catch (NullPointerException e) {
+    // Handle the exception here
+}
+```
+In this test case, the function would throw a `NullPointerException`, and the test case would error, but it would not fail because we handle the exception.
+Another way to avoid this error,  and test the function is to add a null check before accessing the length property and return zero. for example:
+```
+public static int countPositive (int[] x){
+      if(x==null) return 0;
+      int count = 0;
+      for (int i=0; i &lt; x.length; i++)
+      {
+         if (x[i] &gt;= 0)
+         {
+            count++;
+         }
+      }
+      return count;
+   }
+```
+in this way the function return zero on null input and it will not throw any exception.</t>
+  </si>
+  <si>
     <t xml:space="preserve">
 Without a specific test case or fault to address, it is not possible to describe an error state. If you have a specific issue or error in mind that you would like to test, please provide more information about the fault or error you are trying to address. 
 </t>
+  </si>
+  <si>
+    <t>It appears that the given test case is missing, which is necessary to know what the error state would be for this specific method. The error state would depend on the specific input provided as well as the expected output. 
+However generally speaking, the first error state that could occur in this code would be if the input array "x" is null. The method throws a NullPointerException in this case as specified in the function signature. As a result, an error message would be produced indicating that a null array was provided as input.</t>
   </si>
   <si>
     <t xml:space="preserve">
 As I mentioned earlier, the given code is a correct implementation of a function that counts the number of positive elements in an array and there is no need to make any repairs. Therefore, it is not necessary to implement a repair or provide a screen printout or other evidence of the program's correctness.
 If you have a specific issue or error that you would like to address, please provide more information about the fault or error and I will do my best to help you.
 </t>
+  </si>
+  <si>
+    <t>Based on the given code snippet, it looks like the function `countPositive` is intended to take an array of integers as an input and return the number of elements in the array that are greater than or equal to 0. However, the function is missing a check to ensure that the input array is not null, which would cause a `NullPointerException` to be thrown when the code attempts to access the length of the array.
+To fix this issue, you can add a null check before the loop that iterates over the array. Here is an updated version of the `countPositive` function that includes the null check:
+```
+public static int countPositive (int[] x) {
+    if (x == null) {
+        throw new NullPointerException("Input array cannot be null");
+    }
+    int count = 0;
+    for (int i = 0; i &lt; x.length; i++) {
+        if (x[i] &gt;= 0) {
+            count++;
+        }
+    }
+    return count;
+}
+```
+You can also handle the case when x is null in a better way, for example in a way that does not raise an exception but only returns -1 as an output.
+```
+public static int countPositive (int[] x) {
+    if (x == null) {
+        return -1;
+    }
+    int count = 0;
+    for (int i = 0; i &lt; x.length; i++) {
+        if (x[i] &gt;= 0) {
+            count++;
+        }
+    }
+    return count;
+}
+```
+In order to verify that the new program works correctly, you can write test cases that pass different arrays (including a null array) to the `countPositive` function and check that it returns the correct results.
+You can write test cases and test the function using Junit or any other testing library.
+```
+@Test
+    public void test_countPositive(){
+        int[] testArray = {1,2,3,4};
+        int expected = 4;
+        int result = countPositive(testArray);
+        assertEquals(expected,result);
+    }
+    @Test
+    public void test_countPositive_null(){
+        int[] testArray = null;
+        int expected = -1;
+        int result = countPositive(testArray);
+        assertEquals(expected,result);
+    }
+```
+If the new program works as expected, the test cases will pass without any issues, Otherwise, you'll get an assertion error.</t>
   </si>
   <si>
     <t>/**
@@ -455,6 +750,47 @@
 ```</t>
   </si>
   <si>
+    <t>The given code seems to be correctly counting the number of elements in the array 'x' that are either odd or positive (or both), and correctly throwing a `NullPointerException` if the input array is null. However, it could be improved in some ways.
+One issue is that it doesn't check for negative integers, so it could count negative integers as well which is against the requirement of counting positive elements only. In that case  we need to check if the element is greater than zero instead of checking only if the element is not negative.
+```
+  if (x[i]%2 == 1 || x[i] &gt; 0)
+   {
+      count++;
+   }
+```
+can be replaced with
+```
+ if (x[i]%2 == 1 || (x[i] &gt; 0) )
+   {
+      count++;
+   }
+```
+Another issue is that it does not check for empty array, so if an empty array is passed then it will throw ArrayIndexOutOfBoundsException. To handle this we can check if length of array is greater than zero before the loop starts.
+```
+   if (x.length == 0) return 0; 
+```
+Here's the updated code that takes into account these two issues :
+```
+public static int oddOrPos (int[] x)
+   {
+      if (x == null) {
+          throw new NullPointerException("Input array is null");
+      }
+      if (x.length == 0) return 0;
+      int count = 0;
+      for (int i = 0; i &lt; x.length; i++)
+      {
+         if (x[i]%2 == 1 || (x[i] &gt; 0) )
+         {
+            count++;
+         }
+      }
+      return count;
+   }
+```
+By doing so, we have a more robust code that will handle cases where the input array is null, empty or contains only negative elements and also implement the requirement of counting only positive elements.</t>
+  </si>
+  <si>
     <t>It is not possible to give a test case that does not execute the fault, because the fault in the code is that it does not handle the case where an element in the array is negative and odd. Any array that contains at least one negative and odd element will execute the fault.
 For example, the following test case would execute the fault:
 ```
@@ -464,6 +800,11 @@
 In this case, the value of count would be 3, because the negative and odd element (-3) is not counted by the code.</t>
   </si>
   <si>
+    <t>A test case that does not execute the fault would be to pass in an array of integers that contains only positive and/or odd integers. For example, the array `{1, 3, 5, 7, 9}` would not execute the fault, because all of the elements in the array are odd integers and the function would correctly return `5` as the count of odd or positive elements.
+Another test case could be passing in an empty array or even array of zero, which in that case the for loop won't run and the function will return 0 as expected.
+It's worth noting that the function has a null check and throws NullPointerException if the input array is null, meaning that passing a null array will result in the fault in this case, which is desirable and expected.</t>
+  </si>
+  <si>
     <t xml:space="preserve">It is not possible to give a test case that executes the fault but does not result in an error state, because the fault in the code is that it does not handle the case where an element in the array is negative and odd. Any array that contains at least one negative and odd element will execute the fault, and the result of the oddOrPos() function will not be correct.
 For example, the following test case would execute the fault:
 ```
@@ -472,6 +813,11 @@
 ```
 In this case, the value of count would be 3, which is incorrect. The correct value would be 4, because all elements in the array are either odd or positive (or both).
 </t>
+  </si>
+  <si>
+    <t>This code is checking if the elements in the array `x` are either odd or positive, and if so, it increments a count. If the array passed as an argument is null, the code throws a `NullPointerException`.
+It is not possible to give a test case that would execute the fault (i.e., passing a null array as an argument) without resulting in an error state because the code specifically checks for this case and throws an exception. So in this scenario, even if you pass the Null value as argument, it will throw an Exception.
+The function is working as expected and the Exception makes sure that it will not able to run on null input.</t>
   </si>
   <si>
     <t>It is not possible to give a test case that results in an error but not a failure, because the fault in the code is not related to error handling. The fault is that the code does not handle the case where an element in the array is negative and odd. This will not result in an error or a failure, but the result of the oddOrPos() function will not be correct.
@@ -487,11 +833,30 @@
 In this case, the code will throw a NullPointerException when it attempts to access the length of the null array, as expected.</t>
   </si>
   <si>
+    <t>This code will throw a `NullPointerException` if the input array `x` is null. This is because the first line of the method checks for a null value before counting the odd or positive elements in the array, and throws an exception if the input is null.
+A test case that would result in this error would be to call the method with a null array:
+```
+int[] x = null;
+oddOrPos(x);
+```
+This will throw an error, but not a failure, because the error (throwing a `NullPointerException`) is expected behavior and handled by the method itself.
+It should be noted that if test case is covered and handled properly then it should be considered failure. 
+It will fail the test case rather than throwing exception.</t>
+  </si>
+  <si>
     <t>The first error state in the test case occurs when the oddOrPos() function is called with a null array. This results in the following error state:
 - The program counter is at the line where the oddOrPos() function is called.
 - The input array x is null.
 - The NullPointerException has not yet been thrown.
 This error state occurs before the function has a chance to execute any of its code, because the NullPointerException is thrown as soon as the function tries to access the length of the null array.</t>
+  </si>
+  <si>
+    <t>The first error state for this method would be if the input array `x` is `null`. In this case, the method would throw a `NullPointerException` when it attempts to access the length of the array. The complete state at this point would be as follows:
+- `x`: `null`
+- `count`: undefined
+- `i`: undefined
+and the method would throw the NullPointerException at this point.
+Note: Also in addition to `NullPointerException` If array is not initialized and the passed parameter is empty array the same exception would be thrown.</t>
   </si>
   <si>
     <t>Here is the modified code that handles the case where the input array is null:
@@ -532,6 +897,13 @@
 The output of this code is as expected, indicating that the modified code is correct.</t>
   </si>
   <si>
+    <t>This code appears to be a Java method for counting the number of elements in an array that are either odd or positive (or both). The method first checks if the input array `x` is null, and throws a `NullPointerException` if it is. If the input array is not null, the method then iterates through each element of the array, and checks if the element is odd (by using the modulus operator to check if the element is not divisible by 2) or if the element is positive (greater than 0). If either of these conditions is true, the count variable is incremented. Finally, the method returns the count of elements that meet the criteria.
+It appears that the requirement is to fix the code to correctly count all elements of the array that are either odd or positive, and not just odd. To fix the code, we could change the if statement to check 
+```if (x[i] % 2 != 0 || x[i] &gt; 0)``` 
+The current if statement check for x[i] &gt; 0 but in case the element is negative and even it will be considered as not odd or positive. But if we use above if statement it will take care of even positive numbers too.
+Please verify the output for the given test cases and consider it as a evidence for the new program working.</t>
+  </si>
+  <si>
     <t>Consider the following three example classes. These are OO faults taken from Joshua Bloch’s
 Effective Java, Second Edition. Answer the following questions about each.
 class Vehicle implements Cloneable
@@ -604,6 +976,36 @@
 </t>
   </si>
   <si>
+    <t>The code as written has a number of issues with it related to its use of the `clone()` method.
+First, the `Vehicle` class implements the `Cloneable` interface, but its `clone()` method does not properly override the `Object.clone()` method, which is specified to throw a `CloneNotSupportedException`. Instead, it simply creates a new `Vehicle` object and assigns it the value of the current object's `x` field. This can be corrected by adding the `@Override` annotation to the `clone()` method to indicate that it is intended to override a superclass method, and by adding a try-catch block to handle the `CloneNotSupportedException`.
+```
+@Override
+protected Object clone() throws CloneNotSupportedException {
+    return super.clone();
+}
+```
+Second, the `Truck` class attempts to override the `clone()` method inherited from `Vehicle` in order to properly copy its additional `y` field, but it does so in an incorrect way. The method calls the `clone()` method of the superclass and then attempts to cast the result to a `Truck` object, and sets the `y` field of the result to the value of the current object's `y` field. However, the result of calling the `clone()` method of the `Vehicle` class is actually an `Object`, not a `Truck`, so the cast will throw a `ClassCastException`.
+One correct approach to resolve this issue is by using the copy constructor, that is :
+```
+@Override
+public Truck clone() throws CloneNotSupportedException {
+    return new Truck(this);
+}
+private Truck(Truck truck) {
+    super(truck.x);
+    this.y = truck.y;
+}
+```
+Additionally, this class should also override the `getClass()` method so that it returns the correct class name and that it can assert the expected outcome.
+```
+@Override
+public Class&lt;? extends Truck&gt; getClass(){
+    return this.getClass();
+}
+```
+Thus the code will be more robust.</t>
+  </si>
+  <si>
     <t>If possible, give a test case that does not execute the fault. If not, briefly explain why
 not.</t>
   </si>
@@ -614,6 +1016,27 @@
 </t>
   </si>
   <si>
+    <t>In this example, the fault lies in the `Truck.clone()` method at Location "B". When the `super.clone()` method is called in the `Truck` class, it returns an object of type `Vehicle`, which cannot be cast to type `Truck` without throwing a `ClassCastException`. This happens because the `clone()` method in the `Vehicle` class is not implemented correctly. It should be implementing a proper and deep copy of the object and not just returning a new object with the same values.
+A test case that does not execute this fault would involve creating an instance of the `Vehicle` class, instead of the `Truck` class, and calling the `clone()` method on it. For example:
+```
+Vehicle car = new Vehicle(4);
+Vehicle carClone = car.clone();
+```
+In this case, the `clone()` method would execute correctly without any issues, as it only calls `super.clone()` once, and it will return an object of the correct type.
+Another way to avoid the fault is to override the `clone()` method on the parent class, `Vehicle` in a correct way like using `copy constructor` and return the correct type.
+```
+class Vehicle implements Cloneable {
+...
+public Vehicle(Vehicle that) {
+    x = that.x;
+}
+public Vehicle clone(){
+    return new Vehicle(this);
+}
+```
+In this case, when `Truck` class will call `super.clone()`, it will have the correct type.</t>
+  </si>
+  <si>
     <t>If possible, give a test case that executes the fault, but does not result in an error state.
 If not, briefly explain why not.</t>
   </si>
@@ -622,6 +1045,21 @@
 It is not possible to give a test case that executes the fault but does not result in an error state, because the fault in the given code always results in an error state. The fault in the `Vehicle` class is that it does not call the `clone()` method of the `Object` class and handle the `CloneNotSupportedException` that it may throw, and instead simply creates a new instance of the `Vehicle` class. This results in a `CloneNotSupportedException` being thrown when the `clone()` method is called, because the `clone()` method of the `Object` class is not being called to perform the necessary field-by-field copy of the object being cloned.
 The fault in the `Truck` class is that it also does not call the `clone()` method of the `Object` class and handle the `CloneNotSupportedException` that it may throw, and instead relies on the faulty implementation in the `Vehicle` class. Additionally, the `Truck` class casts the result of the call to the `clone()` method of the `Vehicle` class to a `Truck` object without checking if the object is actually an instance of the `Truck` class, which can result in a `ClassCastException` being thrown at runtime. Therefore, any test case that calls the `clone()` method on a `Truck` object will result in either a `CloneNotSupportedException` being thrown (if the `clone()` method of the `Object` class is called and throws the exception) or a `ClassCastException` being thrown (if the `clone()` method of the `Object` class is not called and the result of the call to the `clone()` method of the `Vehicle` class is cast to a `Truck` object without checking its type).
 </t>
+  </si>
+  <si>
+    <t>The code for the `Vehicle` class correctly implements the `clone()` method by creating a new object of the `Vehicle` class and copying the value of the `x` field to the new object. However, the `Truck` class, which extends `Vehicle`, has a problem with its implementation of the `clone()` method.
+The issue with the `Truck` class's implementation is that it calls `super.clone()`, which creates a new object of type `Vehicle`, but then tries to cast it to `Truck` using the line `((Truck) result).y = this.y;`. This is problematic because the new object created by the `Vehicle` class's `clone()` method is not guaranteed to be of type `Truck`, and so the cast will throw a `ClassCastException` at runtime.
+In order for the fault not to result in an error state, one way to fix the code is to change the `clone()` method in the `Truck` class as follows:
+```
+public Object clone()
+{
+    Truck result = new Truck(this.x);
+    result.y = this.y;
+    return result;
+}
+```
+The above modification ensures that the created object will be of type `Truck` and the cast will not be necessary, thus preventing the ClassCast Exception. Also, this overrides the clone method of the super class making it more specific and the expected behaviour of the object when cloned.
+Alternatively, if the class is not supposed to be cloned and its not an important requirement for the class, the Cloneable interface can be removed from the class and the clone method in the truck class can be removed or it can throw a CloneNotSupportedException</t>
   </si>
   <si>
     <t>If possible, give a test case that results in an error, but not a failure. If not, briefly
@@ -633,6 +1071,13 @@
 In the case of the given code, any test case that calls the `clone()` method on a `Truck` object will result in either a `CloneNotSupportedException` being thrown (if the `clone()` method of the `Object` class is called and throws the exception) or a `ClassCastException` being thrown (if the `clone()` method of the `Object` class is not called and the result of the call to the `clone()` method of the `Vehicle` class is cast to a `Truck` object without checking its type). In either case, the program will terminate abruptly, resulting in a failure.
 It is not possible to recover from an error in a program, because the program's execution has been disrupted and it is no longer possible to continue running the program in a predictable and correct manner. Therefore, any test case that executes the fault in the given code will result in a failure.
 </t>
+  </si>
+  <si>
+    <t>In this example, the `Vehicle` class and `Truck` class both implement the `clone()` method. The `Vehicle` class's `clone()` method creates a new `Vehicle` object with the same value for the private variable `x` as the original object, and returns it. The `Truck` class's `clone()` method first calls the `clone()` method in the superclass (`Vehicle`) to create a new object with the same value for `x`, and then sets the private variable `y` of the new object to the same value as the original object.
+In the test case provided, we create a `Truck` object with the value 4 for the variable `z`. We then call the `clone()` method on this object and assign the returned object to a variable named `co`. The expected outcome is that `suv.x = co.x` and `suv.getClass() = co.getClass()`.
+However, there is an issue with this implementation. When the `clone()` method in the `Truck` class is called, it first calls the `clone()` method in the `Vehicle` class, which returns an object of type `Vehicle`. The `Truck` class then tries to cast this `Vehicle` object to a `Truck` object in order to set the private variable `y`, and this will throw a `ClassCastException` at location "B".
+As the code throws an exception the test case will fail, we don't have an error without a failure in this example.
+To fix this issue, Bloch suggests that, a better alternative would be to use the `clone()` method with a `protected` access modifier in the superclass, and then override it in the subclass to use `super.clone()`, this would make the object that is returned is an instance of the correct class.</t>
   </si>
   <si>
     <t>In the given code, describe the first error state. Be sure to describe the complete state.</t>
@@ -650,6 +1095,11 @@
 7. The `clone()` method of the `Truck` class returns control to the calling code, and the `CloneNotSupportedException` is propagated to the calling code.
 In this error state, the program is terminated and a `CloneNotSupportedException` is thrown, indicating that the object being cloned does not support cloning. This error state results in a failure of the program.
 </t>
+  </si>
+  <si>
+    <t>The first error state in the given code occurs when the `clone()` method of the `Truck` class is called, and the returned object is cast to a `Truck` object at location "B". This cast can throw a `ClassCastException`, because the returned object is of type `Vehicle` (the superclass of `Truck`) and not of type `Truck`.
+In the case of this example, the problem is that the `Vehicle` class is implementing the `Cloneable` interface but the implementation of the `clone()` method is returning an object of the type `Vehicle`. The `clone()` method of the `Truck` class is then trying to cast that returned object to a `Truck` which will result in ClassCastException
+To resolve this, Joshua Bloch recommends a better approach which is to use a copy constructor or factory method which is more typesafe and less prone to error.</t>
   </si>
   <si>
     <t>Implement your repair and verify that the given test now produces the expected output.
@@ -701,6 +1151,39 @@
 Test passed
 ```
 </t>
+  </si>
+  <si>
+    <t>The current implementation of the `clone()` method in the `Vehicle` class and the `Truck` class have a few issues that need to be addressed in order for the program to work as expected. 
+First, the `Vehicle` class implements the `Cloneable` interface, which is a marker interface that indicates that an object can be cloned. However, it does not actually override the `clone()` method from `Object`, but instead provides its own implementation of `clone()` that calls the default constructor for the `Vehicle` class to create a new object and then copies the value of the `x` field. But this is not the correct way of implementing the clone, as per the Effective Java, Bloch Suggests to use `super.clone()` in order to create a field-by-field copy of the object.
+Secondly, the `Truck` class overrides the `clone()` method in the `Vehicle` class, but it does not properly handle the field-by-field copy of the object. it's calling `super.clone()` correctly but its also trying to cast the returned object as `Truck` which may throw ClassCastException if returned object is not of type `Truck`.
+To fix these issues, I would suggest the following changes to the code:
+In the `Vehicle` class, I would remove the `Cloneable` interface and instead, override the `clone()` method from `Object` and use `super.clone()` instead of calling the default constructor. Also added a runtime Exception in case of unexpected error:
+```
+@Override
+protected Vehicle clone() {
+    try {
+        return (Vehicle) super.clone();
+    } catch (CloneNotSupportedException e) {
+        throw new RuntimeException(e);
+    }
+}
+```
+In the `Truck` class, I would 
+- remove the `clone()` method as we are using the `clone()` method from `Vehicle` class
+- Add a copy constructor that takes a `Truck` object as its argument and copies its fields
+```
+Truck(Truck truck) {
+    super(truck);
+    this.y = truck.y;
+}
+```
+In the test `Truck suv = new Truck (4); Truck co = suv.clone()`
+- Instead of calling `suv.clone()`, I would call the copy constructor and create a new `Truck` object that is a copy of the `suv` object
+```
+Truck suv = new Truck(4);
+Truck co = new Truck(suv);
+```
+This way, the test `Truck suv = new Truck (4); Truck co = suv.clone()` will produce the expected output, with `suv.x = co.x` and `suv.getClass() = co.getClass()` without throwing any exception, as the program is properly creating a field-by-field copy of the object using the copy constructor.</t>
   </si>
   <si>
     <t xml:space="preserve"> Consider the following three example classes. These are OO faults taken from Joshua Bloch’s
@@ -734,10 +1217,42 @@
 </t>
   </si>
   <si>
+    <t>The problem with the given code is that it uses the `BigDecimal` class, which has an inconsistent implementation of the `equals()` and `compareTo()` methods. Specifically, the code creates two `BigDecimal` objects, `x` and `y`, which have the same value but different internal representations. When these objects are added to a `TreeSet`, the `compareTo()` method is used to determine their relative ordering, so only one element (`x` or `y`) is added to the set. But when they are added to a `HashSet`, the `equals()` method is used to determine equality, so both elements are added to the set.
+To fix this issue, you could modify the `BigDecimal` class to ensure that the `equals()` and `compareTo()` methods are consistent with each other. One way to do this would be to override the `equals()` method in `BigDecimal` so that it uses the same comparison as the `compareTo()` method. For example:
+```
+class BigDecimal {
+    // existing code...
+    @Override
+    public boolean equals(Object o) {
+        if (o == this) return true;
+        if (!(o instanceof BigDecimal)) return false;
+        return this.compareTo((BigDecimal) o) == 0;
+    }
+}
+```
+This modification ensures that two `BigDecimal` objects are equal only if they compare as equal. 
+(b) Explain how the fault could be discovered.
+The fault could be discovered by creating test cases which use a `TreeSet` and `HashSet` and check the output by printing it. In this example, The test case which will cause a bug will be the  `BigDecimalTree.add(x); BigDecimalTree.add(y);` and `BigDecimalHash.add (x); BigDecimalHash.add (y);`  where it is expected that the `BigDecimalTree` will have only one element but it will have 2, and `BigDecimalHash` will have 2 elements but it will have only one.
+It could also be discovered by reviewing the implementation of the `equals()` and `compareTo()` methods in the `BigDecimal` class, and noting that they use different comparison techniques.
+(c) Explain how the fault could be prevented in the future.
+The fault could be prevented in the future by following some of the best practices in implementing `equals()` and `compareTo()` method.
+- The `equals()` method should be consistent with the `compareTo()` method, so that if two objects are equal according to `equals()`, they should compare as equal according to `compareTo()`.
+- The `equals()` method should be reflexive, symmetric, transitive, and consistent.
+- The `compareTo()` method should be consistent with `equals()`, it should also be transitive, and should always return an int.
+- It is also important to follow the contract of `equals()` and `compareTo()` defined by the `Object` and `Comparable` class respectively.
+- Also, it's important to test the classes that has such methods to make sure it's properly working.</t>
+  </si>
+  <si>
     <t xml:space="preserve">
 It is not possible to give a test case that does not execute the fault in the given code, because the fault is inherent in the implementation of the `BigDecimal` class. The fault occurs whenever the `BigDecimal` objects `x` and `y` are used with a collection that relies on either the `equals` or `compareTo` methods for comparison, regardless of the specific values of `x` and `y`.
 The fault occurs because the `equals` and `compareTo` methods of the `BigDecimal` class are implemented in a way that is inconsistent with each other. The `equals` method returns `false` for the `BigDecimal` objects `x` and `y`, but the `compareTo` method returns `0` for the same objects, indicating that they are equal. This inconsistency can lead to unexpected behavior when using the `BigDecimal` objects with collections that rely on either the `equals` or `compareTo` methods for comparison.
 </t>
+  </si>
+  <si>
+    <t>This class demonstrates a problem with the implementation of the `equals()` and `compareTo()` methods in the `BigDecimal` class. The `equals()` method returns `false` when comparing the `x` and `y` variables, even though their values are equal. The `compareTo()` method, on the other hand, returns `0` indicating that the values are equal. This inconsistency causes problems when using a `BigDecimal` with a collection class like `TreeSet` or `HashSet`.
+In the example, a `TreeSet` is created and both `x` and `y` are added to the set. Because `TreeSet` uses the `compareTo()` method to compare elements, the set only contains one element, despite the fact that `x` and `y` have different values according to `equals()`. A `HashSet` is also created and `x` and `y` are added to it. As `HashSet` uses the `equals()` method to compare elements, the set contains two elements, as expected.
+It would be possible to create a test case that does not execute the fault by using `BigDecimal` values that return `true` when passed to the `equals()` method, and `0` when passed to the `compareTo()` method. This would ensure consistency between the two methods, and prevent problems when using `BigDecimal` with collection classes.
+Alternatively, we can use the `java.math.MathContext` class to pass the precision and rounding rule for the BigDecimal value. This way we can be sure that the BigDecimal value will be created with desired precision and rounding rule. And hence it is possible to avoid the faulty behavior.</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -761,16 +1276,31 @@
 </t>
   </si>
   <si>
+    <t>In this example, the problem is that the `BigDecimal` class has inconsistent behavior between its `equals` and `compareTo` methods. Specifically, `x` and `y` are two `BigDecimal` objects that are equal according to `compareTo` (`x.compareTo(y) == 0`), but not equal according to `equals` (`!x.equals(y)`). 
+This causes issues when using `BigDecimal` objects with collections that rely on either `equals` or `compareTo` for their implementation, such as the `TreeSet` and `HashSet` used in this example. 
+If you use a `TreeSet`, which uses `compareTo` for ordering and removing duplicates, it will only contain one element, whereas a `HashSet` which uses `equals`, will contain both of the element
+It's not possible to give a test case that executes the fault and does not result in an error state. Because the fault is in the implementation of the `BigDecimal` class itself, any use of `BigDecimal` objects with collections that rely on `equals` or `compareTo` will result in unexpected behavior. In order to fix this issue, you would need to modify the implementation of the `BigDecimal` class to make the `equals` and `compareTo` methods consistent with each other.</t>
+  </si>
+  <si>
     <t xml:space="preserve">
 It is not possible to give a test case that results in an error but not a failure for the given code, because the code does not contain any syntax errors or runtime exceptions. The code simply creates and uses two `BigDecimal` objects and two collections, which are all valid operations.
 The fault in the given code is not an error, but rather an inconsistency in the implementation of the `equals` and `compareTo` methods of the `BigDecimal` class. This inconsistency can lead to unexpected behavior when using the `BigDecimal` objects with collections that rely on either the `equals` or `compareTo` methods for comparison, such as the `TreeSet` and `HashSet` in the example. However, this behavior is not considered an error, as it does not result in a syntax error or a runtime exception.
 </t>
   </si>
   <si>
+    <t>The code you've provided is an example of a class that demonstrates a problem with the `BigDecimal` class, specifically the inconsistency between its `equals()` and `compareTo()` methods. In this example, `x` and `y` are two `BigDecimal` objects that have the same value but are not considered equal by the `equals()` method. 
+The code creates two sets, `BigDecimalTree` and `BigDecimalHash`, both of which are initialized with the `x` and `y` values. However, because `TreeSet` uses the `compareTo()` method for ordering elements and determining uniqueness, and `HashSet` uses the `equals()` method, the two sets end up with different numbers of elements. 
+In order to demonstrate a case which result in an error, but not a failure one can try use BigDecimal to write a program that performs some computation and compares the results of the computation to an expected value. 
+For example, if you use BigDecimal to perform a financial calculation, and you expect the result to be exactly $1.00, but due to the inconsistency in the equals and compareTo methods it comes out to be $1.0. The program will continue to run correctly but the results will not be as expected. Here the program will not fail but it will give the unexpected results.</t>
+  </si>
+  <si>
     <t xml:space="preserve">
 There is no error state in the given code. The code simply creates and uses two `BigDecimal` objects and two collections, which are all valid operations.
 The fault in the given code is not an error, but rather an inconsistency in the implementation of the `equals` and `compareTo` methods of the `BigDecimal` class. This inconsistency can lead to unexpected behavior when using the `BigDecimal` objects with collections that rely on either the `equals` or `compareTo` methods for comparison, such as the `TreeSet` and `HashSet` in the example. However, this behavior is not considered an error, as it does not result in a syntax error or a runtime exception.
 </t>
+  </si>
+  <si>
+    <t>The first error state in the given code is that the `BigDecimalTree` Set only contains one element (1.0) instead of two (1.0 and 1.00) as expected. This is because the `TreeSet` class uses the `compareTo()` method to determine equality of elements, whereas the `BigDecimal` class has an inconsistent implementation of `compareTo()` and `equals()`, such that `x.compareTo(y) == 0` but `!x.equals(y)`. Since `x` and `y` are not considered equal according to `equals()`, they are both added to the `BigDecimalTree` Set, resulting in only one element in the set.</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -807,6 +1337,26 @@
 </t>
   </si>
   <si>
+    <t>The problem with the given code is that in BigDecimal, the equals() and compareTo() methods are inconsistent, which causes unexpected behavior when using the BigDecimal class in a Set. Specifically, when adding x and y to a TreeSet, only one element is added because TreeSet uses compareTo(), and x.compareTo(y) returns 0. However, when adding x and y to a HashSet, both elements are added because HashSet uses equals() and x.equals(y) returns false.
+One way to "repair" this problem would be to override the equals() method in BigDecimal to be consistent with compareTo(). A possible implementation would be to use the following in the BigDecimal class:
+```
+@Override
+public boolean equals(Object o) {
+    if (o instanceof BigDecimal) {
+        return compareTo((BigDecimal) o) == 0;
+    }
+    return false;
+}
+```
+This implementation of equals uses compareTo() to compare two BigDecimal objects and returns true only if they are equal according to compareTo() (i.e., when compareTo() returns 0). This ensures that the behavior of equals is consistent with the behavior of compareTo.
+The test case you mentioned in your question should now work as expected and will give the output:
+```
+BigDecimalTree = 1
+BigDecimalHash = 1,1
+```
+Please Note that this implementation is based on the assumption that, compareTo() implementation already correct, as you have mentioned "suppose we decide that compareTo() is correct, and that equals() is faulty"</t>
+  </si>
+  <si>
     <t xml:space="preserve">Consider the following three example classes. These are OO faults taken from Joshua Bloch’s
 Effective Java, Second Edition. Answer the following questions about each.
 class Point
@@ -884,22 +1434,75 @@
 </t>
   </si>
   <si>
+    <t>The class `ColorPoint` is a subclass of `Point`, and it extends the state of the `Point` class by adding a color field. However, the implementation of the `equals` method in the `ColorPoint` class fails to take this into account.
+In the `equals` method at Location B, it first checks if the object passed in is an instance of `ColorPoint` using the `instanceof` operator. If it is not, it immediately returns `false`. This means that a `Point` object and a `ColorPoint` object with the same x and y coordinates will be considered not equal, even though they should be.
+To fix this, the check at Location B should be modified to check if the passed in object is an instance of `Point` instead of `ColorPoint`. This way, a `Point` object and a `ColorPoint` object with the same x and y coordinates will be considered equal. Additionally, `ColorPoint` should override `hashCode` method if it also overrode `equals` to be compliant with general contract for `hashCode()` and `equals()`
+```
+@Override public boolean equals (Object o) {
+    if (!(o instanceof Point)) return false;
+    if (!(o instanceof ColorPoint)) {
+        Point p = (Point) o;
+        return (p.x == this.x) &amp;&amp; (p.y == this.y);
+    }
+    ColorPoint cp = (ColorPoint) o;
+    return (super.equals(cp) &amp;&amp; (cp.color == this.color));
+}
+@Override public int hashCode() {
+    int result = super.hashCode();
+    result = 31 * result + (color != null ? color.hashCode() : 0);
+    return result;
+}
+```
+and then use it in the same way as `equals` method:
+```
+Point p = new Point (1,2);
+ColorPoint cp1 = new ColorPoint (1,2,RED);
+ColorPoint cp2 = new ColorPoint (1,2,BLUE);
+p.equals (cp1); // should return true
+cp1.equals (p); // should return true
+cp1.equals (cp2); // should return false
+```
+By doing this, `equals` would now correctly handle the case where it is passed an object of a superclass, and the above test cases would produce the expected results.</t>
+  </si>
+  <si>
     <t xml:space="preserve">
 It is not possible to give a test case that does not execute the fault in the given code because the fault is present in the implementation of the `equals` method in both the `Point` and `ColorPoint` classes. The fault in the `Point` class is that the method does not properly override the `equals` method in the `Object` class, and the fault in the `ColorPoint` class is that the method does not properly handle the case where it is passed an object that is not an instance of `ColorPoint`. These faults are present in the implementation of the `equals` method in both classes and will be executed every time the method is called.
 To avoid executing the fault, the implementation of the `equals` method in both classes must be modified to properly override the `equals` method in the `Object` class and handle the case where it is passed an object that is not an instance of the class. The modified `equals` methods for both classes were provided in the previous response.
 </t>
   </si>
   <si>
+    <t>The fault in this example is that the class `ColorPoint` extends the `Point` class, and adds a new field `color` to represent a color property. However, the `equals` method in `ColorPoint` only checks if the `color` field is equal, but doesn't check the fields in the superclass `Point`. This means that if a `Point` object and a `ColorPoint` object have the same x and y coordinates but different colors, the `equals` method will return `false`, even though they should be considered equal. 
+Test case that does not execute the fault would be : 
+    ColorPoint cp1 = new ColorPoint(1,2, RED);
+    ColorPoint cp2 = new ColorPoint(1,2, RED);
+    cp1.equals(cp2);// both have same x,y,color so this should return true
+As we are using same color for both object and x,y coordinates is also same so it will not execute the fault because in this case it will check both fields of superclass and color field also.</t>
+  </si>
+  <si>
     <t xml:space="preserve">
 It is not possible to give a test case that executes the fault in the given code but does not result in an error state because the fault in the `Point` class will always result in an error state (i.e., a `ClassCastException` will be thrown) when the `equals` method is called with an object that is not an instance of the `Point` class. The fault in the `ColorPoint` class will also always result in an error state (i.e., a `ClassCastException` will be thrown) when the `equals` method is called with an object that is not an instance of the `ColorPoint` class.
 To avoid these error states, the implementation of the `equals` method in both classes must be modified to properly handle the case where it is passed an object that is not an instance of the class. The modified `equals` methods for both classes were provided in a previous response.
 </t>
   </si>
   <si>
+    <t>Class Point defines an `equals` method that compares two points for equality based on their x and y coordinates. Class ColorPoint is a subclass of Point, and adds an additional color field to the Point class. 
+In the implementation of the `equals` method in the ColorPoint class, the method first checks if the object passed as a parameter is an instance of ColorPoint by using the `instanceof` operator. If it is not, the method returns false. Then, it performs an additional check to see if the color field of the ColorPoint instance is equal to the color field of the object passed as a parameter. If this is true, then the method returns true. The implementation also calls `super.equals(cp)` in the overriding method which check if the x and y coordinates of the two objects are equal.
+Test1 : Point p = new Point (1,2); ColorPoint cp1 = new ColorPoint (1,2,RED);
+p.equals (cp1);
+In this test case, the object passed as a parameter to the `equals` method of the Point class is an instance of ColorPoint. Since the implementation of the `equals` method in the Point class does not check the class of the object passed as a parameter, the method simply compares the x and y fields of the Point and ColorPoint instances, which are equal in this case, so the method returns true. However, this is not the expected result. Because the Point class does not have knowledge of the color field of ColorPoint, this test produces an error state.
+This is a example of a common problem known as "Liskov Substitution Principle" violation, where a subclass is not substitutable for its superclass.</t>
+  </si>
+  <si>
     <t xml:space="preserve">
 It is not possible to give a test case that results in an error but not a failure for the given code because the fault in the `Point` class will always result in a failure (i.e., a `ClassCastException` will be thrown) when the `equals` method is called with an object that is not an instance of the `Point` class. The fault in the `ColorPoint` class will also always result in a failure (i.e., a `ClassCastException` will be thrown) when the `equals` method is called with an object that is not an instance of the `ColorPoint` class.
 To avoid these failures, the implementation of the `equals` method in both classes must be modified to properly handle the case where it is passed an object that is not an instance of the class. The modified `equals` methods for both classes were provided in a previous response.
 </t>
+  </si>
+  <si>
+    <t>In this example, there is a problem with the implementation of the equals method in the ColorPoint class. The problem is that the implementation in the ColorPoint class only checks for equality if the compared object is also a ColorPoint, rather than checking for equality with any object of the Point class. This can lead to unexpected behavior.
+Test 1 (p.equals(cp1)) and Test 2 (cp1.equals(p)) results in unexpected behavior as well. It should return true for both cases but because of the implementation it returns true for test 1 and false for test 2.
+As for your question about test cases that result in an error but not failure. If there's no exception is thrown and the method is just not returning the correct value, this means that the error would not lead to a failure. However, it could lead to unexpected behavior or bugs in the program that use these classes.
+An example of a test case that results in an error but not a failure would be, for instance, if you have a Set of Point objects and you add both a Point object and a ColorPoint object with the same x and y coordinates, they would be considered different because of their type, and would both be added to the set, thus breaking the expected semantics of a set.</t>
   </si>
   <si>
     <t xml:space="preserve"> In the given code, describe the first error state. Be sure to describe the complete state.</t>
@@ -1287,26 +1890,6 @@
     <t>Demonstrate the problem with Point using a HashSet.</t>
   </si>
   <si>
-    <t>Write down the mathematical relationship required between equals() and hashCode().</t>
-  </si>
-  <si>
-    <t>Write a simple JUnit test to show that Point objects do not enjoy this property.</t>
-  </si>
-  <si>
-    <t>Repair the Point class to fix the fault.</t>
-  </si>
-  <si>
-    <t>Rewrite your JUnit test as an appropriate JUnit theory. Evaluate it with suitable DataPoints.</t>
-  </si>
-  <si>
-    <t>Replace each occurrence of a set with a list in the JUnit theory removeThenAddDoesNotChangeSet. Is the resulting theory valid or invalid? How many of the tests that pass the precondition also pass the postcondition? Explain.</t>
-  </si>
-  <si>
-    <t>It is not possible for me to accurately answer this question without more information about the JUnit theory "removeThenAddDoesNotChangeSet" and the context in which it is being used.
-In general, replacing a set with a list in a JUnit theory may result in the theory becoming invalid, depending on how the set and list are used in the theory. If the set and list are used in ways that are not interchangeable, such as using set-specific methods on a list, then the theory may become invalid.
-Without knowing more about the theory and the specific replacements being made, it is not possible to determine how many of the tests that pass the precondition will also pass the postcondition. It is also not possible to determine whether the resulting theory will be valid or invalid.</t>
-  </si>
-  <si>
     <t>To demonstrate the problem with the Point class, let's first define the class:
 Copy code
 class Point {
@@ -1363,6 +1946,9 @@
 System.out.println(set.size());  // Outputs: 2</t>
   </si>
   <si>
+    <t>Write down the mathematical relationship required between equals() and hashCode().</t>
+  </si>
+  <si>
     <t xml:space="preserve">The equals() and hashCode() methods are used together in Java to implement the contract of object equality, as defined by the Objects.equals() and Objects.hash() methods.
 According to this contract, if two objects are equal (as determined by the equals() method), then their hashCode() values must be equal as well. Conversely, if two objects have equal hashCode() values, they do not necessarily have to be equal (as determined by the equals() method).
 In other words, the relationship between equals() and hashCode() is defined by the following mathematical relationship:
@@ -1370,6 +1956,9 @@
 This relationship is important because it allows objects to be stored and retrieved efficiently in common data structures such as HashMap, HashSet, and Hashtable.
 It's also worth noting that the hashCode() method should be implemented such that it returns the same value for two equal objects every time it is called on those objects, as long as the objects are not modified. This allows the hashCode() method to be used as a way to identify unique objects and helps to ensure the efficiency of data structures that rely on it.
 </t>
+  </si>
+  <si>
+    <t>Write a simple JUnit test to show that Point objects do not enjoy this property.</t>
   </si>
   <si>
     <t>Here is a simple JUnit test that demonstrates that the Point class does not satisfy the required relationship between equals() and hashCode():
@@ -1387,6 +1976,9 @@
 }
 In this test, we create two Point objects, p1 and p2, which are equal (as determined by the equals() method). However, the test fails because the hashCode() values of p1 and p2 are not equal, indicating that the hashCode() method is not properly implemented.
 To fix this issue, the hashCode() method in the Point class needs to be overridden as described in the previous answer. Once the hashCode() method is properly implemented, the test should pass.</t>
+  </si>
+  <si>
+    <t>Repair the Point class to fix the fault.</t>
   </si>
   <si>
     <t xml:space="preserve">To repair the fault in the Point class, the hashCode() method needs to be overridden as follows:
@@ -1411,6 +2003,9 @@
 With the hashCode() method overridden, the Point class will now satisfy the required relationship between equals() and hashCode() and can be used with common data structures such as HashMap, HashSet, and Hashtable without any issues.
 It's worth noting that the hashCode() method implementation shown above uses the Objects.hash() utility method to compute the hash code for the Point object. This method takes the x and y fields of the Point object as arguments and returns a hash code that is based on their values. This ensures that the hash code is consistent with the definition of equality for the Point class (as defined by the equals() method).
 </t>
+  </si>
+  <si>
+    <t>Rewrite your JUnit test as an appropriate JUnit theory. Evaluate it with suitable DataPoints.</t>
   </si>
   <si>
     <t xml:space="preserve">To rewrite the JUnit test as a JUnit theory, we can use the @Theory annotation and the @DataPoints annotation to specify a set of data points that will be used to evaluate the theory.
@@ -1439,12 +2034,48 @@
 In this case, since the Point class has been repaired and the hashCode() method is properly implemented, the theory should pass for all test cases.
 </t>
   </si>
+  <si>
+    <t>Replace each occurrence of a set with a list in the JUnit theory removeThenAddDoesNotChangeSet. Is the resulting theory valid or invalid? How many of the tests that pass the precondition also pass the postcondition? Explain.</t>
+  </si>
+  <si>
+    <t>It is not possible for me to accurately answer this question without more information about the JUnit theory "removeThenAddDoesNotChangeSet" and the context in which it is being used.
+In general, replacing a set with a list in a JUnit theory may result in the theory becoming invalid, depending on how the set and list are used in the theory. If the set and list are used in ways that are not interchangeable, such as using set-specific methods on a list, then the theory may become invalid.
+Without knowing more about the theory and the specific replacements being made, it is not possible to determine how many of the tests that pass the precondition will also pass the postcondition. It is also not possible to determine whether the resulting theory will be valid or invalid.</t>
+  </si>
+  <si>
+    <t>The first error in the given code is in the ColorPoint class, specifically in the equals method at Location B. In this method, the equals method first checks if the given object o is an instance of ColorPoint by using the instanceof operator. If it is not, the method returns false. However, this creates an error because it violates the symmetry principle of the equals method, which states that if x.equals(y) is true, then y.equals(x) should also be true.
+In this case, when a Point object p is compared to a ColorPoint object cp1 using the equals method, the method returns true as expected because both objects have the same x and y coordinates. But when the comparison is reversed and a ColorPoint object cp1 is compared to a Point object p using the equals method, the method returns false because the equals method in the ColorPoint class specifically checks that the object being compared to is an instance of ColorPoint.
+This causes inconsistency because it violates the symmetry principle of the equals method and also it may create confusion for developers. Because of this it is best for subclasses to always override their parent class equals method to include all of their attributes as well as the attributes of the parent class.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The class Point defines a basic class for representing a point in a 2D space. It has two private fields x and y that represent the coordinates of the point, and a constructor that initializes them. It also overrides the equals method, so that two points are considered equal if their coordinates are the same.
+The ColorPoint class extends the Point class and adds an additional field color that represents the color of the point. It also overrides the equals method, but it has a fault, because it only considers two ColorPoint objects equal if their coordinates and color are the same. This is problematic because it breaks the symmetry of the equals contract, as it will return false for the following test: p.equals(cp1) and cp1.equals(p) even though both points have the same coordinates.
+To fix this issue, I would update the equals method of the ColorPoint class as follows:
+@Override public boolean equals (Object o) {
+    if (o == this) return true;
+    if (!(o instanceof Point)) return false;
+    if (o.getClass() != getClass()) return false;
+    ColorPoint cp = (ColorPoint) o;
+    return (super.equals(cp) &amp;&amp; (cp.color == this.color));
+}
+This way, it will first check if the two objects are the same and if not, it will check that the class of the object is the same as the class of the point being compared with.
+Then, it will call the equals method of super class, instead of only checking for coordinates in the same class.
+With this modification, the following tests will produce the expected results:
+Point p = new Point (1,2);
+ColorPoint cp1 = new ColorPoint (1,2,RED);
+ColorPoint cp2 = new ColorPoint (1,2,BLUE);
+p.equals (cp1); // Test 1: Result = true;
+cp1.equals (p); // Test 2: Result = true;
+cp1.equals (cp2); // Test 3: Result = false;
+It's worth noting that in Java, It's recommended to also override the hashCode() method when we override the equals() method, so the two methods are consistent with each other.
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1458,6 +2089,17 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1467,7 +2109,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1490,16 +2132,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1818,42 +2481,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="2" width="16.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="63.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="51.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="75.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="30.5" style="1" customWidth="1"/>
+    <col min="1" max="5" width="8.83203125" style="1"/>
+    <col min="6" max="6" width="81.6640625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" ht="68">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="409.6">
       <c r="A2" s="1">
         <v>5.0999999999999996</v>
       </c>
@@ -1869,93 +2528,111 @@
       <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="323" x14ac:dyDescent="0.2">
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="409.6">
       <c r="A3" s="1">
         <v>5.0999999999999996</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="323" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="409.6">
       <c r="A4" s="1">
         <v>5.0999999999999996</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="323" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="409.6">
       <c r="A5" s="1">
         <v>5.0999999999999996</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="323" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="409.6">
       <c r="A6" s="1">
         <v>5.0999999999999996</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="409.6">
       <c r="A7" s="1">
         <v>5.0999999999999996</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="409.6">
       <c r="A8" s="1">
         <v>5.2</v>
       </c>
@@ -1963,101 +2640,119 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="306" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="409.6">
       <c r="A9" s="1">
         <v>5.2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="306" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="409.6">
       <c r="A10" s="1">
         <v>5.2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="409.6">
       <c r="A11" s="1">
         <v>5.2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="306" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="409.6">
       <c r="A12" s="1">
         <v>5.2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="409.6">
       <c r="A13" s="1">
         <v>5.2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="340" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="409.6">
       <c r="A14" s="1">
         <v>5.3</v>
       </c>
@@ -2065,101 +2760,119 @@
         <v>6</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="340" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="409.6">
       <c r="A15" s="1">
         <v>5.3</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="340" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="409.6">
       <c r="A16" s="1">
         <v>5.3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="340" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="409.6">
       <c r="A17" s="1">
         <v>5.3</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="340" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="409.6">
       <c r="A18" s="1">
         <v>5.3</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="340" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="409.6">
       <c r="A19" s="1">
         <v>5.3</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="388" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="409.6">
       <c r="A20" s="1">
         <v>5.4</v>
       </c>
@@ -2167,101 +2880,119 @@
         <v>6</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="372" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="409.6">
       <c r="A21" s="1">
         <v>5.4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="372" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="409.6">
       <c r="A22" s="1">
         <v>5.4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="372" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="409.6">
       <c r="A23" s="1">
         <v>5.4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="372" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="409.6">
       <c r="A24" s="1">
         <v>5.4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="409.6">
       <c r="A25" s="1">
         <v>5.4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="409.6">
       <c r="A26" s="1">
         <v>7.1</v>
       </c>
@@ -2269,101 +3000,119 @@
         <v>6</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="409.6">
       <c r="A27" s="1">
         <v>7.1</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="409.6">
       <c r="A28" s="1">
         <v>7.1</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="409.6">
       <c r="A29" s="1">
         <v>7.1</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="409.6">
       <c r="A30" s="1">
         <v>7.1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="409.6">
       <c r="A31" s="1">
         <v>7.1</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="409.6">
       <c r="A32" s="1">
         <v>7.2</v>
       </c>
@@ -2371,101 +3120,119 @@
         <v>6</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="409.6">
       <c r="A33" s="1">
         <v>7.2</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="409.6">
       <c r="A34" s="1">
         <v>7.2</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="409.6">
       <c r="A35" s="1">
         <v>7.2</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="409.6">
       <c r="A36" s="1">
         <v>7.2</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="409.6">
       <c r="A37" s="1">
         <v>7.2</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="409.6">
       <c r="A38" s="1">
         <v>7.3</v>
       </c>
@@ -2473,98 +3240,116 @@
         <v>6</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="409.6">
       <c r="A39" s="1">
         <v>7.3</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="409.6">
       <c r="A40" s="1">
         <v>7.3</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="409.6">
       <c r="A41" s="1">
         <v>7.3</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="409.6">
       <c r="A42" s="1">
         <v>7.3</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>72</v>
+        <v>112</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="409.6">
       <c r="A43" s="1">
         <v>7.3</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>74</v>
+        <v>114</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -2576,22 +3361,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="2" width="11.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="50" style="1" customWidth="1"/>
-    <col min="4" max="4" width="69.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="52.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="2" width="8.83203125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="68" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2607,53 +3387,53 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="409.5" customHeight="1">
       <c r="A2" s="1">
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>75</v>
+        <v>115</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>76</v>
+        <v>116</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="409.5" customHeight="1">
       <c r="A3" s="1">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>78</v>
+        <v>118</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="255" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="409.5" customHeight="1">
       <c r="A4" s="1">
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>81</v>
+        <v>121</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>82</v>
+        <v>122</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="409.5" customHeight="1">
       <c r="A5" s="1">
         <v>6</v>
       </c>
@@ -2661,84 +3441,84 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>84</v>
+        <v>124</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>85</v>
+        <v>125</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="409.5" customHeight="1">
       <c r="A6" s="1">
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>84</v>
+        <v>124</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>87</v>
+        <v>127</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="409.5" customHeight="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>84</v>
+        <v>124</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="409.5" customHeight="1">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>84</v>
+        <v>124</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="409.5" customHeight="1">
       <c r="A9" s="1">
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>84</v>
+        <v>124</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>93</v>
+        <v>133</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="409.5" customHeight="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2746,92 +3526,92 @@
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>95</v>
+        <v>135</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="409.5" customHeight="1">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>95</v>
+        <v>135</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>97</v>
+        <v>138</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="409.5" customHeight="1">
       <c r="A12" s="1">
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>95</v>
+        <v>135</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>98</v>
+        <v>140</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="409.5" customHeight="1">
       <c r="A13" s="1">
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>95</v>
+        <v>135</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>99</v>
+        <v>142</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="409.5" customHeight="1">
       <c r="A14" s="1">
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>95</v>
+        <v>135</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>100</v>
+        <v>144</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="289" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="409.5" customHeight="1">
       <c r="A15" s="1">
         <v>10</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>102</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed chapter 3 (separate Context)
</commit_message>
<xml_diff>
--- a/dataset/testing.xlsx
+++ b/dataset/testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajed/PycharmProjects/Study-on-ChatGPT/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A15395-22B6-D946-AE73-93973852771B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D78966-24C1-4E4F-A2F3-06D4AE970B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="28040" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="28040" windowHeight="17300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ch1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="164">
   <si>
     <t>id</t>
   </si>
@@ -1521,6 +1521,11 @@
 </t>
   </si>
   <si>
+    <t>The first error in the given code is in the ColorPoint class, specifically in the equals method at Location B. In this method, the equals method first checks if the given object o is an instance of ColorPoint by using the instanceof operator. If it is not, the method returns false. However, this creates an error because it violates the symmetry principle of the equals method, which states that if x.equals(y) is true, then y.equals(x) should also be true.
+In this case, when a Point object p is compared to a ColorPoint object cp1 using the equals method, the method returns true as expected because both objects have the same x and y coordinates. But when the comparison is reversed and a ColorPoint object cp1 is compared to a Point object p using the equals method, the method returns false because the equals method in the ColorPoint class specifically checks that the object being compared to is an instance of ColorPoint.
+This causes inconsistency because it violates the symmetry principle of the equals method and also it may create confusion for developers. Because of this it is best for subclasses to always override their parent class equals method to include all of their attributes as well as the attributes of the parent class.</t>
+  </si>
+  <si>
     <t xml:space="preserve">
 To fix the faults in the given code, the implementation of the `equals` method in both the `Point` and `ColorPoint` classes must be modified. The modified `equals` methods should include an `@Override` annotation and a check for object reference equality at the beginning of the method to properly override the `equals` method in the `Object` class and handle the case where the method is passed an object that is not an instance of the class.
 Here is the modified code with the fixed `equals` methods:
@@ -1568,6 +1573,29 @@
 ```
 All tests passed.
 ```
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The class Point defines a basic class for representing a point in a 2D space. It has two private fields x and y that represent the coordinates of the point, and a constructor that initializes them. It also overrides the equals method, so that two points are considered equal if their coordinates are the same.
+The ColorPoint class extends the Point class and adds an additional field color that represents the color of the point. It also overrides the equals method, but it has a fault, because it only considers two ColorPoint objects equal if their coordinates and color are the same. This is problematic because it breaks the symmetry of the equals contract, as it will return false for the following test: p.equals(cp1) and cp1.equals(p) even though both points have the same coordinates.
+To fix this issue, I would update the equals method of the ColorPoint class as follows:
+@Override public boolean equals (Object o) {
+    if (o == this) return true;
+    if (!(o instanceof Point)) return false;
+    if (o.getClass() != getClass()) return false;
+    ColorPoint cp = (ColorPoint) o;
+    return (super.equals(cp) &amp;&amp; (cp.color == this.color));
+}
+This way, it will first check if the two objects are the same and if not, it will check that the class of the object is the same as the class of the point being compared with.
+Then, it will call the equals method of super class, instead of only checking for coordinates in the same class.
+With this modification, the following tests will produce the expected results:
+Point p = new Point (1,2);
+ColorPoint cp1 = new ColorPoint (1,2,RED);
+ColorPoint cp2 = new ColorPoint (1,2,BLUE);
+p.equals (cp1); // Test 1: Result = true;
+cp1.equals (p); // Test 2: Result = true;
+cp1.equals (cp2); // Test 3: Result = false;
+It's worth noting that in Java, It's recommended to also override the hashCode() method when we override the equals() method, so the two methods are consistent with each other.
 </t>
   </si>
   <si>
@@ -1671,6 +1699,55 @@
 </t>
   </si>
   <si>
+    <t>Here's an example of JUnit tests for the BoundedQueue class:
+```
+import static org.junit.Assert.*;
+import org.junit.Test;
+public class BoundedQueueTest {
+    @Test
+    public void testEnqueueAndDequeue() {
+        BoundedQueue q = new BoundedQueue(5);
+        // Test enqueue
+        q.enQueue(1);
+        q.enQueue(2);
+        q.enQueue(3);
+        assertEquals("[1, 2, 3]", q.toString());
+        // Test dequeue
+        assertEquals(1, q.deQueue());
+        assertEquals("[2, 3]", q.toString());
+    }
+    @Test(expected = NullPointerException.class)
+    public void testEnqueueNull() {
+        BoundedQueue q = new BoundedQueue(5);
+        q.enQueue(null);
+    }
+    @Test(expected = IllegalStateException.class)
+    public void testEnqueueFullQueue() {
+        BoundedQueue q = new BoundedQueue(2);
+        q.enQueue(1);
+        q.enQueue(2);
+        q.enQueue(3);
+    }
+    @Test(expected = IllegalStateException.class)
+    public void testDequeueEmptyQueue() {
+        BoundedQueue q = new BoundedQueue(2);
+        q.deQueue();
+    }
+    @Test
+    public void testIsEmptyAndIsFull() {
+        BoundedQueue q = new BoundedQueue(2);
+        assertTrue(q.isEmpty());
+        assertFalse(q.isFull());
+        q.enQueue(1);
+        assertFalse(q.isEmpty());
+        q.enQueue(2);
+        assertTrue(q.isFull());
+    }
+}
+```
+You can run this test by creating a new test class and copying the above code into it. Make sure the classpath is set up to include JUnit 4 or later library. Once you run the test, the results of the test will be displayed, showing you if the tests have passed or failed.</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 
 import java.util.*;
 public class Min
@@ -1736,6 +1813,16 @@
 </t>
   </si>
   <si>
+    <t>To delete the explicit throw of the NullPointerException in the Min program, you would remove the following line of code:
+```
+if (result == null) throw new NullPointerException ("Min.min");
+```
+This line is located after the initialization of the "result" variable and before the while loop that iterates through the elements of the list. This line checks if the first element in the list is null, and if so, it throws a NullPointerException with the message "Min.min".
+Without this line, the program will not check if the first element of the list is null. As a result, if the first element of the list is null and the subsequent elements are not, the program will return null as the minimum element, rather than throwing an exception.
+In the JUnit test for a list with a single null element, if the explicit throw of NPE is removed, the test will fail because the program does not check for null elements in the list any more, and it will return a null which is not the expected result in this case.
+You will have to decide how you want your program to handle the scenario when there is a null element, then update the program and test accordingly.</t>
+  </si>
+  <si>
     <t>The following JUnit test method for the sort() method has a non-syntactic flaw.
 @Test
 public void testSort()
@@ -1757,6 +1844,12 @@
   <si>
     <t xml:space="preserve">The non-syntactic flaw in the test method is that there is a line of code "23" which is not a valid Java statement. This violates the rule of well-formedness in the RIPR model, as a well-formed program must have a syntactically correct structure. 
 </t>
+  </si>
+  <si>
+    <t>The non-syntactic flaw in this JUnit test method is that there is a line of code, `23`, that doesn't perform any function and doesn't affect the outcome of the test. It is not a part of the test case's precondition, execution, or postcondition. 
+In terms of the RIPR model, this line of code violates the 'precondition' and 'postcondition' as it does not set any expectation or validate any behavior, rather it is just a number causing the test case to be an invalid representation of the requirement it's supposed to test.
+It also violates the 'Requirements' part as it's not fulfilling any requirement that's been set.
+It could be said that this line of code is a 'Redundant' element and thus failing the 'Relevant' criteria, thus making the test case not able to understand what's expected in the case of a failure</t>
   </si>
   <si>
     <t>Consider the following example class. PrimeNumbers has three methods. The first, computePrimes(), takes one integer input and computes that many prime numbers. iterator() returns an Iterator that will iterate through the primes, and toString() returns a string representation.
@@ -1830,6 +1923,16 @@
 </t>
   </si>
   <si>
+    <t>A test that does not reach the fault could be as follows:
+1. Create a new instance of the PrimeNumbers class.
+2. Call the computePrimes() method with input 5.
+3. Verify that the list of primes generated contains the numbers 2, 3, 5, 7, 11.
+4. Verify that the output of the toString() method matches the expected output "[2, 3, 5, 7, 11]".
+5. Verify that the iterator() method returns an iterator that returns the expected sequence of primes: 2, 3, 5, 7, 11.
+This test does not reach the fault because the input passed to computePrimes() is 5, which is less than 10, so none of the primes generated will have a last digit of 9, and so none will be excluded.
+Note that a test that can only check if the output is correct is an "oracle problem" because, without another way to compute the prime numbers, it is difficult to say if the output is correct or not, but this  test case is useful in a scenario where the output or the iterator is considered an oracle, where another way to check the prime numbers is available.</t>
+  </si>
+  <si>
     <t>Write a test that reaches the fault, but does not infect. If a test cannot be created, explain why.</t>
   </si>
   <si>
@@ -2043,32 +2146,170 @@
 Without knowing more about the theory and the specific replacements being made, it is not possible to determine how many of the tests that pass the precondition will also pass the postcondition. It is also not possible to determine whether the resulting theory will be valid or invalid.</t>
   </si>
   <si>
-    <t>The first error in the given code is in the ColorPoint class, specifically in the equals method at Location B. In this method, the equals method first checks if the given object o is an instance of ColorPoint by using the instanceof operator. If it is not, the method returns false. However, this creates an error because it violates the symmetry principle of the equals method, which states that if x.equals(y) is true, then y.equals(x) should also be true.
-In this case, when a Point object p is compared to a ColorPoint object cp1 using the equals method, the method returns true as expected because both objects have the same x and y coordinates. But when the comparison is reversed and a ColorPoint object cp1 is compared to a Point object p using the equals method, the method returns false because the equals method in the ColorPoint class specifically checks that the object being compared to is an instance of ColorPoint.
-This causes inconsistency because it violates the symmetry principle of the equals method and also it may create confusion for developers. Because of this it is best for subclasses to always override their parent class equals method to include all of their attributes as well as the attributes of the parent class.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The class Point defines a basic class for representing a point in a 2D space. It has two private fields x and y that represent the coordinates of the point, and a constructor that initializes them. It also overrides the equals method, so that two points are considered equal if their coordinates are the same.
-The ColorPoint class extends the Point class and adds an additional field color that represents the color of the point. It also overrides the equals method, but it has a fault, because it only considers two ColorPoint objects equal if their coordinates and color are the same. This is problematic because it breaks the symmetry of the equals contract, as it will return false for the following test: p.equals(cp1) and cp1.equals(p) even though both points have the same coordinates.
-To fix this issue, I would update the equals method of the ColorPoint class as follows:
-@Override public boolean equals (Object o) {
-    if (o == this) return true;
-    if (!(o instanceof Point)) return false;
-    if (o.getClass() != getClass()) return false;
-    ColorPoint cp = (ColorPoint) o;
-    return (super.equals(cp) &amp;&amp; (cp.color == this.color));
-}
-This way, it will first check if the two objects are the same and if not, it will check that the class of the object is the same as the class of the point being compared with.
-Then, it will call the equals method of super class, instead of only checking for coordinates in the same class.
-With this modification, the following tests will produce the expected results:
-Point p = new Point (1,2);
-ColorPoint cp1 = new ColorPoint (1,2,RED);
-ColorPoint cp2 = new ColorPoint (1,2,BLUE);
-p.equals (cp1); // Test 1: Result = true;
-cp1.equals (p); // Test 2: Result = true;
-cp1.equals (cp2); // Test 3: Result = false;
-It's worth noting that in Java, It's recommended to also override the hashCode() method when we override the equals() method, so the two methods are consistent with each other.
-</t>
+    <t>1. One test you could perform is to compute the first 10 prime numbers and check that none of them end in 9. You would do this by calling the computePrimes method with the input 10, and then calling the iterator method to get an iterator for the primes list, and then iterating through the list and checking that none of the numbers end in 9.
+2. Another test you could perform is to compute the first 20 prime numbers and check that the number 19 is missing from the list. To do this, you would call computePrimes with the input 20, and then check that the iterator does not return 19.
+3. Another test would be to compute the first 100 prime numbers, after that you will check that the primes whose last digits are 9 are not present.
+4. You could test if the first prime number generated is 2 and the second 3
+5. Another test would be to check the primes generated by computePrimes method by comparing it with the well known prime numbers list in the first 1000 numbers. The test oracle would check that the numbers that are in the well-known prime numbers list but not in the generated primes list, should not have a last digit as 9.
+A test that reaches the fault, but does not infect would be to check the first 10 prime numbers and check that the first number is 2 and the next three numbers are 3,5,7 respectively. This test would not infect because it is only checking that the first four primes generated by the algorithm are 2, 3, 5, and 7, and not checking if any other numbers are missing from the list.</t>
+  </si>
+  <si>
+    <t>Here are five tests that can be used to uncover the fault in the computePrimes() method:
+1. Test the class with a small input value (e.g. n=5) and check that the returned primes list does not contain any prime numbers whose last digit is 9. For example, you can call computePrimes(5), then check if the returned primes are [2, 3, 5, 7, 11].
+2. Test the class with a larger input value (e.g. n=10) and check that the returned primes list does not contain any prime numbers whose last digit is 9. For example, you can call computePrimes(10), then check if the returned primes are [2, 3, 5, 7, 11, 13, 17, 19, 23, 29].
+3. Test the class with a large input value (e.g. n=50) and check that the returned primes list does not contain any prime numbers whose last digit is 9. This test will ensure that the fault is not limited to small inputs.
+4. Test the class by calling computePrimes(5) and then calling iterator() and toString() methods and check if the returned primes are [2, 3, 5, 7, 11] and not contain any prime numbers whose last digit is 9 .
+5. Test the class by providing an input value of n=50 and check if the returned primes by iterator() or toString() doesn't contain any prime numbers whose last digit is 9.
+Test that infects the state, but does not propagate
+You can call computePrimes(5) and then call iterator() or toString() and check the primes are [2,3,5,7,11], and you can check if there is any prime number whose last digit is 9.
+It is not possible to create a test that infects the state of the class but does not propagate because the fault is not caused by any external state being passed into the class. Instead, it is caused by the if statement if (isPrime &amp;&amp; (number % 10 != 9)), which checks if the current number is prime and its last digit is not 9. Since this check is always done for every number, there is no way to infect the state of the class without triggering the fault.</t>
+  </si>
+  <si>
+    <t>1. A basic test to check if the first n prime numbers are computed correctly can be created by calling the computePrimes() method with an input of n, and then using the toString() method to check if the first n prime numbers are in the returned string.
+2. A test that checks the correctness of the iterator method can be created by first calling the computePrimes() method with an input of n, and then using the iterator() method to iterate through the primes and check if they are the correct n prime numbers.
+3. A test that checks if prime numbers whose last digit is 9 are included can be created by calling the computePrimes() method with a large input value (e.g. 1000), and then checking if prime numbers whose last digit is 9 are included in the returned string obtained from the toString() method.
+4. A test that checks the upper limit of the prime numbers can be created by calling the computePrimes() method with a large input value (e.g. 10000) and then checking if the last prime number is less or equal to 10000 by calling the iterator() method
+5. A test for a upper boundary input can be created by calling the computePrimes() method with the maximum value allowed for the input, and check the program can handle this limit.
+It is not possible to create a test that propagates but does not reveal the fault because the nature of the bug is that prime numbers whose last digit is 9 are not included, which will be observable in any test that uses the computed primes list generated by the method.</t>
+  </si>
+  <si>
+    <t>When you override the equals() method, it is generally recommended that you also override the hashCode() method, because the hashCode() method is used by certain collection classes (such as HashSet) to determine whether two objects are equal. If you override equals() but not hashCode(), then these collections may not behave as expected.
+Here's an example of how the Point class from Chapter 1 might be defective in this regard:
+class Point {
+    private int x;
+    private int y;
+    public Point(int x, int y) {
+        this.x = x;
+        this.y = y;
+    }
+    @Override
+    public boolean equals(Object o) {
+        if (o == this) return true;
+        if (!(o instanceof Point)) return false;
+        Point p = (Point) o;
+        return p.x == x &amp;&amp; p.y == y;
+    }
+}
+The above Point class overrides the equals() method to check for equality based on the x and y fields, but it does not override the hashCode() method. Therefore, if we try to use it as key in HashMap it will return error.
+Copy code
+    HashSet&lt;Point&gt; set = new HashSet&lt;&gt;();
+    set.add(new Point(1, 2));
+    set.add(new Point(3, 4));
+    set.add(new Point(1, 2)); 
+In this example, we are trying to add three Point objects to a HashSet. The first two Point objects have different x and y values, so they will be added to the set without any problem. However, the third Point object has the same x and y values as the first Point object, so equals() will return true when comparing the two. But HashSet uses the hashCode() method to determine whether two objects are equal, and since the Point class doesn't override hashCode(), the HashSet will treat the first and third Point objects as distinct, and therefore it will be added to the set, even though it's a duplicate.
+To fix this, you would need to override the hashCode() method in Point class, and implement it consistently with the equals() method.
+    @Override
+    public int hashCode() {
+        int result = 17;
+        result = 31 * result + x;
+        result = 31 * result + y;
+        return result;
+    }
+This would ensure that HashSet is able to correctly identify when two Point objects are equal and will prevent duplicate values from being added to the set.</t>
+  </si>
+  <si>
+    <t>Here are five test cases that can reveal the fault in the computePrimes method:
+1. Test case: Call computePrimes(5) and then call iterator(). Compare the list of prime numbers returned by the iterator with a list of the first 5 prime numbers that don't end with 9. Expected outcome: The two lists should not match, revealing the fault.
+2. Test case: Call computePrimes(10) and then call toString(). Compare the string representation of the primes returned with a string representation of the first 10 prime numbers that don't end with 9. Expected outcome: The two strings should not match, revealing the fault.
+3. Test case: Call computePrimes(10) and then check if prime number 19 is present in the list. Expected outcome: It should not be present, revealing the fault.
+4. Test case: Call computePrimes(20) and then check the last element of the list of primes. Expected outcome: The last element should not be a prime number ending with 9, revealing the fault.
+5. Test case: Call computePrimes(10) and then call iterator(). Save the output. Then call computePrimes(20) and call iterator(). Compare the last 10 prime numbers from the second iterator call with the saved output from the first call. Expected outcome: The two lists should not match.
+All test cases are created with the assumption that the oracle for the primality of numbers is correct. All tests cases are checking one specific problem which is the condition in the code "if (isPrime &amp;&amp; (number % 10 != 9))" which cause the problem. The test cases are checking that this condition is not met when the number is prime.</t>
+  </si>
+  <si>
+    <t>When overriding the equals() method in a class, it is generally recommended to also override the hashCode() method, as the two methods should have a consistent relationship. Specifically, if two objects are equal according to the equals() method, then calling hashCode() on each of the objects must produce the same integer result. Additionally, if two objects are unequal according to the equals() method, it is not required but preferable that calling hashCode() on each of the objects produces distinct integer results.
+To put it mathematically:
+- If a.equals(b) returns true, then a.hashCode() == b.hashCode() must also return true.
+- If a.equals(b) returns false, then it is not necessary that a.hashCode() == b.hashCode() returns false, but the distinct hashCode would be preferred.
+It's worth noting that in practice, it's hard to guarantee that hashCode is distinct for all unequal objects, but it's more important that it is consistent with the equals.</t>
+  </si>
+  <si>
+    <t>Here's an example of a JUnit test that demonstrates the issue with the Point class not properly overriding the hashCode() method:
+import static org.junit.Assert.*;
+import java.util.HashSet;
+import org.junit.Test;
+public class PointTest {
+    @Test
+    public void testHashCode() {
+        Point p1 = new Point(1, 2);
+        Point p2 = new Point(1, 2);
+        // assert that p1 and p2 are equal
+        assertTrue(p1.equals(p2));
+        HashSet&lt;Point&gt; set = new HashSet&lt;&gt;();
+        set.add(p1);
+        set.add(p2);
+        // if hashCode() is not properly implemented, the set will contain 2 elements
+        assertEquals(1, set.size());
+    }
+}
+This test creates two Point objects, p1 and p2, that are equal to each other (have the same x and y values). It then adds both of these objects to a HashSet, and checks the size of the set to see if the hashCode() method is properly implemented. If the hashCode() method is not properly overridden, the set will contain 2 elements, because the HashSet considers the two Point objects to be different. If the hashCode() method is correctly overridden, the set will contain only 1 element, because the two Point objects are considered to be equal.
+It is worth noting that if the equals method is overridden and not symmetric, reflexive and transitive, the same issue can appear.</t>
+  </si>
+  <si>
+    <t>Here's an example of how you might repair the Point class to properly override the equals() and hashCode() methods:
+class Point {
+    private int x;
+    private int y;
+    public Point(int x, int y) {
+        this.x = x;
+        this.y = y;
+    }
+    @Override
+    public boolean equals(Object other) {
+        if (!(other instanceof Point)) {
+            return false;
+        }
+        Point otherPoint = (Point) other;
+        return this.x == otherPoint.x &amp;&amp; this.y == otherPoint.y;
+    }
+    @Override
+    public int hashCode() {
+        int result = 17;
+        result = 31 * result + x;
+        result = 31 * result + y;
+        return result;
+    }
+}
+The equals method checks if the other object is an instance of Point and compares the x and y coordinates.
+In the hashCode() method, I use the technique of prime number multiply, where 17 is multiplied by the field x, 31 * the field y .This way, each point's hash code is unique and is based on the point's x and y values, fulfilling the requirement that if two objects are equal, then their hash codes must be equal as well.
+This way, if we store multiple Point objects in a HashSet, the HashSet will be able to properly determine when two Point objects are equal, and it will only store one of them.</t>
+  </si>
+  <si>
+    <t>When overriding the equals() method in a class, it is generally considered a best practice to also override the hashCode() method. This is because hashCode() and equals() are typically used together in data structures such as HashMap and HashSet. If two objects are equal according to the equals() method, they should have the same hash code. Conversely, two objects with the same hash code are not necessarily equal.
+Here is an example of a JUnit theory that tests the equals() and hashCode() methods of a Point class:
+import org.junit.experimental.theories.DataPoints;
+import org.junit.experimental.theories.Theories;
+import org.junit.experimental.theories.Theory;
+import org.junit.runner.RunWith;
+import static org.junit.Assert.*;
+@RunWith(Theories.class)
+public class PointTest {
+    @DataPoints
+    public static Point[] dataPoints = {
+        new Point(0, 0),
+        new Point(1, 1),
+        new Point(2, 2),
+        new Point(-1, -1)
+    };
+    @Theory
+    public void testEquals(Point p1, Point p2) {
+        assertTrue(p1.equals(p2) == (p1.x == p2.x &amp;&amp; p1.y == p2.y));
+    }
+    @Theory
+    public void testHashCode(Point p1, Point p2) {
+        if (p1.equals(p2)) {
+            assertTrue(p1.hashCode() == p2.hashCode());
+        }
+    }
+}
+In this example, the Point class has x and y fields, and the equals() method compares the fields for equality. The testEquals() method tests that the equals() method is implemented correctly by comparing the fields of the two Point objects. The testHashCode() method tests that the hashCode() method is implemented correctly by ensuring that two Point objects with the same x and y fields have the same hash code.
+You can also have custom datapoints as well as use other JUnit annotation like Assume &amp; Before to prepare the test data.</t>
+  </si>
+  <si>
+    <t>It's not clear from the information provided what the original "theory removeThenAddDoesNotChangeSet" looks like, so it's difficult to say whether the resulting theory would be valid or invalid.
+If the original theory tests that removing an element from a set followed by adding the same element back to the set results in the set remaining unchanged, then replacing each occurrence of "set" with "list" would make the theory invalid. This is because in Java, sets are implemented as collections that do not allow duplicate elements, while lists do allow duplicate elements. Therefore, adding an element back to a list after removing it would result in the element being present twice, whereas it would not be present at all if it were a set.
+As for the number of tests that pass the precondition and also pass the postcondition, it would depend on the specific tests included in the original theory. If the tests involve adding and removing elements in such a way that the list would not end up with duplicate elements, then all of the tests would still pass. However, if the tests involve adding and removing elements in such a way that duplicate elements would be introduced to the list, then none of the tests would pass.
+It would be best to check each test and review the expected behavior, also changing the asserts or postcondition in order to reflect that you are testing with a list instead of set.</t>
   </si>
 </sst>
 </file>
@@ -2481,38 +2722,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="5" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="11.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="67.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="41.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="79.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="81.6640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="1"/>
+    <col min="7" max="8" width="8.83203125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="68">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:6" ht="51" customHeight="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="409.6">
+    <row r="2" spans="1:6" ht="409.5" customHeight="1">
       <c r="A2" s="1">
         <v>5.0999999999999996</v>
       </c>
@@ -2532,7 +2778,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="409.6">
+    <row r="3" spans="1:6" ht="409.5" customHeight="1">
       <c r="A3" s="1">
         <v>5.0999999999999996</v>
       </c>
@@ -2552,7 +2798,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="409.6">
+    <row r="4" spans="1:6" ht="409.5" customHeight="1">
       <c r="A4" s="1">
         <v>5.0999999999999996</v>
       </c>
@@ -2572,7 +2818,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="409.6">
+    <row r="5" spans="1:6" ht="409.5" customHeight="1">
       <c r="A5" s="1">
         <v>5.0999999999999996</v>
       </c>
@@ -2592,7 +2838,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="409.6">
+    <row r="6" spans="1:6" ht="409.5" customHeight="1">
       <c r="A6" s="1">
         <v>5.0999999999999996</v>
       </c>
@@ -2612,7 +2858,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="409.6">
+    <row r="7" spans="1:6" ht="409.5" customHeight="1">
       <c r="A7" s="1">
         <v>5.0999999999999996</v>
       </c>
@@ -2632,7 +2878,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="409.6">
+    <row r="8" spans="1:6" ht="409.5" customHeight="1">
       <c r="A8" s="1">
         <v>5.2</v>
       </c>
@@ -2652,7 +2898,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="409.6">
+    <row r="9" spans="1:6" ht="409.5" customHeight="1">
       <c r="A9" s="1">
         <v>5.2</v>
       </c>
@@ -2672,7 +2918,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="409.6">
+    <row r="10" spans="1:6" ht="409.5" customHeight="1">
       <c r="A10" s="1">
         <v>5.2</v>
       </c>
@@ -2692,7 +2938,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="409.6">
+    <row r="11" spans="1:6" ht="409.5" customHeight="1">
       <c r="A11" s="1">
         <v>5.2</v>
       </c>
@@ -2712,7 +2958,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="409.6">
+    <row r="12" spans="1:6" ht="409.5" customHeight="1">
       <c r="A12" s="1">
         <v>5.2</v>
       </c>
@@ -2732,7 +2978,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="409.6">
+    <row r="13" spans="1:6" ht="409.5" customHeight="1">
       <c r="A13" s="1">
         <v>5.2</v>
       </c>
@@ -2752,7 +2998,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="409.6">
+    <row r="14" spans="1:6" ht="409.5" customHeight="1">
       <c r="A14" s="1">
         <v>5.3</v>
       </c>
@@ -2772,7 +3018,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="409.6">
+    <row r="15" spans="1:6" ht="409.5" customHeight="1">
       <c r="A15" s="1">
         <v>5.3</v>
       </c>
@@ -2792,7 +3038,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="409.6">
+    <row r="16" spans="1:6" ht="409.5" customHeight="1">
       <c r="A16" s="1">
         <v>5.3</v>
       </c>
@@ -2812,7 +3058,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="409.6">
+    <row r="17" spans="1:6" ht="409.5" customHeight="1">
       <c r="A17" s="1">
         <v>5.3</v>
       </c>
@@ -2832,7 +3078,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="409.6">
+    <row r="18" spans="1:6" ht="409.5" customHeight="1">
       <c r="A18" s="1">
         <v>5.3</v>
       </c>
@@ -2852,7 +3098,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="409.6">
+    <row r="19" spans="1:6" ht="409.5" customHeight="1">
       <c r="A19" s="1">
         <v>5.3</v>
       </c>
@@ -2872,7 +3118,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="409.6">
+    <row r="20" spans="1:6" ht="409.5" customHeight="1">
       <c r="A20" s="1">
         <v>5.4</v>
       </c>
@@ -2892,7 +3138,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="409.6">
+    <row r="21" spans="1:6" ht="409.5" customHeight="1">
       <c r="A21" s="1">
         <v>5.4</v>
       </c>
@@ -2912,7 +3158,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="409.6">
+    <row r="22" spans="1:6" ht="409.5" customHeight="1">
       <c r="A22" s="1">
         <v>5.4</v>
       </c>
@@ -2932,7 +3178,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="409.6">
+    <row r="23" spans="1:6" ht="409.5" customHeight="1">
       <c r="A23" s="1">
         <v>5.4</v>
       </c>
@@ -2952,7 +3198,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="409.6">
+    <row r="24" spans="1:6" ht="409.5" customHeight="1">
       <c r="A24" s="1">
         <v>5.4</v>
       </c>
@@ -2972,7 +3218,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="409.6">
+    <row r="25" spans="1:6" ht="409.5" customHeight="1">
       <c r="A25" s="1">
         <v>5.4</v>
       </c>
@@ -2992,7 +3238,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="409.6">
+    <row r="26" spans="1:6" ht="409.5" customHeight="1">
       <c r="A26" s="1">
         <v>7.1</v>
       </c>
@@ -3012,7 +3258,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="409.6">
+    <row r="27" spans="1:6" ht="409.5" customHeight="1">
       <c r="A27" s="1">
         <v>7.1</v>
       </c>
@@ -3032,7 +3278,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="409.6">
+    <row r="28" spans="1:6" ht="409.5" customHeight="1">
       <c r="A28" s="1">
         <v>7.1</v>
       </c>
@@ -3052,7 +3298,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="409.6">
+    <row r="29" spans="1:6" ht="409.5" customHeight="1">
       <c r="A29" s="1">
         <v>7.1</v>
       </c>
@@ -3072,7 +3318,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="409.6">
+    <row r="30" spans="1:6" ht="409.5" customHeight="1">
       <c r="A30" s="1">
         <v>7.1</v>
       </c>
@@ -3092,7 +3338,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="409.6">
+    <row r="31" spans="1:6" ht="409.5" customHeight="1">
       <c r="A31" s="1">
         <v>7.1</v>
       </c>
@@ -3112,7 +3358,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="409.6">
+    <row r="32" spans="1:6" ht="409.5" customHeight="1">
       <c r="A32" s="1">
         <v>7.2</v>
       </c>
@@ -3132,7 +3378,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="409.6">
+    <row r="33" spans="1:6" ht="409.5" customHeight="1">
       <c r="A33" s="1">
         <v>7.2</v>
       </c>
@@ -3152,7 +3398,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="409.6">
+    <row r="34" spans="1:6" ht="409.5" customHeight="1">
       <c r="A34" s="1">
         <v>7.2</v>
       </c>
@@ -3172,7 +3418,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="409.6">
+    <row r="35" spans="1:6" ht="409.5" customHeight="1">
       <c r="A35" s="1">
         <v>7.2</v>
       </c>
@@ -3192,7 +3438,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="409.6">
+    <row r="36" spans="1:6" ht="409.5" customHeight="1">
       <c r="A36" s="1">
         <v>7.2</v>
       </c>
@@ -3212,7 +3458,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="409.6">
+    <row r="37" spans="1:6" ht="409.5" customHeight="1">
       <c r="A37" s="1">
         <v>7.2</v>
       </c>
@@ -3232,7 +3478,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="409.6">
+    <row r="38" spans="1:6" ht="409.5" customHeight="1">
       <c r="A38" s="1">
         <v>7.3</v>
       </c>
@@ -3252,7 +3498,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="409.6">
+    <row r="39" spans="1:6" ht="409.5" customHeight="1">
       <c r="A39" s="1">
         <v>7.3</v>
       </c>
@@ -3272,7 +3518,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="409.6">
+    <row r="40" spans="1:6" ht="409.5" customHeight="1">
       <c r="A40" s="1">
         <v>7.3</v>
       </c>
@@ -3292,7 +3538,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="409.6">
+    <row r="41" spans="1:6" ht="409.5" customHeight="1">
       <c r="A41" s="1">
         <v>7.3</v>
       </c>
@@ -3312,7 +3558,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="409.6">
+    <row r="42" spans="1:6" ht="409.5" customHeight="1">
       <c r="A42" s="1">
         <v>7.3</v>
       </c>
@@ -3329,10 +3575,10 @@
         <v>113</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="409.6">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="409.5" customHeight="1">
       <c r="A43" s="1">
         <v>7.3</v>
       </c>
@@ -3346,14 +3592,15 @@
         <v>86</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>149</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -3361,79 +3608,92 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="2" width="8.83203125" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="2" width="8.83203125" style="1"/>
+    <col min="3" max="3" width="74" style="1" customWidth="1"/>
+    <col min="4" max="4" width="63.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="76.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="87.1640625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="68" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" ht="68">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="409.5" customHeight="1">
+    <row r="2" spans="1:6" ht="409.6">
       <c r="A2" s="1">
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="409.5" customHeight="1">
+        <v>119</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="409.6">
       <c r="A3" s="1">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="409.5" customHeight="1">
+        <v>123</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="409.6">
       <c r="A4" s="1">
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="409.5" customHeight="1">
+        <v>127</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="409.6">
       <c r="A5" s="1">
         <v>6</v>
       </c>
@@ -3441,16 +3701,19 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="409.5" customHeight="1">
+        <v>131</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="409.6">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -3458,16 +3721,19 @@
         <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="409.5" customHeight="1">
+        <v>134</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="409.6">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3475,16 +3741,19 @@
         <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="409.5" customHeight="1">
+        <v>136</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="409.6">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -3492,16 +3761,19 @@
         <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="409.5" customHeight="1">
+        <v>138</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="409.6">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -3509,16 +3781,19 @@
         <v>23</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="409.5" customHeight="1">
+        <v>140</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="409.6">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3526,16 +3801,19 @@
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="409.5" customHeight="1">
+        <v>143</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="409.6">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3543,16 +3821,19 @@
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="409.5" customHeight="1">
+        <v>145</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="409.6">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -3560,16 +3841,19 @@
         <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="409.5" customHeight="1">
+        <v>147</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="409.6">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -3577,16 +3861,19 @@
         <v>19</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="409.5" customHeight="1">
+        <v>149</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="409.6">
       <c r="A14" s="1">
         <v>9</v>
       </c>
@@ -3594,24 +3881,30 @@
         <v>23</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="409.5" customHeight="1">
+        <v>151</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="409.6">
       <c r="A15" s="1">
         <v>10</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>147</v>
+        <v>153</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Iteration 3 completed for the both contexts.
</commit_message>
<xml_diff>
--- a/dataset/testing.xlsx
+++ b/dataset/testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajed/PycharmProjects/Study-on-ChatGPT/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B454847-90A2-8541-B0A1-53BFBA1B6734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3A0E4A-683D-5346-AE79-023829542514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="17300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ch1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="411">
   <si>
     <t>id</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>answer (separate_context) - 2</t>
+  </si>
+  <si>
+    <t>answer (separate_context) - 3</t>
   </si>
   <si>
     <t>a</t>
@@ -171,6 +174,24 @@
 This modification ensures that the loop will iterate through all the elements of the array, including the first element at index 0, and return the correct last index of the element if it is present in the array.</t>
   </si>
   <si>
+    <t>The given code is searching for the last index of a given value in an array, but it has a mistake in the for loop. Instead of starting the loop at x.length-1 and ending it at 0, it should be the other way around. Also, the loop condition should be i &gt;=0 instead of i&gt;0.
+The correct code should be:
+```
+public static int findLast (int[] x, int y)
+   {       
+    for (int i=x.length-1; i &gt;= 0; i--)
+      {
+         if (x[i] == y) 
+         {
+            return i;
+         }
+      }
+      return -1;
+   }
+```
+This ensures that the loop starts at the last index of the array and goes backwards, checking each element until it finds the last occurrence of the value or reaches the beginning of the array.</t>
+  </si>
+  <si>
     <t>b</t>
   </si>
   <si>
@@ -230,6 +251,12 @@
 x = [1, 2, 3, 4, 5] and y = 3, it should return 2 as the last index of 3 in array x.</t>
   </si>
   <si>
+    <t>A test case that does not execute the fault would be to call the method with a valid non-null int array and a value that is present in the array at least once. For example:
+findLast([1, 2, 3, 4, 5], 3)
+This test case would return the last index of 3 in the array, which is 2, as expected.
+It is not possible to create a test case that can guarantee that the code will never execute the fault because of the "throws NullPointerException" that is present in the method signature. This means that if the method is called with a null int array, it will throw a NullPointerException, regardless of the value passed in as the second argument.</t>
+  </si>
+  <si>
     <t>c</t>
   </si>
   <si>
@@ -276,6 +303,9 @@
   </si>
   <si>
     <t>It's not possible for this code to execute the fault without resulting in an error state because the code throws a NullPointerException if the input array x is null. Therefore, if a null value is passed as the input for x, the code will throw an exception and the program will be in an error state.</t>
+  </si>
+  <si>
+    <t>A test case that would execute the fault in the code above but not result in an error state would be passing an array "x" with values [1,2,3,4,5,6] and the value "y" as 6. The function will return the last index of 6 which is 5, which is the correct index. However the for loop condition is wrong, it should be i &gt;= 0 instead of i &gt; 0, so it will not find the last element.</t>
   </si>
   <si>
     <t>d</t>
@@ -332,6 +362,9 @@
 findLast(x, y); 
 ``
 This will not halt the program, but will throw a NullPointerException.</t>
+  </si>
+  <si>
+    <t>This code will result in a failure if the input array x is null, as it throws a NullPointerException. However, if the input array x is not null, the code will not result in an error because it does not contain any logical errors. The program counter will reach the end of the function and return -1 if the input value y is not found in the array x.</t>
   </si>
   <si>
     <t>e</t>
@@ -387,6 +420,9 @@
   </si>
   <si>
     <t>The first error state would occur when a NullPointerException is thrown, which would happen if the input array "x" is null. The state of the program would be that the function has been called with a null array as the first argument and an integer as the second argument, and the program would be in the process of throwing the NullPointerException.</t>
+  </si>
+  <si>
+    <t>The first error state for this test case would occur if the input array "x" is null, as it would throw a NullPointerException. The complete state of this error would include the input array "x" being null, the value being searched for "y" being an integer, and the method returning a NullPointerException.</t>
   </si>
   <si>
     <t>f</t>
@@ -597,6 +633,31 @@
 ```
 This should print "Last index of 4: 5"
 You can also test with an empty array and a non-existing element and check if it returns -1 as expected.</t>
+  </si>
+  <si>
+    <t>To fix the issue with the given code, the loop condition should be changed from `i &gt; 0` to `i &gt;= 0`. This ensures that the loop iterates through all elements of the array, including the first element at index 0. 
+Additionally, it would be a good practice to add a null check before the loop to throw a `NullPointerException` if the array passed as the first argument is null, as mentioned in the javadoc.
+Here is the corrected code:
+```
+public static int findLast(int[] x, int y) {
+    if (x == null) {
+        throw new NullPointerException("x is null");
+    }
+    for (int i = x.length - 1; i &gt;= 0; i--) {
+        if (x[i] == y) {
+            return i;
+        }
+    }
+    return -1;
+}
+```
+And here is an example of test case that verifies that the program works as expected
+```
+int[] arr = {1, 2, 3, 4, 5, 6, 7, 8, 9, 10};
+int lastIndex = findLast(arr, 8);
+System.out.println("Last index of 8: " + lastIndex);
+```
+The output will be "Last index of 8: 7" which is the expected value.</t>
   </si>
   <si>
     <t>/**
@@ -742,6 +803,23 @@
 ```</t>
   </si>
   <si>
+    <t>The given code is searching for the last index of zero in the given array 'x' and returning it. However, the code is only searching the array in a forward direction, and not in reverse direction, so it will always return the first zero it encounters in the array, instead of the last. To fix this issue, the code needs to be modified to start the search from the last index of the array and work backwards, like this:
+```
+public static int lastZero (int[] x)
+{
+   for (int i = x.length -1; i &gt;= 0; i--)
+   {
+      if (x[i] == 0)
+      {
+         return i;
+      }
+   }
+   return -1;
+}
+```
+This modification will start the search from the last index of the array, and work backwards towards the first index, ensuring that the last zero in the array is returned.</t>
+  </si>
+  <si>
     <t xml:space="preserve">
 Since the given code does not contain any faults, any test case that passes a valid input (i.e., an non-null array of integers) to the method would not execute the fault.
 For example, the following test case would not execute the fault:
@@ -788,6 +866,9 @@
   </si>
   <si>
     <t>Test case that does not execute the fault: x = [1, 2, 3]; Expected output = -1. This test case does not execute the fault because it does not contain any 0s, so the loop will not find any 0s and return -1 as expected.</t>
+  </si>
+  <si>
+    <t>A test case that does not execute the fault would be an array where the last element is not 0. For example, x = [1, 2, 3]. In this case, the function would return -1 as expected, as there are no 0's in the array.</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -847,6 +928,10 @@
 One test case that executes the fault, but does not result in an error state, is when the input array is empty. The method will correctly return -1 indicating that there are no zeroes in the array.</t>
   </si>
   <si>
+    <t>A test case that executes the fault would be an input of an array that contains multiple zeroes, such as x = [0, 1, 2, 0, 3, 0], as the method will only return the index of the first occurrence of 0, which is 0, instead of the last occurrence, which is 5.
+This test case will not result in an error state, as the method will still return a valid integer value, it just doesn't meet the requirement of returning the last occurrence of 0.</t>
+  </si>
+  <si>
     <t xml:space="preserve">
 Since the given code does not contain any faults, it is not possible to provide a test case that results in an error but not a failure.
 The code simply searches for the last occurrence of the value 0 in an array of integers and returns the index of that occurrence. If the value 0 is not found in the array, the method returns -1. There is no way for the method to produce an error in this behavior.
@@ -913,6 +998,9 @@
 int result = lastZero(x);
 ```
 This would throw a `NullPointerException` when the method tries to access the first element of the array but it is null.</t>
+  </si>
+  <si>
+    <t>The given code throws a `NullPointerException` if the input array `x` is null. So, a test case that results in an error would be `lastZero(null)`. This will result in an error, but not a failure, as the code is handling the error by throwing an exception.</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -960,6 +1048,13 @@
   </si>
   <si>
     <t>The first error state would occur if the input array 'x' passed to the method is null, which would result in a NullPointerException being thrown. The complete state at this point would be that the input array 'x' is null and the code is trying to access elements in the array, causing the exception to be thrown.</t>
+  </si>
+  <si>
+    <t>The first error state would be if the input array is null, which would trigger a NullPointerException. 
+The complete state would be:
+- x: null 
+- i: not defined 
+- Return value: None (as it throws exception)</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -1087,6 +1182,22 @@
 ```
 In this version, I've added a variable `lastIndex` initialized to -1, to keep track of the last index of 0 that we come across in the loop. I've also changed the return statement inside the loop to update the `lastIndex` variable instead of returning the index immediately. This way, the loop will continue to iterate through the entire array, and the `lastIndex` variable will hold the last index of 0 that was found in the array.
 Testing the code with the input `x = [0, 1, 0]` will give the output `2`, which is the expected result.</t>
+  </si>
+  <si>
+    <t>I'm sorry, I am an AI language model and I am not able to take screenshots or execute code. However, I can help you implement the repair to the given function.
+The given function iterates through the array and returns the index of the first zero it finds. To make it return the index of the last zero, you need to update the loop to start at the end of the array and iterate backwards. Additionally, you should initialize a variable to store the last zero index found, and update it only if a zero is found at a higher index than the previously found index. Here is an example of how to implement this:
+```
+    public static int lastZero (int[] x) {
+        int lastZeroIndex = -1;
+        for (int i = x.length - 1; i &gt;= 0; i--) {
+            if (x[i] == 0) {
+                lastZeroIndex = i;
+            }
+        }
+        return lastZeroIndex;
+    }
+```
+You can then test the function with the given test case and verify that the expected output is produced.</t>
   </si>
   <si>
     <t>/** 
@@ -1214,6 +1325,13 @@
 This modification checks if the input array is null, and if it is, throws an IllegalArgumentException with a message indicating that the input array cannot be null. This way, the program will handle the null input scenario and the user will get a more informative error message.</t>
   </si>
   <si>
+    <t>The given code does not handle the case where the input array `x` is null. If the input array is null, the code will throw a NullPointerException when trying to access the length of the array. To fix this, I would propose adding a null check before the for loop that iterates through the array:
+```
+   if(x == null)
+   throw new NullPointerException("Input array is null");
+```</t>
+  </si>
+  <si>
     <t xml:space="preserve">
 Since there is no fault or error present in the given code, there is no need to provide a test case to demonstrate the absence of a fault. Any valid test case (that is, a test case that passes in an array of integers as a parameter) will execute correctly with the given implementation. 
 If you have a specific issue or error in mind that you would like to test, please provide more information about the fault or error you are trying to address. 
@@ -1259,6 +1377,12 @@
 It is not possible to give a test case that does not execute the fault, because a null x will always throw a NullPointerException.</t>
   </si>
   <si>
+    <t>A test case that does not execute the fault would be to provide a non-null array x that contains only positive integers as input. For example, the following test case should not execute the fault:
+int[] testArray = {1, 2, 3, 4, 5};
+countPositive(testArray);
+The reason that this test case does not execute the fault is because the provided array is not null, and all elements of the array are greater than or equal to 0, which satisfies the condition in the if statement.</t>
+  </si>
+  <si>
     <t xml:space="preserve">
 Since there is no fault or error present in the given code, there is no need to provide a test case to demonstrate the execution of a fault. The code will execute correctly for any valid input. 
 If you have a specific issue or error in mind that you would like to test, please provide more information about the fault or error you are trying to address. 
@@ -1288,6 +1412,9 @@
   </si>
   <si>
     <t>It is not possible for this code to execute a fault but not result in an error state, because the code throws a NullPointerException if the input array "x" is null. This means that if a null array is passed as input, the code will throw an exception and the program will enter an error state.</t>
+  </si>
+  <si>
+    <t>It is not possible for this code to execute the fault, but not result in an error state because a `NullPointerException` will be thrown if the input array `x` is `null`. This exception is explicitly thrown in the method's signature and will be caught by the runtime system, resulting in an error state. Therefore, there is no test case that can execute the fault without resulting in an error state.</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -1356,6 +1483,11 @@
 ```</t>
   </si>
   <si>
+    <t>A test case that results in an error would be passing a null value to the "x" parameter of the "countPositive" method. This would cause a "NullPointerException" to be thrown, as specified in the method's documentation. An example of this test case would be:
+countPositive(null);
+This test case would not result in a failure as the program would not crash, but it would throw an exception and the program would not execute the rest of the method.</t>
+  </si>
+  <si>
     <t xml:space="preserve">
 Without a specific test case or fault to address, it is not possible to describe an error state. If you have a specific issue or error in mind that you would like to test, please provide more information about the fault or error you are trying to address. 
 </t>
@@ -1395,6 +1527,9 @@
   </si>
   <si>
     <t>The first error state for the given test case would occur if the input array 'x' passed to the countPositive method is null. This would result in a NullPointerException being thrown when the for loop attempts to access the length of the array, as x would be null and therefore have no length property. The complete state at this point would include the count variable being initialized to 0, the for loop being in the process of executing and the NullPointerException being thrown.</t>
+  </si>
+  <si>
+    <t>The first error state for the given test case would occur if the input array "x" is null. This would cause a NullPointerException to be thrown when the for loop attempts to access the length of the array. The complete state of the error would include the null input array and the exception being thrown at the line where the for loop is attempting to access the length of the array.</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -1547,6 +1682,31 @@
 To verify that the new program works, I would create test cases that include passing a null value as the argument, and check that a NullPointerException is thrown as expected. I would also test the method with different arrays of integers, both positive and negative, to ensure that the count of positive elements is returned correctly.</t>
   </si>
   <si>
+    <t>I'm sorry, I'm a text-based AI model and I'm not able to provide a screen printout or other evidence that your program works. However, I can help you with a code review and suggest a repair for the given function.
+The given function seems to be counting the number of positive elements in an array. The function takes an array of integers as an argument and returns an integer that represents the number of positive elements in the array. The function also throws a NullPointerException if the array passed as an argument is null.
+One issue in the given function is that it doesn't handle negative numbers, It only counts elements that are greater or equal to 0.
+A possible repair would be to change the if statement to check if the element is greater than 0 instead of greater than or equal to 0.
+```
+if (x[i] &gt; 0)
+{
+   count++;
+}
+```
+Another solution is to add a check to check if x is null before iterating over the array and throw a NullPointerException if x is null.
+```
+if(x == null){
+   throw new NullPointerException("Array is null");
+}
+```
+It is also good practice to check if x.length is greater than 0 before iterating over it, otherwise it will throw an exception if x is empty.
+```
+if(x.length == 0){
+   throw new IllegalArgumentException("Array is empty");
+}
+```
+By making these changes, the function should now correctly count the number of positive elements in an array and throw appropriate exceptions when the array passed as an argument is null or empty.</t>
+  </si>
+  <si>
     <t>/**
    * Count odd or positive elements in an array
    *
@@ -1695,6 +1855,27 @@
 ```</t>
   </si>
   <si>
+    <t>There is nothing inherently wrong with the given code, it appears to be a correct implementation of counting the number of elements in an array that are either odd or positive (or both). However, if the input array is null, the code will throw a NullPointerException. To prevent this, we can add a null check at the beginning of the function, before the for loop, like this:
+```
+   public static int oddOrPos (int[] x)
+   {
+      if (x == null) {
+          throw new IllegalArgumentException("Array should not be null");
+      }
+      int count = 0;
+      for (int i = 0; i &lt; x.length; i++)
+      {
+         if (x[i]%2 == 1 || x[i] &gt; 0)
+         {
+            count++;
+         }
+      }
+      return count;
+   }
+```
+This will ensure that the function throws an IllegalArgumentException instead of a NullPointerException when the input array is null.</t>
+  </si>
+  <si>
     <t>It is not possible to give a test case that does not execute the fault, because the fault in the code is that it does not handle the case where an element in the array is negative and odd. Any array that contains at least one negative and odd element will execute the fault.
 For example, the following test case would execute the fault:
 ```
@@ -1735,6 +1916,9 @@
     <t>A test case that does not execute the fault would be an input array of all even and non-positive integers, such as [0, -2, -4, -6]. The method would return 0 as the count of elements in the array that are either odd or positive is 0.</t>
   </si>
   <si>
+    <t>A test case that does not execute the fault would be: x = [2, 4, 6, 8, 10]; In this case, none of the elements in the array are odd or positive (or both) so the count variable will remain at 0 and the function will return 0.</t>
+  </si>
+  <si>
     <t xml:space="preserve">It is not possible to give a test case that executes the fault but does not result in an error state, because the fault in the code is that it does not handle the case where an element in the array is negative and odd. Any array that contains at least one negative and odd element will execute the fault, and the result of the oddOrPos() function will not be correct.
 For example, the following test case would execute the fault:
 ```
@@ -1768,6 +1952,9 @@
   </si>
   <si>
     <t>It is not possible to give a test case that executes the fault, but does not result in an error state because the method throws a `NullPointerException` if the input array `x` is null. If `x` is null, the method will not execute and will immediately throw an exception, resulting in an error state.</t>
+  </si>
+  <si>
+    <t>It is not possible to give a test case that executes the fault of this method but does not result in an error state because the method throws a `NullPointerException` if the input array `x` is null. If `x` is null, the code will not execute any further and will immediately throw the exception. This is because the method has a precondition that `x` should not be null and it checks for it in the beginning itself.</t>
   </si>
   <si>
     <t>It is not possible to give a test case that results in an error but not a failure, because the fault in the code is not related to error handling. The fault is that the code does not handle the case where an element in the array is negative and odd. This will not result in an error or a failure, but the result of the oddOrPos() function will not be correct.
@@ -1815,6 +2002,9 @@
 oddOrPos(null);
 ```
 If the array is not null and the input array is well-formed, this function will run correctly and return the expected output for any given test cases. There is no other way to cause an error in this function.</t>
+  </si>
+  <si>
+    <t>A test case that results in an error would be passing a null value for the parameter x, as the method throws a NullPointerException in this case. This is not a failure as the method is correctly handling the error condition by throwing an exception.</t>
   </si>
   <si>
     <t>The first error state in the test case occurs when the oddOrPos() function is called with a null array. This results in the following error state:
@@ -1859,6 +2049,9 @@
   </si>
   <si>
     <t>The first error state in this given test case would occur when the input array 'x' is null, as the method throws a NullPointerException in this scenario. The complete state of the error would be that the variable 'x' is null and the method is unable to perform the iteration to count the number of odd or positive elements, resulting in the NullPointerException being thrown.</t>
+  </si>
+  <si>
+    <t>The first error state in this test case would be if the input array 'x' is null, causing a NullPointerException to be thrown in the method. This would occur on the first line of the method before any logic is executed, as the method checks for a null value before counting the elements in the array. The complete state of the error would be that the input array 'x' is null and a NullPointerException is thrown.</t>
   </si>
   <si>
     <t>Here is the modified code that handles the case where the input array is null:
@@ -1960,6 +2153,28 @@
     <t>I'm sorry, I am an AI language model and do not have the capability to execute code or take screenshots. However, based on the provided code, it looks like the function "oddOrPos" is counting the number of elements in the input array "x" that are either odd or positive. The given test case, where x = [-3, -2, 0, 1, 4], should return 3 as there are 3 elements (1, -2 and 4) that are either odd or positive in the array x. If this test case returns the expected output, then the function should be working correctly.</t>
   </si>
   <si>
+    <t>The given code appears to be a Java method that counts the number of elements in an array that are either odd or positive (or both). The method takes in an array of integers as its only parameter, and uses a for loop to iterate through the array and check if each element is odd or positive. If it is, the count variable is incremented. The method then returns the final count.
+To fix the issue that the test case x = [-3, -2, 0, 1, 4]  is not producing the expected output of 3. I would suggest changing the condition in the if statement from (x[i]%2 == 1 || x[i] &gt; 0)  to (x[i]%2 != 0 || x[i] &gt; 0). This would include both positive even numbers and negative numbers in the count, which would give us the expected output.
+The fixed code should look like this:
+```
+public static int oddOrPos (int[] x)
+   {  // Effects:  if x is null throw NullPointerException
+      // else return the number of elements in x that
+      //      are either odd or positive (or both)
+      int count = 0;
+      for (int i = 0; i &lt; x.length; i++)
+      {
+         if (x[i]%2 != 0 || x[i] &gt; 0)
+         {
+            count++;
+         }
+      }
+      return count;
+   }
+```
+After this implementation, the test case x = [-3, -2, 0, 1, 4]  should produce the expected output of 3.</t>
+  </si>
+  <si>
     <t>Consider the following three example classes. These are OO faults taken from Joshua Bloch’s
 Effective Java, Second Edition. Answer the following questions about each.
 class Vehicle implements Cloneable
@@ -2140,6 +2355,21 @@
 Also, in the Truck class, the clone method should override the superclass's method and return a Truck type, and also use the keyword "override" to avoid the potential confusion.</t>
   </si>
   <si>
+    <t>The given code has a problem with the implementation of the clone method in the Truck class. The problem is that the clone method in the Truck class is calling the clone method of the superclass (Vehicle), which returns an object of type Vehicle. However, the Truck class is then trying to cast this object to type Truck, which will throw a ClassCastException at runtime.
+To fix this problem, the clone method in the Truck class should be modified to create and return a new object of type Truck, rather than calling the clone method of the superclass and then trying to cast the result. This can be done by adding a new constructor to the Truck class that takes a Truck object as a parameter and copies its fields, and then calling this constructor in the clone method:
+```
+public Truck (Truck truck) {
+    super(truck.x);
+    y = truck.y;
+}
+@Override
+public Truck clone() {
+    return new Truck(this);
+}
+```
+This way the returned object is guaranteed to be of the same class as the original object and the class cast exception will not occur.</t>
+  </si>
+  <si>
     <t>If possible, give a test case that does not execute the fault. If not, briefly explain why
 not.</t>
   </si>
@@ -2191,6 +2421,10 @@
   </si>
   <si>
     <t>It is not possible to give a test case that does not execute the fault as the fault is present in the implementation of the `clone()` method in the `Truck` class. The `clone()` method in the `Truck` class calls the `clone()` method of its superclass `Vehicle` and then attempts to cast the returned object to a `Truck` object. However, since the returned object is actually an instance of `Vehicle`, the cast will throw a `ClassCastException`. This exception will be thrown regardless of how the `Truck` object is created or how the `clone()` method is called.</t>
+  </si>
+  <si>
+    <t>The fault in this example is that the `clone()` method in the `Truck` class throws a `ClassCastException` when trying to cast the result of the `super.clone()` call to a `Truck` object. This is because the `clone()` method in the `Vehicle` class is not implemented correctly and does not create a proper copy of the object, resulting in the returned object not being an instance of the `Truck` class. 
+It is not possible to give a test case that does not execute the fault, as the fault is present in the `Truck` class's `clone()` method, which would always be called when attempting to clone a `Truck` object. The only way to avoid this fault would be to correct the implementation of the `clone()` method in the `Vehicle` class to correctly create a copy of the object.</t>
   </si>
   <si>
     <t>If possible, give a test case that executes the fault, but does not result in an error state.
@@ -2246,6 +2480,11 @@
 It's not possible to give a test case that executes the fault but does not result in an error state. Because the error occurs because of the class cast exception, it's not possible to fix the error without changing the design of the classes and their implementations.</t>
   </si>
   <si>
+    <t>This code contains a fault in the implementation of the clone method in the Truck class. The issue is that the result of the call to super.clone() is cast to a Truck object before its y field is set, but the result of the call to super.clone() is actually an object of type Vehicle, not Truck, so the cast throws a ClassCastException.
+A test case that executes the fault, but does not result in an error state would be to use the code as it is and test the clone method on a object of type Vehicle and not Truck. As the error is thrown in the Truck class's clone method, it will not be thrown in the Vehicle class's clone method.
+Alternatively, the fault could be corrected by implementing the Cloneable interface and the clone method correctly in the Vehicle class to properly create and return a new instance of the Truck class in the clone method of the Truck class.</t>
+  </si>
+  <si>
     <t>If possible, give a test case that results in an error, but not a failure. If not, briefly
 explain why not. Hint: Don’t forget about the program counter.</t>
   </si>
@@ -2280,6 +2519,9 @@
   </si>
   <si>
     <t>The test case that results in an error is when the code at location "B" is executed and the attempt is made to cast the Object returned by the super.clone() method to a Truck object. This will result in a ClassCastException being thrown because the Object returned by the super.clone() method is actually an instance of the Vehicle class and not the Truck class. This is an error, but not a failure because the program will continue to execute after the exception is thrown, provided that the exception is caught and handled properly.</t>
+  </si>
+  <si>
+    <t>The test case provided in the question, "Truck suv = new Truck (4); Truck co = suv.clone()" will result in an error, specifically a ClassCastException, because the Object returned by the super.clone() method in the Truck class's clone() method is being cast to a Truck object, but it is actually a Vehicle object. This is because the super.clone() method in the Truck class calls the clone() method defined in the Vehicle class, which only creates a new Vehicle object and does not properly handle cloning of the additional state in the Truck class. To avoid this error, the clone() method in the Vehicle class should be properly implemented to create a new object of the same class and properly copy all relevant state, and the clone() method in the Truck class should call this method and then properly copy any additional state specific to the Truck class.</t>
   </si>
   <si>
     <t>In the given code, describe the first error state. Be sure to describe the complete state.</t>
@@ -2331,6 +2573,9 @@
     <t>The first error in the given code is that the `clone()` method in the `Truck` class throws a `ClassCastException` when it tries to cast the result of the superclass's `clone()` method (which is of type `Object`) to a `Truck` object. This occurs at Location "B" in the `Truck` class's `clone()` method. The exception is thrown because the object returned by the `Vehicle` class's `clone()` method is not guaranteed to be an instance of the `Truck` class, so the cast is not guaranteed to succeed. This is a violation of the Liskov Substitution Principle, which states that objects of a superclass should be able to be replaced with objects of a subclass without causing errors.</t>
   </si>
   <si>
+    <t>The first error in the given code is in the `Truck` class's implementation of the `clone()` method. At Location "B", the `result` object is cast to a `Truck` object, but it is actually still an instance of the `Vehicle` class. This will throw a `ClassCastException` at runtime when the code attempts to cast the `Vehicle` object to a `Truck` object. The complete state of this error is that the `Truck.clone()` method is attempting to access a field (`y`) that is not present in the `Vehicle` class, and this is causing a class cast exception to be thrown at runtime.</t>
+  </si>
+  <si>
     <t>Implement your repair and verify that the given test now produces the expected output.
 Submit a screen printout or other evidence that your new program works.</t>
   </si>
@@ -2482,6 +2727,32 @@
 suv.x = co.x; suv.getClass() = co.getClass()
 ```
 It is important to note that this is a shallow copy of the object, if you have any references to mutable objects within the class, those references will be shared between the original and the cloned object.</t>
+  </si>
+  <si>
+    <t>In the above code, the `Vehicle` class implements the `Cloneable` interface and overrides the `clone()` method. The `Truck` class extends the `Vehicle` class and also overrides the `clone()` method. However, the `Truck` class's `clone()` method is flawed because it attempts to cast the result of the `super.clone()` method to a `Truck` object, which may throw a `ClassCastException` if the object is not actually an instance of `Truck`.
+To fix this issue, the `clone()` method in the `Truck` class should be changed to create a new instance of `Truck` using the constructor, passing the value of the current object's `x` and `y` fields to the constructor, instead of trying to cast the result of `super.clone()`.
+```
+class Truck extends Vehicle
+{
+    private int y;
+    public Truck (int z) { super (z); y = z;}
+    @Override
+    public Truck clone()
+    {
+        return new Truck(this.x, this.y);
+    }
+    // other methods omitted
+}
+```
+Also, the return type of clone method should be `Truck` instead of `Object` to prevent ClassCastException.
+This will fix the issue and create a new instance of `Truck` rather than trying to cast the result of `super.clone()`, avoiding the `ClassCastException`.
+You can test the class by creating an instance of Truck class, cloning it and checking if the x and y attributes are equal. 
+```
+    Truck suv = new Truck (4); 
+    Truck co = suv.clone();
+    //expected: suv.x = co.x; suv.getClass() = co.getClass()
+```
+This will work as expected and will not throw any exception.</t>
   </si>
   <si>
     <t xml:space="preserve"> Consider the following three example classes. These are OO faults taken from Joshua Bloch’s
@@ -2571,6 +2842,16 @@
 Note: This is just a example, and it's not a real code and real classes, so it doesn't make sense to test the example.</t>
   </si>
   <si>
+    <t>The problem with the given code is that the `BigDecimal` class has inconsistent behavior between its `equals()` and `compareTo()` methods. In the code, `x` and `y` are two `BigDecimal` objects with different string representations but are equal according to `compareTo()` method, however, the `equals()` method returns false. This causes the `TreeSet` to only contain one element, while the `HashSet` contains both `x` and `y` as separate elements. 
+To fix this, one possible modification would be to override the `equals()` method in the `BigDecimal` class to ensure that it returns true when `compareTo()` returns 0. This would make the behavior of `equals()` consistent with `compareTo()`, and the `TreeSet` would contain both `x` and `y` as separate elements. Additionally, the `HashSet` would also contain both `x` and `y` as separate elements. 
+Another solution would be to use BigDecimal.compareTo() for adding elements to the TreeSet and HashSet, like this: 
+```
+BigDecimalTree.add(x.compareTo(y) == 0 ? x : y);
+BigDecimalHash.add(x.compareTo(y) == 0 ? x : y);
+```
+This way, while adding the elements, only one of the elements with same value but different representation would be added, thus maintaining consistency.</t>
+  </si>
+  <si>
     <t xml:space="preserve">
 It is not possible to give a test case that does not execute the fault in the given code, because the fault is inherent in the implementation of the `BigDecimal` class. The fault occurs whenever the `BigDecimal` objects `x` and `y` are used with a collection that relies on either the `equals` or `compareTo` methods for comparison, regardless of the specific values of `x` and `y`.
 The fault occurs because the `equals` and `compareTo` methods of the `BigDecimal` class are implemented in a way that is inconsistent with each other. The `equals` method returns `false` for the `BigDecimal` objects `x` and `y`, but the `compareTo` method returns `0` for the same objects, indicating that they are equal. This inconsistency can lead to unexpected behavior when using the `BigDecimal` objects with collections that rely on either the `equals` or `compareTo` methods for comparison.
@@ -2606,6 +2887,9 @@
 });
 ```
 This will ensure that the TreeSet uses equals() method to compare the BigDecimal values and will add both x and y to the set.</t>
+  </si>
+  <si>
+    <t>It is not possible to give a test case that does not execute the fault in this example, because the fault is inherent in the implementation of the `BigDecimal` class. The `equals()` and `compareTo()` methods in `BigDecimal` are inconsistent, meaning that they do not return the same result for the same input. In this example, `x` and `y` are two `BigDecimal` objects with the same value, but the `equals()` method returns `false` for them, while the `compareTo()` method returns `0`. As a result, when `x` and `y` are added to a `TreeSet`, only one of them is added, while both are added to a `HashSet`. This behavior cannot be avoided without changing the implementation of the `BigDecimal` class.</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -2689,6 +2973,11 @@
 This test case demonstrates the inconsistency between equals() and compareTo() in the BigDecimal class, but it does not result in an error state as the program runs successfully.</t>
   </si>
   <si>
+    <t>In the given example, the problem is that the BigDecimal class's equals() and compareTo() methods are inconsistent. The code creates two BigDecimal objects, x and y, with the values "1.0" and "1.00" respectively. Even though x and y are not equal according to the equals() method (!x.equals(y)), the compareTo() method returns 0, indicating that they are equal.
+When these objects are added to a TreeSet, the set uses the compareTo() method to determine equality, so only one element is added to the set. However, when added to a HashSet, the set uses the equals() method, so both x and y are added to the set.
+A test case that executes this fault but does not result in an error state would be to create two BigDecimal objects with slightly different values, and add them to both a TreeSet and a HashSet. The output of the test would show that the TreeSet only has one element, while the HashSet has two elements, which would demonstrate the inconsistency between the equals() and compareTo() methods in the BigDecimal class.</t>
+  </si>
+  <si>
     <t>If possible, give a test case that results in an error, but not a failure. If not, briefly explain why not. Hint: Don’t forget about the program counter.</t>
   </si>
   <si>
@@ -2737,6 +3026,11 @@
 However, this would not result in an error or a failure in the program. The program would simply output the expected results, and the only indication of a problem would be the discrepancy between the output of the two sets. So in this case, it is not possible to give a test case that results in an error but not a failure.</t>
   </si>
   <si>
+    <t>The given code creates two instances of BigDecimal, x and y, with the values "1.0" and "1.00" respectively. It then adds these instances to two different Sets, a TreeSet and a HashSet. The TreeSet uses the compareTo() method of the BigDecimal class to compare and add elements, while the HashSet uses the equals() method. Since the compareTo() method of BigDecimal returns 0 for x and y, the TreeSet only contains one element, while the HashSet contains both x and y.
+A test case that results in an error but not a failure would be one where the program expects the TreeSet to contain both x and y, but it only contains one element due to the inconsistent behavior of the equals() and compareTo() methods in BigDecimal. For example, a test case could check the size of the TreeSet and assert that it is equal to 2, which would throw an error if the TreeSet only contains one element.
+As for why this test case would not result in a failure, is because it's just a test case that check if the size of the TreeSet is 2, but the program is still running as expected and the program counter is not affected by it.</t>
+  </si>
+  <si>
     <t xml:space="preserve">
 There is no error state in the given code. The code simply creates and uses two `BigDecimal` objects and two collections, which are all valid operations.
 The fault in the given code is not an error, but rather an inconsistency in the implementation of the `equals` and `compareTo` methods of the `BigDecimal` class. This inconsistency can lead to unexpected behavior when using the `BigDecimal` objects with collections that rely on either the `equals` or `compareTo` methods for comparison, such as the `TreeSet` and `HashSet` in the example. However, this behavior is not considered an error, as it does not result in a syntax error or a runtime exception.
@@ -2769,6 +3063,9 @@
   </si>
   <si>
     <t>The first error state in the given code is that the TreeSet, BigDecimalTree, only contains one element, whereas the HashSet, BigDecimalHash, contains two elements. This is because the TreeSet uses the compareTo() method to determine if elements are equal, while the HashSet uses the equals() method. In this case, the BigDecimal class has an inconsistency where the equals() method returns false for the BigDecimal objects x and y, but the compareTo() method returns 0, indicating that they are equal. This causes the TreeSet to only contain one element, while the HashSet contains both elements.</t>
+  </si>
+  <si>
+    <t>The first error state in the given code occurs when the elements x and y, which are instances of the BigDecimal class with the values "1.0" and "1.00" respectively, are added to the BigDecimalTree Set. Since the TreeSet uses the compareTo() method for comparison, the element y is considered equal to the element x and is not added to the set, resulting in the BigDecimalTree Set having only 1 element. This is an error state as the expected behavior is that the BigDecimalTree Set should have 2 elements, x and y, as they have different values.</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -2932,6 +3229,21 @@
 ```
 With this modification, the test code would produce the expected output of "BigDecimalTree = 1; BigDecimalHash = 1".
 It is better to use a wrapper class that wraps BigDecimal and override the equals method, rather than modifying BigDecimal class which is a final class.</t>
+  </si>
+  <si>
+    <t>The provided code demonstrates an issue with the implementation of the `equals()` and `compareTo()` methods in the `BigDecimal` class. The `equals()` method returns `false` when comparing `x` and `y`, even though `x.compareTo(y)` returns `0`, indicating that they are equal. As a result, when adding `x` and `y` to a `TreeSet`, only one element is added to the set (since `TreeSet` uses `compareTo()` for element ordering and comparison), while adding them to a `HashSet` results in both elements being added (since `HashSet` uses `equals()` for element comparison).
+To repair this issue, the `equals()` method in the `BigDecimal` class should be overridden to use the same comparison logic as the `compareTo()` method. This can be done by adding the following code to the `BigDecimal` class:
+```
+@Override
+public boolean equals(Object obj) {
+    if (!(obj instanceof BigDecimal)) {
+        return false;
+    }
+    return compareTo((BigDecimal) obj) == 0;
+}
+```
+With this modification, when adding `x` and `y` to a `TreeSet` and `HashSet`, both sets will have only one element. Thus, the test output will be "BigDecimalTree = 1; BigDecimalHash = 1" which is the expected output.
+It is advisable to also override the hashCode method as well to follow the contract of hashcode and equals.</t>
   </si>
   <si>
     <t xml:space="preserve">Consider the following three example classes. These are OO faults taken from Joshua Bloch’s
@@ -3086,6 +3398,20 @@
 This modification would ensure that the ColorPoint class correctly implements the equals method by taking the additional color field into account and the expected results from the tests would be produced.</t>
   </si>
   <si>
+    <t>The code defines two classes, Point and ColorPoint, where ColorPoint extends Point. The problem with the code is that the equals method in the ColorPoint class incorrectly checks for equality only between the color instance variables, and not the x and y instance variables inherited from the Point class. This means that a Point and a ColorPoint with the same x and y values will not be considered equal.
+To fix this fault, the equals method in the ColorPoint class should be modified to check for equality between all of the instance variables, including those inherited from the Point class. This can be done by calling the equals method of the superclass within the ColorPoint's equals method, and also checking for equality between the color instance variables.
+For example:
+```
+@Override public boolean equals (Object o) {
+    if (!(o instanceof ColorPoint)) return false;
+    if (!super.equals(o)) return false;
+    ColorPoint cp = (ColorPoint) o;
+    return cp.color == this.color;
+}
+```
+This way the `super.equals(o)` will check for equality of x and y which is inherited from Point class and `cp.color == this.color` will check for equality of color specific to ColorPoint class.</t>
+  </si>
+  <si>
     <t xml:space="preserve">
 It is not possible to give a test case that does not execute the fault in the given code because the fault is present in the implementation of the `equals` method in both the `Point` and `ColorPoint` classes. The fault in the `Point` class is that the method does not properly override the `equals` method in the `Object` class, and the fault in the `ColorPoint` class is that the method does not properly handle the case where it is passed an object that is not an instance of `ColorPoint`. These faults are present in the implementation of the `equals` method in both classes and will be executed every time the method is called.
 To avoid executing the fault, the implementation of the `equals` method in both classes must be modified to properly override the `equals` method in the `Object` class and handle the case where it is passed an object that is not an instance of the class. The modified `equals` methods for both classes were provided in the previous response.
@@ -3120,6 +3446,10 @@
 As you can see, this test case does not execute the fault because it does not involve any instances of the `ColorPoint` class.</t>
   </si>
   <si>
+    <t>The class ColorPoint extends Point, and adds the additional state of 'color'. The class overrides the equals method, but the implementation is faulty as it only compares the color state of the ColorPoint class, it does not consider the Point class' state of x and y. In the test cases, p.equals(cp1) returns true, but cp1.equals(p) returns false, and cp1.equals(cp2) also returns false, while they are expected to return true.
+It is not possible to give a test case that does not execute the fault because the fault is in the implementation of the equals method in the ColorPoint class. The correct implementation would be to use "super.equals(cp) &amp;&amp; (cp.color == this.color)" instead of just "(cp.color == this.color)".</t>
+  </si>
+  <si>
     <t xml:space="preserve">
 It is not possible to give a test case that executes the fault in the given code but does not result in an error state because the fault in the `Point` class will always result in an error state (i.e., a `ClassCastException` will be thrown) when the `equals` method is called with an object that is not an instance of the `Point` class. The fault in the `ColorPoint` class will also always result in an error state (i.e., a `ClassCastException` will be thrown) when the `equals` method is called with an object that is not an instance of the `ColorPoint` class.
 To avoid these error states, the implementation of the `equals` method in both classes must be modified to properly handle the case where it is passed an object that is not an instance of the class. The modified `equals` methods for both classes were provided in a previous response.
@@ -3161,6 +3491,18 @@
 The fault in ColorPoint class can be seen in the test case where cp1.equals(p) is expected to be true but it returns false.</t>
   </si>
   <si>
+    <t>The class Point defines an equals method that checks if two Point objects have the same x and y values. The class ColorPoint extends Point and also defines an equals method that checks if two ColorPoint objects have the same x, y, and color values. 
+However, the equals method in ColorPoint is faulted because it only returns true if the object being compared to is also an instance of ColorPoint, instead of checking if it's an instance of the superclass Point. This means that the following test cases will have unexpected results: 
+- p.equals (cp1) should return true, but it actually returns false
+- cp1.equals (p) should return true, but it actually returns false
+- cp1.equals (cp2) should return false, and it returns false
+A test case that executes the fault but doesn't result in an error state would be:
+- Point p = new Point (1,2);
+- ColorPoint cp1 = new ColorPoint (1,2,RED);
+- cp1.equals(p) 
+As this test case calls the equals method on an instance of ColorPoint and compares it to an instance of Point, it should return true according to the expected behavior. However, it returns false because of the fault in the equals method of ColorPoint.</t>
+  </si>
+  <si>
     <t xml:space="preserve">
 It is not possible to give a test case that results in an error but not a failure for the given code because the fault in the `Point` class will always result in a failure (i.e., a `ClassCastException` will be thrown) when the `equals` method is called with an object that is not an instance of the `Point` class. The fault in the `ColorPoint` class will also always result in a failure (i.e., a `ClassCastException` will be thrown) when the `equals` method is called with an object that is not an instance of the `ColorPoint` class.
 To avoid these failures, the implementation of the `equals` method in both classes must be modified to properly handle the case where it is passed an object that is not an instance of the class. The modified `equals` methods for both classes were provided in a previous response.
@@ -3188,6 +3530,14 @@
 The class ColorPoint extends Point and also overrides the equals method. However, this implementation is incorrect as it only checks if the passed in object is an instance of ColorPoint and then compares the x and y values inherited from Point and the color field of the two ColorPoint objects. This means that if a plain Point object is passed to the equals method of a ColorPoint object, the method will return false. 
 The tests provided in the question demonstrate this issue. Test 1, p.equals (cp1) should return true, but it returns false because the equals method of ColorPoint only checks if the passed in object is an instance of ColorPoint. Test 2, cp1.equals (p) also returns false, but it should return true since the x and y values of the two Point objects are the same.
 It is not possible to give a test case that results in an error but not a failure because the issue is with the implementation of the equals method, not with the test cases. The issue is with the logic of the equals method which will always return false if passed a Point object, and this will result in a failure.</t>
+  </si>
+  <si>
+    <t>In the example above, the class ColorPoint extends Point and overrides the equals method. However, the equals method in ColorPoint only checks if the object is an instance of ColorPoint and compares the color of the two ColorPoints, while ignoring the x and y fields inherited from the Point class. This means that if a Point object and a ColorPoint object with the same x and y coordinates are compared, the equals method in ColorPoint will return false, while the expected result is true. This can be seen in the test case p.equals(cp1) which returns false, while the expected result is true.
+A test case that results in an error, but not a failure, could be calling the equals method on a null object. For example: 
+ColorPoint cp = new ColorPoint(1,2, RED);
+cp.equals(null); //this will throw a NullPointerException when it try to check the color of the null object.
+Another test case that results in an error would be passing an object of a different type other than Point or ColorPoint to the equals method.
+As for a test case that results in an error but not a failure, it is not possible here because the equals method does not have any error handling for unexpected input, and thus will throw an exception in such cases.</t>
   </si>
   <si>
     <t xml:space="preserve"> In the given code, describe the first error state. Be sure to describe the complete state.</t>
@@ -3227,6 +3577,10 @@
   </si>
   <si>
     <t>The first error state in the given code is in the implementation of the `equals` method in the `ColorPoint` class at Location B. In this method, the implementation first checks if the passed in object is an instance of `ColorPoint` using the `instanceof` operator. If it is not, the method immediately returns `false`. This results in a problem when comparing `ColorPoint` objects to `Point` objects, because `ColorPoint` objects are not considered equal to `Point` objects even if they have the same x and y coordinates. This can be seen in Test 2, where `cp1.equals(p)` returns `false` even though the x and y coordinates of both `p` and `cp1` are the same. This violates the symmetric property of the `equals` contract, as `p.equals(cp1)` returns `true` but `cp1.equals(p)` returns `false`.</t>
+  </si>
+  <si>
+    <t>The first error state in the given code is in the implementation of the `equals` method in the `ColorPoint` class. The implementation overrides the `equals` method inherited from the `Point` class, but it only returns `true` if the passed-in object is an instance of `ColorPoint` and if the color of the two objects match. This means that if an instance of `Point` is passed to the `equals` method of an instance of `ColorPoint`, the method will always return `false`, even if the x and y coordinates of the two points are the same. This violates the symmetric and transitive requirements of the `equals` method, as described in the `Object` class.
+Another error state in the given code is the class hierarchy, `ColorPoint` extends `Point` and `Point` is instantiable and the subclass state is extended by adding `color` attribute. This design decision can lead to many issues like tests 1 and 2 returning different results, whereas they should return the same results.</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -3382,6 +3736,44 @@
 I hope this helps!</t>
   </si>
   <si>
+    <t>The class Point defines a simple class that represents a point in 2D space. It has two private instance variables, x and y, that represent the x and y coordinates of the point. The class has a constructor that initializes these variables and an equals method that compares the x and y coordinates of this point with another point object.
+The class ColorPoint is a subclass of Point. It extends the state of the Point class by adding a private instance variable, color, that represents the color of the point. The class has a constructor that calls the constructor of the superclass and initializes the color variable. It also overrides the equals method of the superclass to include a comparison of the color instance variable in addition to the x and y coordinates.
+The fault in this class hierarchy is that the equals method in the ColorPoint class does not properly handle the case when it is passed a Point object instead of a ColorPoint object. The current implementation returns false in that case, which is incorrect. The expected behavior is that the equals method should return true when a Point object and a ColorPoint object have the same x and y coordinates, regardless of the color of the ColorPoint object.
+To fix this issue, the equals method in the ColorPoint class should be modified to first check if the passed object is an instance of Point, and if so, call the equals method of the superclass to compare the x and y coordinates. If the passed object is not an instance of Point, then it should continue to check if it is an instance of ColorPoint and compare the color variable as well.
+Here's the fixed code:
+```
+class ColorPoint extends Point
+{
+private Color color;
+// Fault: Superclass instantiable; subclass state extended
+public ColorPoint (int x, int y, Color color)
+{
+super (x,y);
+this.color=color;
+}
+@Override public boolean equals (Object o)
+{
+if (!(o instanceof Point)) return false;
+if (o instanceof ColorPoint) {
+ColorPoint cp = (ColorPoint) o;
+return (super.equals(cp) &amp;&amp; (cp.color == this.color));
+} else {
+    return super.equals(o);
+}
+}
+```
+With above modification, the tests:
+```
+Point p = new Point (1,2);
+ColorPoint cp1 = new ColorPoint (1,2,RED);
+ColorPoint cp2 = new ColorPoint (1,2,BLUE);
+p.equals (cp1); // Test 1: Result = true;
+cp1.equals (p); // Test 2: Result = true;
+cp1.equals (cp2); // Test 3: Result = false;
+```
+Will produce the expected output.</t>
+  </si>
+  <si>
     <t>How are faults and failures related to testing and debugging?</t>
   </si>
   <si>
@@ -3400,6 +3792,9 @@
   </si>
   <si>
     <t>Faults and failures are related to testing and debugging in that testing and debugging are used to identify and fix faults and failures in a system or application. Faults are mistakes or errors in the design or implementation of a system or application, while failures are instances of a system or application not performing as expected. Testing is used to identify faults by exposing a system or application to various inputs and conditions and observing its behavior, while debugging is used to find and fix faults by identifying the source of the problem and making changes to the system or application to correct it. Together, testing and debugging help ensure that a system or application is functioning correctly and is free of faults and failures.</t>
+  </si>
+  <si>
+    <t>Faults and failures are related to testing and debugging because testing is used to identify faults (bugs or defects) in a system and debugging is used to determine the cause of a failure (when the system does not behave as expected) and fix the underlying fault. In other words, testing is used to find problems and debugging is used to solve them.</t>
   </si>
   <si>
     <t>public class BoundedQueue
@@ -3790,6 +4185,82 @@
 It is important to note that these test cases are just examples, you might have different test cases, or different test input or expected outputs depending on the implementation of the class.</t>
   </si>
   <si>
+    <t>Here is an example of JUnit tests for the BoundedQueue class:
+```
+import static org.junit.jupiter.api.Assertions.*;
+import org.junit.jupiter.api.Test;
+class BoundedQueueTest {
+    BoundedQueue bq;
+    @Test
+    void testConstructor() {
+        bq = new BoundedQueue(5);
+        assertEquals(0, bq.size);
+        assertEquals(5, bq.capacity);
+        assertEquals(0, bq.front);
+        assertEquals(0, bq.back);
+    }
+    @Test
+    void testEnQueue() {
+        bq = new BoundedQueue(5);
+        bq.enQueue(1);
+        assertEquals(1, bq.size);
+        assertEquals(1, bq.elements[bq.back - 1]);
+        bq.enQueue(2);
+        assertEquals(2, bq.size);
+        assertEquals(2, bq.elements[bq.back - 1]);
+    }
+    @Test
+    void testEnQueueFull() {
+        bq = new BoundedQueue(2);
+        bq.enQueue(1);
+        bq.enQueue(2);
+        assertThrows(IllegalStateException.class, () -&gt; bq.enQueue(3));
+    }
+    @Test
+    void testEnQueueNull() {
+        bq = new BoundedQueue(2);
+        assertThrows(NullPointerException.class, () -&gt; bq.enQueue(null));
+    }
+    @Test
+    void testDeQueue() {
+        bq = new BoundedQueue(5);
+        bq.enQueue(1);
+        bq.enQueue(2);
+        assertEquals(1, bq.deQueue());
+        assertEquals(1, bq.size);
+    }
+    @Test
+    void testDeQueueEmpty() {
+        bq = new BoundedQueue(2);
+        assertThrows(IllegalStateException.class, () -&gt; bq.deQueue());
+    }
+    @Test
+    void testIsEmpty() {
+        bq = new BoundedQueue(2);
+        assertTrue(bq.isEmpty());
+        bq.enQueue(1);
+        assertFalse(bq.isEmpty());
+    }
+    @Test
+    void testIsFull() {
+        bq = new BoundedQueue(2);
+        assertFalse(bq.isFull());
+        bq.enQueue(1);
+        bq.enQueue(2);
+        assertTrue(bq.isFull());
+    }
+    @Test
+    void testToString() {
+        bq = new BoundedQueue(2);
+        bq.enQueue(1);
+        bq.enQueue(2);
+        assertEquals("[1, 2]", bq.toString());
+    }
+}
+```
+You can run this test class and see the test results by using a JUnit testing framework such as JUnit 5.</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 
 import java.util.*;
 public class Min
@@ -3885,6 +4356,11 @@
 After removing this line, the JUnit test for a list with a single null element will fail because the NullPointerException will no longer be thrown and the program will not handle the null element properly.</t>
   </si>
   <si>
+    <t>To delete the explicit throw of NullPointerException in the Min program, you can remove the following line of code:
+if (result == null) throw new NullPointerException ("Min.min");
+After removing this line of code, you should verify that the JUnit test for a list with a single null element now fails. This is because the explicit throw of the NullPointerException is used to handle the case where the list contains a null element, and without it, the program will not know how to handle a null element in the list, resulting in a failure of the JUnit test.</t>
+  </si>
+  <si>
     <t>The following JUnit test method for the sort() method has a non-syntactic flaw.
 @Test
 public void testSort()
@@ -3926,6 +4402,9 @@
   </si>
   <si>
     <t>The non-syntactic flaw in the test method is that it does not have a proper oracle. The oracle in this case, is the expected output of the sort() method. The test method only asserts that the first element of the names object after sorting should be "Alex" using the assertTrue() method, but it does not check if the rest of the elements are sorted in the correct order. This means that the test method only checks for a partial correctness of the sort() method, and does not guarantee that the sort() method works correctly in all cases.</t>
+  </si>
+  <si>
+    <t>The non-syntactic flaw in the test method is that it is not specifying the desired output of the sort() method. It is only checking if the first element of the sorted list is "Alex", without specifying what the expected order of the entire sorted list should be. This violates the requirement of the "Result" aspect of the RIPR model, which states that a test should specify the expected output of the tested code.</t>
   </si>
   <si>
     <t>Consider the following example class. PrimeNumbers has three methods. The first, computePrimes(), takes one integer input and computes that many prime numbers. iterator() returns an Iterator that will iterate through the primes, and toString() returns a string representation.
@@ -4070,6 +4549,28 @@
 This test would also not reach the fault as only 1 prime number is computed, and it is the first prime number which is 2 and it doesn't end with 9.</t>
   </si>
   <si>
+    <t>Test 1: 
+- Call computePrimes(3) 
+- Check if the returned list of primes contains 2, 3, and 5
+- The test would not reach the fault, as none of the primes generated by the method should have a last digit of 9, thus the test will pass.
+Test 2:
+- Call computePrimes(5)
+- Check if the returned list of primes contains 2, 3, 5, 7, 11
+- The test would not reach the fault, as none of the primes generated by the method should have a last digit of 9, thus the test will pass.
+Test 3:
+- Call computePrimes(10)
+- Check if the returned list of primes contains 2, 3, 5, 7, 11, 13, 17, 19, 23, 29
+- The test would reach the fault, as the returned list of primes should contain 29, but it will be omitted by the fault in the method, thus the test will fail.
+Test 4:
+- Call computePrimes(20)
+- Check if the returned list of primes contains 2, 3, 5, 7, 11, 13, 17, 19, 23, 29, 31, 37, 41, 43, 47, 53, 59, 61, 67, 71
+- The test would reach the fault, as the returned list of primes should contain 59, but it will be omitted by the fault in the method, thus the test will fail.
+Test 5:
+- Call computePrimes(50)
+- Check if the returned list of primes matches the list of primes generated by an oracle, such as a mathematical library or a list of primes found on a website
+- The test would reach the fault, as the returned list of primes will be different from the list of primes generated by the oracle, due to the omitted primes with a last digit of 9, thus the test will fail.</t>
+  </si>
+  <si>
     <t>Write a test that reaches the fault, but does not infect. If a test cannot be created, explain why.</t>
   </si>
   <si>
@@ -4133,6 +4634,14 @@
 The reason why it does not infect is that it is testing the specific case of the fault, and it does not affect the other test cases.</t>
   </si>
   <si>
+    <t>1. A test that calls computePrimes(5) and then calls toString(). This test would verify that the class correctly computes the first 5 prime numbers and stores them in the list, and that the toString method correctly returns a string representation of the list.
+2. A test that calls computePrimes(10) and then calls iterator(). This test would verify that the class correctly computes the first 10 prime numbers and stores them in the list, and that the iterator method correctly returns an iterator that can iterate through the list of primes.
+3. A test that calls computePrimes(20) and then calls toString(). This test would verify that the class correctly computes the first 20 prime numbers and stores them in the list, and that the toString method correctly returns a string representation of the list.
+4. A test that calls computePrimes(50) and then calls iterator(). This test would verify that the class correctly computes the first 50 prime numbers and stores them in the list, and that the iterator method correctly returns an iterator that can iterate through the list of primes.
+5. The test oracle would be to check if the last digit of the prime number is 9 or not.
+A test that calls computePrimes(10) and checks that the list of primes generated does not contain any prime number whose last digit is 9. This test would reach the fault, but it would not infect other tests as it is only checking for the absence of a specific condition in the generated list of primes.</t>
+  </si>
+  <si>
     <t>Write a test that infects the state, but does not propagate. If a test cannot be created, explain why.</t>
   </si>
   <si>
@@ -4185,6 +4694,14 @@
 4. A test that calls computePrimes(50) and checks that the size of the primes list is 49 (as 1 prime number ending in 9 is expected to be omitted)
 5. A test that calls computePrimes(50) and uses a test oracle to check that the primes list only includes prime numbers, and that none of them end in 9.
 For infecting state but not propagating, we can test with computePrimes(1) and check the primes list, if it has only one element and that element is not prime number or it is prime but ends with 9. It will confirm that the fault is only infecting the state and not propagating.</t>
+  </si>
+  <si>
+    <t>1. Test computePrimes(5) and then call toString(). The resulting string should be "[2, 3, 5, 7, 11]" and not include prime numbers whose last digit is 9.
+2. Test computePrimes(10) and then call iterator(). The iterator should iterate through the first 10 prime numbers, not including those whose last digit is 9.
+3. Test computePrimes(3) and then call toString(). The resulting string should be "[2, 3, 5]" and not include the prime number 7, whose last digit is 9.
+4. Test computePrimes(15) and then check that the last element of the list is 89. It should be, since 89 is the 15th prime number and the method is not including prime numbers whose last digit is 9.
+5. Test computePrimes(50) and check that the last element of the list is 449. It should be, since 449 is the 50th prime number and the method is not including prime numbers whose last digit is 9.
+A test that infects the state, but does not propagate, is not possible in this case. Since the method computePrimes() is not returning any value and it is only updating the internal state of the class, there is no way to infect the state without propagating it.</t>
   </si>
   <si>
     <t>Write a test that propagates, but does not reveal. If a test cannot be created, explain why.</t>
@@ -4229,6 +4746,23 @@
 </t>
   </si>
   <si>
+    <t>1. Test that checks if computePrimes() computes the correct number of prime numbers. This can be done by calling computePrimes(5) and then checking if the size of the primes list is 5.
+2. Test that checks if the iterator() method correctly iterates through the primes list. This can be done by calling computePrimes(5), then using the iterator() method to iterate through the primes and checking if the values match the expected prime numbers.
+3. Test that checks if the toString() method correctly represents the primes list. This can be done by calling computePrimes(5), then using the toString() method to get a string representation of the primes list and checking if the string matches the expected output.
+4. Test that checks if the computePrimes() method correctly omits prime numbers whose last digit is 9. This can be done by calling computePrimes(10) and then checking if the primes list contains any prime numbers whose last digit is 9. (Test oracle: manual check)
+5. Test that checks if the computePrimes() method correctly includes prime numbers whose last digit is not 9. This can be done by calling computePrimes(10) and then checking if the primes list contains prime numbers whose last digit is not 9. (Test oracle: manual check)
+A test that propagates but does not reveal the fault is to call computePrimes(5) and then check that the size of the primes list is equal to 5. This test will pass even if the fault is present as the computePrimes() method is still computing the correct number of prime numbers, but it does not reveal the fact that it is not including prime numbers whose last digit is 9.</t>
+  </si>
+  <si>
+    <t>1. Test the method computePrimes() by passing an input of 5 and verifying that the prime numbers generated do not include those with a last digit of 9.
+2. Test the method iterator() by calling it after computePrimes() is called with an input of 10 and verifying that the iterator does not return any prime numbers with a last digit of 9.
+3. Test the method toString() by calling it after computePrimes() is called with an input of 15 and verifying that the string representation does not include any prime numbers with a last digit of 9.
+4. Test the method computePrimes() by passing an input of 100 and comparing the output to a known list of prime numbers to verify that none with last digit 9 are missing.
+5. Test the method computePrimes() by passing an input of 100 and using a test oracle that verifies that no prime numbers whose last digit is 9 are missing. 
+For an example of a test that propagates but does not reveal:
+Test the method computePrimes() by passing an input of 100 and verifying that the output has 100 prime numbers, this test will propagate the fault but will not reveal it.</t>
+  </si>
+  <si>
     <t>Write a test that reveals the fault. If a test cannot be created, explain why.</t>
   </si>
   <si>
@@ -4270,6 +4804,24 @@
 5. Call the computePrimes() method with an input of 10 again
 6. Verify that the returned primes list contains prime numbers whose last digit is 9 (19, 29, 59, 79, 89, etc.)
 This test reveals the fault by calling the computePrimes() method twice with the same input and verifying that the primes list does not contain the expected prime numbers whose last digit is 9 the first time, but contains them the second time. This indicates that the fault is present in the computePrimes() method and causes it to not include prime numbers whose last digit is 9 in the primes list when called with a specific input of 10.</t>
+  </si>
+  <si>
+    <t>1. Test that computePrimes() correctly computes the first 10 prime numbers. Call computePrimes(10) and then call toString() to check that the output matches the expected list of prime numbers.
+2. Test that computePrimes() correctly computes the first 100 prime numbers. Call computePrimes(100) and then call toString() to check that the output matches the expected list of prime numbers.
+3. Test that computePrimes() correctly computes the first 100 prime numbers and then test that the iterator() method correctly iterates through them. Call computePrimes(100), then call iterator() and iterate through the output, comparing each element to the expected prime numbers.
+4. Test that computePrimes() correctly computes the first 20 prime numbers and check that it does not include any prime numbers whose last digit is 9. Call computePrimes(20), then call toString() and check that the output does not include any prime numbers whose last digit is 9.
+5. Test that computePrimes() correctly computes the first 20 prime numbers and check that it does not include any prime numbers whose last digit is 9. Call computePrimes(20) and check the output of iterator() by comparing the elements in the iterator to the expected prime numbers and check that none of them end with 9.
+Test oracle: The expected list of prime numbers generated by computePrimes() should match the list of prime numbers generated by an independent method or algorithm.
+e. A test that reveal the fault would be to check that computePrimes() correctly computes the first 100 prime numbers, but check that it does not include any prime numbers whose last digit is 9. 
+You can call computePrimes(100) and then call toString() to check that the output does not include any prime numbers whose last digit is 9.</t>
+  </si>
+  <si>
+    <t>1. A test that calls the computePrimes() method with an input of 10, then calls the toString() method and compares the output to a known list of the first 10 prime numbers (excluding those ending in 9).
+2. A test that calls the computePrimes() method with an input of 100, then calls the iterator() method and iterates through the primes, counting the number of primes that end in 9 and comparing that to the expected number (0).
+3. A test that calls the computePrimes() method with an input of 50, then calls the toString() method and compares the output to a known list of the first 50 prime numbers (excluding those ending in 9). Then, call the computePrimes() method again with an input of 50 and calls the toString() method and compares the output to a known list of the next 50 prime numbers (excluding those ending in 9)
+4. A test that calls the computePrimes() method with an input of 1000, then calls the iterator() method and iterates through the primes, comparing each prime to a known list of primes (excluding those ending in 9) and checking if any prime from the known list is missing.
+5. A test that calls the computePrimes() method with an input of 100, then calls the iterator() method and iterates through the primes, checking if any prime whose last digit is 9 is present or not.
+Note: The oracle in these test cases would be a known list of prime numbers (excluding those ending in 9) that can be used for comparison.</t>
   </si>
   <si>
     <t>When overriding the equals() method, programmers are also required to override the hashCode() method; otherwise clients cannot store instances of these objects in common Collection structures such as HashSet. For example, the Point class from Chapter 1 is defective in this regard.</t>
@@ -4410,6 +4962,46 @@
 </t>
   </si>
   <si>
+    <t>If the Point class has not overridden the hashCode() method, and the equals() method is used to compare two Point objects in a HashSet, the HashSet may not properly identify the two Point objects as equal. This can cause issues with adding, removing, or searching for the Point objects in the HashSet.
+For example, if we create two Point objects with the same x and y coordinates, the HashSet may not recognize them as equal and add them both to the set. 
+```
+HashSet&lt;Point&gt; pointSet = new HashSet&lt;&gt;();
+Point point1 = new Point(1, 2);
+Point point2 = new Point(1, 2);
+pointSet.add(point1);
+pointSet.add(point2);
+System.out.println(pointSet.size());  // Output: 2
+```
+This is because the HashSet uses the hashCode() method to determine where to store the object in its internal data structure and also uses it to compare objects for equality. If the hashCode() method is not overridden, the HashSet will use the default implementation which may not be appropriate for the Point class.</t>
+  </si>
+  <si>
+    <t>Here is an example of the problem with the Point class from Chapter 1 when using a HashSet:
+```
+import java.util.HashSet;
+public class Main {
+    public static void main(String[] args) {
+        HashSet&lt;Point&gt; points = new HashSet&lt;Point&gt;();
+        Point p1 = new Point(1, 2);
+        Point p2 = new Point(1, 2);
+        points.add(p1);
+        points.add(p2);
+        System.out.println(points.size()); // prints "2" instead of "1"
+    }
+}
+class Point {
+    int x;
+    int y;
+    Point(int x, int y) {
+        this.x = x;
+        this.y = y;
+    }
+    // equals() method is not overridden
+}
+```
+In this example, we create a HashSet of Point objects and add two Point objects, p1 and p2, that have the same x and y values. However, since the Point class does not override the equals() method, the HashSet considers these two Point objects to be distinct and adds both to the set. As a result, the size of the set is 2 instead of 1. 
+This problem could be avoided if the Point class overrides the equals() method and hashCode() method, so that two Point objects with the same x and y values are considered equal by the HashSet and only one is added to the set.</t>
+  </si>
+  <si>
     <t>Write down the mathematical relationship required between equals() and hashCode().</t>
   </si>
   <si>
@@ -4442,6 +5034,14 @@
 - It is not required that if two objects are unequal according to the `equals(Object)` method, then calling the `hashCode()` method on each of the two objects must produce distinct integer results. However, the programmer should be aware that producing distinct integer results for unequal objects may improve the performance of hash tables.
 In other words, if two objects are equal, they must have the same hash code. However, if two objects have different hash codes, they may still be equal. Therefore, it is important to make sure that the hash code is based on the same attributes used by the equals method.
 </t>
+  </si>
+  <si>
+    <t>When overriding the equals() method, it is generally recommended to also override the hashCode() method. This is because the hashCode() method is used by common Collection structures such as HashSet to determine if two objects are equal, and if the hashCode() method is not overridden, it may not return the correct value.
+The mathematical relationship required between equals() and hashCode() is that if two objects are equal according to the equals(Object) method, then calling the hashCode() method on each of the two objects must produce the same integer result. This means that if two objects are equal then their hashcode should be same.</t>
+  </si>
+  <si>
+    <t>(a) When overriding the equals() method, it is generally recommended to also override the hashCode() method. This is because the hashCode method is used by certain collection classes (such as HashSet and HashMap) to determine where to store an object, and if the hashCode method is not overridden, these classes may not be able to properly store instances of the class.
+(b) The mathematical relationship required between equals() and hashCode() is that if two objects are equal according to the equals(Object) method, then calling the hashCode method on each of the two objects must produce the same integer result. This means that if a.equals(b) returns true, then a.hashCode() == b.hashCode() must also be true. Additionally, it is required that if two objects are not equal according to the equals(Object) method, then calling the hashCode method on each of the two objects must produce distinct integer results, unless the two objects are null.</t>
   </si>
   <si>
     <t>Write a simple JUnit test to show that Point objects do not enjoy this property.</t>
@@ -4554,6 +5154,44 @@
 </t>
   </si>
   <si>
+    <t>```
+import static org.junit.Assert.*;
+import java.util.HashSet;
+import org.junit.Test;
+public class PointTest {
+    @Test
+    public void testEqualityInHashSet() {
+        Point p1 = new Point(1, 2);
+        Point p2 = new Point(1, 2);
+        HashSet&lt;Point&gt; set = new HashSet&lt;Point&gt;();
+        set.add(p1);
+        assertFalse(set.contains(p2));
+    }
+}
+```
+In this JUnit test, two Point objects `p1` and `p2` are created with the same x and y coordinates. These objects are added to a HashSet, and it is asserted that the HashSet does not contain the second Point object `p2`. This is because the `equals()` and `hashCode()` methods have not been overridden, so the HashSet uses the default implementation which only considers objects to be equal if they are the same instance.</t>
+  </si>
+  <si>
+    <t>Here is a simple JUnit test that demonstrates that Point objects do not have the property of being able to be stored in common Collection structures such as HashSet when the equals() method is overridden without also overriding the hashCode() method:
+```
+import static org.junit.Assert.*;
+import java.util.HashSet;
+import org.junit.Test;
+public class PointTest {
+    @Test
+    public void testHashCodeProperty() {
+        Point p1 = new Point(1, 2);
+        Point p2 = new Point(1, 2);
+        HashSet&lt;Point&gt; set = new HashSet&lt;Point&gt;();
+        set.add(p1);
+        // This should return false, since p1 and p2 are equal but have different hash codes
+        assertFalse(set.contains(p2));
+    }
+}
+```
+Note that this is just an example and you need to import the class point in your test class.</t>
+  </si>
+  <si>
     <t>Repair the Point class to fix the fault.</t>
   </si>
   <si>
@@ -4675,6 +5313,63 @@
 In this example, the Point class overrides the `hashCode()` method and uses the `Objects.hash()` method to generate a hash code based on the x and y values of the Point objects. The `Objects.hash()` method generates a hash code based on the values of all the parameters passed to it. This ensures that if two Point objects are equal, they will have the same hash code and can be stored in a Collection structure such as HashSet without any problem.
 Note that the use of the `Objects.hash()` method is available since Java 7. If you're using an older version of Java, you can implement your own hash function using a similar approach.
 </t>
+  </si>
+  <si>
+    <t>To repair the Point class and fix the fault, the programmer should override both the `equals()` and `hashCode()` methods. The `equals()` method should be used to determine if two Point objects are equal, and the `hashCode()` method should return a unique hash code for each Point object. 
+Here is an example of how to override the `equals()` and `hashCode()` methods in the Point class:
+```
+class Point {
+    private int x;
+    private int y;
+    public Point(int x, int y) {
+        this.x = x;
+        this.y = y;
+    }
+    @Override
+    public boolean equals(Object o) {
+        if (o == this) return true;
+        if (!(o instanceof Point)) return false;
+        Point p = (Point) o;
+        return p.x == x &amp;&amp; p.y == y;
+    }
+    @Override
+    public int hashCode() {
+        int result = 17;
+        result = 31 * result + x;
+        result = 31 * result + y;
+        return result;
+    }
+}
+```
+It is also important to keep in mind that if the equals method is changed, the hashCode method should also be updated accordingly.</t>
+  </si>
+  <si>
+    <t>Here's one way to repair the Point class to fix the fault:
+```
+public class Point {
+    private int x;
+    private int y;
+    public Point(int x, int y) {
+        this.x = x;
+        this.y = y;
+    }
+    @Override
+    public boolean equals(Object o) {
+        if (o == this) return true;
+        if (!(o instanceof Point)) return false;
+        Point p = (Point) o;
+        return p.x == x &amp;&amp; p.y == y;
+    }
+    @Override
+    public int hashCode() {
+        int result = 17;
+        result = 31 * result + x;
+        result = 31 * result + y;
+        return result;
+    }
+}
+```
+Note that in the above example, We are using the fields x and y to calculate the hashCode, this is because fields used in equals() method should also be used to calculate hashCode() method.</t>
   </si>
   <si>
     <t>Rewrite your JUnit test as an appropriate JUnit theory. Evaluate it with suitable DataPoints.</t>
@@ -4828,6 +5523,55 @@
 </t>
   </si>
   <si>
+    <t>To rewrite the JUnit test as a theory, the @Theory annotation should be used instead of the @Test annotation, and the test method should be parameterized with DataPoints.
+Here is an example of how the test for the Point class's equals() and hashCode() methods could be written as a theory:
+```
+import org.junit.experimental.theories.DataPoints;
+import org.junit.experimental.theories.Theories;
+import org.junit.experimental.theories.Theory;
+import org.junit.runner.RunWith;
+@RunWith(Theories.class)
+public class PointTest {
+    @DataPoints
+    public static Point[] dataPoints = { new Point(1, 2), new Point(3, 4), new Point(5, 6) };
+    @Theory
+    public void testEqualsAndHashCode(Point p1, Point p2) {
+        // Test that the equals() method is consistent
+        assertEquals(p1.equals(p2), p1.equals(p2));
+        assertEquals(p1.equals(p2), p2.equals(p1));
+        // Test that the hashCode() method is consistent with equals()
+        if (p1.equals(p2)) {
+            assertEquals(p1.hashCode(), p2.hashCode());
+        }
+    }
+}
+```
+In this example, the test method is parameterized with two Point objects, p1 and p2. The theory is that for any two Point objects, if they are equal according to the equals() method, then their hashCode() method should return the same value. The @DataPoints annotation is used to specify an array of Point objects to be used as the inputs for the theory.
+This test can be run by the JUnit test runner, and it will automatically generate test cases by selecting all possible combinations of the data points.</t>
+  </si>
+  <si>
+    <t>```java
+import org.junit.experimental.theories.DataPoints;
+import org.junit.experimental.theories.Theories;
+import org.junit.experimental.theories.Theory;
+import org.junit.runner.RunWith;
+@RunWith(Theories.class)
+public class PointTest {
+    @DataPoints
+    public static Point[] dataPoints = {new Point(1, 2), new Point(3, 4), new Point(5, 6)};
+    @Theory
+    public void testEquals(Point point1, Point point2) {
+        if (point1.equals(point2)) {
+            assertTrue(point1.hashCode() == point2.hashCode());
+        }
+    }
+}
+```
+This JUnit test uses the `@RunWith(Theories.class)` annotation to run the test as a theory, and the `@DataPoints` annotation to define the data points for the theory. In this case, the data points are instances of the `Point` class. The `testEquals` method is annotated with `@Theory`, which tells JUnit to run the method for each combination of data points.
+The method checks if the `equals()` method returns true for two `Point` instances, it also checks that the `hashCode()` method returns the same value for both instances.
+The test will be run for each possible pair of data points defined in the `dataPoints` array, 3*3 =9 times.</t>
+  </si>
+  <si>
     <t>Replace each occurrence of a set with a list in the JUnit theory removeThenAddDoesNotChangeSet. Is the resulting theory valid or invalid? How many of the tests that pass the precondition also pass the postcondition? Explain.</t>
   </si>
   <si>
@@ -4849,6 +5593,16 @@
     <t xml:space="preserve">It depends on the specific implementation of the theory and the methods being used. In general, replacing a set with a list in the theory would likely result in the theory being invalid, as the behavior of sets and lists are different in Java. Sets are designed to not allow duplicate elements, while lists can have duplicate elements. This would change the behavior of the methods being tested and could cause the theory to fail.
 As for the number of tests that pass the precondition and also pass the postcondition, it would depend on the specific implementation of the theory and the methods being used. Without more information, it is not possible to determine how many tests would pass both the precondition and postcondition.
 </t>
+  </si>
+  <si>
+    <t>It is not possible to determine if the resulting theory is valid or invalid without more information on the specific implementation of the JUnit theory "removeThenAddDoesNotChangeSet." 
+In order to determine if the tests pass the precondition and postcondition, one would need to see the specific test cases being run and the expected results.
+In general, replacing a set with a list in a JUnit theory could change the behavior of the tests, as sets and lists have different characteristics and methods. Sets do not allow duplicate elements and have no defined order, while lists do allow duplicate elements and have a defined order. This means that the tests would have to be re-written or adapted to account for these differences, and it's possible that the original tests would no longer pass the precondition or postcondition.</t>
+  </si>
+  <si>
+    <t>It is not possible for me to determine whether the resulting theory is valid or invalid without more information about the specific JUnit theory in question, as well as the specific set and list implementations being used.
+However, in general, replacing a set with a list in a JUnit theory could potentially make the theory invalid. This is because sets and lists have different characteristics and behaviors. Sets do not allow duplicate elements, while lists do. Sets are typically unordered, while lists have a specific order. Therefore, replacing a set with a list in a JUnit theory could change the behavior of the theory and the results of the tests.
+Without more information, I cannot determine how many of the tests that pass the precondition also pass the postcondition. The tests that pass the precondition may fail the postcondition and vice versa.</t>
   </si>
 </sst>
 </file>
@@ -4924,18 +5678,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5252,13 +6003,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="2" width="8.83203125" style="1"/>
+    <col min="3" max="3" width="33.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="41.5" style="1" customWidth="1"/>
+    <col min="7" max="9" width="8.83203125" style="1"/>
+    <col min="10" max="10" width="43.83203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="45.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="44.1640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="43.1640625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13" ht="68">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -5295,1367 +6061,1496 @@
       <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:12">
-      <c r="A2">
+    <row r="2" spans="1:13" ht="409.6">
+      <c r="A2" s="1">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
+      <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K2" t="s">
+      <c r="J2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L2" t="s">
+      <c r="K2" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="L2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:12">
-      <c r="A3">
+    <row r="3" spans="1:13" ht="409.6">
+      <c r="A3" s="1">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="409.6">
+      <c r="A4" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="409.6">
+      <c r="A5" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="409.6">
+      <c r="A6" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="409.6">
+      <c r="A7" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="409.6">
+      <c r="A8" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="C8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="409.6">
+      <c r="A9" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F3" t="s">
+      <c r="C9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" t="s">
-        <v>26</v>
+      <c r="E9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
-      <c r="A4">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="10" spans="1:13" ht="409.6">
+      <c r="A10" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="409.6">
+      <c r="A11" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="409.6">
+      <c r="A12" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="409.6">
+      <c r="A13" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="409.6">
+      <c r="A14" s="1">
+        <v>5.3</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="C14" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="409.6">
+      <c r="A15" s="1">
+        <v>5.3</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="409.6">
+      <c r="A16" s="1">
+        <v>5.3</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J4" t="s">
+      <c r="C16" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K4" t="s">
-        <v>32</v>
-      </c>
-      <c r="L4" t="s">
-        <v>33</v>
+      <c r="E16" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
-      <c r="A5">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="17" spans="1:13" ht="409.6">
+      <c r="A17" s="1">
+        <v>5.3</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="409.6">
+      <c r="A18" s="1">
+        <v>5.3</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="409.6">
+      <c r="A19" s="1">
+        <v>5.3</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="409.6">
+      <c r="A20" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="C20" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="409.6">
+      <c r="A21" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="409.6">
+      <c r="A22" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="409.6">
+      <c r="A23" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K5" t="s">
+      <c r="C23" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L5" t="s">
-        <v>40</v>
+      <c r="E23" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
-      <c r="A6">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" t="s">
+    <row r="24" spans="1:13" ht="409.6">
+      <c r="A24" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="409.6">
+      <c r="A25" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="409.6">
+      <c r="A26" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" t="s">
-        <v>44</v>
-      </c>
-      <c r="J6" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="C26" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="409.6">
+      <c r="A27" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="409.6">
+      <c r="A28" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="409.6">
+      <c r="A29" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="409.6">
+      <c r="A30" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L6" t="s">
-        <v>47</v>
+      <c r="C30" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>213</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
-      <c r="A7">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" t="s">
+    <row r="31" spans="1:13" ht="409.6">
+      <c r="A31" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="409.6">
+      <c r="A32" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" t="s">
-        <v>51</v>
-      </c>
-      <c r="J7" t="s">
-        <v>52</v>
-      </c>
-      <c r="K7" t="s">
-        <v>53</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="C32" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="409.6">
+      <c r="A33" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="409.6">
+      <c r="A34" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="409.6">
+      <c r="A35" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="409.6">
+      <c r="A36" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="409.6">
+      <c r="A37" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="C37" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>260</v>
+      </c>
     </row>
-    <row r="8" spans="1:12">
-      <c r="A8">
-        <v>5.2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" t="s">
-        <v>57</v>
-      </c>
-      <c r="G8" t="s">
-        <v>58</v>
-      </c>
-      <c r="H8" t="s">
-        <v>59</v>
-      </c>
-      <c r="J8" t="s">
-        <v>60</v>
-      </c>
-      <c r="K8" t="s">
-        <v>61</v>
-      </c>
-      <c r="L8" t="s">
-        <v>62</v>
+    <row r="38" spans="1:13" ht="409.6">
+      <c r="A38" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>268</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
-      <c r="A9">
-        <v>5.2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" t="s">
-        <v>63</v>
-      </c>
-      <c r="F9" t="s">
-        <v>64</v>
-      </c>
-      <c r="G9" t="s">
-        <v>58</v>
-      </c>
-      <c r="H9" t="s">
-        <v>59</v>
-      </c>
-      <c r="J9" t="s">
+    <row r="39" spans="1:13" ht="409.6">
+      <c r="A39" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="409.6">
+      <c r="A40" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="K9" t="s">
+      <c r="H40" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="L9" t="s">
-        <v>67</v>
+      <c r="J40" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>280</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
-      <c r="A10">
-        <v>5.2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" t="s">
-        <v>68</v>
-      </c>
-      <c r="F10" t="s">
-        <v>69</v>
-      </c>
-      <c r="G10" t="s">
-        <v>58</v>
-      </c>
-      <c r="H10" t="s">
-        <v>59</v>
-      </c>
-      <c r="J10" t="s">
-        <v>70</v>
-      </c>
-      <c r="K10" t="s">
-        <v>71</v>
-      </c>
-      <c r="L10" t="s">
-        <v>72</v>
+    <row r="41" spans="1:13" ht="409.6">
+      <c r="A41" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>286</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
-      <c r="A11">
-        <v>5.2</v>
-      </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" t="s">
-        <v>73</v>
-      </c>
-      <c r="F11" t="s">
-        <v>74</v>
-      </c>
-      <c r="G11" t="s">
-        <v>58</v>
-      </c>
-      <c r="H11" t="s">
-        <v>59</v>
-      </c>
-      <c r="J11" t="s">
-        <v>75</v>
-      </c>
-      <c r="K11" t="s">
-        <v>76</v>
-      </c>
-      <c r="L11" t="s">
-        <v>77</v>
+    <row r="42" spans="1:13" ht="409.6">
+      <c r="A42" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
-      <c r="A12">
-        <v>5.2</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" t="s">
-        <v>78</v>
-      </c>
-      <c r="F12" t="s">
-        <v>79</v>
-      </c>
-      <c r="G12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12" t="s">
-        <v>59</v>
-      </c>
-      <c r="J12" t="s">
-        <v>80</v>
-      </c>
-      <c r="K12" t="s">
-        <v>81</v>
-      </c>
-      <c r="L12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13">
-        <v>5.2</v>
-      </c>
-      <c r="B13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" t="s">
-        <v>83</v>
-      </c>
-      <c r="F13" t="s">
-        <v>84</v>
-      </c>
-      <c r="G13" t="s">
-        <v>58</v>
-      </c>
-      <c r="H13" t="s">
-        <v>59</v>
-      </c>
-      <c r="J13" t="s">
-        <v>85</v>
-      </c>
-      <c r="K13" t="s">
-        <v>86</v>
-      </c>
-      <c r="L13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14">
-        <v>5.3</v>
-      </c>
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" t="s">
-        <v>88</v>
-      </c>
-      <c r="D14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" t="s">
-        <v>89</v>
-      </c>
-      <c r="F14" t="s">
-        <v>90</v>
-      </c>
-      <c r="J14" t="s">
-        <v>91</v>
-      </c>
-      <c r="K14" t="s">
-        <v>92</v>
-      </c>
-      <c r="L14" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15">
-        <v>5.3</v>
-      </c>
-      <c r="B15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" t="s">
-        <v>88</v>
-      </c>
-      <c r="D15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" t="s">
-        <v>94</v>
-      </c>
-      <c r="F15" t="s">
-        <v>95</v>
-      </c>
-      <c r="J15" t="s">
-        <v>96</v>
-      </c>
-      <c r="K15" t="s">
-        <v>97</v>
-      </c>
-      <c r="L15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16">
-        <v>5.3</v>
-      </c>
-      <c r="B16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" t="s">
-        <v>99</v>
-      </c>
-      <c r="F16" t="s">
-        <v>100</v>
-      </c>
-      <c r="J16" t="s">
-        <v>101</v>
-      </c>
-      <c r="K16" t="s">
-        <v>102</v>
-      </c>
-      <c r="L16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17">
-        <v>5.3</v>
-      </c>
-      <c r="B17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" t="s">
-        <v>88</v>
-      </c>
-      <c r="D17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" t="s">
-        <v>104</v>
-      </c>
-      <c r="F17" t="s">
-        <v>105</v>
-      </c>
-      <c r="J17" t="s">
-        <v>106</v>
-      </c>
-      <c r="K17" t="s">
-        <v>107</v>
-      </c>
-      <c r="L17" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="A18">
-        <v>5.3</v>
-      </c>
-      <c r="B18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" t="s">
-        <v>88</v>
-      </c>
-      <c r="D18" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" t="s">
-        <v>109</v>
-      </c>
-      <c r="F18" t="s">
-        <v>110</v>
-      </c>
-      <c r="J18" t="s">
-        <v>111</v>
-      </c>
-      <c r="K18" t="s">
-        <v>112</v>
-      </c>
-      <c r="L18" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="A19">
-        <v>5.3</v>
-      </c>
-      <c r="B19" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" t="s">
-        <v>88</v>
-      </c>
-      <c r="D19" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" t="s">
-        <v>114</v>
-      </c>
-      <c r="F19" t="s">
-        <v>115</v>
-      </c>
-      <c r="J19" t="s">
-        <v>116</v>
-      </c>
-      <c r="K19" t="s">
-        <v>117</v>
-      </c>
-      <c r="L19" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="A20">
-        <v>5.4</v>
-      </c>
-      <c r="B20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" t="s">
-        <v>119</v>
-      </c>
-      <c r="D20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" t="s">
-        <v>120</v>
-      </c>
-      <c r="F20" t="s">
-        <v>121</v>
-      </c>
-      <c r="G20" t="s">
-        <v>122</v>
-      </c>
-      <c r="H20" t="s">
-        <v>123</v>
-      </c>
-      <c r="J20" t="s">
-        <v>124</v>
-      </c>
-      <c r="K20" t="s">
-        <v>125</v>
-      </c>
-      <c r="L20" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="A21">
-        <v>5.4</v>
-      </c>
-      <c r="B21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" t="s">
-        <v>119</v>
-      </c>
-      <c r="D21" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" t="s">
-        <v>127</v>
-      </c>
-      <c r="F21" t="s">
-        <v>128</v>
-      </c>
-      <c r="G21" t="s">
-        <v>58</v>
-      </c>
-      <c r="H21" t="s">
-        <v>59</v>
-      </c>
-      <c r="J21" t="s">
-        <v>129</v>
-      </c>
-      <c r="K21" t="s">
-        <v>130</v>
-      </c>
-      <c r="L21" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="A22">
-        <v>5.4</v>
-      </c>
-      <c r="B22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" t="s">
-        <v>119</v>
-      </c>
-      <c r="D22" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" t="s">
-        <v>132</v>
-      </c>
-      <c r="F22" t="s">
-        <v>133</v>
-      </c>
-      <c r="G22" t="s">
-        <v>58</v>
-      </c>
-      <c r="H22" t="s">
-        <v>59</v>
-      </c>
-      <c r="J22" t="s">
-        <v>134</v>
-      </c>
-      <c r="K22" t="s">
-        <v>135</v>
-      </c>
-      <c r="L22" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23">
-        <v>5.4</v>
-      </c>
-      <c r="B23" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" t="s">
-        <v>119</v>
-      </c>
-      <c r="D23" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" t="s">
-        <v>137</v>
-      </c>
-      <c r="F23" t="s">
-        <v>138</v>
-      </c>
-      <c r="G23" t="s">
-        <v>58</v>
-      </c>
-      <c r="H23" t="s">
-        <v>139</v>
-      </c>
-      <c r="J23" t="s">
-        <v>140</v>
-      </c>
-      <c r="K23" t="s">
-        <v>141</v>
-      </c>
-      <c r="L23" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="A24">
-        <v>5.4</v>
-      </c>
-      <c r="B24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" t="s">
-        <v>119</v>
-      </c>
-      <c r="D24" t="s">
-        <v>42</v>
-      </c>
-      <c r="E24" t="s">
-        <v>143</v>
-      </c>
-      <c r="F24" t="s">
-        <v>144</v>
-      </c>
-      <c r="G24" t="s">
-        <v>58</v>
-      </c>
-      <c r="H24" t="s">
-        <v>59</v>
-      </c>
-      <c r="J24" t="s">
-        <v>145</v>
-      </c>
-      <c r="K24" t="s">
-        <v>146</v>
-      </c>
-      <c r="L24" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25">
-        <v>5.4</v>
-      </c>
-      <c r="B25" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" t="s">
-        <v>119</v>
-      </c>
-      <c r="D25" t="s">
-        <v>49</v>
-      </c>
-      <c r="E25" t="s">
-        <v>148</v>
-      </c>
-      <c r="F25" t="s">
-        <v>149</v>
-      </c>
-      <c r="G25" t="s">
-        <v>58</v>
-      </c>
-      <c r="H25" t="s">
-        <v>59</v>
-      </c>
-      <c r="J25" t="s">
-        <v>150</v>
-      </c>
-      <c r="K25" t="s">
-        <v>151</v>
-      </c>
-      <c r="L25" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26">
-        <v>7.1</v>
-      </c>
-      <c r="B26" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" t="s">
-        <v>153</v>
-      </c>
-      <c r="D26" t="s">
-        <v>154</v>
-      </c>
-      <c r="E26" t="s">
-        <v>155</v>
-      </c>
-      <c r="F26" t="s">
-        <v>156</v>
-      </c>
-      <c r="J26" t="s">
-        <v>157</v>
-      </c>
-      <c r="K26" t="s">
-        <v>158</v>
-      </c>
-      <c r="L26" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27">
-        <v>7.1</v>
-      </c>
-      <c r="B27" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" t="s">
-        <v>153</v>
-      </c>
-      <c r="D27" t="s">
-        <v>160</v>
-      </c>
-      <c r="E27" t="s">
-        <v>161</v>
-      </c>
-      <c r="F27" t="s">
-        <v>162</v>
-      </c>
-      <c r="J27" t="s">
-        <v>163</v>
-      </c>
-      <c r="K27" t="s">
-        <v>164</v>
-      </c>
-      <c r="L27" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28">
-        <v>7.1</v>
-      </c>
-      <c r="B28" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" t="s">
-        <v>153</v>
-      </c>
-      <c r="D28" t="s">
-        <v>166</v>
-      </c>
-      <c r="E28" t="s">
-        <v>167</v>
-      </c>
-      <c r="F28" t="s">
-        <v>168</v>
-      </c>
-      <c r="J28" t="s">
-        <v>169</v>
-      </c>
-      <c r="K28" t="s">
-        <v>170</v>
-      </c>
-      <c r="L28" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29">
-        <v>7.1</v>
-      </c>
-      <c r="B29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" t="s">
-        <v>153</v>
-      </c>
-      <c r="D29" t="s">
-        <v>172</v>
-      </c>
-      <c r="E29" t="s">
-        <v>173</v>
-      </c>
-      <c r="F29" t="s">
-        <v>174</v>
-      </c>
-      <c r="J29" t="s">
-        <v>175</v>
-      </c>
-      <c r="K29" t="s">
-        <v>176</v>
-      </c>
-      <c r="L29" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="A30">
-        <v>7.1</v>
-      </c>
-      <c r="B30" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" t="s">
-        <v>153</v>
-      </c>
-      <c r="D30" t="s">
-        <v>178</v>
-      </c>
-      <c r="E30" t="s">
-        <v>179</v>
-      </c>
-      <c r="F30" t="s">
-        <v>180</v>
-      </c>
-      <c r="J30" t="s">
-        <v>181</v>
-      </c>
-      <c r="K30" t="s">
-        <v>182</v>
-      </c>
-      <c r="L30" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="A31">
-        <v>7.1</v>
-      </c>
-      <c r="B31" t="s">
-        <v>48</v>
-      </c>
-      <c r="C31" t="s">
-        <v>153</v>
-      </c>
-      <c r="D31" t="s">
-        <v>184</v>
-      </c>
-      <c r="E31" t="s">
-        <v>185</v>
-      </c>
-      <c r="F31" t="s">
-        <v>186</v>
-      </c>
-      <c r="J31" t="s">
-        <v>187</v>
-      </c>
-      <c r="K31" t="s">
-        <v>188</v>
-      </c>
-      <c r="L31" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12">
-      <c r="A32">
-        <v>7.2</v>
-      </c>
-      <c r="B32" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" t="s">
-        <v>190</v>
-      </c>
-      <c r="D32" t="s">
-        <v>14</v>
-      </c>
-      <c r="E32" t="s">
-        <v>191</v>
-      </c>
-      <c r="F32" t="s">
-        <v>192</v>
-      </c>
-      <c r="G32" t="s">
-        <v>193</v>
-      </c>
-      <c r="H32" t="s">
-        <v>139</v>
-      </c>
-      <c r="J32" t="s">
-        <v>194</v>
-      </c>
-      <c r="K32" t="s">
-        <v>195</v>
-      </c>
-      <c r="L32" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12">
-      <c r="A33">
-        <v>7.2</v>
-      </c>
-      <c r="B33" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" t="s">
-        <v>190</v>
-      </c>
-      <c r="D33" t="s">
-        <v>21</v>
-      </c>
-      <c r="E33" t="s">
-        <v>197</v>
-      </c>
-      <c r="F33" t="s">
-        <v>198</v>
-      </c>
-      <c r="G33" t="s">
-        <v>193</v>
-      </c>
-      <c r="H33" t="s">
-        <v>139</v>
-      </c>
-      <c r="J33" t="s">
-        <v>199</v>
-      </c>
-      <c r="K33" t="s">
-        <v>200</v>
-      </c>
-      <c r="L33" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12">
-      <c r="A34">
-        <v>7.2</v>
-      </c>
-      <c r="B34" t="s">
-        <v>27</v>
-      </c>
-      <c r="C34" t="s">
-        <v>190</v>
-      </c>
-      <c r="D34" t="s">
-        <v>166</v>
-      </c>
-      <c r="E34" t="s">
-        <v>202</v>
-      </c>
-      <c r="F34" t="s">
-        <v>203</v>
-      </c>
-      <c r="G34" t="s">
-        <v>58</v>
-      </c>
-      <c r="H34" t="s">
-        <v>59</v>
-      </c>
-      <c r="J34" t="s">
-        <v>204</v>
-      </c>
-      <c r="K34" t="s">
-        <v>205</v>
-      </c>
-      <c r="L34" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12">
-      <c r="A35">
-        <v>7.2</v>
-      </c>
-      <c r="B35" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" t="s">
-        <v>190</v>
-      </c>
-      <c r="D35" t="s">
-        <v>207</v>
-      </c>
-      <c r="E35" t="s">
-        <v>208</v>
-      </c>
-      <c r="F35" t="s">
-        <v>209</v>
-      </c>
-      <c r="G35" t="s">
-        <v>58</v>
-      </c>
-      <c r="H35" t="s">
-        <v>210</v>
-      </c>
-      <c r="J35" t="s">
-        <v>211</v>
-      </c>
-      <c r="K35" t="s">
-        <v>212</v>
-      </c>
-      <c r="L35" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12">
-      <c r="A36">
-        <v>7.2</v>
-      </c>
-      <c r="B36" t="s">
-        <v>41</v>
-      </c>
-      <c r="C36" t="s">
-        <v>190</v>
-      </c>
-      <c r="D36" t="s">
-        <v>178</v>
-      </c>
-      <c r="E36" t="s">
+    <row r="43" spans="1:13" ht="409.6">
+      <c r="A43" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="F36" t="s">
-        <v>215</v>
-      </c>
-      <c r="G36" t="s">
-        <v>58</v>
-      </c>
-      <c r="H36" t="s">
-        <v>59</v>
-      </c>
-      <c r="J36" t="s">
-        <v>216</v>
-      </c>
-      <c r="K36" t="s">
-        <v>217</v>
-      </c>
-      <c r="L36" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12">
-      <c r="A37">
-        <v>7.2</v>
-      </c>
-      <c r="B37" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37" t="s">
-        <v>190</v>
-      </c>
-      <c r="D37" t="s">
-        <v>184</v>
-      </c>
-      <c r="E37" t="s">
-        <v>219</v>
-      </c>
-      <c r="F37" t="s">
-        <v>220</v>
-      </c>
-      <c r="G37" t="s">
-        <v>193</v>
-      </c>
-      <c r="H37" t="s">
-        <v>139</v>
-      </c>
-      <c r="J37" t="s">
-        <v>221</v>
-      </c>
-      <c r="K37" t="s">
-        <v>222</v>
-      </c>
-      <c r="L37" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12">
-      <c r="A38">
-        <v>7.3</v>
-      </c>
-      <c r="B38" t="s">
-        <v>12</v>
-      </c>
-      <c r="C38" t="s">
-        <v>224</v>
-      </c>
-      <c r="D38" t="s">
-        <v>225</v>
-      </c>
-      <c r="E38" t="s">
-        <v>226</v>
-      </c>
-      <c r="F38" t="s">
-        <v>227</v>
-      </c>
-      <c r="G38" t="s">
-        <v>122</v>
-      </c>
-      <c r="H38" t="s">
-        <v>123</v>
-      </c>
-      <c r="J38" t="s">
-        <v>228</v>
-      </c>
-      <c r="K38" t="s">
-        <v>229</v>
-      </c>
-      <c r="L38" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12">
-      <c r="A39">
-        <v>7.3</v>
-      </c>
-      <c r="B39" t="s">
-        <v>20</v>
-      </c>
-      <c r="C39" t="s">
-        <v>224</v>
-      </c>
-      <c r="D39" t="s">
-        <v>160</v>
-      </c>
-      <c r="E39" t="s">
-        <v>231</v>
-      </c>
-      <c r="F39" t="s">
-        <v>232</v>
-      </c>
-      <c r="G39" t="s">
-        <v>193</v>
-      </c>
-      <c r="H39" t="s">
-        <v>139</v>
-      </c>
-      <c r="J39" t="s">
-        <v>233</v>
-      </c>
-      <c r="K39" t="s">
-        <v>234</v>
-      </c>
-      <c r="L39" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12">
-      <c r="A40">
-        <v>7.3</v>
-      </c>
-      <c r="B40" t="s">
-        <v>27</v>
-      </c>
-      <c r="C40" t="s">
-        <v>224</v>
-      </c>
-      <c r="D40" t="s">
-        <v>166</v>
-      </c>
-      <c r="E40" t="s">
-        <v>236</v>
-      </c>
-      <c r="F40" t="s">
-        <v>237</v>
-      </c>
-      <c r="G40" t="s">
-        <v>58</v>
-      </c>
-      <c r="H40" t="s">
-        <v>59</v>
-      </c>
-      <c r="J40" t="s">
-        <v>238</v>
-      </c>
-      <c r="K40" t="s">
-        <v>239</v>
-      </c>
-      <c r="L40" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12">
-      <c r="A41">
-        <v>7.3</v>
-      </c>
-      <c r="B41" t="s">
-        <v>34</v>
-      </c>
-      <c r="C41" t="s">
-        <v>224</v>
-      </c>
-      <c r="D41" t="s">
-        <v>172</v>
-      </c>
-      <c r="E41" t="s">
-        <v>241</v>
-      </c>
-      <c r="F41" t="s">
-        <v>242</v>
-      </c>
-      <c r="G41" t="s">
-        <v>193</v>
-      </c>
-      <c r="H41" t="s">
-        <v>139</v>
-      </c>
-      <c r="J41" t="s">
-        <v>243</v>
-      </c>
-      <c r="K41" t="s">
-        <v>244</v>
-      </c>
-      <c r="L41" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12">
-      <c r="A42">
-        <v>7.3</v>
-      </c>
-      <c r="B42" t="s">
-        <v>41</v>
-      </c>
-      <c r="C42" t="s">
-        <v>224</v>
-      </c>
-      <c r="D42" t="s">
-        <v>246</v>
-      </c>
-      <c r="E42" t="s">
-        <v>247</v>
-      </c>
-      <c r="F42" t="s">
-        <v>248</v>
-      </c>
-      <c r="G42" t="s">
-        <v>58</v>
-      </c>
-      <c r="H42" t="s">
-        <v>59</v>
-      </c>
-      <c r="J42" t="s">
-        <v>249</v>
-      </c>
-      <c r="K42" t="s">
-        <v>250</v>
-      </c>
-      <c r="L42" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12">
-      <c r="A43">
-        <v>7.3</v>
-      </c>
-      <c r="B43" t="s">
-        <v>48</v>
-      </c>
-      <c r="C43" t="s">
-        <v>224</v>
-      </c>
-      <c r="D43" t="s">
-        <v>184</v>
-      </c>
-      <c r="E43" t="s">
-        <v>252</v>
-      </c>
-      <c r="F43" t="s">
-        <v>253</v>
-      </c>
-      <c r="G43" t="s">
-        <v>58</v>
-      </c>
-      <c r="H43" t="s">
-        <v>59</v>
-      </c>
-      <c r="J43" t="s">
-        <v>254</v>
-      </c>
-      <c r="K43" t="s">
-        <v>255</v>
-      </c>
-      <c r="L43" t="s">
-        <v>256</v>
+      <c r="E43" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -6665,77 +7560,98 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="2" width="8.83203125" style="1"/>
+    <col min="3" max="3" width="9.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27" style="1" customWidth="1"/>
+    <col min="6" max="6" width="33.6640625" style="1" customWidth="1"/>
+    <col min="7" max="9" width="8.83203125" style="1"/>
+    <col min="10" max="10" width="28" style="1" customWidth="1"/>
+    <col min="11" max="11" width="28.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="29.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="34.83203125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:13" ht="68">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:12">
-      <c r="A2">
+    <row r="2" spans="1:13" ht="409.6">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>257</v>
-      </c>
-      <c r="E2" t="s">
-        <v>258</v>
-      </c>
-      <c r="F2" t="s">
-        <v>259</v>
-      </c>
-      <c r="G2" t="s">
-        <v>193</v>
-      </c>
-      <c r="H2" t="s">
-        <v>139</v>
-      </c>
-      <c r="J2" t="s">
-        <v>260</v>
-      </c>
-      <c r="K2" t="s">
-        <v>261</v>
-      </c>
-      <c r="L2" t="s">
-        <v>262</v>
+      <c r="D2" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -6745,471 +7661,550 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="2" width="8.83203125" style="1"/>
+    <col min="3" max="3" width="21" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.33203125" style="1" customWidth="1"/>
+    <col min="7" max="9" width="8.83203125" style="1"/>
+    <col min="10" max="10" width="27.83203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="27.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="29.5" style="1" customWidth="1"/>
+    <col min="13" max="13" width="31.5" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="68">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:13" ht="68">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" ht="409.6">
+    <row r="2" spans="1:13" ht="409.6">
       <c r="A2" s="1">
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>263</v>
+        <v>307</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>264</v>
+        <v>308</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>265</v>
+        <v>309</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>266</v>
+        <v>310</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>267</v>
+        <v>311</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>268</v>
+        <v>312</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>269</v>
+        <v>313</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>314</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="409.6">
+    <row r="3" spans="1:13" ht="409.6">
       <c r="A3" s="1">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>270</v>
+        <v>315</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>271</v>
+        <v>316</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>272</v>
+        <v>317</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>273</v>
+        <v>318</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>193</v>
+        <v>224</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>274</v>
+        <v>319</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>275</v>
+        <v>320</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>276</v>
+        <v>321</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>277</v>
+        <v>322</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>323</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="409.6">
+    <row r="4" spans="1:13" ht="409.6">
       <c r="A4" s="1">
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>278</v>
+        <v>324</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>279</v>
+        <v>325</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>280</v>
+        <v>326</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>281</v>
+        <v>327</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>193</v>
+        <v>224</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>282</v>
+        <v>328</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>283</v>
+        <v>329</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>284</v>
+        <v>330</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>331</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="409.6">
+    <row r="5" spans="1:13" ht="409.6">
       <c r="A5" s="1">
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>285</v>
+        <v>332</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>286</v>
+        <v>333</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>287</v>
+        <v>334</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>288</v>
+        <v>335</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>289</v>
+        <v>336</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>290</v>
+        <v>337</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>291</v>
+        <v>338</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>339</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="409.6">
+    <row r="6" spans="1:13" ht="409.6">
       <c r="A6" s="1">
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>285</v>
+        <v>332</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>292</v>
+        <v>340</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>293</v>
+        <v>341</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>294</v>
+        <v>342</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>295</v>
+        <v>343</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>296</v>
+        <v>344</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>297</v>
+        <v>345</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>346</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="409.6">
+    <row r="7" spans="1:13" ht="409.6">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>285</v>
+        <v>332</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>298</v>
+        <v>347</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>299</v>
+        <v>348</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>300</v>
+        <v>349</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>301</v>
+        <v>350</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>302</v>
+        <v>351</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>303</v>
+        <v>352</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>353</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="409.6">
+    <row r="8" spans="1:13" ht="409.6">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>285</v>
+        <v>332</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>304</v>
+        <v>354</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>305</v>
+        <v>355</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>306</v>
+        <v>356</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>307</v>
+        <v>357</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>308</v>
+        <v>358</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>360</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="409.6">
+    <row r="9" spans="1:13" ht="409.6">
       <c r="A9" s="1">
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>285</v>
+        <v>332</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>309</v>
+        <v>361</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>310</v>
+        <v>362</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>311</v>
+        <v>363</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>312</v>
+        <v>364</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>313</v>
+        <v>365</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>367</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="409.6">
+    <row r="10" spans="1:13" ht="409.6">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>314</v>
+        <v>368</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>315</v>
+        <v>369</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>316</v>
+        <v>370</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>317</v>
+        <v>371</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>193</v>
+        <v>224</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>318</v>
+        <v>372</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>319</v>
+        <v>373</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>375</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="409.6">
+    <row r="11" spans="1:13" ht="409.6">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>314</v>
+        <v>368</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>320</v>
+        <v>376</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>321</v>
+        <v>377</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>322</v>
+        <v>378</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>193</v>
+        <v>224</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>323</v>
+        <v>379</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>324</v>
+        <v>380</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>382</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="409.6">
+    <row r="12" spans="1:13" ht="409.6">
       <c r="A12" s="1">
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>314</v>
+        <v>368</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>325</v>
+        <v>383</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>326</v>
+        <v>384</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>327</v>
+        <v>385</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>193</v>
+        <v>224</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>328</v>
+        <v>386</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>329</v>
+        <v>387</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>389</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="409.6">
+    <row r="13" spans="1:13" ht="409.6">
       <c r="A13" s="1">
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>314</v>
+        <v>368</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>330</v>
+        <v>390</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>331</v>
+        <v>391</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>332</v>
+        <v>392</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>193</v>
+        <v>224</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>333</v>
+        <v>393</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>334</v>
+        <v>394</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>396</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="409.6">
+    <row r="14" spans="1:13" ht="409.6">
       <c r="A14" s="1">
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>314</v>
+        <v>368</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>335</v>
+        <v>397</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>336</v>
+        <v>398</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>337</v>
+        <v>399</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>122</v>
+        <v>141</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>123</v>
+        <v>142</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>338</v>
+        <v>400</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>339</v>
+        <v>401</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>403</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="409.6">
+    <row r="15" spans="1:13" ht="409.6">
       <c r="A15" s="1">
         <v>10</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>340</v>
+        <v>404</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>341</v>
+        <v>405</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>342</v>
+        <v>406</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>122</v>
+        <v>141</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>123</v>
+        <v>142</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>343</v>
+        <v>407</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>344</v>
+        <v>408</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>410</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Chapter 1 & 2 feedback completed
</commit_message>
<xml_diff>
--- a/dataset/testing.xlsx
+++ b/dataset/testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajed/PycharmProjects/Study-on-ChatGPT/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3A0E4A-683D-5346-AE79-023829542514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF0FDD7-B4F7-2244-9C35-3D216437411A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="17300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ch1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="434">
   <si>
     <t>id</t>
   </si>
@@ -1140,28 +1140,6 @@
 Will now produce the expected output of 2, as the method will start from the end of the array and return the first zero it encounters which is the last zero in the array.
 Also, I have added a check for the null input arrays so that it returns -1 if array is null.
 It's worth mentioning that this is a simulation and I don't have access to any system to run this code and show the output, however, you can run this code on your local machine and check the output.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-As I am a text-based AI model I can't provide a screen printout or other evidence that my new program works. However, I can provide the modified code to fix the error:
-```java
-public static int lastZero (int[] x) {
-    if (x == null) {
-        throw new NullPointerException("Input array is null");
-    }
-    int lastZeroIndex = -1;
-    for (int i = 0; i &lt; x.length; i++) {
-        if (x[i] == 0) {
-            lastZeroIndex = i;
-        }
-    }
-    return lastZeroIndex;
-}
-```
-In this new version of the code, I've added a null check at the beginning of the function to check if the input array is null. If it is, it throws a `NullPointerException` with an appropriate error message.
-This modification will handle the case where the input array is null, and it will prevent the program from throwing a `NullPointerException` and also it will give a proper error message to handle it.
-This modification will work on all test cases including the one where the input array is null and will give the expected output.
 </t>
   </si>
   <si>
@@ -5604,12 +5582,103 @@
 However, in general, replacing a set with a list in a JUnit theory could potentially make the theory invalid. This is because sets and lists have different characteristics and behaviors. Sets do not allow duplicate elements, while lists do. Sets are typically unordered, while lists have a specific order. Therefore, replacing a set with a list in a JUnit theory could change the behavior of the theory and the results of the tests.
 Without more information, I cannot determine how many of the tests that pass the precondition also pass the postcondition. The tests that pass the precondition may fail the postcondition and vice versa.</t>
   </si>
+  <si>
+    <t>EPC</t>
+  </si>
+  <si>
+    <t>APC</t>
+  </si>
+  <si>
+    <t>Provies wrong idea about null checks</t>
+  </si>
+  <si>
+    <t>Misses the NPE case</t>
+  </si>
+  <si>
+    <t>Treats execution as failure</t>
+  </si>
+  <si>
+    <t>Could not find the case where every element occurs once</t>
+  </si>
+  <si>
+    <t>Did not talk about the initialization</t>
+  </si>
+  <si>
+    <t>Although correct, It did not executed the commented test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+As I am a text-based AI model I can't provide a screen printout or other evidence that my new program works. However, I can provide the modified code to fix the error:
+```
+public static int lastZero (int[] x) {
+    if (x == null) {
+        throw new NullPointerException("Input array is null");
+    }
+    int lastZeroIndex = -1;
+    for (int i = 0; i &lt; x.length; i++) {
+        if (x[i] == 0) {
+            lastZeroIndex = i;
+        }
+    }
+    return lastZeroIndex;
+}
+```
+In this new version of the code, I've added a null check at the beginning of the function to check if the input array is null. If it is, it throws a `NullPointerException` with an appropriate error message.
+This modification will handle the case where the input array is null, and it will prevent the program from throwing a `NullPointerException` and also it will give a proper error message to handle it.
+This modification will work on all test cases including the one where the input array is null and will give the expected output.
+</t>
+  </si>
+  <si>
+    <t>Finds the correct issue but fails to give a fix for the code</t>
+  </si>
+  <si>
+    <t>Talks about the empty cases but misses the null case</t>
+  </si>
+  <si>
+    <t>Did not talk about the commented test case</t>
+  </si>
+  <si>
+    <t>Finds a solution that the writer did not talk about</t>
+  </si>
+  <si>
+    <t>Treats error equavalent to exception</t>
+  </si>
+  <si>
+    <t>Explanation correct from the prespective that assumption about equality is not corrent to the tester</t>
+  </si>
+  <si>
+    <t>Wrong assumption by chatGPT</t>
+  </si>
+  <si>
+    <t>Writer differs in the sense that it is a part of JAVA API and cannot be modified without consequences in the client code all over the world. But chatGPT provides a fix that would be the soultion if it was written properly.</t>
+  </si>
+  <si>
+    <t>Talks about hashcode which the author missed</t>
+  </si>
+  <si>
+    <t>There will be no valid code solution</t>
+  </si>
+  <si>
+    <t>Talks about the problem in both equals()</t>
+  </si>
+  <si>
+    <t>Exception is treated as error</t>
+  </si>
+  <si>
+    <t>Also talks about design perspective</t>
+  </si>
+  <si>
+    <t>Just need to remove extends Point. Otherwise correctly provides solution in terms of composition</t>
+  </si>
+  <si>
+    <t>Talks about composition indirectly</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5627,13 +5696,32 @@
       <sz val="12"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -5678,7 +5766,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -5688,6 +5776,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6003,28 +6100,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M43"/>
+  <dimension ref="A1:AE43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="2" width="8.83203125" style="1"/>
-    <col min="3" max="3" width="33.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="33.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="41.5" style="1" customWidth="1"/>
-    <col min="7" max="9" width="8.83203125" style="1"/>
-    <col min="10" max="10" width="43.83203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="45.83203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="44.1640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="43.1640625" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.83203125" style="1"/>
+    <col min="3" max="3" width="45.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="46.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="57.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" style="1" customWidth="1"/>
+    <col min="9" max="11" width="8.83203125" style="1"/>
+    <col min="12" max="12" width="60.1640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.1640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.83203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="63.5" style="1" customWidth="1"/>
+    <col min="17" max="17" width="14.1640625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.33203125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="15.1640625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="65.1640625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="14.1640625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="12.33203125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="12.83203125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="71.33203125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="14.1640625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="12.33203125" style="1" customWidth="1"/>
+    <col min="27" max="27" width="12.83203125" style="1" customWidth="1"/>
+    <col min="28" max="28" width="78.83203125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="14.1640625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="12.33203125" style="1" customWidth="1"/>
+    <col min="31" max="31" width="12.83203125" style="1" customWidth="1"/>
+    <col min="32" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="68">
+    <row r="1" spans="1:31" ht="68">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -6040,32 +6155,86 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="M1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="N1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="O1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="Q1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="U1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="X1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="Y1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB1" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="AC1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE1" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" ht="409.6">
+    <row r="2" spans="1:31" ht="409.6">
       <c r="A2" s="1">
         <v>5.0999999999999996</v>
       </c>
@@ -6082,22 +6251,61 @@
         <v>16</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="M2" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="U2" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="X2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB2" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="AC2" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" ht="409.6">
+    <row r="3" spans="1:31" ht="409.6">
       <c r="A3" s="1">
         <v>5.0999999999999996</v>
       </c>
@@ -6114,22 +6322,64 @@
         <v>24</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="M3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="Q3" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="U3" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="V3" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="X3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="Y3" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z3" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB3" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="AC3" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD3" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE3" s="6" t="s">
+        <v>413</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" ht="409.6">
+    <row r="4" spans="1:31" ht="409.6">
       <c r="A4" s="1">
         <v>5.0999999999999996</v>
       </c>
@@ -6145,23 +6395,26 @@
       <c r="E4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="T4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="X4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="AB4" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="409.6">
+    <row r="5" spans="1:31" ht="409.6">
       <c r="A5" s="1">
         <v>5.0999999999999996</v>
       </c>
@@ -6177,23 +6430,23 @@
       <c r="E5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="X5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="AB5" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="409.6">
+    <row r="6" spans="1:31" ht="409.6">
       <c r="A6" s="1">
         <v>5.0999999999999996</v>
       </c>
@@ -6209,23 +6462,23 @@
       <c r="E6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="T6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="X6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="AB6" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="409.6">
+    <row r="7" spans="1:31" ht="409.6">
       <c r="A7" s="1">
         <v>5.0999999999999996</v>
       </c>
@@ -6241,23 +6494,23 @@
       <c r="E7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="T7" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="X7" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="AB7" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="409.6">
+    <row r="8" spans="1:31" ht="409.6">
       <c r="A8" s="1">
         <v>5.2</v>
       </c>
@@ -6274,28 +6527,64 @@
         <v>63</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J8" s="1" t="s">
+      <c r="M8" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="P8" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="Q8" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="T8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="U8" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="X8" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="Y8" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB8" s="1" t="s">
         <v>70</v>
       </c>
+      <c r="AC8" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="9" spans="1:13" ht="409.6">
+    <row r="9" spans="1:31" ht="409.6">
       <c r="A9" s="1">
         <v>5.2</v>
       </c>
@@ -6312,28 +6601,67 @@
         <v>71</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J9" s="1" t="s">
+      <c r="M9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P9" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="Q9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="T9" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="U9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="X9" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="Y9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB9" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="AC9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="10" spans="1:13" ht="409.6">
+    <row r="10" spans="1:31" ht="409.6">
       <c r="A10" s="1">
         <v>5.2</v>
       </c>
@@ -6350,28 +6678,64 @@
         <v>77</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J10" s="1" t="s">
+      <c r="M10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P10" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="Q10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="T10" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="U10" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="V10" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="X10" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="Y10" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z10" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB10" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="AC10" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD10" s="6" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="11" spans="1:13" ht="409.6">
+    <row r="11" spans="1:31" ht="409.6">
       <c r="A11" s="1">
         <v>5.2</v>
       </c>
@@ -6387,29 +6751,68 @@
       <c r="E11" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J11" s="1" t="s">
+      <c r="M11" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="P11" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="Q11" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="T11" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="U11" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="X11" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="Y11" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB11" s="1" t="s">
         <v>88</v>
       </c>
+      <c r="AC11" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD11" s="1" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="12" spans="1:13" ht="409.6">
+    <row r="12" spans="1:31" ht="409.6">
       <c r="A12" s="1">
         <v>5.2</v>
       </c>
@@ -6426,28 +6829,67 @@
         <v>89</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L12" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J12" s="1" t="s">
+      <c r="M12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P12" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="Q12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="T12" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="U12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="X12" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="Y12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB12" s="1" t="s">
         <v>94</v>
       </c>
+      <c r="AC12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD12" s="1" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="13" spans="1:13" ht="409.6">
+    <row r="13" spans="1:31" ht="409.6">
       <c r="A13" s="1">
         <v>5.2</v>
       </c>
@@ -6463,29 +6905,68 @@
       <c r="E13" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L13" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J13" s="1" t="s">
+      <c r="M13" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="P13" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="Q13" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="U13" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="X13" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="Y13" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z13" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB13" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="M13" s="1" t="s">
-        <v>100</v>
+      <c r="AC13" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="AD13" s="1" t="s">
+        <v>411</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="409.6">
+    <row r="14" spans="1:31" ht="409.6">
       <c r="A14" s="1">
         <v>5.3</v>
       </c>
@@ -6493,31 +6974,31 @@
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L14" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="P14" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="T14" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="X14" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="AB14" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="M14" s="1" t="s">
-        <v>107</v>
-      </c>
     </row>
-    <row r="15" spans="1:13" ht="409.6">
+    <row r="15" spans="1:31" ht="340">
       <c r="A15" s="1">
         <v>5.3</v>
       </c>
@@ -6525,31 +7006,31 @@
         <v>22</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="L15" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="P15" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="T15" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="X15" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="AB15" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="M15" s="1" t="s">
-        <v>113</v>
-      </c>
     </row>
-    <row r="16" spans="1:13" ht="409.6">
+    <row r="16" spans="1:31" ht="340">
       <c r="A16" s="1">
         <v>5.3</v>
       </c>
@@ -6557,31 +7038,31 @@
         <v>30</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L16" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="P16" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="T16" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="X16" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="AB16" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="M16" s="1" t="s">
-        <v>119</v>
-      </c>
     </row>
-    <row r="17" spans="1:13" ht="409.6">
+    <row r="17" spans="1:31" ht="409.6">
       <c r="A17" s="1">
         <v>5.3</v>
       </c>
@@ -6589,31 +7070,31 @@
         <v>38</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="L17" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="P17" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="T17" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="X17" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="AB17" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="M17" s="1" t="s">
-        <v>125</v>
-      </c>
     </row>
-    <row r="18" spans="1:13" ht="409.6">
+    <row r="18" spans="1:31" ht="409.6">
       <c r="A18" s="1">
         <v>5.3</v>
       </c>
@@ -6621,31 +7102,31 @@
         <v>46</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="L18" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="P18" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="T18" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="X18" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="AB18" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="M18" s="1" t="s">
-        <v>131</v>
-      </c>
     </row>
-    <row r="19" spans="1:13" ht="409.6">
+    <row r="19" spans="1:31" ht="409.6">
       <c r="A19" s="1">
         <v>5.3</v>
       </c>
@@ -6653,31 +7134,31 @@
         <v>54</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>55</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="L19" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="P19" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="T19" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="X19" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="AB19" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="M19" s="1" t="s">
-        <v>137</v>
-      </c>
     </row>
-    <row r="20" spans="1:13" ht="409.6">
+    <row r="20" spans="1:31" ht="409.6">
       <c r="A20" s="1">
         <v>5.4</v>
       </c>
@@ -6685,37 +7166,79 @@
         <v>13</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="L20" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="H20" s="1" t="s">
+      <c r="M20" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="P20" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="Q20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="T20" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="U20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="V20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="X20" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="L20" s="1" t="s">
+      <c r="Y20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB20" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="M20" s="1" t="s">
-        <v>146</v>
+      <c r="AC20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD20" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="409.6">
+    <row r="21" spans="1:31" ht="388">
       <c r="A21" s="1">
         <v>5.4</v>
       </c>
@@ -6723,37 +7246,76 @@
         <v>22</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L21" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="M21" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="P21" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J21" s="1" t="s">
+      <c r="Q21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="T21" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="U21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="X21" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="L21" s="1" t="s">
+      <c r="Y21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB21" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="M21" s="1" t="s">
-        <v>152</v>
+      <c r="AC21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD21" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="409.6">
+    <row r="22" spans="1:31" ht="388">
       <c r="A22" s="1">
         <v>5.4</v>
       </c>
@@ -6761,37 +7323,73 @@
         <v>30</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L22" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="M22" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="N22" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="P22" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J22" s="1" t="s">
+      <c r="Q22" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="R22" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="T22" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="U22" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="V22" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="X22" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="L22" s="1" t="s">
+      <c r="Y22" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z22" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB22" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="M22" s="1" t="s">
-        <v>158</v>
+      <c r="AC22" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD22" s="6" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="409.6">
+    <row r="23" spans="1:31" ht="388">
       <c r="A23" s="1">
         <v>5.4</v>
       </c>
@@ -6799,37 +7397,73 @@
         <v>38</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="L23" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H23" s="1" t="s">
+      <c r="M23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P23" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="Q23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="T23" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="U23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="X23" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="L23" s="1" t="s">
+      <c r="Y23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB23" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="M23" s="1" t="s">
-        <v>165</v>
+      <c r="AC23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD23" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="409.6">
+    <row r="24" spans="1:31" ht="388">
       <c r="A24" s="1">
         <v>5.4</v>
       </c>
@@ -6837,37 +7471,91 @@
         <v>46</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L24" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="M24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="P24" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J24" s="1" t="s">
+      <c r="Q24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="T24" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="U24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="V24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="W24" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="X24" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="L24" s="1" t="s">
+      <c r="Y24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA24" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="AB24" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="M24" s="1" t="s">
-        <v>171</v>
+      <c r="AC24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE24" s="1" t="s">
+        <v>421</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="409.6">
+    <row r="25" spans="1:31" ht="409.6">
       <c r="A25" s="1">
         <v>5.4</v>
       </c>
@@ -6875,37 +7563,91 @@
         <v>54</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>55</v>
       </c>
       <c r="E25" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L25" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="M25" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="P25" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J25" s="1" t="s">
+      <c r="Q25" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="R25" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="S25" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="T25" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="U25" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="V25" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="W25" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="X25" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="L25" s="1" t="s">
+      <c r="Y25" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z25" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA25" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="AB25" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="M25" s="1" t="s">
-        <v>177</v>
+      <c r="AC25" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD25" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AE25" s="1" t="s">
+        <v>422</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="409.6">
+    <row r="26" spans="1:31" ht="409.6">
       <c r="A26" s="1">
         <v>7.1</v>
       </c>
@@ -6913,31 +7655,31 @@
         <v>13</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="L26" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="P26" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="T26" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="X26" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="L26" s="1" t="s">
+      <c r="AB26" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="M26" s="1" t="s">
-        <v>185</v>
-      </c>
     </row>
-    <row r="27" spans="1:13" ht="409.6">
+    <row r="27" spans="1:31" ht="409.6">
       <c r="A27" s="1">
         <v>7.1</v>
       </c>
@@ -6945,31 +7687,31 @@
         <v>22</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D27" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="L27" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="P27" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="T27" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="X27" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="L27" s="1" t="s">
+      <c r="AB27" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="M27" s="1" t="s">
-        <v>192</v>
-      </c>
     </row>
-    <row r="28" spans="1:13" ht="409.6">
+    <row r="28" spans="1:31" ht="409.6">
       <c r="A28" s="1">
         <v>7.1</v>
       </c>
@@ -6977,31 +7719,31 @@
         <v>30</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D28" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="L28" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="P28" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="T28" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="X28" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="L28" s="1" t="s">
+      <c r="AB28" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="M28" s="1" t="s">
-        <v>199</v>
-      </c>
     </row>
-    <row r="29" spans="1:13" ht="409.6">
+    <row r="29" spans="1:31" ht="409.6">
       <c r="A29" s="1">
         <v>7.1</v>
       </c>
@@ -7009,31 +7751,31 @@
         <v>38</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D29" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="L29" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="P29" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="T29" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="K29" s="1" t="s">
+      <c r="X29" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="L29" s="1" t="s">
+      <c r="AB29" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="M29" s="1" t="s">
-        <v>206</v>
-      </c>
     </row>
-    <row r="30" spans="1:13" ht="409.6">
+    <row r="30" spans="1:31" ht="409.6">
       <c r="A30" s="1">
         <v>7.1</v>
       </c>
@@ -7041,31 +7783,31 @@
         <v>46</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="L30" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="P30" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="T30" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="K30" s="1" t="s">
+      <c r="X30" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="L30" s="1" t="s">
+      <c r="AB30" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="M30" s="1" t="s">
-        <v>213</v>
-      </c>
     </row>
-    <row r="31" spans="1:13" ht="409.6">
+    <row r="31" spans="1:31" ht="409.6">
       <c r="A31" s="1">
         <v>7.1</v>
       </c>
@@ -7073,31 +7815,31 @@
         <v>54</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D31" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="L31" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="P31" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="T31" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="K31" s="1" t="s">
+      <c r="X31" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="L31" s="1" t="s">
+      <c r="AB31" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="M31" s="1" t="s">
-        <v>220</v>
-      </c>
     </row>
-    <row r="32" spans="1:13" ht="409.6">
+    <row r="32" spans="1:31" ht="409.6">
       <c r="A32" s="1">
         <v>7.2</v>
       </c>
@@ -7105,37 +7847,73 @@
         <v>13</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>223</v>
       </c>
       <c r="G32" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="P32" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="H32" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="J32" s="1" t="s">
+      <c r="Q32" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="T32" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="K32" s="1" t="s">
+      <c r="U32" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="V32" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="X32" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="L32" s="1" t="s">
+      <c r="Y32" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z32" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB32" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="M32" s="1" t="s">
-        <v>228</v>
+      <c r="AC32" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD32" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="409.6">
+    <row r="33" spans="1:31" ht="409.6">
       <c r="A33" s="1">
         <v>7.2</v>
       </c>
@@ -7143,37 +7921,73 @@
         <v>22</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E33" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="L33" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="M33" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P33" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="G33" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="J33" s="1" t="s">
+      <c r="Q33" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R33" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="T33" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="K33" s="1" t="s">
+      <c r="U33" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="V33" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="X33" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="L33" s="1" t="s">
+      <c r="Y33" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z33" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB33" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="M33" s="1" t="s">
-        <v>234</v>
+      <c r="AC33" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD33" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="409.6">
+    <row r="34" spans="1:31" ht="409.6">
       <c r="A34" s="1">
         <v>7.2</v>
       </c>
@@ -7181,37 +7995,73 @@
         <v>30</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E34" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L34" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="M34" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="N34" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="P34" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="G34" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J34" s="1" t="s">
+      <c r="Q34" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="R34" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="T34" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="K34" s="1" t="s">
+      <c r="U34" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="V34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="X34" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="L34" s="1" t="s">
+      <c r="Y34" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="Z34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB34" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="M34" s="1" t="s">
-        <v>240</v>
+      <c r="AC34" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD34" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="409.6">
+    <row r="35" spans="1:31" ht="409.6">
       <c r="A35" s="1">
         <v>7.2</v>
       </c>
@@ -7219,37 +8069,82 @@
         <v>38</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D35" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="F35" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="L35" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="M35" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N35" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="G35" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H35" s="1" t="s">
+      <c r="P35" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="J35" s="1" t="s">
+      <c r="Q35" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R35" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="T35" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="K35" s="1" t="s">
+      <c r="U35" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="V35" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="W35" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="X35" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="L35" s="1" t="s">
+      <c r="Y35" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z35" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA35" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="AB35" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="M35" s="1" t="s">
-        <v>248</v>
+      <c r="AC35" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD35" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE35" s="1" t="s">
+        <v>424</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="409.6">
+    <row r="36" spans="1:31" ht="409.6">
       <c r="A36" s="1">
         <v>7.2</v>
       </c>
@@ -7257,37 +8152,88 @@
         <v>46</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E36" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L36" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="M36" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="N36" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="P36" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="G36" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J36" s="1" t="s">
+      <c r="Q36" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="R36" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="S36" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="T36" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="K36" s="1" t="s">
+      <c r="U36" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="V36" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="W36" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="X36" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="L36" s="1" t="s">
+      <c r="Y36" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z36" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA36" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="AB36" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="M36" s="1" t="s">
-        <v>254</v>
+      <c r="AC36" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD36" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE36" s="1" t="s">
+        <v>425</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="409.6">
+    <row r="37" spans="1:31" ht="409.6">
       <c r="A37" s="1">
         <v>7.2</v>
       </c>
@@ -7295,37 +8241,91 @@
         <v>54</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E37" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="L37" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="M37" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="P37" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="G37" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="J37" s="1" t="s">
+      <c r="Q37" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R37" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="S37" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="T37" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="K37" s="1" t="s">
+      <c r="U37" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="V37" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="W37" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="X37" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="L37" s="1" t="s">
+      <c r="Y37" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z37" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA37" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="AB37" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="M37" s="1" t="s">
-        <v>260</v>
+      <c r="AC37" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD37" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AE37" s="1" t="s">
+        <v>426</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="409.6">
+    <row r="38" spans="1:31" ht="409.6">
       <c r="A38" s="1">
         <v>7.3</v>
       </c>
@@ -7333,37 +8333,88 @@
         <v>13</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="F38" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="L38" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="M38" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="P38" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="G38" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="J38" s="1" t="s">
+      <c r="Q38" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R38" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="S38" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="T38" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="K38" s="1" t="s">
+      <c r="U38" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="V38" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="W38" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="X38" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="L38" s="1" t="s">
+      <c r="Y38" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z38" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="AA38" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="AB38" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="M38" s="1" t="s">
-        <v>268</v>
+      <c r="AC38" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD38" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="AE38" s="1" t="s">
+        <v>428</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="409.6">
+    <row r="39" spans="1:31" ht="409.6">
       <c r="A39" s="1">
         <v>7.3</v>
       </c>
@@ -7371,37 +8422,76 @@
         <v>22</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E39" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="L39" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="M39" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P39" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="J39" s="1" t="s">
+      <c r="Q39" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="R39" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="T39" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="K39" s="1" t="s">
+      <c r="U39" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="V39" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="X39" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="L39" s="1" t="s">
+      <c r="Y39" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="Z39" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA39" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="AB39" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="M39" s="1" t="s">
-        <v>274</v>
+      <c r="AC39" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD39" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="409.6">
+    <row r="40" spans="1:31" ht="409.6">
       <c r="A40" s="1">
         <v>7.3</v>
       </c>
@@ -7409,37 +8499,73 @@
         <v>30</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E40" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L40" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="M40" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P40" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="G40" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J40" s="1" t="s">
+      <c r="Q40" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R40" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="T40" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="K40" s="1" t="s">
+      <c r="U40" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="V40" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="X40" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="L40" s="1" t="s">
+      <c r="Y40" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z40" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB40" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="M40" s="1" t="s">
-        <v>280</v>
+      <c r="AC40" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD40" s="6" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="409.6">
+    <row r="41" spans="1:31" ht="409.6">
       <c r="A41" s="1">
         <v>7.3</v>
       </c>
@@ -7447,37 +8573,73 @@
         <v>38</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E41" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="L41" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="M41" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P41" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="G41" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="J41" s="1" t="s">
+      <c r="Q41" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="R41" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="T41" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="K41" s="1" t="s">
+      <c r="U41" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="V41" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="X41" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="L41" s="1" t="s">
+      <c r="Y41" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z41" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB41" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="M41" s="1" t="s">
-        <v>286</v>
+      <c r="AC41" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD41" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="409.6">
+    <row r="42" spans="1:31" ht="409.6">
       <c r="A42" s="1">
         <v>7.3</v>
       </c>
@@ -7485,37 +8647,79 @@
         <v>46</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D42" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="F42" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L42" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="M42" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="P42" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="G42" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J42" s="1" t="s">
+      <c r="Q42" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R42" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="T42" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="K42" s="1" t="s">
+      <c r="U42" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="V42" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="X42" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="L42" s="1" t="s">
+      <c r="Y42" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z42" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB42" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="M42" s="1" t="s">
-        <v>293</v>
+      <c r="AC42" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD42" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AE42" s="1" t="s">
+        <v>431</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="409.6">
+    <row r="43" spans="1:31" ht="409.6">
       <c r="A43" s="1">
         <v>7.3</v>
       </c>
@@ -7523,34 +8727,79 @@
         <v>54</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E43" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L43" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="M43" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P43" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="G43" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J43" s="1" t="s">
+      <c r="Q43" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R43" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="T43" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="K43" s="1" t="s">
+      <c r="U43" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="V43" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="X43" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="L43" s="1" t="s">
+      <c r="Y43" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="Z43" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="AA43" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="AB43" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="M43" s="1" t="s">
-        <v>299</v>
+      <c r="AC43" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD43" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="AE43" s="1" t="s">
+        <v>433</v>
       </c>
     </row>
   </sheetData>
@@ -7560,10 +8809,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2:AD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -7572,16 +8821,34 @@
     <col min="3" max="3" width="9.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="30.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="27" style="1" customWidth="1"/>
-    <col min="6" max="6" width="33.6640625" style="1" customWidth="1"/>
-    <col min="7" max="9" width="8.83203125" style="1"/>
-    <col min="10" max="10" width="28" style="1" customWidth="1"/>
-    <col min="11" max="11" width="28.1640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="29.33203125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="34.83203125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.83203125" style="1"/>
+    <col min="6" max="6" width="11.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" style="1" customWidth="1"/>
+    <col min="9" max="11" width="8.83203125" style="1"/>
+    <col min="12" max="12" width="33.6640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12.1640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.1640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="28" style="1" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.1640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="11.1640625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="28.1640625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="11.6640625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="12.1640625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="11.1640625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="29.33203125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="11.6640625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="12.1640625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="11.1640625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="34.83203125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="11.6640625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="12.1640625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="11.1640625" style="1" customWidth="1"/>
+    <col min="32" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="68">
+    <row r="1" spans="1:31" ht="68">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -7597,61 +8864,151 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="M1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="N1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="O1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="Q1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="U1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="X1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="Y1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB1" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="AC1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE1" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" ht="409.6">
+    <row r="2" spans="1:31" ht="409.6">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="M2" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="U2" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="X2" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB2" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>306</v>
+      <c r="AC2" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -7728,28 +9085,28 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>313</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="409.6">
@@ -7757,37 +9114,37 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="409.6">
@@ -7795,34 +9152,34 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>330</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="409.6">
@@ -7833,28 +9190,28 @@
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>338</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="409.6">
@@ -7865,28 +9222,28 @@
         <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>345</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="409.6">
@@ -7897,28 +9254,28 @@
         <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>352</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="409.6">
@@ -7929,28 +9286,28 @@
         <v>38</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>359</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="409.6">
@@ -7961,28 +9318,28 @@
         <v>46</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>366</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="409.6">
@@ -7993,34 +9350,34 @@
         <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>374</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="409.6">
@@ -8031,34 +9388,34 @@
         <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="M11" s="1" t="s">
         <v>381</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="409.6">
@@ -8069,34 +9426,34 @@
         <v>30</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="J12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="M12" s="1" t="s">
         <v>388</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="409.6">
@@ -8107,34 +9464,34 @@
         <v>38</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="J13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="M13" s="1" t="s">
         <v>395</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="409.6">
@@ -8145,34 +9502,34 @@
         <v>46</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="J14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="M14" s="1" t="s">
         <v>402</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="409.6">
@@ -8180,31 +9537,31 @@
         <v>10</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>409</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>410</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Chapter 3 feedback completed (Student sol)
</commit_message>
<xml_diff>
--- a/dataset/testing.xlsx
+++ b/dataset/testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajed/PycharmProjects/Study-on-ChatGPT/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF0FDD7-B4F7-2244-9C35-3D216437411A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B4C7848-0CCA-4144-A369-1F59AA5B7DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="17300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="17300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ch1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="436">
   <si>
     <t>id</t>
   </si>
@@ -4808,8 +4808,817 @@
     <t>Demonstrate the problem with Point using a HashSet.</t>
   </si>
   <si>
+    <t>When you override the equals() method, it is generally recommended that you also override the hashCode() method, because the hashCode() method is used by certain collection classes (such as HashSet) to determine whether two objects are equal. If you override equals() but not hashCode(), then these collections may not behave as expected.
+Here's an example of how the Point class from Chapter 1 might be defective in this regard:
+class Point {
+    private int x;
+    private int y;
+    public Point(int x, int y) {
+        this.x = x;
+        this.y = y;
+    }
+    @Override
+    public boolean equals(Object o) {
+        if (o == this) return true;
+        if (!(o instanceof Point)) return false;
+        Point p = (Point) o;
+        return p.x == x &amp;&amp; p.y == y;
+    }
+}
+The above Point class overrides the equals() method to check for equality based on the x and y fields, but it does not override the hashCode() method. Therefore, if we try to use it as key in HashMap it will return error.
+Copy code
+    HashSet&lt;Point&gt; set = new HashSet&lt;&gt;();
+    set.add(new Point(1, 2));
+    set.add(new Point(3, 4));
+    set.add(new Point(1, 2)); 
+In this example, we are trying to add three Point objects to a HashSet. The first two Point objects have different x and y values, so they will be added to the set without any problem. However, the third Point object has the same x and y values as the first Point object, so equals() will return true when comparing the two. But HashSet uses the hashCode() method to determine whether two objects are equal, and since the Point class doesn't override hashCode(), the HashSet will treat the first and third Point objects as distinct, and therefore it will be added to the set, even though it's a duplicate.
+To fix this, you would need to override the hashCode() method in Point class, and implement it consistently with the equals() method.
+    @Override
+    public int hashCode() {
+        int result = 17;
+        result = 31 * result + x;
+        result = 31 * result + y;
+        return result;
+    }
+This would ensure that HashSet is able to correctly identify when two Point objects are equal and will prevent duplicate values from being added to the set.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the Point class overrides the equals() method but does not also override the hashCode() method, then instances of Point may not behave correctly when stored in a HashSet. For example, if two Point instances have the same x and y coordinates, the equals() method may return true for these instances, indicating that they are equal. However, the HashSet will use the hashCode() method to determine where to store the instances, and if the hashCode() method is not overridden, the HashSet will consider the instances to be different, even though the equals() method considers them to be equal. This can lead to unexpected behavior, such as the HashSet storing multiple copies of the same Point instance.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Here is an example of how the problem with the Point class from Chapter 1 can be demonstrated using a HashSet:
+```
+import java.util.HashSet;
+class Point {
+    int x, y;
+    public Point(int x, int y) {
+        this.x = x;
+        this.y = y;
+    }
+    @Override
+    public boolean equals(Object obj) {
+        if (obj == this) {
+            return true;
+        }
+        if (!(obj instanceof Point)) {
+            return false;
+        }
+        Point p = (Point) obj;
+        return p.x == x &amp;&amp; p.y == y;
+    }
+}
+public class Main {
+    public static void main(String[] args) {
+        HashSet&lt;Point&gt; set = new HashSet&lt;Point&gt;();
+        Point p1 = new Point(1, 2);
+        Point p2 = new Point(1, 2);
+        set.add(p1);
+        set.add(p2);
+        System.out.println(set.size()); // prints 2 instead of 1
+    }
+}
+```
+In this example, two Point objects (p1 and p2) are created with the same x and y values, and they are added to a HashSet. Since the Point class does not override the hashCode() method, the HashSet uses the default implementation of the Object class, which generates a unique hash code based on the memory address of the object. As a result, the HashSet considers p1 and p2 to be different objects and does not remove the duplicate. This causes the set.size() to return 2 instead of 1.
+To fix this problem, the Point class should override the hashCode() method and implement a proper hash function based on the x and y values of the Point objects.
+</t>
+  </si>
+  <si>
+    <t>If the Point class has not overridden the hashCode() method, and the equals() method is used to compare two Point objects in a HashSet, the HashSet may not properly identify the two Point objects as equal. This can cause issues with adding, removing, or searching for the Point objects in the HashSet.
+For example, if we create two Point objects with the same x and y coordinates, the HashSet may not recognize them as equal and add them both to the set. 
+```
+HashSet&lt;Point&gt; pointSet = new HashSet&lt;&gt;();
+Point point1 = new Point(1, 2);
+Point point2 = new Point(1, 2);
+pointSet.add(point1);
+pointSet.add(point2);
+System.out.println(pointSet.size());  // Output: 2
+```
+This is because the HashSet uses the hashCode() method to determine where to store the object in its internal data structure and also uses it to compare objects for equality. If the hashCode() method is not overridden, the HashSet will use the default implementation which may not be appropriate for the Point class.</t>
+  </si>
+  <si>
+    <t>Here is an example of the problem with the Point class from Chapter 1 when using a HashSet:
+```
+import java.util.HashSet;
+public class Main {
+    public static void main(String[] args) {
+        HashSet&lt;Point&gt; points = new HashSet&lt;Point&gt;();
+        Point p1 = new Point(1, 2);
+        Point p2 = new Point(1, 2);
+        points.add(p1);
+        points.add(p2);
+        System.out.println(points.size()); // prints "2" instead of "1"
+    }
+}
+class Point {
+    int x;
+    int y;
+    Point(int x, int y) {
+        this.x = x;
+        this.y = y;
+    }
+    // equals() method is not overridden
+}
+```
+In this example, we create a HashSet of Point objects and add two Point objects, p1 and p2, that have the same x and y values. However, since the Point class does not override the equals() method, the HashSet considers these two Point objects to be distinct and adds both to the set. As a result, the size of the set is 2 instead of 1. 
+This problem could be avoided if the Point class overrides the equals() method and hashCode() method, so that two Point objects with the same x and y values are considered equal by the HashSet and only one is added to the set.</t>
+  </si>
+  <si>
+    <t>Write down the mathematical relationship required between equals() and hashCode().</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The equals() and hashCode() methods are used together in Java to implement the contract of object equality, as defined by the Objects.equals() and Objects.hash() methods.
+According to this contract, if two objects are equal (as determined by the equals() method), then their hashCode() values must be equal as well. Conversely, if two objects have equal hashCode() values, they do not necessarily have to be equal (as determined by the equals() method).
+In other words, the relationship between equals() and hashCode() is defined by the following mathematical relationship:
+if a.equals(b) then a.hashCode() == b.hashCode()
+This relationship is important because it allows objects to be stored and retrieved efficiently in common data structures such as HashMap, HashSet, and Hashtable.
+It's also worth noting that the hashCode() method should be implemented such that it returns the same value for two equal objects every time it is called on those objects, as long as the objects are not modified. This allows the hashCode() method to be used as a way to identify unique objects and helps to ensure the efficiency of data structures that rely on it.
+</t>
+  </si>
+  <si>
+    <t>When overriding the equals() method in a class, it is generally recommended to also override the hashCode() method, as the two methods should have a consistent relationship. Specifically, if two objects are equal according to the equals() method, then calling hashCode() on each of the objects must produce the same integer result. Additionally, if two objects are unequal according to the equals() method, it is not required but preferable that calling hashCode() on each of the objects produces distinct integer results.
+To put it mathematically:
+- If a.equals(b) returns true, then a.hashCode() == b.hashCode() must also return true.
+- If a.equals(b) returns false, then it is not necessary that a.hashCode() == b.hashCode() returns false, but the distinct hashCode would be preferred.
+It's worth noting that in practice, it's hard to guarantee that hashCode is distinct for all unequal objects, but it's more important that it is consistent with the equals.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+The mathematical relationship required between the equals() and hashCode() methods is known as the "general contract" and it states that if two objects are equal, according to the equals(Object) method, then calling the hashCode() method on each of the two objects must produce the same integer result. 
+Additionally, it is not required but strongly recommended that if two objects are unequal according to the equals(java.lang.Object) method, then calling the hashCode() method on each of the two objects should produce distinct integer results. In other words, the hashCode() method should return distinct values for distinct objects.
+It's worth noting that this relationship is not symmetric, meaning that if two objects have the same hashCode() it doesn't mean they are equal.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+The relationship between the `equals()` and `hashCode()` methods in Java is defined by the following contract:
+- If two objects are equal according to the `equals(Object)` method, then calling the `hashCode()` method on each of the two objects must produce the same integer result.
+- It is not required that if two objects are unequal according to the `equals(Object)` method, then calling the `hashCode()` method on each of the two objects must produce distinct integer results. However, the programmer should be aware that producing distinct integer results for unequal objects may improve the performance of hash tables.
+In other words, if two objects are equal, they must have the same hash code. However, if two objects have different hash codes, they may still be equal. Therefore, it is important to make sure that the hash code is based on the same attributes used by the equals method.
+</t>
+  </si>
+  <si>
+    <t>When overriding the equals() method, it is generally recommended to also override the hashCode() method. This is because the hashCode() method is used by common Collection structures such as HashSet to determine if two objects are equal, and if the hashCode() method is not overridden, it may not return the correct value.
+The mathematical relationship required between equals() and hashCode() is that if two objects are equal according to the equals(Object) method, then calling the hashCode() method on each of the two objects must produce the same integer result. This means that if two objects are equal then their hashcode should be same.</t>
+  </si>
+  <si>
+    <t>(a) When overriding the equals() method, it is generally recommended to also override the hashCode() method. This is because the hashCode method is used by certain collection classes (such as HashSet and HashMap) to determine where to store an object, and if the hashCode method is not overridden, these classes may not be able to properly store instances of the class.
+(b) The mathematical relationship required between equals() and hashCode() is that if two objects are equal according to the equals(Object) method, then calling the hashCode method on each of the two objects must produce the same integer result. This means that if a.equals(b) returns true, then a.hashCode() == b.hashCode() must also be true. Additionally, it is required that if two objects are not equal according to the equals(Object) method, then calling the hashCode method on each of the two objects must produce distinct integer results, unless the two objects are null.</t>
+  </si>
+  <si>
+    <t>Write a simple JUnit test to show that Point objects do not enjoy this property.</t>
+  </si>
+  <si>
+    <t>Here is a simple JUnit test that demonstrates that the Point class does not satisfy the required relationship between equals() and hashCode():
+import org.junit.Test;
+import static org.junit.Assert.*;
+public class PointTest {
+  @Test
+  public void testEqualsAndHashCode() {
+    Point p1 = new Point(1, 2);
+    Point p2 = new Point(1, 2);
+    Point p3 = new Point(3, 4);
+    assertTrue(p1.equals(p2));
+    assertFalse(p1.hashCode() == p2.hashCode());  // Fails
+  }
+}
+In this test, we create two Point objects, p1 and p2, which are equal (as determined by the equals() method). However, the test fails because the hashCode() values of p1 and p2 are not equal, indicating that the hashCode() method is not properly implemented.
+To fix this issue, the hashCode() method in the Point class needs to be overridden as described in the previous answer. Once the hashCode() method is properly implemented, the test should pass.</t>
+  </si>
+  <si>
+    <t>Here's an example of a JUnit test that demonstrates the issue with the Point class not properly overriding the hashCode() method:
+import static org.junit.Assert.*;
+import java.util.HashSet;
+import org.junit.Test;
+public class PointTest {
+    @Test
+    public void testHashCode() {
+        Point p1 = new Point(1, 2);
+        Point p2 = new Point(1, 2);
+        // assert that p1 and p2 are equal
+        assertTrue(p1.equals(p2));
+        HashSet&lt;Point&gt; set = new HashSet&lt;&gt;();
+        set.add(p1);
+        set.add(p2);
+        // if hashCode() is not properly implemented, the set will contain 2 elements
+        assertEquals(1, set.size());
+    }
+}
+This test creates two Point objects, p1 and p2, that are equal to each other (have the same x and y values). It then adds both of these objects to a HashSet, and checks the size of the set to see if the hashCode() method is properly implemented. If the hashCode() method is not properly overridden, the set will contain 2 elements, because the HashSet considers the two Point objects to be different. If the hashCode() method is correctly overridden, the set will contain only 1 element, because the two Point objects are considered to be equal.
+It is worth noting that if the equals method is overridden and not symmetric, reflexive and transitive, the same issue can appear.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Here is an example of a JUnit test that demonstrates that Point objects do not have the proper relationship between equals() and hashCode():
+```
+import static org.junit.Assert.*;
+import java.util.HashSet;
+import java.util.Set;
+import org.junit.Test;
+public class PointTest {
+    @Test
+    public void testEqualsAndHashCode() {
+        Point p1 = new Point(1, 2);
+        Point p2 = new Point(1, 2);
+        // Assert that p1 and p2 are equal according to the equals() method
+        assertTrue(p1.equals(p2));
+        // Assert that p1 and p2 have different hash codes
+        assertNotEquals(p1.hashCode(), p2.hashCode());
+        // Create a HashSet and add p1 and p2 to it
+        Set&lt;Point&gt; set = new HashSet&lt;Point&gt;();
+        set.add(p1);
+        set.add(p2);
+        // Assert that the HashSet only contains one Point
+        // even though p1 and p2 are equal
+        assertEquals(1, set.size());
+    }
+}
+```
+This test creates two Point objects, p1 and p2, that have the same x and y coordinates. The test then asserts that the equals() method considers p1 and p2 to be equal, but that their hash codes are different. Finally, the test adds p1 and p2 to a HashSet, and asserts that the HashSet only contains one Point, even though p1 and p2 are equal. This behavior is caused by the Point class not overriding the hashCode() method, and demonstrate that the Point objects do not have the proper relationship between equals() and hashCode().
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Here is a simple JUnit test that demonstrates that Point objects do not satisfy the contract between `equals()` and `hashCode()`:
+```
+import org.junit.Test;
+import java.util.HashSet;
+import static org.junit.Assert.*;
+class Point {
+    int x, y;
+    public Point(int x, int y) {
+        this.x = x;
+        this.y = y;
+    }
+    @Override
+    public boolean equals(Object obj) {
+        if (obj == this) {
+            return true;
+        }
+        if (!(obj instanceof Point)) {
+            return false;
+        }
+        Point p = (Point) obj;
+        return p.x == x &amp;&amp; p.y == y;
+    }
+}
+public class PointTest {
+    @Test
+    public void testHashCode() {
+        Point p1 = new Point(1, 2);
+        Point p2 = new Point(1, 2);
+        assertTrue(p1.equals(p2));
+        assertFalse(p1.hashCode() == p2.hashCode());
+    }
+}
+```
+This test creates two Point objects (p1 and p2) with the same x and y values and checks if they are equal using the `equals()` method. Then it checks if the hash codes of these two objects are the same. Since the Point class does not override the `hashCode()` method, it uses the default implementation of the `Object` class which generates a unique hash code based on the memory address of the object. As a result, the test fails, indicating that the Point objects do not satisfy the contract between `equals()` and `hashCode()`.
+</t>
+  </si>
+  <si>
+    <t>```
+import static org.junit.Assert.*;
+import java.util.HashSet;
+import org.junit.Test;
+public class PointTest {
+    @Test
+    public void testEqualityInHashSet() {
+        Point p1 = new Point(1, 2);
+        Point p2 = new Point(1, 2);
+        HashSet&lt;Point&gt; set = new HashSet&lt;Point&gt;();
+        set.add(p1);
+        assertFalse(set.contains(p2));
+    }
+}
+```
+In this JUnit test, two Point objects `p1` and `p2` are created with the same x and y coordinates. These objects are added to a HashSet, and it is asserted that the HashSet does not contain the second Point object `p2`. This is because the `equals()` and `hashCode()` methods have not been overridden, so the HashSet uses the default implementation which only considers objects to be equal if they are the same instance.</t>
+  </si>
+  <si>
+    <t>Here is a simple JUnit test that demonstrates that Point objects do not have the property of being able to be stored in common Collection structures such as HashSet when the equals() method is overridden without also overriding the hashCode() method:
+```
+import static org.junit.Assert.*;
+import java.util.HashSet;
+import org.junit.Test;
+public class PointTest {
+    @Test
+    public void testHashCodeProperty() {
+        Point p1 = new Point(1, 2);
+        Point p2 = new Point(1, 2);
+        HashSet&lt;Point&gt; set = new HashSet&lt;Point&gt;();
+        set.add(p1);
+        // This should return false, since p1 and p2 are equal but have different hash codes
+        assertFalse(set.contains(p2));
+    }
+}
+```
+Note that this is just an example and you need to import the class point in your test class.</t>
+  </si>
+  <si>
+    <t>Repair the Point class to fix the fault.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To repair the fault in the Point class, the hashCode() method needs to be overridden as follows:
+class Point {
+  int x;
+  int y;
+  public Point(int x, int y) {
+    this.x = x;
+    this.y = y;
+  }
+  // Overrides equals() method
+  public boolean equals(Object o) {
+    if (!(o instanceof Point)) return false;
+    Point p = (Point) o;
+    return p.x == x &amp;&amp; p.y == y;
+  }
+  // Overrides hashCode() method
+  public int hashCode() {
+    return Objects.hash(x, y);
+  }
+}
+With the hashCode() method overridden, the Point class will now satisfy the required relationship between equals() and hashCode() and can be used with common data structures such as HashMap, HashSet, and Hashtable without any issues.
+It's worth noting that the hashCode() method implementation shown above uses the Objects.hash() utility method to compute the hash code for the Point object. This method takes the x and y fields of the Point object as arguments and returns a hash code that is based on their values. This ensures that the hash code is consistent with the definition of equality for the Point class (as defined by the equals() method).
+</t>
+  </si>
+  <si>
+    <t>Here's an example of how you might repair the Point class to properly override the equals() and hashCode() methods:
+class Point {
+    private int x;
+    private int y;
+    public Point(int x, int y) {
+        this.x = x;
+        this.y = y;
+    }
+    @Override
+    public boolean equals(Object other) {
+        if (!(other instanceof Point)) {
+            return false;
+        }
+        Point otherPoint = (Point) other;
+        return this.x == otherPoint.x &amp;&amp; this.y == otherPoint.y;
+    }
+    @Override
+    public int hashCode() {
+        int result = 17;
+        result = 31 * result + x;
+        result = 31 * result + y;
+        return result;
+    }
+}
+The equals method checks if the other object is an instance of Point and compares the x and y coordinates.
+In the hashCode() method, I use the technique of prime number multiply, where 17 is multiplied by the field x, 31 * the field y .This way, each point's hash code is unique and is based on the point's x and y values, fulfilling the requirement that if two objects are equal, then their hash codes must be equal as well.
+This way, if we store multiple Point objects in a HashSet, the HashSet will be able to properly determine when two Point objects are equal, and it will only store one of them.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Here is an example of how the Point class can be repaired to fix the fault and satisfy the mathematical relationship between equals() and hashCode():
+```java
+class Point {
+    private final int x;
+    private final int y;
+    public Point(int x, int y) {
+        this.x = x;
+        this.y = y;
+    }
+    @Override
+    public boolean equals(Object o) {
+        if (o == this) {
+            return true;
+        }
+        if (!(o instanceof Point)) {
+            return false;
+        }
+        Point p = (Point) o;
+        return p.x == x &amp;&amp; p.y == y;
+    }
+    @Override
+    public int hashCode() {
+        int result = 17;
+        result = 31 * result + x;
+        result = 31 * result + y;
+        return result;
+    }
+}
+```
+In this example, the equals() method checks if the passed object is the same object, then checks if the passed object is an instance of Point, and finally compares the x and y coordinates of the Point objects.
+The hashCode() method uses the common approach of combining the hash codes of the individual fields (x and y) using a prime number and the result of a previous calculation.
+When this class is used in the test case provided earlier, it should pass all the asserts, meaning that it's fixed the problem and satisfy the general contract.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Here is an example of how the Point class can be repaired to fix the fault:
+```
+class Point {
+    int x, y;
+    public Point(int x, int y) {
+        this.x = x;
+        this.y = y;
+    }
+    @Override
+    public boolean equals(Object obj) {
+        if (obj == this) {
+            return true;
+        }
+        if (!(obj instanceof Point)) {
+            return false;
+        }
+        Point p = (Point) obj;
+        return p.x == x &amp;&amp; p.y == y;
+    }
+    @Override
+    public int hashCode() {
+        return Objects.hash(x, y);
+    }
+}
+```
+In this example, the Point class overrides the `hashCode()` method and uses the `Objects.hash()` method to generate a hash code based on the x and y values of the Point objects. The `Objects.hash()` method generates a hash code based on the values of all the parameters passed to it. This ensures that if two Point objects are equal, they will have the same hash code and can be stored in a Collection structure such as HashSet without any problem.
+Note that the use of the `Objects.hash()` method is available since Java 7. If you're using an older version of Java, you can implement your own hash function using a similar approach.
+</t>
+  </si>
+  <si>
+    <t>To repair the Point class and fix the fault, the programmer should override both the `equals()` and `hashCode()` methods. The `equals()` method should be used to determine if two Point objects are equal, and the `hashCode()` method should return a unique hash code for each Point object. 
+Here is an example of how to override the `equals()` and `hashCode()` methods in the Point class:
+```
+class Point {
+    private int x;
+    private int y;
+    public Point(int x, int y) {
+        this.x = x;
+        this.y = y;
+    }
+    @Override
+    public boolean equals(Object o) {
+        if (o == this) return true;
+        if (!(o instanceof Point)) return false;
+        Point p = (Point) o;
+        return p.x == x &amp;&amp; p.y == y;
+    }
+    @Override
+    public int hashCode() {
+        int result = 17;
+        result = 31 * result + x;
+        result = 31 * result + y;
+        return result;
+    }
+}
+```
+It is also important to keep in mind that if the equals method is changed, the hashCode method should also be updated accordingly.</t>
+  </si>
+  <si>
+    <t>Here's one way to repair the Point class to fix the fault:
+```
+public class Point {
+    private int x;
+    private int y;
+    public Point(int x, int y) {
+        this.x = x;
+        this.y = y;
+    }
+    @Override
+    public boolean equals(Object o) {
+        if (o == this) return true;
+        if (!(o instanceof Point)) return false;
+        Point p = (Point) o;
+        return p.x == x &amp;&amp; p.y == y;
+    }
+    @Override
+    public int hashCode() {
+        int result = 17;
+        result = 31 * result + x;
+        result = 31 * result + y;
+        return result;
+    }
+}
+```
+Note that in the above example, We are using the fields x and y to calculate the hashCode, this is because fields used in equals() method should also be used to calculate hashCode() method.</t>
+  </si>
+  <si>
+    <t>Rewrite your JUnit test as an appropriate JUnit theory. Evaluate it with suitable DataPoints.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To rewrite the JUnit test as a JUnit theory, we can use the @Theory annotation and the @DataPoints annotation to specify a set of data points that will be used to evaluate the theory.
+Here is the revised JUnit test:
+import org.junit.experimental.theories.DataPoint;
+import org.junit.experimental.theories.Theories;
+import org.junit.experimental.theories.Theory;
+import org.junit.runner.RunWith;
+import static org.junit.Assert.*;
+@RunWith(Theories.class)
+public class PointTest {
+  @DataPoint
+  public static Point p1 = new Point(1, 2);
+  @DataPoint
+  public static Point p2 = new Point(1, 2);
+  @DataPoint
+  public static Point p3 = new Point(3, 4);
+  @Theory
+  public void testEqualsAndHashCode(Point p1, Point p2) {
+    assertTrue(p1.equals(p2));
+    assertTrue(p1.hashCode() == p2.hashCode());
+  }
+}
+In this revised test, the @DataPoint annotation is used to define three Point objects that will be used as data points for the theory. The theory itself is defined using the @Theory annotation and takes two Point objects as arguments. The theory asserts that if two Point objects are equal (as determined by the equals() method), then their hashCode() values must also be equal.
+To evaluate the theory, JUnit will generate a set of test cases using the data points defined in the test class. For each test case, JUnit will pass two Point objects to the theory and evaluate the assertions. If any of the assertions fail, the theory will be considered to have failed.
+In this case, since the Point class has been repaired and the hashCode() method is properly implemented, the theory should pass for all test cases.
+</t>
+  </si>
+  <si>
+    <t>When overriding the equals() method in a class, it is generally considered a best practice to also override the hashCode() method. This is because hashCode() and equals() are typically used together in data structures such as HashMap and HashSet. If two objects are equal according to the equals() method, they should have the same hash code. Conversely, two objects with the same hash code are not necessarily equal.
+Here is an example of a JUnit theory that tests the equals() and hashCode() methods of a Point class:
+import org.junit.experimental.theories.DataPoints;
+import org.junit.experimental.theories.Theories;
+import org.junit.experimental.theories.Theory;
+import org.junit.runner.RunWith;
+import static org.junit.Assert.*;
+@RunWith(Theories.class)
+public class PointTest {
+    @DataPoints
+    public static Point[] dataPoints = {
+        new Point(0, 0),
+        new Point(1, 1),
+        new Point(2, 2),
+        new Point(-1, -1)
+    };
+    @Theory
+    public void testEquals(Point p1, Point p2) {
+        assertTrue(p1.equals(p2) == (p1.x == p2.x &amp;&amp; p1.y == p2.y));
+    }
+    @Theory
+    public void testHashCode(Point p1, Point p2) {
+        if (p1.equals(p2)) {
+            assertTrue(p1.hashCode() == p2.hashCode());
+        }
+    }
+}
+In this example, the Point class has x and y fields, and the equals() method compares the fields for equality. The testEquals() method tests that the equals() method is implemented correctly by comparing the fields of the two Point objects. The testHashCode() method tests that the hashCode() method is implemented correctly by ensuring that two Point objects with the same x and y fields have the same hash code.
+You can also have custom datapoints as well as use other JUnit annotation like Assume &amp; Before to prepare the test data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Here is an example of the JUnit test from (c) rewritten as a JUnit theory using appropriate DataPoints:
+```java
+import static org.junit.Assert.*;
+import org.junit.experimental.theories.DataPoints;
+import org.junit.experimental.theories.Theories;
+import org.junit.experimental.theories.Theory;
+import org.junit.runner.RunWith;
+import java.util.HashSet;
+import java.util.Set;
+@RunWith(Theories.class)
+public class PointTheoryTest {
+    @DataPoints
+    public static Point[] pointData() {
+        return new Point[]{
+                new Point(1, 2),
+                new Point(3, 4),
+                new Point(5, 6)
+        };
+    }
+    @Theory
+    public void equalsAndHashCode(Point p1, Point p2) {
+        // Assert that p1 and p2 are equal according to the equals() method
+        assertTrue(p1.equals(p2));
+        // Assert that p1 and p2 have the same hash code
+        assertEquals(p1.hashCode(), p2.hashCode());
+        // Create a HashSet and add p1 and p2 to it
+        Set&lt;Point&gt; set = new HashSet&lt;Point&gt;();
+        set.add(p1);
+        set.add(p2);
+        // Assert that the HashSet contains only one Point
+        assertEquals(1, set.size());
+    }
+}
+```
+In this example, the test method is annotated with the `@Theory` annotation, indicating that it is a theory, and it takes two `Point` objects as parameters. The `@DataPoints` annotation is used to define an array of Point objects that will be used as the data points for the theory. The test asserts that the two `Point` objects passed as parameters are equal, have the same hashCode, and that when added to a set, the set only contains one element. Since it uses the @Theory annotation, JUnit will automatically run the test for all possible combinations of the data points.
+It's worth noting that the test passed in (c) is checking that the Point class is not following the contract, that's why it's checking for different hashCodes and not equal one. In this case, the test is checking that the Point class is following the contract, that's why it's checking for the same hashCodes and only one element in the set.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Here is an example of how the JUnit test can be rewritten as a JUnit theory with appropriate DataPoints:
+```
+import org.junit.experimental.theories.DataPoints;
+import org.junit.experimental.theories.Theories;
+import org.junit.experimental.theories.Theory;
+import org.junit.runner.RunWith;
+import java.util.Objects;
+class Point {
+    int x, y;
+    public Point(int x, int y) {
+        this.x = x;
+        this.y = y;
+    }
+    @Override
+    public boolean equals(Object obj) {
+        if (obj == this) {
+            return true;
+        }
+        if (!(obj instanceof Point)) {
+            return false;
+        }
+        Point p = (Point) obj;
+        return p.x == x &amp;&amp; p.y == y;
+    }
+    @Override
+    public int hashCode() {
+        return Objects.hash(x, y);
+    }
+}
+@RunWith(Theories.class)
+public class PointTest {
+    @DataPoints
+    public static Point[] points() {
+        return new Point[]{new Point(1, 2), new Point(3, 4), new Point(5, 6), new Point(7, 8)};
+    }
+    @Theory
+    public void testHashCode(Point p1, Point p2) {
+        if (p1.equals(p2)) {
+            assertEquals(p1.hashCode(), p2.hashCode());
+        }
+    }
+}
+```
+This test uses JUnit theories, which allow to test the same method with multiple sets of inputs. The `@DataPoints` annotation is used to define a set of input data. The `@Theory` annotation is used to specify that a method should be run as a theory. 
+In this case, the test uses the `points()` method, which returns an array of Point objects, as the DataPoints. The `testHashCode()` method is run for all possible combinations of the Point objects in the array, and it checks if the hashCode() method returns the same value for two Point objects if they are equals.
+This theory test is more robust than the previous one as it will test the hashCode() method for all the combinations of the Point objects in the array which ensures that the hashCode() method is working correctly for all possible inputs.
+</t>
+  </si>
+  <si>
+    <t>To rewrite the JUnit test as a theory, the @Theory annotation should be used instead of the @Test annotation, and the test method should be parameterized with DataPoints.
+Here is an example of how the test for the Point class's equals() and hashCode() methods could be written as a theory:
+```
+import org.junit.experimental.theories.DataPoints;
+import org.junit.experimental.theories.Theories;
+import org.junit.experimental.theories.Theory;
+import org.junit.runner.RunWith;
+@RunWith(Theories.class)
+public class PointTest {
+    @DataPoints
+    public static Point[] dataPoints = { new Point(1, 2), new Point(3, 4), new Point(5, 6) };
+    @Theory
+    public void testEqualsAndHashCode(Point p1, Point p2) {
+        // Test that the equals() method is consistent
+        assertEquals(p1.equals(p2), p1.equals(p2));
+        assertEquals(p1.equals(p2), p2.equals(p1));
+        // Test that the hashCode() method is consistent with equals()
+        if (p1.equals(p2)) {
+            assertEquals(p1.hashCode(), p2.hashCode());
+        }
+    }
+}
+```
+In this example, the test method is parameterized with two Point objects, p1 and p2. The theory is that for any two Point objects, if they are equal according to the equals() method, then their hashCode() method should return the same value. The @DataPoints annotation is used to specify an array of Point objects to be used as the inputs for the theory.
+This test can be run by the JUnit test runner, and it will automatically generate test cases by selecting all possible combinations of the data points.</t>
+  </si>
+  <si>
+    <t>```java
+import org.junit.experimental.theories.DataPoints;
+import org.junit.experimental.theories.Theories;
+import org.junit.experimental.theories.Theory;
+import org.junit.runner.RunWith;
+@RunWith(Theories.class)
+public class PointTest {
+    @DataPoints
+    public static Point[] dataPoints = {new Point(1, 2), new Point(3, 4), new Point(5, 6)};
+    @Theory
+    public void testEquals(Point point1, Point point2) {
+        if (point1.equals(point2)) {
+            assertTrue(point1.hashCode() == point2.hashCode());
+        }
+    }
+}
+```
+This JUnit test uses the `@RunWith(Theories.class)` annotation to run the test as a theory, and the `@DataPoints` annotation to define the data points for the theory. In this case, the data points are instances of the `Point` class. The `testEquals` method is annotated with `@Theory`, which tells JUnit to run the method for each combination of data points.
+The method checks if the `equals()` method returns true for two `Point` instances, it also checks that the `hashCode()` method returns the same value for both instances.
+The test will be run for each possible pair of data points defined in the `dataPoints` array, 3*3 =9 times.</t>
+  </si>
+  <si>
+    <t>Replace each occurrence of a set with a list in the JUnit theory removeThenAddDoesNotChangeSet. Is the resulting theory valid or invalid? How many of the tests that pass the precondition also pass the postcondition? Explain.</t>
+  </si>
+  <si>
+    <t>It is not possible for me to accurately answer this question without more information about the JUnit theory "removeThenAddDoesNotChangeSet" and the context in which it is being used.
+In general, replacing a set with a list in a JUnit theory may result in the theory becoming invalid, depending on how the set and list are used in the theory. If the set and list are used in ways that are not interchangeable, such as using set-specific methods on a list, then the theory may become invalid.
+Without knowing more about the theory and the specific replacements being made, it is not possible to determine how many of the tests that pass the precondition will also pass the postcondition. It is also not possible to determine whether the resulting theory will be valid or invalid.</t>
+  </si>
+  <si>
+    <t>It's not clear from the information provided what the original "theory removeThenAddDoesNotChangeSet" looks like, so it's difficult to say whether the resulting theory would be valid or invalid.
+If the original theory tests that removing an element from a set followed by adding the same element back to the set results in the set remaining unchanged, then replacing each occurrence of "set" with "list" would make the theory invalid. This is because in Java, sets are implemented as collections that do not allow duplicate elements, while lists do allow duplicate elements. Therefore, adding an element back to a list after removing it would result in the element being present twice, whereas it would not be present at all if it were a set.
+As for the number of tests that pass the precondition and also pass the postcondition, it would depend on the specific tests included in the original theory. If the tests involve adding and removing elements in such a way that the list would not end up with duplicate elements, then all of the tests would still pass. However, if the tests involve adding and removing elements in such a way that duplicate elements would be introduced to the list, then none of the tests would pass.
+It would be best to check each test and review the expected behavior, also changing the asserts or postcondition in order to reflect that you are testing with a list instead of set.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It is difficult to determine the validity of the resulting theory and the number of tests that pass the precondition also pass the postcondition without more information about the specific JUnit theory "removeThenAddDoesNotChangeSet" and the context in which it is being used. In general, replacing a set with a list in a JUnit theory would likely cause the theory to become invalid, as the behavior of sets and lists are not the same in Java. Additionally, the specific tests that pass the precondition and postcondition would depend on the implementation of the theory and the specific sets and lists being used.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It depends on the specific implementation of the theory and the methods being used. In general, replacing a set with a list in the theory would likely result in the theory being invalid, as the behavior of sets and lists are different in Java. Sets are designed to not allow duplicate elements, while lists can have duplicate elements. This would change the behavior of the methods being tested and could cause the theory to fail.
+As for the number of tests that pass the precondition and also pass the postcondition, it would depend on the specific implementation of the theory and the methods being used. Without more information, it is not possible to determine how many tests would pass both the precondition and postcondition.
+</t>
+  </si>
+  <si>
+    <t>It is not possible to determine if the resulting theory is valid or invalid without more information on the specific implementation of the JUnit theory "removeThenAddDoesNotChangeSet." 
+In order to determine if the tests pass the precondition and postcondition, one would need to see the specific test cases being run and the expected results.
+In general, replacing a set with a list in a JUnit theory could change the behavior of the tests, as sets and lists have different characteristics and methods. Sets do not allow duplicate elements and have no defined order, while lists do allow duplicate elements and have a defined order. This means that the tests would have to be re-written or adapted to account for these differences, and it's possible that the original tests would no longer pass the precondition or postcondition.</t>
+  </si>
+  <si>
+    <t>It is not possible for me to determine whether the resulting theory is valid or invalid without more information about the specific JUnit theory in question, as well as the specific set and list implementations being used.
+However, in general, replacing a set with a list in a JUnit theory could potentially make the theory invalid. This is because sets and lists have different characteristics and behaviors. Sets do not allow duplicate elements, while lists do. Sets are typically unordered, while lists have a specific order. Therefore, replacing a set with a list in a JUnit theory could change the behavior of the theory and the results of the tests.
+Without more information, I cannot determine how many of the tests that pass the precondition also pass the postcondition. The tests that pass the precondition may fail the postcondition and vice versa.</t>
+  </si>
+  <si>
+    <t>EPC</t>
+  </si>
+  <si>
+    <t>APC</t>
+  </si>
+  <si>
+    <t>Provies wrong idea about null checks</t>
+  </si>
+  <si>
+    <t>Misses the NPE case</t>
+  </si>
+  <si>
+    <t>Treats execution as failure</t>
+  </si>
+  <si>
+    <t>Could not find the case where every element occurs once</t>
+  </si>
+  <si>
+    <t>Did not talk about the initialization</t>
+  </si>
+  <si>
+    <t>Although correct, It did not executed the commented test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+As I am a text-based AI model I can't provide a screen printout or other evidence that my new program works. However, I can provide the modified code to fix the error:
+```
+public static int lastZero (int[] x) {
+    if (x == null) {
+        throw new NullPointerException("Input array is null");
+    }
+    int lastZeroIndex = -1;
+    for (int i = 0; i &lt; x.length; i++) {
+        if (x[i] == 0) {
+            lastZeroIndex = i;
+        }
+    }
+    return lastZeroIndex;
+}
+```
+In this new version of the code, I've added a null check at the beginning of the function to check if the input array is null. If it is, it throws a `NullPointerException` with an appropriate error message.
+This modification will handle the case where the input array is null, and it will prevent the program from throwing a `NullPointerException` and also it will give a proper error message to handle it.
+This modification will work on all test cases including the one where the input array is null and will give the expected output.
+</t>
+  </si>
+  <si>
+    <t>Finds the correct issue but fails to give a fix for the code</t>
+  </si>
+  <si>
+    <t>Talks about the empty cases but misses the null case</t>
+  </si>
+  <si>
+    <t>Did not talk about the commented test case</t>
+  </si>
+  <si>
+    <t>Finds a solution that the writer did not talk about</t>
+  </si>
+  <si>
+    <t>Treats error equavalent to exception</t>
+  </si>
+  <si>
+    <t>Explanation correct from the prespective that assumption about equality is not corrent to the tester</t>
+  </si>
+  <si>
+    <t>Wrong assumption by chatGPT</t>
+  </si>
+  <si>
+    <t>Writer differs in the sense that it is a part of JAVA API and cannot be modified without consequences in the client code all over the world. But chatGPT provides a fix that would be the soultion if it was written properly.</t>
+  </si>
+  <si>
+    <t>Talks about hashcode which the author missed</t>
+  </si>
+  <si>
+    <t>There will be no valid code solution</t>
+  </si>
+  <si>
+    <t>Talks about the problem in both equals()</t>
+  </si>
+  <si>
+    <t>Exception is treated as error</t>
+  </si>
+  <si>
+    <t>Also talks about design perspective</t>
+  </si>
+  <si>
+    <t>Just need to remove extends Point. Otherwise correctly provides solution in terms of composition</t>
+  </si>
+  <si>
+    <t>Talks about composition indirectly</t>
+  </si>
+  <si>
     <t>To demonstrate the problem with the Point class, let's first define the class:
-Copy code
 class Point {
   int x;
   int y;
@@ -4864,814 +5673,10 @@
 System.out.println(set.size());  // Outputs: 2</t>
   </si>
   <si>
-    <t>When you override the equals() method, it is generally recommended that you also override the hashCode() method, because the hashCode() method is used by certain collection classes (such as HashSet) to determine whether two objects are equal. If you override equals() but not hashCode(), then these collections may not behave as expected.
-Here's an example of how the Point class from Chapter 1 might be defective in this regard:
-class Point {
-    private int x;
-    private int y;
-    public Point(int x, int y) {
-        this.x = x;
-        this.y = y;
-    }
-    @Override
-    public boolean equals(Object o) {
-        if (o == this) return true;
-        if (!(o instanceof Point)) return false;
-        Point p = (Point) o;
-        return p.x == x &amp;&amp; p.y == y;
-    }
-}
-The above Point class overrides the equals() method to check for equality based on the x and y fields, but it does not override the hashCode() method. Therefore, if we try to use it as key in HashMap it will return error.
-Copy code
-    HashSet&lt;Point&gt; set = new HashSet&lt;&gt;();
-    set.add(new Point(1, 2));
-    set.add(new Point(3, 4));
-    set.add(new Point(1, 2)); 
-In this example, we are trying to add three Point objects to a HashSet. The first two Point objects have different x and y values, so they will be added to the set without any problem. However, the third Point object has the same x and y values as the first Point object, so equals() will return true when comparing the two. But HashSet uses the hashCode() method to determine whether two objects are equal, and since the Point class doesn't override hashCode(), the HashSet will treat the first and third Point objects as distinct, and therefore it will be added to the set, even though it's a duplicate.
-To fix this, you would need to override the hashCode() method in Point class, and implement it consistently with the equals() method.
-    @Override
-    public int hashCode() {
-        int result = 17;
-        result = 31 * result + x;
-        result = 31 * result + y;
-        return result;
-    }
-This would ensure that HashSet is able to correctly identify when two Point objects are equal and will prevent duplicate values from being added to the set.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the Point class overrides the equals() method but does not also override the hashCode() method, then instances of Point may not behave correctly when stored in a HashSet. For example, if two Point instances have the same x and y coordinates, the equals() method may return true for these instances, indicating that they are equal. However, the HashSet will use the hashCode() method to determine where to store the instances, and if the hashCode() method is not overridden, the HashSet will consider the instances to be different, even though the equals() method considers them to be equal. This can lead to unexpected behavior, such as the HashSet storing multiple copies of the same Point instance.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Here is an example of how the problem with the Point class from Chapter 1 can be demonstrated using a HashSet:
-```
-import java.util.HashSet;
-class Point {
-    int x, y;
-    public Point(int x, int y) {
-        this.x = x;
-        this.y = y;
-    }
-    @Override
-    public boolean equals(Object obj) {
-        if (obj == this) {
-            return true;
-        }
-        if (!(obj instanceof Point)) {
-            return false;
-        }
-        Point p = (Point) obj;
-        return p.x == x &amp;&amp; p.y == y;
-    }
-}
-public class Main {
-    public static void main(String[] args) {
-        HashSet&lt;Point&gt; set = new HashSet&lt;Point&gt;();
-        Point p1 = new Point(1, 2);
-        Point p2 = new Point(1, 2);
-        set.add(p1);
-        set.add(p2);
-        System.out.println(set.size()); // prints 2 instead of 1
-    }
-}
-```
-In this example, two Point objects (p1 and p2) are created with the same x and y values, and they are added to a HashSet. Since the Point class does not override the hashCode() method, the HashSet uses the default implementation of the Object class, which generates a unique hash code based on the memory address of the object. As a result, the HashSet considers p1 and p2 to be different objects and does not remove the duplicate. This causes the set.size() to return 2 instead of 1.
-To fix this problem, the Point class should override the hashCode() method and implement a proper hash function based on the x and y values of the Point objects.
-</t>
-  </si>
-  <si>
-    <t>If the Point class has not overridden the hashCode() method, and the equals() method is used to compare two Point objects in a HashSet, the HashSet may not properly identify the two Point objects as equal. This can cause issues with adding, removing, or searching for the Point objects in the HashSet.
-For example, if we create two Point objects with the same x and y coordinates, the HashSet may not recognize them as equal and add them both to the set. 
-```
-HashSet&lt;Point&gt; pointSet = new HashSet&lt;&gt;();
-Point point1 = new Point(1, 2);
-Point point2 = new Point(1, 2);
-pointSet.add(point1);
-pointSet.add(point2);
-System.out.println(pointSet.size());  // Output: 2
-```
-This is because the HashSet uses the hashCode() method to determine where to store the object in its internal data structure and also uses it to compare objects for equality. If the hashCode() method is not overridden, the HashSet will use the default implementation which may not be appropriate for the Point class.</t>
-  </si>
-  <si>
-    <t>Here is an example of the problem with the Point class from Chapter 1 when using a HashSet:
-```
-import java.util.HashSet;
-public class Main {
-    public static void main(String[] args) {
-        HashSet&lt;Point&gt; points = new HashSet&lt;Point&gt;();
-        Point p1 = new Point(1, 2);
-        Point p2 = new Point(1, 2);
-        points.add(p1);
-        points.add(p2);
-        System.out.println(points.size()); // prints "2" instead of "1"
-    }
-}
-class Point {
-    int x;
-    int y;
-    Point(int x, int y) {
-        this.x = x;
-        this.y = y;
-    }
-    // equals() method is not overridden
-}
-```
-In this example, we create a HashSet of Point objects and add two Point objects, p1 and p2, that have the same x and y values. However, since the Point class does not override the equals() method, the HashSet considers these two Point objects to be distinct and adds both to the set. As a result, the size of the set is 2 instead of 1. 
-This problem could be avoided if the Point class overrides the equals() method and hashCode() method, so that two Point objects with the same x and y values are considered equal by the HashSet and only one is added to the set.</t>
-  </si>
-  <si>
-    <t>Write down the mathematical relationship required between equals() and hashCode().</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The equals() and hashCode() methods are used together in Java to implement the contract of object equality, as defined by the Objects.equals() and Objects.hash() methods.
-According to this contract, if two objects are equal (as determined by the equals() method), then their hashCode() values must be equal as well. Conversely, if two objects have equal hashCode() values, they do not necessarily have to be equal (as determined by the equals() method).
-In other words, the relationship between equals() and hashCode() is defined by the following mathematical relationship:
-if a.equals(b) then a.hashCode() == b.hashCode()
-This relationship is important because it allows objects to be stored and retrieved efficiently in common data structures such as HashMap, HashSet, and Hashtable.
-It's also worth noting that the hashCode() method should be implemented such that it returns the same value for two equal objects every time it is called on those objects, as long as the objects are not modified. This allows the hashCode() method to be used as a way to identify unique objects and helps to ensure the efficiency of data structures that rely on it.
-</t>
-  </si>
-  <si>
-    <t>When overriding the equals() method in a class, it is generally recommended to also override the hashCode() method, as the two methods should have a consistent relationship. Specifically, if two objects are equal according to the equals() method, then calling hashCode() on each of the objects must produce the same integer result. Additionally, if two objects are unequal according to the equals() method, it is not required but preferable that calling hashCode() on each of the objects produces distinct integer results.
-To put it mathematically:
-- If a.equals(b) returns true, then a.hashCode() == b.hashCode() must also return true.
-- If a.equals(b) returns false, then it is not necessary that a.hashCode() == b.hashCode() returns false, but the distinct hashCode would be preferred.
-It's worth noting that in practice, it's hard to guarantee that hashCode is distinct for all unequal objects, but it's more important that it is consistent with the equals.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-The mathematical relationship required between the equals() and hashCode() methods is known as the "general contract" and it states that if two objects are equal, according to the equals(Object) method, then calling the hashCode() method on each of the two objects must produce the same integer result. 
-Additionally, it is not required but strongly recommended that if two objects are unequal according to the equals(java.lang.Object) method, then calling the hashCode() method on each of the two objects should produce distinct integer results. In other words, the hashCode() method should return distinct values for distinct objects.
-It's worth noting that this relationship is not symmetric, meaning that if two objects have the same hashCode() it doesn't mean they are equal.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-The relationship between the `equals()` and `hashCode()` methods in Java is defined by the following contract:
-- If two objects are equal according to the `equals(Object)` method, then calling the `hashCode()` method on each of the two objects must produce the same integer result.
-- It is not required that if two objects are unequal according to the `equals(Object)` method, then calling the `hashCode()` method on each of the two objects must produce distinct integer results. However, the programmer should be aware that producing distinct integer results for unequal objects may improve the performance of hash tables.
-In other words, if two objects are equal, they must have the same hash code. However, if two objects have different hash codes, they may still be equal. Therefore, it is important to make sure that the hash code is based on the same attributes used by the equals method.
-</t>
-  </si>
-  <si>
-    <t>When overriding the equals() method, it is generally recommended to also override the hashCode() method. This is because the hashCode() method is used by common Collection structures such as HashSet to determine if two objects are equal, and if the hashCode() method is not overridden, it may not return the correct value.
-The mathematical relationship required between equals() and hashCode() is that if two objects are equal according to the equals(Object) method, then calling the hashCode() method on each of the two objects must produce the same integer result. This means that if two objects are equal then their hashcode should be same.</t>
-  </si>
-  <si>
-    <t>(a) When overriding the equals() method, it is generally recommended to also override the hashCode() method. This is because the hashCode method is used by certain collection classes (such as HashSet and HashMap) to determine where to store an object, and if the hashCode method is not overridden, these classes may not be able to properly store instances of the class.
-(b) The mathematical relationship required between equals() and hashCode() is that if two objects are equal according to the equals(Object) method, then calling the hashCode method on each of the two objects must produce the same integer result. This means that if a.equals(b) returns true, then a.hashCode() == b.hashCode() must also be true. Additionally, it is required that if two objects are not equal according to the equals(Object) method, then calling the hashCode method on each of the two objects must produce distinct integer results, unless the two objects are null.</t>
-  </si>
-  <si>
-    <t>Write a simple JUnit test to show that Point objects do not enjoy this property.</t>
-  </si>
-  <si>
-    <t>Here is a simple JUnit test that demonstrates that the Point class does not satisfy the required relationship between equals() and hashCode():
-import org.junit.Test;
-import static org.junit.Assert.*;
-public class PointTest {
-  @Test
-  public void testEqualsAndHashCode() {
-    Point p1 = new Point(1, 2);
-    Point p2 = new Point(1, 2);
-    Point p3 = new Point(3, 4);
-    assertTrue(p1.equals(p2));
-    assertFalse(p1.hashCode() == p2.hashCode());  // Fails
-  }
-}
-In this test, we create two Point objects, p1 and p2, which are equal (as determined by the equals() method). However, the test fails because the hashCode() values of p1 and p2 are not equal, indicating that the hashCode() method is not properly implemented.
-To fix this issue, the hashCode() method in the Point class needs to be overridden as described in the previous answer. Once the hashCode() method is properly implemented, the test should pass.</t>
-  </si>
-  <si>
-    <t>Here's an example of a JUnit test that demonstrates the issue with the Point class not properly overriding the hashCode() method:
-import static org.junit.Assert.*;
-import java.util.HashSet;
-import org.junit.Test;
-public class PointTest {
-    @Test
-    public void testHashCode() {
-        Point p1 = new Point(1, 2);
-        Point p2 = new Point(1, 2);
-        // assert that p1 and p2 are equal
-        assertTrue(p1.equals(p2));
-        HashSet&lt;Point&gt; set = new HashSet&lt;&gt;();
-        set.add(p1);
-        set.add(p2);
-        // if hashCode() is not properly implemented, the set will contain 2 elements
-        assertEquals(1, set.size());
-    }
-}
-This test creates two Point objects, p1 and p2, that are equal to each other (have the same x and y values). It then adds both of these objects to a HashSet, and checks the size of the set to see if the hashCode() method is properly implemented. If the hashCode() method is not properly overridden, the set will contain 2 elements, because the HashSet considers the two Point objects to be different. If the hashCode() method is correctly overridden, the set will contain only 1 element, because the two Point objects are considered to be equal.
-It is worth noting that if the equals method is overridden and not symmetric, reflexive and transitive, the same issue can appear.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Here is an example of a JUnit test that demonstrates that Point objects do not have the proper relationship between equals() and hashCode():
-```
-import static org.junit.Assert.*;
-import java.util.HashSet;
-import java.util.Set;
-import org.junit.Test;
-public class PointTest {
-    @Test
-    public void testEqualsAndHashCode() {
-        Point p1 = new Point(1, 2);
-        Point p2 = new Point(1, 2);
-        // Assert that p1 and p2 are equal according to the equals() method
-        assertTrue(p1.equals(p2));
-        // Assert that p1 and p2 have different hash codes
-        assertNotEquals(p1.hashCode(), p2.hashCode());
-        // Create a HashSet and add p1 and p2 to it
-        Set&lt;Point&gt; set = new HashSet&lt;Point&gt;();
-        set.add(p1);
-        set.add(p2);
-        // Assert that the HashSet only contains one Point
-        // even though p1 and p2 are equal
-        assertEquals(1, set.size());
-    }
-}
-```
-This test creates two Point objects, p1 and p2, that have the same x and y coordinates. The test then asserts that the equals() method considers p1 and p2 to be equal, but that their hash codes are different. Finally, the test adds p1 and p2 to a HashSet, and asserts that the HashSet only contains one Point, even though p1 and p2 are equal. This behavior is caused by the Point class not overriding the hashCode() method, and demonstrate that the Point objects do not have the proper relationship between equals() and hashCode().
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Here is a simple JUnit test that demonstrates that Point objects do not satisfy the contract between `equals()` and `hashCode()`:
-```
-import org.junit.Test;
-import java.util.HashSet;
-import static org.junit.Assert.*;
-class Point {
-    int x, y;
-    public Point(int x, int y) {
-        this.x = x;
-        this.y = y;
-    }
-    @Override
-    public boolean equals(Object obj) {
-        if (obj == this) {
-            return true;
-        }
-        if (!(obj instanceof Point)) {
-            return false;
-        }
-        Point p = (Point) obj;
-        return p.x == x &amp;&amp; p.y == y;
-    }
-}
-public class PointTest {
-    @Test
-    public void testHashCode() {
-        Point p1 = new Point(1, 2);
-        Point p2 = new Point(1, 2);
-        assertTrue(p1.equals(p2));
-        assertFalse(p1.hashCode() == p2.hashCode());
-    }
-}
-```
-This test creates two Point objects (p1 and p2) with the same x and y values and checks if they are equal using the `equals()` method. Then it checks if the hash codes of these two objects are the same. Since the Point class does not override the `hashCode()` method, it uses the default implementation of the `Object` class which generates a unique hash code based on the memory address of the object. As a result, the test fails, indicating that the Point objects do not satisfy the contract between `equals()` and `hashCode()`.
-</t>
-  </si>
-  <si>
-    <t>```
-import static org.junit.Assert.*;
-import java.util.HashSet;
-import org.junit.Test;
-public class PointTest {
-    @Test
-    public void testEqualityInHashSet() {
-        Point p1 = new Point(1, 2);
-        Point p2 = new Point(1, 2);
-        HashSet&lt;Point&gt; set = new HashSet&lt;Point&gt;();
-        set.add(p1);
-        assertFalse(set.contains(p2));
-    }
-}
-```
-In this JUnit test, two Point objects `p1` and `p2` are created with the same x and y coordinates. These objects are added to a HashSet, and it is asserted that the HashSet does not contain the second Point object `p2`. This is because the `equals()` and `hashCode()` methods have not been overridden, so the HashSet uses the default implementation which only considers objects to be equal if they are the same instance.</t>
-  </si>
-  <si>
-    <t>Here is a simple JUnit test that demonstrates that Point objects do not have the property of being able to be stored in common Collection structures such as HashSet when the equals() method is overridden without also overriding the hashCode() method:
-```
-import static org.junit.Assert.*;
-import java.util.HashSet;
-import org.junit.Test;
-public class PointTest {
-    @Test
-    public void testHashCodeProperty() {
-        Point p1 = new Point(1, 2);
-        Point p2 = new Point(1, 2);
-        HashSet&lt;Point&gt; set = new HashSet&lt;Point&gt;();
-        set.add(p1);
-        // This should return false, since p1 and p2 are equal but have different hash codes
-        assertFalse(set.contains(p2));
-    }
-}
-```
-Note that this is just an example and you need to import the class point in your test class.</t>
-  </si>
-  <si>
-    <t>Repair the Point class to fix the fault.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To repair the fault in the Point class, the hashCode() method needs to be overridden as follows:
-class Point {
-  int x;
-  int y;
-  public Point(int x, int y) {
-    this.x = x;
-    this.y = y;
-  }
-  // Overrides equals() method
-  public boolean equals(Object o) {
-    if (!(o instanceof Point)) return false;
-    Point p = (Point) o;
-    return p.x == x &amp;&amp; p.y == y;
-  }
-  // Overrides hashCode() method
-  public int hashCode() {
-    return Objects.hash(x, y);
-  }
-}
-With the hashCode() method overridden, the Point class will now satisfy the required relationship between equals() and hashCode() and can be used with common data structures such as HashMap, HashSet, and Hashtable without any issues.
-It's worth noting that the hashCode() method implementation shown above uses the Objects.hash() utility method to compute the hash code for the Point object. This method takes the x and y fields of the Point object as arguments and returns a hash code that is based on their values. This ensures that the hash code is consistent with the definition of equality for the Point class (as defined by the equals() method).
-</t>
-  </si>
-  <si>
-    <t>Here's an example of how you might repair the Point class to properly override the equals() and hashCode() methods:
-class Point {
-    private int x;
-    private int y;
-    public Point(int x, int y) {
-        this.x = x;
-        this.y = y;
-    }
-    @Override
-    public boolean equals(Object other) {
-        if (!(other instanceof Point)) {
-            return false;
-        }
-        Point otherPoint = (Point) other;
-        return this.x == otherPoint.x &amp;&amp; this.y == otherPoint.y;
-    }
-    @Override
-    public int hashCode() {
-        int result = 17;
-        result = 31 * result + x;
-        result = 31 * result + y;
-        return result;
-    }
-}
-The equals method checks if the other object is an instance of Point and compares the x and y coordinates.
-In the hashCode() method, I use the technique of prime number multiply, where 17 is multiplied by the field x, 31 * the field y .This way, each point's hash code is unique and is based on the point's x and y values, fulfilling the requirement that if two objects are equal, then their hash codes must be equal as well.
-This way, if we store multiple Point objects in a HashSet, the HashSet will be able to properly determine when two Point objects are equal, and it will only store one of them.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Here is an example of how the Point class can be repaired to fix the fault and satisfy the mathematical relationship between equals() and hashCode():
-```java
-class Point {
-    private final int x;
-    private final int y;
-    public Point(int x, int y) {
-        this.x = x;
-        this.y = y;
-    }
-    @Override
-    public boolean equals(Object o) {
-        if (o == this) {
-            return true;
-        }
-        if (!(o instanceof Point)) {
-            return false;
-        }
-        Point p = (Point) o;
-        return p.x == x &amp;&amp; p.y == y;
-    }
-    @Override
-    public int hashCode() {
-        int result = 17;
-        result = 31 * result + x;
-        result = 31 * result + y;
-        return result;
-    }
-}
-```
-In this example, the equals() method checks if the passed object is the same object, then checks if the passed object is an instance of Point, and finally compares the x and y coordinates of the Point objects.
-The hashCode() method uses the common approach of combining the hash codes of the individual fields (x and y) using a prime number and the result of a previous calculation.
-When this class is used in the test case provided earlier, it should pass all the asserts, meaning that it's fixed the problem and satisfy the general contract.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Here is an example of how the Point class can be repaired to fix the fault:
-```
-class Point {
-    int x, y;
-    public Point(int x, int y) {
-        this.x = x;
-        this.y = y;
-    }
-    @Override
-    public boolean equals(Object obj) {
-        if (obj == this) {
-            return true;
-        }
-        if (!(obj instanceof Point)) {
-            return false;
-        }
-        Point p = (Point) obj;
-        return p.x == x &amp;&amp; p.y == y;
-    }
-    @Override
-    public int hashCode() {
-        return Objects.hash(x, y);
-    }
-}
-```
-In this example, the Point class overrides the `hashCode()` method and uses the `Objects.hash()` method to generate a hash code based on the x and y values of the Point objects. The `Objects.hash()` method generates a hash code based on the values of all the parameters passed to it. This ensures that if two Point objects are equal, they will have the same hash code and can be stored in a Collection structure such as HashSet without any problem.
-Note that the use of the `Objects.hash()` method is available since Java 7. If you're using an older version of Java, you can implement your own hash function using a similar approach.
-</t>
-  </si>
-  <si>
-    <t>To repair the Point class and fix the fault, the programmer should override both the `equals()` and `hashCode()` methods. The `equals()` method should be used to determine if two Point objects are equal, and the `hashCode()` method should return a unique hash code for each Point object. 
-Here is an example of how to override the `equals()` and `hashCode()` methods in the Point class:
-```
-class Point {
-    private int x;
-    private int y;
-    public Point(int x, int y) {
-        this.x = x;
-        this.y = y;
-    }
-    @Override
-    public boolean equals(Object o) {
-        if (o == this) return true;
-        if (!(o instanceof Point)) return false;
-        Point p = (Point) o;
-        return p.x == x &amp;&amp; p.y == y;
-    }
-    @Override
-    public int hashCode() {
-        int result = 17;
-        result = 31 * result + x;
-        result = 31 * result + y;
-        return result;
-    }
-}
-```
-It is also important to keep in mind that if the equals method is changed, the hashCode method should also be updated accordingly.</t>
-  </si>
-  <si>
-    <t>Here's one way to repair the Point class to fix the fault:
-```
-public class Point {
-    private int x;
-    private int y;
-    public Point(int x, int y) {
-        this.x = x;
-        this.y = y;
-    }
-    @Override
-    public boolean equals(Object o) {
-        if (o == this) return true;
-        if (!(o instanceof Point)) return false;
-        Point p = (Point) o;
-        return p.x == x &amp;&amp; p.y == y;
-    }
-    @Override
-    public int hashCode() {
-        int result = 17;
-        result = 31 * result + x;
-        result = 31 * result + y;
-        return result;
-    }
-}
-```
-Note that in the above example, We are using the fields x and y to calculate the hashCode, this is because fields used in equals() method should also be used to calculate hashCode() method.</t>
-  </si>
-  <si>
-    <t>Rewrite your JUnit test as an appropriate JUnit theory. Evaluate it with suitable DataPoints.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To rewrite the JUnit test as a JUnit theory, we can use the @Theory annotation and the @DataPoints annotation to specify a set of data points that will be used to evaluate the theory.
-Here is the revised JUnit test:
-import org.junit.experimental.theories.DataPoint;
-import org.junit.experimental.theories.Theories;
-import org.junit.experimental.theories.Theory;
-import org.junit.runner.RunWith;
-import static org.junit.Assert.*;
-@RunWith(Theories.class)
-public class PointTest {
-  @DataPoint
-  public static Point p1 = new Point(1, 2);
-  @DataPoint
-  public static Point p2 = new Point(1, 2);
-  @DataPoint
-  public static Point p3 = new Point(3, 4);
-  @Theory
-  public void testEqualsAndHashCode(Point p1, Point p2) {
-    assertTrue(p1.equals(p2));
-    assertTrue(p1.hashCode() == p2.hashCode());
-  }
-}
-In this revised test, the @DataPoint annotation is used to define three Point objects that will be used as data points for the theory. The theory itself is defined using the @Theory annotation and takes two Point objects as arguments. The theory asserts that if two Point objects are equal (as determined by the equals() method), then their hashCode() values must also be equal.
-To evaluate the theory, JUnit will generate a set of test cases using the data points defined in the test class. For each test case, JUnit will pass two Point objects to the theory and evaluate the assertions. If any of the assertions fail, the theory will be considered to have failed.
-In this case, since the Point class has been repaired and the hashCode() method is properly implemented, the theory should pass for all test cases.
-</t>
-  </si>
-  <si>
-    <t>When overriding the equals() method in a class, it is generally considered a best practice to also override the hashCode() method. This is because hashCode() and equals() are typically used together in data structures such as HashMap and HashSet. If two objects are equal according to the equals() method, they should have the same hash code. Conversely, two objects with the same hash code are not necessarily equal.
-Here is an example of a JUnit theory that tests the equals() and hashCode() methods of a Point class:
-import org.junit.experimental.theories.DataPoints;
-import org.junit.experimental.theories.Theories;
-import org.junit.experimental.theories.Theory;
-import org.junit.runner.RunWith;
-import static org.junit.Assert.*;
-@RunWith(Theories.class)
-public class PointTest {
-    @DataPoints
-    public static Point[] dataPoints = {
-        new Point(0, 0),
-        new Point(1, 1),
-        new Point(2, 2),
-        new Point(-1, -1)
-    };
-    @Theory
-    public void testEquals(Point p1, Point p2) {
-        assertTrue(p1.equals(p2) == (p1.x == p2.x &amp;&amp; p1.y == p2.y));
-    }
-    @Theory
-    public void testHashCode(Point p1, Point p2) {
-        if (p1.equals(p2)) {
-            assertTrue(p1.hashCode() == p2.hashCode());
-        }
-    }
-}
-In this example, the Point class has x and y fields, and the equals() method compares the fields for equality. The testEquals() method tests that the equals() method is implemented correctly by comparing the fields of the two Point objects. The testHashCode() method tests that the hashCode() method is implemented correctly by ensuring that two Point objects with the same x and y fields have the same hash code.
-You can also have custom datapoints as well as use other JUnit annotation like Assume &amp; Before to prepare the test data.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Here is an example of the JUnit test from (c) rewritten as a JUnit theory using appropriate DataPoints:
-```java
-import static org.junit.Assert.*;
-import org.junit.experimental.theories.DataPoints;
-import org.junit.experimental.theories.Theories;
-import org.junit.experimental.theories.Theory;
-import org.junit.runner.RunWith;
-import java.util.HashSet;
-import java.util.Set;
-@RunWith(Theories.class)
-public class PointTheoryTest {
-    @DataPoints
-    public static Point[] pointData() {
-        return new Point[]{
-                new Point(1, 2),
-                new Point(3, 4),
-                new Point(5, 6)
-        };
-    }
-    @Theory
-    public void equalsAndHashCode(Point p1, Point p2) {
-        // Assert that p1 and p2 are equal according to the equals() method
-        assertTrue(p1.equals(p2));
-        // Assert that p1 and p2 have the same hash code
-        assertEquals(p1.hashCode(), p2.hashCode());
-        // Create a HashSet and add p1 and p2 to it
-        Set&lt;Point&gt; set = new HashSet&lt;Point&gt;();
-        set.add(p1);
-        set.add(p2);
-        // Assert that the HashSet contains only one Point
-        assertEquals(1, set.size());
-    }
-}
-```
-In this example, the test method is annotated with the `@Theory` annotation, indicating that it is a theory, and it takes two `Point` objects as parameters. The `@DataPoints` annotation is used to define an array of Point objects that will be used as the data points for the theory. The test asserts that the two `Point` objects passed as parameters are equal, have the same hashCode, and that when added to a set, the set only contains one element. Since it uses the @Theory annotation, JUnit will automatically run the test for all possible combinations of the data points.
-It's worth noting that the test passed in (c) is checking that the Point class is not following the contract, that's why it's checking for different hashCodes and not equal one. In this case, the test is checking that the Point class is following the contract, that's why it's checking for the same hashCodes and only one element in the set.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Here is an example of how the JUnit test can be rewritten as a JUnit theory with appropriate DataPoints:
-```
-import org.junit.experimental.theories.DataPoints;
-import org.junit.experimental.theories.Theories;
-import org.junit.experimental.theories.Theory;
-import org.junit.runner.RunWith;
-import java.util.Objects;
-class Point {
-    int x, y;
-    public Point(int x, int y) {
-        this.x = x;
-        this.y = y;
-    }
-    @Override
-    public boolean equals(Object obj) {
-        if (obj == this) {
-            return true;
-        }
-        if (!(obj instanceof Point)) {
-            return false;
-        }
-        Point p = (Point) obj;
-        return p.x == x &amp;&amp; p.y == y;
-    }
-    @Override
-    public int hashCode() {
-        return Objects.hash(x, y);
-    }
-}
-@RunWith(Theories.class)
-public class PointTest {
-    @DataPoints
-    public static Point[] points() {
-        return new Point[]{new Point(1, 2), new Point(3, 4), new Point(5, 6), new Point(7, 8)};
-    }
-    @Theory
-    public void testHashCode(Point p1, Point p2) {
-        if (p1.equals(p2)) {
-            assertEquals(p1.hashCode(), p2.hashCode());
-        }
-    }
-}
-```
-This test uses JUnit theories, which allow to test the same method with multiple sets of inputs. The `@DataPoints` annotation is used to define a set of input data. The `@Theory` annotation is used to specify that a method should be run as a theory. 
-In this case, the test uses the `points()` method, which returns an array of Point objects, as the DataPoints. The `testHashCode()` method is run for all possible combinations of the Point objects in the array, and it checks if the hashCode() method returns the same value for two Point objects if they are equals.
-This theory test is more robust than the previous one as it will test the hashCode() method for all the combinations of the Point objects in the array which ensures that the hashCode() method is working correctly for all possible inputs.
-</t>
-  </si>
-  <si>
-    <t>To rewrite the JUnit test as a theory, the @Theory annotation should be used instead of the @Test annotation, and the test method should be parameterized with DataPoints.
-Here is an example of how the test for the Point class's equals() and hashCode() methods could be written as a theory:
-```
-import org.junit.experimental.theories.DataPoints;
-import org.junit.experimental.theories.Theories;
-import org.junit.experimental.theories.Theory;
-import org.junit.runner.RunWith;
-@RunWith(Theories.class)
-public class PointTest {
-    @DataPoints
-    public static Point[] dataPoints = { new Point(1, 2), new Point(3, 4), new Point(5, 6) };
-    @Theory
-    public void testEqualsAndHashCode(Point p1, Point p2) {
-        // Test that the equals() method is consistent
-        assertEquals(p1.equals(p2), p1.equals(p2));
-        assertEquals(p1.equals(p2), p2.equals(p1));
-        // Test that the hashCode() method is consistent with equals()
-        if (p1.equals(p2)) {
-            assertEquals(p1.hashCode(), p2.hashCode());
-        }
-    }
-}
-```
-In this example, the test method is parameterized with two Point objects, p1 and p2. The theory is that for any two Point objects, if they are equal according to the equals() method, then their hashCode() method should return the same value. The @DataPoints annotation is used to specify an array of Point objects to be used as the inputs for the theory.
-This test can be run by the JUnit test runner, and it will automatically generate test cases by selecting all possible combinations of the data points.</t>
-  </si>
-  <si>
-    <t>```java
-import org.junit.experimental.theories.DataPoints;
-import org.junit.experimental.theories.Theories;
-import org.junit.experimental.theories.Theory;
-import org.junit.runner.RunWith;
-@RunWith(Theories.class)
-public class PointTest {
-    @DataPoints
-    public static Point[] dataPoints = {new Point(1, 2), new Point(3, 4), new Point(5, 6)};
-    @Theory
-    public void testEquals(Point point1, Point point2) {
-        if (point1.equals(point2)) {
-            assertTrue(point1.hashCode() == point2.hashCode());
-        }
-    }
-}
-```
-This JUnit test uses the `@RunWith(Theories.class)` annotation to run the test as a theory, and the `@DataPoints` annotation to define the data points for the theory. In this case, the data points are instances of the `Point` class. The `testEquals` method is annotated with `@Theory`, which tells JUnit to run the method for each combination of data points.
-The method checks if the `equals()` method returns true for two `Point` instances, it also checks that the `hashCode()` method returns the same value for both instances.
-The test will be run for each possible pair of data points defined in the `dataPoints` array, 3*3 =9 times.</t>
-  </si>
-  <si>
-    <t>Replace each occurrence of a set with a list in the JUnit theory removeThenAddDoesNotChangeSet. Is the resulting theory valid or invalid? How many of the tests that pass the precondition also pass the postcondition? Explain.</t>
-  </si>
-  <si>
-    <t>It is not possible for me to accurately answer this question without more information about the JUnit theory "removeThenAddDoesNotChangeSet" and the context in which it is being used.
-In general, replacing a set with a list in a JUnit theory may result in the theory becoming invalid, depending on how the set and list are used in the theory. If the set and list are used in ways that are not interchangeable, such as using set-specific methods on a list, then the theory may become invalid.
-Without knowing more about the theory and the specific replacements being made, it is not possible to determine how many of the tests that pass the precondition will also pass the postcondition. It is also not possible to determine whether the resulting theory will be valid or invalid.</t>
-  </si>
-  <si>
-    <t>It's not clear from the information provided what the original "theory removeThenAddDoesNotChangeSet" looks like, so it's difficult to say whether the resulting theory would be valid or invalid.
-If the original theory tests that removing an element from a set followed by adding the same element back to the set results in the set remaining unchanged, then replacing each occurrence of "set" with "list" would make the theory invalid. This is because in Java, sets are implemented as collections that do not allow duplicate elements, while lists do allow duplicate elements. Therefore, adding an element back to a list after removing it would result in the element being present twice, whereas it would not be present at all if it were a set.
-As for the number of tests that pass the precondition and also pass the postcondition, it would depend on the specific tests included in the original theory. If the tests involve adding and removing elements in such a way that the list would not end up with duplicate elements, then all of the tests would still pass. However, if the tests involve adding and removing elements in such a way that duplicate elements would be introduced to the list, then none of the tests would pass.
-It would be best to check each test and review the expected behavior, also changing the asserts or postcondition in order to reflect that you are testing with a list instead of set.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It is difficult to determine the validity of the resulting theory and the number of tests that pass the precondition also pass the postcondition without more information about the specific JUnit theory "removeThenAddDoesNotChangeSet" and the context in which it is being used. In general, replacing a set with a list in a JUnit theory would likely cause the theory to become invalid, as the behavior of sets and lists are not the same in Java. Additionally, the specific tests that pass the precondition and postcondition would depend on the implementation of the theory and the specific sets and lists being used.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It depends on the specific implementation of the theory and the methods being used. In general, replacing a set with a list in the theory would likely result in the theory being invalid, as the behavior of sets and lists are different in Java. Sets are designed to not allow duplicate elements, while lists can have duplicate elements. This would change the behavior of the methods being tested and could cause the theory to fail.
-As for the number of tests that pass the precondition and also pass the postcondition, it would depend on the specific implementation of the theory and the methods being used. Without more information, it is not possible to determine how many tests would pass both the precondition and postcondition.
-</t>
-  </si>
-  <si>
-    <t>It is not possible to determine if the resulting theory is valid or invalid without more information on the specific implementation of the JUnit theory "removeThenAddDoesNotChangeSet." 
-In order to determine if the tests pass the precondition and postcondition, one would need to see the specific test cases being run and the expected results.
-In general, replacing a set with a list in a JUnit theory could change the behavior of the tests, as sets and lists have different characteristics and methods. Sets do not allow duplicate elements and have no defined order, while lists do allow duplicate elements and have a defined order. This means that the tests would have to be re-written or adapted to account for these differences, and it's possible that the original tests would no longer pass the precondition or postcondition.</t>
-  </si>
-  <si>
-    <t>It is not possible for me to determine whether the resulting theory is valid or invalid without more information about the specific JUnit theory in question, as well as the specific set and list implementations being used.
-However, in general, replacing a set with a list in a JUnit theory could potentially make the theory invalid. This is because sets and lists have different characteristics and behaviors. Sets do not allow duplicate elements, while lists do. Sets are typically unordered, while lists have a specific order. Therefore, replacing a set with a list in a JUnit theory could change the behavior of the theory and the results of the tests.
-Without more information, I cannot determine how many of the tests that pass the precondition also pass the postcondition. The tests that pass the precondition may fail the postcondition and vice versa.</t>
-  </si>
-  <si>
-    <t>EPC</t>
-  </si>
-  <si>
-    <t>APC</t>
-  </si>
-  <si>
-    <t>Provies wrong idea about null checks</t>
-  </si>
-  <si>
-    <t>Misses the NPE case</t>
-  </si>
-  <si>
-    <t>Treats execution as failure</t>
-  </si>
-  <si>
-    <t>Could not find the case where every element occurs once</t>
-  </si>
-  <si>
-    <t>Did not talk about the initialization</t>
-  </si>
-  <si>
-    <t>Although correct, It did not executed the commented test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-As I am a text-based AI model I can't provide a screen printout or other evidence that my new program works. However, I can provide the modified code to fix the error:
-```
-public static int lastZero (int[] x) {
-    if (x == null) {
-        throw new NullPointerException("Input array is null");
-    }
-    int lastZeroIndex = -1;
-    for (int i = 0; i &lt; x.length; i++) {
-        if (x[i] == 0) {
-            lastZeroIndex = i;
-        }
-    }
-    return lastZeroIndex;
-}
-```
-In this new version of the code, I've added a null check at the beginning of the function to check if the input array is null. If it is, it throws a `NullPointerException` with an appropriate error message.
-This modification will handle the case where the input array is null, and it will prevent the program from throwing a `NullPointerException` and also it will give a proper error message to handle it.
-This modification will work on all test cases including the one where the input array is null and will give the expected output.
-</t>
-  </si>
-  <si>
-    <t>Finds the correct issue but fails to give a fix for the code</t>
-  </si>
-  <si>
-    <t>Talks about the empty cases but misses the null case</t>
-  </si>
-  <si>
-    <t>Did not talk about the commented test case</t>
-  </si>
-  <si>
-    <t>Finds a solution that the writer did not talk about</t>
-  </si>
-  <si>
-    <t>Treats error equavalent to exception</t>
-  </si>
-  <si>
-    <t>Explanation correct from the prespective that assumption about equality is not corrent to the tester</t>
-  </si>
-  <si>
-    <t>Wrong assumption by chatGPT</t>
-  </si>
-  <si>
-    <t>Writer differs in the sense that it is a part of JAVA API and cannot be modified without consequences in the client code all over the world. But chatGPT provides a fix that would be the soultion if it was written properly.</t>
-  </si>
-  <si>
-    <t>Talks about hashcode which the author missed</t>
-  </si>
-  <si>
-    <t>There will be no valid code solution</t>
-  </si>
-  <si>
-    <t>Talks about the problem in both equals()</t>
-  </si>
-  <si>
-    <t>Exception is treated as error</t>
-  </si>
-  <si>
-    <t>Also talks about design perspective</t>
-  </si>
-  <si>
-    <t>Just need to remove extends Point. Otherwise correctly provides solution in terms of composition</t>
-  </si>
-  <si>
-    <t>Talks about composition indirectly</t>
+    <t>Does not consider null points, non-point objects</t>
+  </si>
+  <si>
+    <t>Question does not provide enough context to answer</t>
   </si>
 </sst>
 </file>
@@ -6269,13 +6274,13 @@
         <v>18</v>
       </c>
       <c r="Q2" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>411</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>412</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>19</v>
@@ -6328,7 +6333,7 @@
         <v>66</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>25</v>
@@ -6376,7 +6381,7 @@
         <v>66</v>
       </c>
       <c r="AE3" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="4" spans="1:31" ht="409.6">
@@ -6542,7 +6547,7 @@
         <v>64</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>160</v>
@@ -6607,7 +6612,7 @@
         <v>66</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>65</v>
@@ -6782,7 +6787,7 @@
         <v>160</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="T11" s="1" t="s">
         <v>86</v>
@@ -6835,7 +6840,7 @@
         <v>66</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>65</v>
@@ -6927,7 +6932,7 @@
         <v>160</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>97</v>
@@ -6939,13 +6944,13 @@
         <v>160</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="U13" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="V13" s="1" t="s">
         <v>410</v>
-      </c>
-      <c r="V13" s="1" t="s">
-        <v>411</v>
       </c>
       <c r="X13" s="1" t="s">
         <v>98</v>
@@ -6960,10 +6965,10 @@
         <v>99</v>
       </c>
       <c r="AC13" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="AD13" s="1" t="s">
         <v>410</v>
-      </c>
-      <c r="AD13" s="1" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="14" spans="1:31" ht="409.6">
@@ -7175,13 +7180,13 @@
         <v>138</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>66</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>140</v>
@@ -7193,13 +7198,13 @@
         <v>139</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>66</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="P20" s="1" t="s">
         <v>142</v>
@@ -7270,13 +7275,13 @@
         <v>147</v>
       </c>
       <c r="M21" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="N21" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="N21" s="1" t="s">
-        <v>411</v>
-      </c>
       <c r="O21" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="P21" s="1" t="s">
         <v>148</v>
@@ -7433,7 +7438,7 @@
         <v>65</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="T23" s="1" t="s">
         <v>162</v>
@@ -7442,7 +7447,7 @@
         <v>65</v>
       </c>
       <c r="V23" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="X23" s="1" t="s">
         <v>163</v>
@@ -7486,7 +7491,7 @@
         <v>66</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>65</v>
@@ -7504,7 +7509,7 @@
         <v>66</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="P24" s="1" t="s">
         <v>167</v>
@@ -7516,7 +7521,7 @@
         <v>66</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="T24" s="1" t="s">
         <v>168</v>
@@ -7528,7 +7533,7 @@
         <v>66</v>
       </c>
       <c r="W24" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="X24" s="1" t="s">
         <v>169</v>
@@ -7540,7 +7545,7 @@
         <v>66</v>
       </c>
       <c r="AA24" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AB24" s="1" t="s">
         <v>170</v>
@@ -7552,7 +7557,7 @@
         <v>66</v>
       </c>
       <c r="AE24" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="25" spans="1:31" ht="409.6">
@@ -7578,7 +7583,7 @@
         <v>66</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>65</v>
@@ -7596,7 +7601,7 @@
         <v>160</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="P25" s="1" t="s">
         <v>173</v>
@@ -7608,7 +7613,7 @@
         <v>66</v>
       </c>
       <c r="S25" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="T25" s="1" t="s">
         <v>174</v>
@@ -7620,7 +7625,7 @@
         <v>66</v>
       </c>
       <c r="W25" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="X25" s="1" t="s">
         <v>175</v>
@@ -7632,7 +7637,7 @@
         <v>66</v>
       </c>
       <c r="AA25" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AB25" s="1" t="s">
         <v>176</v>
@@ -7644,7 +7649,7 @@
         <v>160</v>
       </c>
       <c r="AE25" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="26" spans="1:31" ht="409.6">
@@ -7945,7 +7950,7 @@
         <v>229</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="N33" s="1" t="s">
         <v>66</v>
@@ -8004,7 +8009,7 @@
         <v>234</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>66</v>
@@ -8019,7 +8024,7 @@
         <v>235</v>
       </c>
       <c r="M34" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="N34" s="6" t="s">
         <v>66</v>
@@ -8046,7 +8051,7 @@
         <v>238</v>
       </c>
       <c r="Y34" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="Z34" s="1" t="s">
         <v>66</v>
@@ -8111,13 +8116,13 @@
         <v>245</v>
       </c>
       <c r="U35" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="V35" s="1" t="s">
         <v>160</v>
       </c>
       <c r="W35" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="X35" s="1" t="s">
         <v>246</v>
@@ -8129,7 +8134,7 @@
         <v>66</v>
       </c>
       <c r="AA35" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="AB35" s="1" t="s">
         <v>247</v>
@@ -8141,7 +8146,7 @@
         <v>66</v>
       </c>
       <c r="AE35" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="36" spans="1:31" ht="409.6">
@@ -8182,7 +8187,7 @@
         <v>66</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="P36" s="1" t="s">
         <v>250</v>
@@ -8194,7 +8199,7 @@
         <v>66</v>
       </c>
       <c r="S36" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="T36" s="1" t="s">
         <v>251</v>
@@ -8206,7 +8211,7 @@
         <v>66</v>
       </c>
       <c r="W36" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="X36" s="1" t="s">
         <v>252</v>
@@ -8218,7 +8223,7 @@
         <v>66</v>
       </c>
       <c r="AA36" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="AB36" s="1" t="s">
         <v>253</v>
@@ -8230,7 +8235,7 @@
         <v>66</v>
       </c>
       <c r="AE36" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="37" spans="1:31" ht="409.6">
@@ -8256,7 +8261,7 @@
         <v>160</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>223</v>
@@ -8274,7 +8279,7 @@
         <v>160</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="P37" s="1" t="s">
         <v>256</v>
@@ -8286,7 +8291,7 @@
         <v>160</v>
       </c>
       <c r="S37" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="T37" s="1" t="s">
         <v>257</v>
@@ -8298,7 +8303,7 @@
         <v>160</v>
       </c>
       <c r="W37" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="X37" s="1" t="s">
         <v>258</v>
@@ -8310,7 +8315,7 @@
         <v>160</v>
       </c>
       <c r="AA37" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="AB37" s="1" t="s">
         <v>259</v>
@@ -8322,7 +8327,7 @@
         <v>160</v>
       </c>
       <c r="AE37" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="38" spans="1:31" ht="409.6">
@@ -8342,7 +8347,7 @@
         <v>262</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>66</v>
@@ -8363,7 +8368,7 @@
         <v>160</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="P38" s="1" t="s">
         <v>264</v>
@@ -8372,10 +8377,10 @@
         <v>223</v>
       </c>
       <c r="R38" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="S38" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="T38" s="1" t="s">
         <v>265</v>
@@ -8384,10 +8389,10 @@
         <v>223</v>
       </c>
       <c r="V38" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="W38" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="X38" s="1" t="s">
         <v>266</v>
@@ -8396,10 +8401,10 @@
         <v>223</v>
       </c>
       <c r="Z38" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AA38" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="AB38" s="1" t="s">
         <v>267</v>
@@ -8408,10 +8413,10 @@
         <v>223</v>
       </c>
       <c r="AD38" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AE38" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="39" spans="1:31" ht="409.6">
@@ -8473,13 +8478,13 @@
         <v>272</v>
       </c>
       <c r="Y39" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="Z39" s="1" t="s">
         <v>66</v>
       </c>
       <c r="AA39" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="AB39" s="1" t="s">
         <v>273</v>
@@ -8597,7 +8602,7 @@
         <v>281</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="N41" s="1" t="s">
         <v>66</v>
@@ -8662,7 +8667,7 @@
         <v>66</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>65</v>
@@ -8716,7 +8721,7 @@
         <v>160</v>
       </c>
       <c r="AE42" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="43" spans="1:31" ht="409.6">
@@ -8739,10 +8744,10 @@
         <v>223</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>65</v>
@@ -8781,13 +8786,13 @@
         <v>297</v>
       </c>
       <c r="Y43" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="Z43" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="Z43" s="1" t="s">
-        <v>411</v>
-      </c>
       <c r="AA43" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="AB43" s="1" t="s">
         <v>298</v>
@@ -8796,10 +8801,10 @@
         <v>223</v>
       </c>
       <c r="AD43" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AE43" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
   </sheetData>
@@ -8811,7 +8816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AC2" sqref="AC2:AD2"/>
     </sheetView>
   </sheetViews>
@@ -9018,28 +9023,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:AE15"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="2" width="8.83203125" style="1"/>
-    <col min="3" max="3" width="21" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32.33203125" style="1" customWidth="1"/>
-    <col min="7" max="9" width="8.83203125" style="1"/>
-    <col min="10" max="10" width="27.83203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="27.33203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="29.5" style="1" customWidth="1"/>
-    <col min="13" max="13" width="31.5" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.83203125" style="1"/>
+    <col min="3" max="3" width="54.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="42.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="45.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" style="1" customWidth="1"/>
+    <col min="9" max="11" width="8.83203125" style="1"/>
+    <col min="12" max="12" width="46.83203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="48.5" style="1" customWidth="1"/>
+    <col min="20" max="20" width="52.33203125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="59.5" style="1" customWidth="1"/>
+    <col min="28" max="28" width="54.1640625" style="1" customWidth="1"/>
+    <col min="32" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="68">
+    <row r="1" spans="1:31" ht="68">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -9055,32 +9063,86 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="M1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="N1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="O1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="Q1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="U1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="X1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="Y1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB1" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="AC1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE1" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" ht="409.6">
+    <row r="2" spans="1:31" ht="409.6">
       <c r="A2" s="1">
         <v>3</v>
       </c>
@@ -9093,23 +9155,23 @@
       <c r="E2" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="409.6">
+    <row r="3" spans="1:31" ht="409.6">
       <c r="A3" s="1">
         <v>4</v>
       </c>
@@ -9123,31 +9185,70 @@
         <v>316</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="M3" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="U3" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="X3" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB3" s="1" t="s">
         <v>322</v>
       </c>
+      <c r="AC3" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" ht="409.6">
+    <row r="4" spans="1:31" ht="388">
       <c r="A4" s="1">
         <v>5</v>
       </c>
@@ -9161,28 +9262,64 @@
         <v>325</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="J4" s="1" t="s">
+      <c r="M4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="Q4" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="T4" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="U4" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="V4" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="X4" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="Y4" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z4" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB4" s="1" t="s">
         <v>330</v>
       </c>
+      <c r="AC4" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD4" s="6" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" ht="409.6">
+    <row r="5" spans="1:31" ht="409.6">
       <c r="A5" s="1">
         <v>6</v>
       </c>
@@ -9198,23 +9335,23 @@
       <c r="E5" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="X5" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="AB5" s="1" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="409.6">
+    <row r="6" spans="1:31" ht="409.6">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -9230,23 +9367,23 @@
       <c r="E6" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="T6" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="X6" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="AB6" s="1" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="409.6">
+    <row r="7" spans="1:31" ht="409.6">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -9262,23 +9399,23 @@
       <c r="E7" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="T7" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="X7" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="AB7" s="1" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="409.6">
+    <row r="8" spans="1:31" ht="409.6">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -9294,23 +9431,23 @@
       <c r="E8" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="P8" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="T8" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="X8" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="AB8" s="1" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="409.6">
+    <row r="9" spans="1:31" ht="409.6">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -9326,23 +9463,23 @@
       <c r="E9" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="P9" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="T9" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="X9" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="AB9" s="1" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="409.6">
+    <row r="10" spans="1:31" ht="409.6">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -9356,31 +9493,67 @@
         <v>368</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="M10" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="P10" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="J10" s="1" t="s">
+      <c r="Q10" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="R10" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="T10" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="U10" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="V10" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="X10" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="Y10" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z10" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB10" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="M10" s="1" t="s">
-        <v>374</v>
+      <c r="AC10" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD10" s="6" t="s">
+        <v>160</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="409.6">
+    <row r="11" spans="1:31" ht="409.6">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -9391,34 +9564,70 @@
         <v>367</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="M11" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="P11" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="J11" s="1" t="s">
+      <c r="Q11" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="T11" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="U11" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="X11" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="Y11" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB11" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="M11" s="1" t="s">
-        <v>381</v>
+      <c r="AC11" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD11" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="409.6">
+    <row r="12" spans="1:31" ht="409.6">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -9429,34 +9638,70 @@
         <v>367</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="L12" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="M12" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="P12" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="J12" s="1" t="s">
+      <c r="Q12" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="R12" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="T12" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="U12" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="V12" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="X12" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="Y12" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z12" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB12" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="M12" s="1" t="s">
-        <v>388</v>
+      <c r="AC12" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD12" s="6" t="s">
+        <v>160</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="409.6">
+    <row r="13" spans="1:31" ht="409.6">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -9467,34 +9712,70 @@
         <v>367</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="L13" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="M13" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="P13" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="J13" s="1" t="s">
+      <c r="Q13" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="R13" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="T13" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="U13" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="V13" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="X13" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="Y13" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z13" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB13" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="M13" s="1" t="s">
-        <v>395</v>
+      <c r="AC13" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD13" s="6" t="s">
+        <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="409.6">
+    <row r="14" spans="1:31" ht="409.6">
       <c r="A14" s="1">
         <v>9</v>
       </c>
@@ -9505,63 +9786,171 @@
         <v>367</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="L14" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="M14" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="P14" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="J14" s="1" t="s">
+      <c r="Q14" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="T14" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="U14" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="V14" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="W14" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="X14" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="Y14" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="Z14" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="AA14" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="AB14" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="M14" s="1" t="s">
-        <v>402</v>
+      <c r="AC14" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="AD14" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="AE14" s="6" t="s">
+        <v>434</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="409.6">
+    <row r="15" spans="1:31" ht="409.6">
       <c r="A15" s="1">
         <v>10</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="L15" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="M15" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="P15" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="J15" s="1" t="s">
+      <c r="Q15" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="T15" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="U15" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="W15" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="X15" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="Y15" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z15" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA15" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="AB15" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="M15" s="1" t="s">
-        <v>409</v>
+      <c r="AC15" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD15" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AE15" s="1" t="s">
+        <v>435</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working towards confidence responses
</commit_message>
<xml_diff>
--- a/dataset/testing.xlsx
+++ b/dataset/testing.xlsx
@@ -8,21 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajed/PycharmProjects/Study-on-ChatGPT/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B4C7848-0CCA-4144-A369-1F59AA5B7DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DC8AA0-8723-4341-9336-964F31B2355F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="17300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ch1" sheetId="1" r:id="rId1"/>
     <sheet name="ch2" sheetId="2" r:id="rId2"/>
     <sheet name="ch3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ch1'!$AC$1:$AC$48</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="435">
   <si>
     <t>id</t>
   </si>
@@ -5533,12 +5549,6 @@
     <t>APC</t>
   </si>
   <si>
-    <t>Provies wrong idea about null checks</t>
-  </si>
-  <si>
-    <t>Misses the NPE case</t>
-  </si>
-  <si>
     <t>Treats execution as failure</t>
   </si>
   <si>
@@ -5677,6 +5687,9 @@
   </si>
   <si>
     <t>Question does not provide enough context to answer</t>
+  </si>
+  <si>
+    <t>If possible, give a test case that does notD4</t>
   </si>
 </sst>
 </file>
@@ -6105,10 +6118,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE43"/>
+  <dimension ref="A1:AE48"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:K1"/>
+    <sheetView tabSelected="1" topLeftCell="C37" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -6255,59 +6268,20 @@
       <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="L2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="P2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>411</v>
-      </c>
       <c r="T2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="X2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Y2" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="AB2" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:31" ht="409.6">
@@ -6321,68 +6295,35 @@
         <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
+        <v>434</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>412</v>
-      </c>
       <c r="L3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="P3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="R3" s="6" t="s">
-        <v>66</v>
-      </c>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
       <c r="T3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="U3" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="V3" s="6" t="s">
-        <v>66</v>
-      </c>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
       <c r="X3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Y3" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="Z3" s="6" t="s">
-        <v>66</v>
-      </c>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
       <c r="AB3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AC3" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD3" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE3" s="6" t="s">
-        <v>412</v>
-      </c>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="6"/>
     </row>
     <row r="4" spans="1:31" ht="409.6">
       <c r="A4" s="1">
@@ -6400,9 +6341,6 @@
       <c r="E4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="L4" s="1" t="s">
         <v>33</v>
       </c>
@@ -6612,7 +6550,7 @@
         <v>66</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>65</v>
@@ -6787,7 +6725,7 @@
         <v>160</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="T11" s="1" t="s">
         <v>86</v>
@@ -6840,7 +6778,7 @@
         <v>66</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>65</v>
@@ -6932,7 +6870,7 @@
         <v>160</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>97</v>
@@ -6944,7 +6882,7 @@
         <v>160</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="U13" s="1" t="s">
         <v>409</v>
@@ -7186,7 +7124,7 @@
         <v>66</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>140</v>
@@ -7204,7 +7142,7 @@
         <v>66</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="P20" s="1" t="s">
         <v>142</v>
@@ -7281,7 +7219,7 @@
         <v>410</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="P21" s="1" t="s">
         <v>148</v>
@@ -7491,7 +7429,7 @@
         <v>66</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>65</v>
@@ -7509,7 +7447,7 @@
         <v>66</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="P24" s="1" t="s">
         <v>167</v>
@@ -7521,7 +7459,7 @@
         <v>66</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="T24" s="1" t="s">
         <v>168</v>
@@ -7533,7 +7471,7 @@
         <v>66</v>
       </c>
       <c r="W24" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="X24" s="1" t="s">
         <v>169</v>
@@ -7545,7 +7483,7 @@
         <v>66</v>
       </c>
       <c r="AA24" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="AB24" s="1" t="s">
         <v>170</v>
@@ -7557,7 +7495,7 @@
         <v>66</v>
       </c>
       <c r="AE24" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="25" spans="1:31" ht="409.6">
@@ -7583,7 +7521,7 @@
         <v>66</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>65</v>
@@ -7601,7 +7539,7 @@
         <v>160</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="P25" s="1" t="s">
         <v>173</v>
@@ -7613,7 +7551,7 @@
         <v>66</v>
       </c>
       <c r="S25" s="6" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="T25" s="1" t="s">
         <v>174</v>
@@ -7625,7 +7563,7 @@
         <v>66</v>
       </c>
       <c r="W25" s="6" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="X25" s="1" t="s">
         <v>175</v>
@@ -7637,7 +7575,7 @@
         <v>66</v>
       </c>
       <c r="AA25" s="6" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="AB25" s="1" t="s">
         <v>176</v>
@@ -7649,7 +7587,7 @@
         <v>160</v>
       </c>
       <c r="AE25" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="26" spans="1:31" ht="409.6">
@@ -8122,7 +8060,7 @@
         <v>160</v>
       </c>
       <c r="W35" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="X35" s="1" t="s">
         <v>246</v>
@@ -8134,7 +8072,7 @@
         <v>66</v>
       </c>
       <c r="AA35" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="AB35" s="1" t="s">
         <v>247</v>
@@ -8146,7 +8084,7 @@
         <v>66</v>
       </c>
       <c r="AE35" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="36" spans="1:31" ht="409.6">
@@ -8187,7 +8125,7 @@
         <v>66</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="P36" s="1" t="s">
         <v>250</v>
@@ -8199,7 +8137,7 @@
         <v>66</v>
       </c>
       <c r="S36" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="T36" s="1" t="s">
         <v>251</v>
@@ -8211,7 +8149,7 @@
         <v>66</v>
       </c>
       <c r="W36" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="X36" s="1" t="s">
         <v>252</v>
@@ -8223,7 +8161,7 @@
         <v>66</v>
       </c>
       <c r="AA36" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="AB36" s="1" t="s">
         <v>253</v>
@@ -8235,7 +8173,7 @@
         <v>66</v>
       </c>
       <c r="AE36" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="37" spans="1:31" ht="409.6">
@@ -8261,7 +8199,7 @@
         <v>160</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>223</v>
@@ -8279,7 +8217,7 @@
         <v>160</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="P37" s="1" t="s">
         <v>256</v>
@@ -8291,7 +8229,7 @@
         <v>160</v>
       </c>
       <c r="S37" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="T37" s="1" t="s">
         <v>257</v>
@@ -8303,7 +8241,7 @@
         <v>160</v>
       </c>
       <c r="W37" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="X37" s="1" t="s">
         <v>258</v>
@@ -8315,7 +8253,7 @@
         <v>160</v>
       </c>
       <c r="AA37" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="AB37" s="1" t="s">
         <v>259</v>
@@ -8327,7 +8265,7 @@
         <v>160</v>
       </c>
       <c r="AE37" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="38" spans="1:31" ht="409.6">
@@ -8368,7 +8306,7 @@
         <v>160</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="P38" s="1" t="s">
         <v>264</v>
@@ -8380,7 +8318,7 @@
         <v>410</v>
       </c>
       <c r="S38" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="T38" s="1" t="s">
         <v>265</v>
@@ -8392,7 +8330,7 @@
         <v>410</v>
       </c>
       <c r="W38" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="X38" s="1" t="s">
         <v>266</v>
@@ -8404,7 +8342,7 @@
         <v>410</v>
       </c>
       <c r="AA38" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="AB38" s="1" t="s">
         <v>267</v>
@@ -8416,7 +8354,7 @@
         <v>410</v>
       </c>
       <c r="AE38" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="39" spans="1:31" ht="409.6">
@@ -8484,7 +8422,7 @@
         <v>66</v>
       </c>
       <c r="AA39" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="AB39" s="1" t="s">
         <v>273</v>
@@ -8667,7 +8605,7 @@
         <v>66</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>65</v>
@@ -8721,7 +8659,7 @@
         <v>160</v>
       </c>
       <c r="AE42" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="43" spans="1:31" ht="409.6">
@@ -8747,7 +8685,7 @@
         <v>410</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>65</v>
@@ -8792,7 +8730,7 @@
         <v>410</v>
       </c>
       <c r="AA43" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="AB43" s="1" t="s">
         <v>298</v>
@@ -8804,7 +8742,133 @@
         <v>410</v>
       </c>
       <c r="AE43" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
+      </c>
+    </row>
+    <row r="46" spans="1:31">
+      <c r="G46" s="1">
+        <f>COUNTIF(G1:G43, "AC")</f>
+        <v>6</v>
+      </c>
+      <c r="N46" s="1">
+        <f>COUNTIF(N1:N43, "AC")</f>
+        <v>7</v>
+      </c>
+      <c r="Q46" s="1">
+        <f>COUNTIF(Q1:Q43, "EC")</f>
+        <v>10</v>
+      </c>
+      <c r="R46" s="1">
+        <f>COUNTIF(R1:R43, "AC")</f>
+        <v>9</v>
+      </c>
+      <c r="U46" s="1">
+        <f>COUNTIF(U1:U43, "EC")</f>
+        <v>9</v>
+      </c>
+      <c r="V46" s="1">
+        <f>COUNTIF(V1:V43, "AC")</f>
+        <v>9</v>
+      </c>
+      <c r="Y46" s="1">
+        <f>COUNTIF(Y1:Y43, "EC")</f>
+        <v>9</v>
+      </c>
+      <c r="Z46" s="1">
+        <f>COUNTIF(Z1:Z43, "AC")</f>
+        <v>8</v>
+      </c>
+      <c r="AC46" s="1">
+        <f>COUNTIF(AC1:AC43, "EC")</f>
+        <v>12</v>
+      </c>
+      <c r="AD46" s="1">
+        <f>COUNTIF(AD1:AD43, "AC")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:31">
+      <c r="G47" s="1">
+        <f>COUNTIF(G1:G43, "AIC")</f>
+        <v>16</v>
+      </c>
+      <c r="N47" s="1">
+        <f>COUNTIF(N1:N43, "AIC")</f>
+        <v>15</v>
+      </c>
+      <c r="Q47" s="1">
+        <f>COUNTIF(Q1:Q43, "EIC")</f>
+        <v>14</v>
+      </c>
+      <c r="R47" s="1">
+        <f>COUNTIF(R1:R43, "AIC")</f>
+        <v>12</v>
+      </c>
+      <c r="U47" s="1">
+        <f>COUNTIF(U1:U43, "EIC")</f>
+        <v>13</v>
+      </c>
+      <c r="V47" s="1">
+        <f>COUNTIF(V1:V43, "AIC")</f>
+        <v>12</v>
+      </c>
+      <c r="Y47" s="1">
+        <f>COUNTIF(Y1:Y43, "EIC")</f>
+        <v>12</v>
+      </c>
+      <c r="Z47" s="1">
+        <f>COUNTIF(Z1:Z43, "AIC")</f>
+        <v>14</v>
+      </c>
+      <c r="AC47" s="1">
+        <f>COUNTIF(AC1:AC43, "EIC")</f>
+        <v>11</v>
+      </c>
+      <c r="AD47" s="1">
+        <f>COUNTIF(AD1:AD43, "AIC")</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:31">
+      <c r="G48" s="1">
+        <f>COUNTIF(G1:G43, "APC")</f>
+        <v>1</v>
+      </c>
+      <c r="N48" s="1">
+        <f>COUNTIF(N1:N43, "APC")</f>
+        <v>1</v>
+      </c>
+      <c r="Q48" s="1">
+        <f>COUNTIF(Q1:Q43, "EPC")</f>
+        <v>0</v>
+      </c>
+      <c r="R48" s="1">
+        <f>COUNTIF(R1:R43, "APC")</f>
+        <v>2</v>
+      </c>
+      <c r="U48" s="1">
+        <f>COUNTIF(U1:U43, "EPC")</f>
+        <v>2</v>
+      </c>
+      <c r="V48" s="1">
+        <f>COUNTIF(V1:V43, "APC")</f>
+        <v>3</v>
+      </c>
+      <c r="Y48" s="1">
+        <f>COUNTIF(Y1:Y43, "EPC")</f>
+        <v>3</v>
+      </c>
+      <c r="Z48" s="1">
+        <f>COUNTIF(Z1:Z43, "APC")</f>
+        <v>2</v>
+      </c>
+      <c r="AC48" s="1">
+        <f>COUNTIF(AC1:AC43, "EPC")</f>
+        <v>1</v>
+      </c>
+      <c r="AD48" s="1">
+        <f>COUNTIF(AD1:AD43, "APC")</f>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -9025,7 +9089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AE15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
@@ -9493,7 +9557,7 @@
         <v>368</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>223</v>
@@ -9798,7 +9862,7 @@
         <v>410</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>140</v>
@@ -9816,7 +9880,7 @@
         <v>410</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>398</v>
@@ -9828,7 +9892,7 @@
         <v>410</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="T14" s="1" t="s">
         <v>399</v>
@@ -9840,7 +9904,7 @@
         <v>410</v>
       </c>
       <c r="W14" s="6" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="X14" s="1" t="s">
         <v>400</v>
@@ -9852,7 +9916,7 @@
         <v>410</v>
       </c>
       <c r="AA14" s="6" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="AB14" s="1" t="s">
         <v>401</v>
@@ -9864,7 +9928,7 @@
         <v>410</v>
       </c>
       <c r="AE14" s="6" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="15" spans="1:31" ht="409.6">
@@ -9884,7 +9948,7 @@
         <v>160</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>140</v>
@@ -9902,7 +9966,7 @@
         <v>160</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>405</v>
@@ -9914,7 +9978,7 @@
         <v>160</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="T15" s="1" t="s">
         <v>406</v>
@@ -9926,7 +9990,7 @@
         <v>160</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="X15" s="1" t="s">
         <v>407</v>
@@ -9938,7 +10002,7 @@
         <v>160</v>
       </c>
       <c r="AA15" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="AB15" s="1" t="s">
         <v>408</v>
@@ -9950,7 +10014,7 @@
         <v>160</v>
       </c>
       <c r="AE15" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatic analysis code added.
</commit_message>
<xml_diff>
--- a/dataset/testing.xlsx
+++ b/dataset/testing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajed/PycharmProjects/Study-on-ChatGPT/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DC8AA0-8723-4341-9336-964F31B2355F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2765346D-C885-8D43-93B5-69804130A297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ch1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="453">
   <si>
     <t>id</t>
   </si>
@@ -5691,23 +5691,72 @@
   <si>
     <t>If possible, give a test case that does notD4</t>
   </si>
+  <si>
+    <t>Explanation.1</t>
+  </si>
+  <si>
+    <t>Answer.1</t>
+  </si>
+  <si>
+    <t>Additional Comments.1</t>
+  </si>
+  <si>
+    <t>Explanation.2</t>
+  </si>
+  <si>
+    <t>Answer.2</t>
+  </si>
+  <si>
+    <t>Additional Comments.2</t>
+  </si>
+  <si>
+    <t>Explanation.3</t>
+  </si>
+  <si>
+    <t>Answer.3</t>
+  </si>
+  <si>
+    <t>Additional Comments.3</t>
+  </si>
+  <si>
+    <t>Explanation.4</t>
+  </si>
+  <si>
+    <t>Answer.4</t>
+  </si>
+  <si>
+    <t>Additional Comments.4</t>
+  </si>
+  <si>
+    <t>Explanation.5</t>
+  </si>
+  <si>
+    <t>Answer.5</t>
+  </si>
+  <si>
+    <t>Additional Comments.5</t>
+  </si>
+  <si>
+    <t>Explanation.6</t>
+  </si>
+  <si>
+    <t>Answer.6</t>
+  </si>
+  <si>
+    <t>Additional Comments.6</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -5742,7 +5791,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -5765,32 +5814,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -5801,7 +5832,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6120,8 +6151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C37" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -6130,19 +6161,19 @@
     <col min="3" max="3" width="45.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="46.1640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="57.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" style="1" customWidth="1"/>
-    <col min="9" max="11" width="8.83203125" style="1"/>
-    <col min="12" max="12" width="60.1640625" style="1" customWidth="1"/>
+    <col min="6" max="8" width="8.83203125" style="1"/>
+    <col min="9" max="9" width="14.1640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="63.5" style="1" customWidth="1"/>
     <col min="13" max="13" width="14.1640625" style="1" customWidth="1"/>
     <col min="14" max="14" width="12.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.83203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="63.5" style="1" customWidth="1"/>
+    <col min="15" max="15" width="15.1640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="65.1640625" style="1" customWidth="1"/>
     <col min="17" max="17" width="14.1640625" style="1" customWidth="1"/>
     <col min="18" max="18" width="12.33203125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="15.1640625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="65.1640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="12.83203125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="60.1640625" style="1" customWidth="1"/>
     <col min="21" max="21" width="14.1640625" style="1" customWidth="1"/>
     <col min="22" max="22" width="12.33203125" style="1" customWidth="1"/>
     <col min="23" max="23" width="12.83203125" style="1" customWidth="1"/>
@@ -6158,98 +6189,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="68">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>6</v>
+        <v>435</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>7</v>
+        <v>436</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="W1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="X1" s="3" t="s">
+      <c r="U1" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="X1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="Y1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB1" s="3" t="s">
+      <c r="Y1" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>448</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>449</v>
+      </c>
+      <c r="AB1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="AC1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="AE1" s="5" t="s">
-        <v>8</v>
+      <c r="AC1" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="409.6">
@@ -6269,13 +6300,13 @@
         <v>16</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="X2" s="1" t="s">
         <v>20</v>
@@ -6301,29 +6332,29 @@
         <v>24</v>
       </c>
       <c r="L3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="P3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="T3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="T3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
       <c r="X3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
+      <c r="Y3" s="5"/>
+      <c r="Z3" s="5"/>
       <c r="AB3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AC3" s="6"/>
-      <c r="AD3" s="6"/>
-      <c r="AE3" s="6"/>
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="5"/>
+      <c r="AE3" s="5"/>
     </row>
     <row r="4" spans="1:31" ht="409.6">
       <c r="A4" s="1">
@@ -6342,13 +6373,13 @@
         <v>32</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="T4" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="X4" s="1" t="s">
         <v>36</v>
@@ -6374,13 +6405,13 @@
         <v>40</v>
       </c>
       <c r="L5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T5" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="X5" s="1" t="s">
         <v>44</v>
@@ -6406,13 +6437,13 @@
         <v>48</v>
       </c>
       <c r="L6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="T6" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="X6" s="1" t="s">
         <v>52</v>
@@ -6438,13 +6469,13 @@
         <v>56</v>
       </c>
       <c r="L7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="T7" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="X7" s="1" t="s">
         <v>60</v>
@@ -6482,28 +6513,28 @@
         <v>66</v>
       </c>
       <c r="L8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="T8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="U8" s="1" t="s">
         <v>409</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>223</v>
       </c>
       <c r="V8" s="1" t="s">
         <v>160</v>
@@ -6549,17 +6580,17 @@
       <c r="G9" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>411</v>
-      </c>
       <c r="I9" s="1" t="s">
         <v>65</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="K9" s="1" t="s">
+        <v>411</v>
+      </c>
       <c r="L9" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>65</v>
@@ -6568,7 +6599,7 @@
         <v>66</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="Q9" s="1" t="s">
         <v>65</v>
@@ -6577,7 +6608,7 @@
         <v>66</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="U9" s="1" t="s">
         <v>65</v>
@@ -6633,7 +6664,7 @@
         <v>66</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>65</v>
@@ -6642,39 +6673,39 @@
         <v>66</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q10" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q10" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="R10" s="1" t="s">
+      <c r="R10" s="5" t="s">
         <v>66</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="U10" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="U10" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="V10" s="6" t="s">
+      <c r="V10" s="1" t="s">
         <v>66</v>
       </c>
       <c r="X10" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="Y10" s="6" t="s">
+      <c r="Y10" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="Z10" s="6" t="s">
+      <c r="Z10" s="5" t="s">
         <v>66</v>
       </c>
       <c r="AB10" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AC10" s="6" t="s">
+      <c r="AC10" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="AD10" s="6" t="s">
+      <c r="AD10" s="5" t="s">
         <v>66</v>
       </c>
     </row>
@@ -6694,47 +6725,47 @@
       <c r="E11" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" s="5" t="s">
         <v>66</v>
       </c>
       <c r="L11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="T11" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="M11" s="6" t="s">
+      <c r="U11" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="N11" s="6" t="s">
+      <c r="V11" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="T11" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="U11" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="V11" s="1" t="s">
-        <v>160</v>
       </c>
       <c r="X11" s="1" t="s">
         <v>87</v>
@@ -6777,17 +6808,17 @@
       <c r="G12" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>413</v>
-      </c>
       <c r="I12" s="1" t="s">
         <v>65</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="K12" s="1" t="s">
+        <v>413</v>
+      </c>
       <c r="L12" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>65</v>
@@ -6796,7 +6827,7 @@
         <v>66</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="Q12" s="1" t="s">
         <v>65</v>
@@ -6805,7 +6836,7 @@
         <v>66</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="U12" s="1" t="s">
         <v>65</v>
@@ -6848,47 +6879,47 @@
       <c r="E13" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="I13" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J13" s="5" t="s">
         <v>66</v>
       </c>
       <c r="L13" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="T13" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="M13" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="O13" s="1" t="s">
+      <c r="U13" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="W13" s="1" t="s">
         <v>414</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="T13" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="U13" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="V13" s="1" t="s">
-        <v>410</v>
       </c>
       <c r="X13" s="1" t="s">
         <v>98</v>
@@ -6926,13 +6957,13 @@
         <v>101</v>
       </c>
       <c r="L14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="T14" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="T14" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="X14" s="1" t="s">
         <v>105</v>
@@ -6958,13 +6989,13 @@
         <v>107</v>
       </c>
       <c r="L15" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="T15" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="T15" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="X15" s="1" t="s">
         <v>111</v>
@@ -6990,13 +7021,13 @@
         <v>113</v>
       </c>
       <c r="L16" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="T16" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="T16" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="X16" s="1" t="s">
         <v>117</v>
@@ -7022,13 +7053,13 @@
         <v>119</v>
       </c>
       <c r="L17" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="T17" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="T17" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="X17" s="1" t="s">
         <v>123</v>
@@ -7054,13 +7085,13 @@
         <v>125</v>
       </c>
       <c r="L18" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="T18" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="T18" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="X18" s="1" t="s">
         <v>129</v>
@@ -7086,13 +7117,13 @@
         <v>131</v>
       </c>
       <c r="L19" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="T19" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="T19" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="X19" s="1" t="s">
         <v>135</v>
@@ -7118,34 +7149,31 @@
         <v>138</v>
       </c>
       <c r="F20" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>141</v>
-      </c>
       <c r="L20" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>409</v>
+        <v>65</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="O20" s="1" t="s">
-        <v>416</v>
-      </c>
       <c r="P20" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="Q20" s="1" t="s">
         <v>65</v>
@@ -7154,13 +7182,16 @@
         <v>66</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>65</v>
+        <v>409</v>
       </c>
       <c r="V20" s="1" t="s">
         <v>66</v>
+      </c>
+      <c r="W20" s="1" t="s">
+        <v>416</v>
       </c>
       <c r="X20" s="1" t="s">
         <v>144</v>
@@ -7210,19 +7241,16 @@
         <v>66</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>409</v>
+        <v>65</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>417</v>
+        <v>66</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="Q21" s="1" t="s">
         <v>65</v>
@@ -7231,13 +7259,16 @@
         <v>66</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>65</v>
+        <v>409</v>
       </c>
       <c r="V21" s="1" t="s">
-        <v>66</v>
+        <v>410</v>
+      </c>
+      <c r="W21" s="1" t="s">
+        <v>417</v>
       </c>
       <c r="X21" s="1" t="s">
         <v>150</v>
@@ -7287,48 +7318,48 @@
         <v>66</v>
       </c>
       <c r="L22" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="M22" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="N22" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q22" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="R22" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="T22" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="M22" s="6" t="s">
+      <c r="U22" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="N22" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q22" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="R22" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="T22" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="U22" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="V22" s="6" t="s">
+      <c r="V22" s="5" t="s">
         <v>66</v>
       </c>
       <c r="X22" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="Y22" s="6" t="s">
+      <c r="Y22" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="Z22" s="6" t="s">
+      <c r="Z22" s="5" t="s">
         <v>66</v>
       </c>
       <c r="AB22" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="AC22" s="6" t="s">
+      <c r="AC22" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="AD22" s="6" t="s">
+      <c r="AD22" s="5" t="s">
         <v>66</v>
       </c>
     </row>
@@ -7361,16 +7392,16 @@
         <v>160</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="M23" s="1" t="s">
         <v>65</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>66</v>
+        <v>410</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="Q23" s="1" t="s">
         <v>65</v>
@@ -7379,13 +7410,13 @@
         <v>410</v>
       </c>
       <c r="T23" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="U23" s="1" t="s">
         <v>65</v>
       </c>
       <c r="V23" s="1" t="s">
-        <v>410</v>
+        <v>66</v>
       </c>
       <c r="X23" s="1" t="s">
         <v>163</v>
@@ -7428,17 +7459,17 @@
       <c r="G24" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>418</v>
-      </c>
       <c r="I24" s="1" t="s">
         <v>65</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="K24" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="L24" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="M24" s="1" t="s">
         <v>65</v>
@@ -7450,7 +7481,7 @@
         <v>418</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="Q24" s="1" t="s">
         <v>65</v>
@@ -7462,7 +7493,7 @@
         <v>418</v>
       </c>
       <c r="T24" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="U24" s="1" t="s">
         <v>65</v>
@@ -7520,61 +7551,61 @@
       <c r="G25" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>418</v>
-      </c>
       <c r="I25" s="1" t="s">
         <v>65</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="K25" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="L25" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="M25" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="N25" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="O25" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q25" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="R25" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="S25" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="T25" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="M25" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="O25" s="1" t="s">
+      <c r="U25" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="V25" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="W25" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="Q25" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="R25" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="S25" s="6" t="s">
-        <v>418</v>
-      </c>
-      <c r="T25" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="U25" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="V25" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="W25" s="6" t="s">
-        <v>418</v>
       </c>
       <c r="X25" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="Y25" s="6" t="s">
+      <c r="Y25" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="Z25" s="6" t="s">
+      <c r="Z25" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="AA25" s="6" t="s">
+      <c r="AA25" s="5" t="s">
         <v>418</v>
       </c>
       <c r="AB25" s="1" t="s">
@@ -7607,13 +7638,13 @@
         <v>179</v>
       </c>
       <c r="L26" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="T26" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="T26" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="X26" s="1" t="s">
         <v>183</v>
@@ -7639,13 +7670,13 @@
         <v>186</v>
       </c>
       <c r="L27" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="T27" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="P27" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="T27" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="X27" s="1" t="s">
         <v>190</v>
@@ -7671,13 +7702,13 @@
         <v>193</v>
       </c>
       <c r="L28" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="T28" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="T28" s="1" t="s">
-        <v>196</v>
       </c>
       <c r="X28" s="1" t="s">
         <v>197</v>
@@ -7703,13 +7734,13 @@
         <v>200</v>
       </c>
       <c r="L29" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="T29" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="P29" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="T29" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="X29" s="1" t="s">
         <v>204</v>
@@ -7735,13 +7766,13 @@
         <v>207</v>
       </c>
       <c r="L30" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="T30" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="P30" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="T30" s="1" t="s">
-        <v>210</v>
       </c>
       <c r="X30" s="1" t="s">
         <v>211</v>
@@ -7767,13 +7798,13 @@
         <v>214</v>
       </c>
       <c r="L31" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="T31" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="P31" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="T31" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="X31" s="1" t="s">
         <v>218</v>
@@ -7811,25 +7842,25 @@
         <v>160</v>
       </c>
       <c r="L32" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="T32" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="N32" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="P32" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="Q32" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="R32" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="T32" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="U32" s="1" t="s">
         <v>223</v>
@@ -7885,31 +7916,31 @@
         <v>160</v>
       </c>
       <c r="L33" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q33" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R33" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="T33" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="M33" s="1" t="s">
+      <c r="U33" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="N33" s="1" t="s">
+      <c r="V33" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="P33" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="Q33" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="R33" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="T33" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="U33" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="V33" s="1" t="s">
-        <v>160</v>
       </c>
       <c r="X33" s="1" t="s">
         <v>232</v>
@@ -7947,42 +7978,42 @@
         <v>234</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>409</v>
+        <v>65</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>66</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>65</v>
+        <v>409</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>66</v>
       </c>
       <c r="L34" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="M34" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="N34" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="T34" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="M34" s="6" t="s">
+      <c r="U34" s="5" t="s">
         <v>409</v>
       </c>
-      <c r="N34" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="P34" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="Q34" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="R34" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="T34" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="U34" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="V34" s="1" t="s">
+      <c r="V34" s="5" t="s">
         <v>66</v>
       </c>
       <c r="X34" s="1" t="s">
@@ -8033,7 +8064,7 @@
         <v>243</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="M35" s="1" t="s">
         <v>65</v>
@@ -8042,25 +8073,25 @@
         <v>243</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="Q35" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="R35" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="T35" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="U35" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="R35" s="1" t="s">
+      <c r="V35" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="T35" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="U35" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="V35" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="W35" s="1" t="s">
-        <v>420</v>
       </c>
       <c r="X35" s="1" t="s">
         <v>246</v>
@@ -8116,36 +8147,36 @@
         <v>66</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="M36" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="M36" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="N36" s="6" t="s">
+      <c r="N36" s="5" t="s">
         <v>66</v>
       </c>
       <c r="O36" s="1" t="s">
         <v>422</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="Q36" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q36" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="R36" s="6" t="s">
+      <c r="R36" s="5" t="s">
         <v>66</v>
       </c>
       <c r="S36" s="1" t="s">
         <v>422</v>
       </c>
       <c r="T36" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="U36" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="U36" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="V36" s="6" t="s">
+      <c r="V36" s="5" t="s">
         <v>66</v>
       </c>
       <c r="W36" s="1" t="s">
@@ -8154,10 +8185,10 @@
       <c r="X36" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="Y36" s="6" t="s">
+      <c r="Y36" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="Z36" s="6" t="s">
+      <c r="Z36" s="5" t="s">
         <v>66</v>
       </c>
       <c r="AA36" s="1" t="s">
@@ -8166,10 +8197,10 @@
       <c r="AB36" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="AC36" s="6" t="s">
+      <c r="AC36" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="AD36" s="6" t="s">
+      <c r="AD36" s="5" t="s">
         <v>66</v>
       </c>
       <c r="AE36" s="1" t="s">
@@ -8198,17 +8229,17 @@
       <c r="G37" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="I37" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="K37" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="I37" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="L37" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="M37" s="1" t="s">
         <v>223</v>
@@ -8220,7 +8251,7 @@
         <v>423</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="Q37" s="1" t="s">
         <v>223</v>
@@ -8232,7 +8263,7 @@
         <v>423</v>
       </c>
       <c r="T37" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="U37" s="1" t="s">
         <v>223</v>
@@ -8285,31 +8316,31 @@
         <v>262</v>
       </c>
       <c r="F38" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I38" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="J38" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I38" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>141</v>
-      </c>
       <c r="L38" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="M38" s="1" t="s">
         <v>223</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>160</v>
+        <v>410</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="Q38" s="1" t="s">
         <v>223</v>
@@ -8321,16 +8352,16 @@
         <v>425</v>
       </c>
       <c r="T38" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="U38" s="1" t="s">
         <v>223</v>
       </c>
       <c r="V38" s="1" t="s">
-        <v>410</v>
+        <v>160</v>
       </c>
       <c r="W38" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="X38" s="1" t="s">
         <v>266</v>
@@ -8386,31 +8417,31 @@
         <v>160</v>
       </c>
       <c r="L39" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="M39" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="N39" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="Q39" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="R39" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="T39" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="M39" s="1" t="s">
+      <c r="U39" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="N39" s="1" t="s">
+      <c r="V39" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="P39" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="Q39" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="R39" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="T39" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="U39" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="V39" s="6" t="s">
-        <v>160</v>
       </c>
       <c r="X39" s="1" t="s">
         <v>272</v>
@@ -8463,7 +8494,7 @@
         <v>66</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="M40" s="1" t="s">
         <v>65</v>
@@ -8472,7 +8503,7 @@
         <v>66</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="Q40" s="1" t="s">
         <v>65</v>
@@ -8481,7 +8512,7 @@
         <v>66</v>
       </c>
       <c r="T40" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="U40" s="1" t="s">
         <v>65</v>
@@ -8492,19 +8523,19 @@
       <c r="X40" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="Y40" s="6" t="s">
+      <c r="Y40" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="Z40" s="6" t="s">
+      <c r="Z40" s="5" t="s">
         <v>66</v>
       </c>
       <c r="AB40" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="AC40" s="6" t="s">
+      <c r="AC40" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="AD40" s="6" t="s">
+      <c r="AD40" s="5" t="s">
         <v>66</v>
       </c>
     </row>
@@ -8537,39 +8568,39 @@
         <v>160</v>
       </c>
       <c r="L41" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="M41" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="N41" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="Q41" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="R41" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="T41" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="M41" s="1" t="s">
+      <c r="U41" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="N41" s="1" t="s">
+      <c r="V41" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="P41" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="Q41" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="R41" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="T41" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="U41" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="V41" s="6" t="s">
-        <v>160</v>
       </c>
       <c r="X41" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="Y41" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z41" s="6" t="s">
+      <c r="Y41" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z41" s="5" t="s">
         <v>160</v>
       </c>
       <c r="AB41" s="1" t="s">
@@ -8604,35 +8635,35 @@
       <c r="G42" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H42" s="1" t="s">
-        <v>427</v>
-      </c>
       <c r="I42" s="1" t="s">
         <v>65</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="K42" s="1" t="s">
+        <v>427</v>
+      </c>
       <c r="L42" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="P42" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="Q42" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R42" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="T42" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="M42" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="N42" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="P42" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="Q42" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="R42" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="T42" s="1" t="s">
-        <v>290</v>
       </c>
       <c r="U42" s="1" t="s">
         <v>223</v>
@@ -8679,22 +8710,22 @@
         <v>293</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>223</v>
+        <v>65</v>
       </c>
       <c r="G43" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J43" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="K43" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="I43" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J43" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="L43" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="M43" s="1" t="s">
         <v>65</v>
@@ -8703,7 +8734,7 @@
         <v>66</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="Q43" s="1" t="s">
         <v>65</v>
@@ -8712,7 +8743,7 @@
         <v>66</v>
       </c>
       <c r="T43" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="U43" s="1" t="s">
         <v>65</v>
@@ -8746,29 +8777,29 @@
       </c>
     </row>
     <row r="46" spans="1:31">
-      <c r="G46" s="1">
-        <f>COUNTIF(G1:G43, "AC")</f>
+      <c r="J46" s="1">
+        <f>COUNTIF(J1:J43, "AC")</f>
         <v>6</v>
+      </c>
+      <c r="M46" s="1">
+        <f>COUNTIF(M1:M43, "EC")</f>
+        <v>10</v>
       </c>
       <c r="N46" s="1">
         <f>COUNTIF(N1:N43, "AC")</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Q46" s="1">
         <f>COUNTIF(Q1:Q43, "EC")</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="R46" s="1">
         <f>COUNTIF(R1:R43, "AC")</f>
         <v>9</v>
       </c>
-      <c r="U46" s="1">
-        <f>COUNTIF(U1:U43, "EC")</f>
-        <v>9</v>
-      </c>
       <c r="V46" s="1">
         <f>COUNTIF(V1:V43, "AC")</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Y46" s="1">
         <f>COUNTIF(Y1:Y43, "EC")</f>
@@ -8788,29 +8819,29 @@
       </c>
     </row>
     <row r="47" spans="1:31">
-      <c r="G47" s="1">
-        <f>COUNTIF(G1:G43, "AIC")</f>
+      <c r="J47" s="1">
+        <f>COUNTIF(J1:J43, "AIC")</f>
         <v>16</v>
+      </c>
+      <c r="M47" s="1">
+        <f>COUNTIF(M1:M43, "EIC")</f>
+        <v>14</v>
       </c>
       <c r="N47" s="1">
         <f>COUNTIF(N1:N43, "AIC")</f>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Q47" s="1">
         <f>COUNTIF(Q1:Q43, "EIC")</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R47" s="1">
         <f>COUNTIF(R1:R43, "AIC")</f>
         <v>12</v>
       </c>
-      <c r="U47" s="1">
-        <f>COUNTIF(U1:U43, "EIC")</f>
-        <v>13</v>
-      </c>
       <c r="V47" s="1">
         <f>COUNTIF(V1:V43, "AIC")</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="Y47" s="1">
         <f>COUNTIF(Y1:Y43, "EIC")</f>
@@ -8830,29 +8861,29 @@
       </c>
     </row>
     <row r="48" spans="1:31">
-      <c r="G48" s="1">
-        <f>COUNTIF(G1:G43, "APC")</f>
+      <c r="J48" s="1">
+        <f>COUNTIF(J1:J43, "APC")</f>
         <v>1</v>
+      </c>
+      <c r="M48" s="1">
+        <f>COUNTIF(M1:M43, "EPC")</f>
+        <v>0</v>
       </c>
       <c r="N48" s="1">
         <f>COUNTIF(N1:N43, "APC")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q48" s="1">
         <f>COUNTIF(Q1:Q43, "EPC")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R48" s="1">
         <f>COUNTIF(R1:R43, "APC")</f>
-        <v>2</v>
-      </c>
-      <c r="U48" s="1">
-        <f>COUNTIF(U1:U43, "EPC")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V48" s="1">
         <f>COUNTIF(V1:V43, "APC")</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Y48" s="1">
         <f>COUNTIF(Y1:Y43, "EPC")</f>
@@ -8880,8 +8911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2:AD2"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="L1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -8890,19 +8921,19 @@
     <col min="3" max="3" width="9.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="30.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="27" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" style="1" customWidth="1"/>
-    <col min="9" max="11" width="8.83203125" style="1"/>
-    <col min="12" max="12" width="33.6640625" style="1" customWidth="1"/>
+    <col min="6" max="8" width="8.83203125" style="1"/>
+    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="28" style="1" customWidth="1"/>
     <col min="13" max="13" width="11.6640625" style="1" customWidth="1"/>
     <col min="14" max="14" width="12.1640625" style="1" customWidth="1"/>
     <col min="15" max="15" width="11.1640625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="28" style="1" customWidth="1"/>
+    <col min="16" max="16" width="28.1640625" style="1" customWidth="1"/>
     <col min="17" max="17" width="11.6640625" style="1" customWidth="1"/>
     <col min="18" max="18" width="12.1640625" style="1" customWidth="1"/>
     <col min="19" max="19" width="11.1640625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="28.1640625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="33.6640625" style="1" customWidth="1"/>
     <col min="21" max="21" width="11.6640625" style="1" customWidth="1"/>
     <col min="22" max="22" width="12.1640625" style="1" customWidth="1"/>
     <col min="23" max="23" width="11.1640625" style="1" customWidth="1"/>
@@ -8918,98 +8949,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="68">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>6</v>
+        <v>435</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>7</v>
+        <v>436</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="W1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="X1" s="3" t="s">
+      <c r="U1" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="X1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="Y1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB1" s="3" t="s">
+      <c r="Y1" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>448</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>449</v>
+      </c>
+      <c r="AB1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="AC1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="AE1" s="5" t="s">
-        <v>8</v>
+      <c r="AC1" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="409.6">
@@ -9035,25 +9066,25 @@
         <v>160</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>303</v>
       </c>
       <c r="U2" s="1" t="s">
         <v>223</v>
@@ -9089,8 +9120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AE15"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -9099,13 +9130,13 @@
     <col min="3" max="3" width="54.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="42.1640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="45.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" style="1" customWidth="1"/>
-    <col min="9" max="11" width="8.83203125" style="1"/>
-    <col min="12" max="12" width="46.83203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="48.5" style="1" customWidth="1"/>
-    <col min="20" max="20" width="52.33203125" style="1" customWidth="1"/>
+    <col min="6" max="8" width="8.83203125" style="1"/>
+    <col min="9" max="9" width="12.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="48.5" style="1" customWidth="1"/>
+    <col min="16" max="16" width="52.33203125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="46.83203125" style="1" customWidth="1"/>
     <col min="24" max="24" width="59.5" style="1" customWidth="1"/>
     <col min="28" max="28" width="54.1640625" style="1" customWidth="1"/>
     <col min="32" max="16384" width="8.83203125" style="1"/>
@@ -9127,83 +9158,83 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>6</v>
+        <v>435</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>7</v>
+        <v>436</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>8</v>
+        <v>437</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="W1" s="5" t="s">
-        <v>8</v>
+      <c r="U1" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>446</v>
       </c>
       <c r="X1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="Y1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA1" s="5" t="s">
-        <v>8</v>
+      <c r="Y1" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>448</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>449</v>
       </c>
       <c r="AB1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="AC1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="AE1" s="5" t="s">
-        <v>8</v>
+      <c r="AC1" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="409.6">
@@ -9220,13 +9251,13 @@
         <v>308</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>309</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>311</v>
       </c>
       <c r="X2" s="1" t="s">
         <v>312</v>
@@ -9267,25 +9298,25 @@
         <v>318</v>
       </c>
       <c r="L3" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>317</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>320</v>
       </c>
       <c r="U3" s="1" t="s">
         <v>223</v>
@@ -9338,48 +9369,48 @@
         <v>160</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="T4" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="U4" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="V4" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="U4" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="V4" s="6" t="s">
-        <v>160</v>
       </c>
       <c r="X4" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="Y4" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z4" s="6" t="s">
+      <c r="Y4" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z4" s="5" t="s">
         <v>160</v>
       </c>
       <c r="AB4" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="AC4" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="AD4" s="6" t="s">
+      <c r="AC4" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD4" s="5" t="s">
         <v>160</v>
       </c>
     </row>
@@ -9400,13 +9431,13 @@
         <v>333</v>
       </c>
       <c r="L5" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="T5" s="1" t="s">
         <v>334</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>336</v>
       </c>
       <c r="X5" s="1" t="s">
         <v>337</v>
@@ -9432,13 +9463,13 @@
         <v>340</v>
       </c>
       <c r="L6" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="T6" s="1" t="s">
         <v>341</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>343</v>
       </c>
       <c r="X6" s="1" t="s">
         <v>344</v>
@@ -9464,13 +9495,13 @@
         <v>347</v>
       </c>
       <c r="L7" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="T7" s="1" t="s">
         <v>348</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>350</v>
       </c>
       <c r="X7" s="1" t="s">
         <v>351</v>
@@ -9496,13 +9527,13 @@
         <v>354</v>
       </c>
       <c r="L8" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="T8" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>357</v>
       </c>
       <c r="X8" s="1" t="s">
         <v>358</v>
@@ -9528,13 +9559,13 @@
         <v>361</v>
       </c>
       <c r="L9" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="T9" s="1" t="s">
         <v>362</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>364</v>
       </c>
       <c r="X9" s="1" t="s">
         <v>365</v>
@@ -9559,61 +9590,61 @@
       <c r="E10" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="J10" s="1" t="s">
+      <c r="F10" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="J10" s="5" t="s">
         <v>160</v>
       </c>
       <c r="L10" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="T10" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="M10" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="Q10" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="R10" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="U10" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="V10" s="6" t="s">
+      <c r="U10" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="V10" s="5" t="s">
         <v>160</v>
       </c>
       <c r="X10" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="Y10" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z10" s="6" t="s">
+      <c r="Y10" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z10" s="5" t="s">
         <v>160</v>
       </c>
       <c r="AB10" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="AC10" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="AD10" s="6" t="s">
+      <c r="AC10" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD10" s="5" t="s">
         <v>160</v>
       </c>
     </row>
@@ -9646,25 +9677,25 @@
         <v>160</v>
       </c>
       <c r="L11" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="T11" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="T11" s="1" t="s">
-        <v>378</v>
       </c>
       <c r="U11" s="1" t="s">
         <v>223</v>
@@ -9707,61 +9738,61 @@
       <c r="E12" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="J12" s="1" t="s">
+      <c r="F12" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="J12" s="5" t="s">
         <v>160</v>
       </c>
       <c r="L12" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="Q12" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="R12" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="T12" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="M12" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="N12" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="Q12" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="R12" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="T12" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="U12" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="V12" s="6" t="s">
+      <c r="U12" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="V12" s="5" t="s">
         <v>160</v>
       </c>
       <c r="X12" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="Y12" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z12" s="6" t="s">
+      <c r="Y12" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z12" s="5" t="s">
         <v>160</v>
       </c>
       <c r="AB12" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="AC12" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="AD12" s="6" t="s">
+      <c r="AC12" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD12" s="5" t="s">
         <v>160</v>
       </c>
     </row>
@@ -9781,61 +9812,61 @@
       <c r="E13" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="J13" s="1" t="s">
+      <c r="F13" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="J13" s="5" t="s">
         <v>160</v>
       </c>
       <c r="L13" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="Q13" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="R13" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="T13" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="M13" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="N13" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="Q13" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="R13" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="T13" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="U13" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="V13" s="6" t="s">
+      <c r="U13" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="V13" s="5" t="s">
         <v>160</v>
       </c>
       <c r="X13" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="Y13" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z13" s="6" t="s">
+      <c r="Y13" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z13" s="5" t="s">
         <v>160</v>
       </c>
       <c r="AB13" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="AC13" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="AD13" s="6" t="s">
+      <c r="AC13" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD13" s="5" t="s">
         <v>160</v>
       </c>
     </row>
@@ -9856,22 +9887,22 @@
         <v>396</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>141</v>
-      </c>
       <c r="L14" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="M14" s="1" t="s">
         <v>409</v>
@@ -9883,51 +9914,51 @@
         <v>432</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="Q14" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="Q14" s="5" t="s">
         <v>409</v>
       </c>
-      <c r="R14" s="1" t="s">
+      <c r="R14" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="S14" s="1" t="s">
+      <c r="S14" s="5" t="s">
         <v>432</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="U14" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="U14" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="V14" s="6" t="s">
+      <c r="V14" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="W14" s="6" t="s">
+      <c r="W14" s="1" t="s">
         <v>432</v>
       </c>
       <c r="X14" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="Y14" s="6" t="s">
+      <c r="Y14" s="5" t="s">
         <v>409</v>
       </c>
-      <c r="Z14" s="6" t="s">
+      <c r="Z14" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="AA14" s="6" t="s">
+      <c r="AA14" s="5" t="s">
         <v>432</v>
       </c>
       <c r="AB14" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="AC14" s="6" t="s">
+      <c r="AC14" s="5" t="s">
         <v>409</v>
       </c>
-      <c r="AD14" s="6" t="s">
+      <c r="AD14" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="AE14" s="6" t="s">
+      <c r="AE14" s="5" t="s">
         <v>432</v>
       </c>
     </row>
@@ -9942,22 +9973,22 @@
         <v>403</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>223</v>
+        <v>140</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="H15" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>141</v>
-      </c>
       <c r="L15" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>223</v>
@@ -9969,7 +10000,7 @@
         <v>433</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="Q15" s="1" t="s">
         <v>223</v>
@@ -9981,7 +10012,7 @@
         <v>433</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="U15" s="1" t="s">
         <v>223</v>

</xml_diff>

<commit_message>
Data labelled for chapter 4 & 5
</commit_message>
<xml_diff>
--- a/dataset/testing.xlsx
+++ b/dataset/testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajed/PycharmProjects/Study-on-ChatGPT/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC6B576-7C8D-0B40-A4BC-0B5A96A35F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11EB56B6-F4CB-9842-8FC7-659D2F51E4C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ch1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1267" uniqueCount="510">
   <si>
     <t>id</t>
   </si>
@@ -5881,42 +5881,6 @@
 In this example, I used the Test-Driven Development (TDD) approach to add additional functionality to the Calc class. First, I created a failing test for one of the new functionalities (subtraction), then I modified the Calc class until the test passed. After that, I performed any refactoring needed and repeated the process for the remaining functionalities (multiplication and division). Finally, I submitted printouts of all tests, my final version of Calc, and a screenshot showing that all tests passed.</t>
   </si>
   <si>
-    <t>I'm sorry, I am unable to submit printouts or screenshots as I am a text-based AI. However, I can guide you through the process of Test-Driven Development (TDD) for the Calc class.
-1. Create a failing test for subtraction: 
-```
-@Test
-public void testSubtract() {
-    assertEquals(5, Calc.subtract(10, 5));
-}
-```
-2. Modify the Calc class to include the subtract method:
-```
-static public int subtract (int a, int b) {
-    return a - b;
-}
-```
-3. Run the test and ensure it passes.
-4. Repeat steps 1-3 for the multiply and divide methods.
-5. Test for divide by zero case
-```
-@Test
-public void testDivideByZero() {
-    assertThrows(ArithmeticException.class, () -&gt; Calc.divide(10, 0));
-}
-```
-6. Modify the Calc class to handle divide by zero case
-```
-static public double divide (int a, int b) {
-    if(b==0)
-    throw new ArithmeticException();
-    return (double) a / b;
-}
-```
-7. Run the test and ensure it passes.
-8. Refactor the code if necessary to improve readability and maintainability.
-At the end of the process, you should have a Calc class that implements the add, subtract, multiply, and divide methods and has passing tests for each of these functionalities.</t>
-  </si>
-  <si>
     <t>Test 1: Subtraction
 1. Create a failing test for the subtraction method by adding the following test case to the test file:
 ```
@@ -6309,12 +6273,98 @@
     <t xml:space="preserve">No, T2 does not necessarily satisfy C1. If C1 subsumes C2, it means that C1 is a stronger or more comprehensive criterion than C2. Therefore, a test set that satisfies C2 may not satisfy all the requirements of C1. For example, C1 may require testing for additional edge cases or input conditions that are not covered by C2. Therefore, even though T1 satisfies C1 and T2 satisfies C2 on program P, T2 may not satisfy all the requirements of C1.
 </t>
   </si>
+  <si>
+    <t>Shows where to add screen prinouts</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>Just says screenshot is not available.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Step by step answer.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Better than book solution</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Handles division by zero
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Book Solution do not say anything about division by zero</t>
+    </r>
+  </si>
+  <si>
+    <t>Detailed instruction for travis CI</t>
+  </si>
+  <si>
+    <t>Partially correct because it explains the necessary steps to build the CI sever first.
+Does not talk about static analysis or code coverage</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Partially correct because it explains the necessary steps to build the CI sever first.
+Does not talk about static analysis or code coverage
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Incomplete response</t>
+    </r>
+  </si>
+  <si>
+    <t>Did not find any project.
+Just talked about the general steps.
+Expected code</t>
+  </si>
+  <si>
+    <t>Does not demonstrate any faulty code or any failed test</t>
+  </si>
+  <si>
+    <t>Acknowleges inability to run/print code</t>
+  </si>
+  <si>
+    <t>Understands what subsume means. But makes logical error in decision.</t>
+  </si>
+  <si>
+    <t>Does not say that C1 is stronger than C2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -6334,6 +6384,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="3">
@@ -6707,7 +6762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -9382,7 +9437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AB15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F1" sqref="F1:H1048576"/>
     </sheetView>
   </sheetViews>
@@ -10260,8 +10315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AB6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10270,17 +10325,24 @@
     <col min="3" max="3" width="32.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="47.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="44.33203125" style="1" customWidth="1"/>
-    <col min="6" max="8" width="8.83203125" style="1"/>
+    <col min="6" max="7" width="8.83203125" style="1"/>
+    <col min="8" max="8" width="20" style="1" customWidth="1"/>
     <col min="9" max="9" width="47" style="1" customWidth="1"/>
-    <col min="10" max="12" width="8.83203125" style="1"/>
+    <col min="10" max="11" width="8.83203125" style="1"/>
+    <col min="12" max="12" width="23.83203125" style="1" customWidth="1"/>
     <col min="13" max="13" width="48.33203125" style="1" customWidth="1"/>
-    <col min="14" max="16" width="8.83203125" style="1"/>
+    <col min="14" max="15" width="8.83203125" style="1"/>
+    <col min="16" max="16" width="23.1640625" style="1" customWidth="1"/>
     <col min="17" max="17" width="42.1640625" style="1" customWidth="1"/>
-    <col min="18" max="20" width="8.83203125" style="1"/>
+    <col min="18" max="19" width="8.83203125" style="1"/>
+    <col min="20" max="20" width="21.33203125" style="1" customWidth="1"/>
     <col min="21" max="21" width="55" style="1" customWidth="1"/>
-    <col min="22" max="24" width="8.83203125" style="1"/>
+    <col min="22" max="23" width="8.83203125" style="1"/>
+    <col min="24" max="24" width="23.1640625" style="1" customWidth="1"/>
     <col min="25" max="25" width="48.33203125" style="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.83203125" style="1"/>
+    <col min="26" max="27" width="8.83203125" style="1"/>
+    <col min="28" max="28" width="26.5" style="1" customWidth="1"/>
+    <col min="29" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="68" customHeight="1" x14ac:dyDescent="0.2">
@@ -10382,46 +10444,136 @@
       <c r="E2" s="1" t="s">
         <v>450</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="I2" s="1" t="s">
         <v>451</v>
       </c>
+      <c r="J2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="M2" s="1" t="s">
         <v>452</v>
       </c>
+      <c r="N2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>507</v>
+      </c>
       <c r="Q2" s="1" t="s">
         <v>453</v>
       </c>
+      <c r="R2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>497</v>
+      </c>
       <c r="U2" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="Y2" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="Y2" s="1" t="s">
-        <v>455</v>
+      <c r="Z2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>499</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" ht="408" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="U3" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="V3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y3" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="Y3" s="1" t="s">
-        <v>462</v>
+      <c r="Z3" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="409.6" x14ac:dyDescent="0.2">
@@ -10429,25 +10581,79 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="U4" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="V4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>504</v>
+      </c>
+      <c r="Y4" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="Y4" s="1" t="s">
-        <v>468</v>
+      <c r="Z4" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="409.6" x14ac:dyDescent="0.2">
@@ -10455,25 +10661,79 @@
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="N5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="Q5" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="R5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="U5" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="V5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="W5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="Y5" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="Y5" s="1" t="s">
-        <v>475</v>
+      <c r="Z5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB5" s="4" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="409.6" x14ac:dyDescent="0.2">
@@ -10481,25 +10741,79 @@
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="Q6" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="R6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="U6" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="V6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="Y6" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="Y6" s="1" t="s">
-        <v>482</v>
+      <c r="Z6" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA6" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB6" s="4" t="s">
+        <v>506</v>
       </c>
     </row>
   </sheetData>
@@ -10511,8 +10825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AB3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="Z3" sqref="Z3:AA3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10523,7 +10837,8 @@
     <col min="5" max="5" width="44" style="1" customWidth="1"/>
     <col min="6" max="8" width="8.83203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="46.33203125" style="1" customWidth="1"/>
-    <col min="10" max="12" width="8.83203125" style="1" customWidth="1"/>
+    <col min="10" max="11" width="8.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16" style="1" customWidth="1"/>
     <col min="13" max="13" width="50.33203125" style="1" customWidth="1"/>
     <col min="14" max="16" width="8.83203125" style="1" customWidth="1"/>
     <col min="17" max="17" width="56.33203125" style="1" customWidth="1"/>
@@ -10629,28 +10944,79 @@
         <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="Y2" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="Y2" s="1" t="s">
-        <v>490</v>
+      <c r="Z2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="388" customHeight="1" x14ac:dyDescent="0.2">
@@ -10661,28 +11027,67 @@
         <v>37</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="U3" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="V3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y3" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="Y3" s="1" t="s">
-        <v>497</v>
+      <c r="Z3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Included chapter 4&5 answers
</commit_message>
<xml_diff>
--- a/dataset/testing.xlsx
+++ b/dataset/testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajed/PycharmProjects/Study-on-ChatGPT/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11EB56B6-F4CB-9842-8FC7-659D2F51E4C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6577ED0-7057-984A-9C9B-ABFCC5E28C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ch1" sheetId="1" r:id="rId1"/>
@@ -6762,7 +6762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -10431,7 +10431,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -10656,7 +10656,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -10736,7 +10736,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -10825,8 +10825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AB3"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="Z3" sqref="Z3:AA3"/>
+    <sheetView tabSelected="1" topLeftCell="R2" workbookViewId="0">
+      <selection activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Changed the testing.xlsx with Suzzana's opinion
</commit_message>
<xml_diff>
--- a/dataset/testing.xlsx
+++ b/dataset/testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajed/PycharmProjects/Study-on-ChatGPT/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6577ED0-7057-984A-9C9B-ABFCC5E28C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737CC19D-9144-344A-AB2E-E10FC511588D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ch1" sheetId="1" r:id="rId1"/>
@@ -6277,9 +6277,6 @@
     <t>Shows where to add screen prinouts</t>
   </si>
   <si>
-    <t>w</t>
-  </si>
-  <si>
     <t>Just says screenshot is not available.</t>
   </si>
   <si>
@@ -6358,6 +6355,42 @@
   </si>
   <si>
     <t>Does not say that C1 is stronger than C2</t>
+  </si>
+  <si>
+    <t>I'm sorry, I am unable to submit printouts or screenshots as I am a text-based AI. However, I can guide you through the process of Test-Driven Development (TDD) for the Calc class.
+1. Create a failing test for subtraction: 
+```
+@Test
+public void testSubtract() {
+    assertEquals(5, Calc.subtract(10, 5));
+}
+```
+2. Modify the Calc class to include the subtract method:
+```
+static public int subtract (int a, int b) {
+    return a - b;
+}
+```
+3. Run the test and ensure it passes.
+4. Repeat steps 1-3 for the multiply and divide methods.
+5. Test for divide by zero case
+```
+@Test
+public void testDivideByZero() {
+    assertThrows(ArithmeticException.class, () -&gt; Calc.divide(10, 0));
+}
+```
+6. Modify the Calc class to handle divide by zero case
+```
+static public double divide (int a, int b) {
+    if(b==0)
+    throw new ArithmeticException();
+    return (double) a / b;
+}
+```
+7. Run the test and ensure it passes.
+8. Refactor the code if necessary to improve readability and maintainability.
+At the end of the process, you should have a Calc class that implements the add, subtract, multiply, and divide methods and has passing tests for each of these functionalities.</t>
   </si>
 </sst>
 </file>
@@ -6762,8 +6795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9437,8 +9470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AB15"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:H1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10315,8 +10348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AB6"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView topLeftCell="I2" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10431,7 +10464,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -10469,7 +10502,7 @@
         <v>83</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>453</v>
@@ -10484,7 +10517,7 @@
         <v>497</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>498</v>
+        <v>509</v>
       </c>
       <c r="V2" s="1" t="s">
         <v>82</v>
@@ -10493,7 +10526,7 @@
         <v>83</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="Y2" s="1" t="s">
         <v>454</v>
@@ -10505,7 +10538,7 @@
         <v>83</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="408" customHeight="1" x14ac:dyDescent="0.2">
@@ -10525,7 +10558,7 @@
         <v>83</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>457</v>
@@ -10573,7 +10606,7 @@
         <v>83</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="409.6" x14ac:dyDescent="0.2">
@@ -10593,7 +10626,7 @@
         <v>80</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>463</v>
@@ -10605,7 +10638,7 @@
         <v>80</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>464</v>
@@ -10617,7 +10650,7 @@
         <v>80</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>465</v>
@@ -10629,7 +10662,7 @@
         <v>80</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="U4" s="1" t="s">
         <v>466</v>
@@ -10641,7 +10674,7 @@
         <v>80</v>
       </c>
       <c r="X4" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="Y4" s="1" t="s">
         <v>467</v>
@@ -10653,7 +10686,7 @@
         <v>80</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="409.5" x14ac:dyDescent="0.2">
@@ -10673,7 +10706,7 @@
         <v>80</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>470</v>
@@ -10685,7 +10718,7 @@
         <v>80</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>471</v>
@@ -10697,7 +10730,7 @@
         <v>80</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>472</v>
@@ -10709,7 +10742,7 @@
         <v>80</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="U5" s="1" t="s">
         <v>473</v>
@@ -10721,7 +10754,7 @@
         <v>80</v>
       </c>
       <c r="X5" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="Y5" s="1" t="s">
         <v>474</v>
@@ -10733,7 +10766,7 @@
         <v>80</v>
       </c>
       <c r="AB5" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="409.5" x14ac:dyDescent="0.2">
@@ -10753,7 +10786,7 @@
         <v>80</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>477</v>
@@ -10765,7 +10798,7 @@
         <v>80</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>478</v>
@@ -10777,7 +10810,7 @@
         <v>80</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>479</v>
@@ -10789,7 +10822,7 @@
         <v>80</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="U6" s="1" t="s">
         <v>480</v>
@@ -10801,7 +10834,7 @@
         <v>80</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="Y6" s="1" t="s">
         <v>481</v>
@@ -10813,7 +10846,7 @@
         <v>80</v>
       </c>
       <c r="AB6" s="4" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
   </sheetData>
@@ -10825,7 +10858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AB3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
@@ -10968,7 +11001,7 @@
         <v>80</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>486</v>
@@ -10980,7 +11013,7 @@
         <v>80</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>487</v>
@@ -10992,7 +11025,7 @@
         <v>80</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="U2" s="1" t="s">
         <v>488</v>
@@ -11004,7 +11037,7 @@
         <v>80</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y2" s="1" t="s">
         <v>489</v>
@@ -11016,7 +11049,7 @@
         <v>80</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="388" customHeight="1" x14ac:dyDescent="0.2">
@@ -11051,7 +11084,7 @@
         <v>83</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>493</v>

</xml_diff>